<commit_message>
Add data for 2024-11-25
</commit_message>
<xml_diff>
--- a/マイジャグラーV_塗りつぶし済み.xlsx
+++ b/マイジャグラーV_塗りつぶし済み.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BY53"/>
+  <dimension ref="A1:BZ53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -516,6 +516,7 @@
     <col width="12" customWidth="1" min="75" max="75"/>
     <col width="12" customWidth="1" min="76" max="76"/>
     <col width="12" customWidth="1" min="77" max="77"/>
+    <col width="12" customWidth="1" min="78" max="78"/>
   </cols>
   <sheetData>
     <row r="1" ht="20" customHeight="1">
@@ -904,6 +905,11 @@
           <t>2024/11/24</t>
         </is>
       </c>
+      <c r="BZ1" s="1" t="inlineStr">
+        <is>
+          <t>2024/11/25</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="20" customHeight="1">
       <c r="A2" s="1" t="n">
@@ -1137,6 +1143,9 @@
       <c r="BY2" s="1" t="n">
         <v>207.1</v>
       </c>
+      <c r="BZ2" s="2" t="n">
+        <v>103.4</v>
+      </c>
     </row>
     <row r="3" ht="20" customHeight="1">
       <c r="A3" s="1" t="n">
@@ -1370,6 +1379,9 @@
       <c r="BY3" s="2" t="n">
         <v>120.9</v>
       </c>
+      <c r="BZ3" s="3" t="n">
+        <v>130.3</v>
+      </c>
     </row>
     <row r="4" ht="20" customHeight="1">
       <c r="A4" s="1" t="n">
@@ -1603,6 +1615,9 @@
       <c r="BY4" s="1" t="n">
         <v>165.4</v>
       </c>
+      <c r="BZ4" s="1" t="n">
+        <v>140.1</v>
+      </c>
     </row>
     <row r="5" ht="20" customHeight="1">
       <c r="A5" s="1" t="n">
@@ -1836,6 +1851,9 @@
       <c r="BY5" s="1" t="n">
         <v>218.6</v>
       </c>
+      <c r="BZ5" s="1" t="n">
+        <v>177</v>
+      </c>
     </row>
     <row r="6" ht="20" customHeight="1">
       <c r="A6" s="1" t="n">
@@ -2069,6 +2087,9 @@
       <c r="BY6" s="1" t="n">
         <v>180</v>
       </c>
+      <c r="BZ6" s="1" t="n">
+        <v>151.8</v>
+      </c>
     </row>
     <row r="7" ht="20" customHeight="1">
       <c r="A7" s="1" t="n">
@@ -2302,6 +2323,9 @@
       <c r="BY7" s="1" t="n">
         <v>142.4</v>
       </c>
+      <c r="BZ7" s="1" t="n">
+        <v>152.8</v>
+      </c>
     </row>
     <row r="8" ht="20" customHeight="1">
       <c r="A8" s="1" t="n">
@@ -2535,6 +2559,9 @@
       <c r="BY8" s="1" t="n">
         <v>144.3</v>
       </c>
+      <c r="BZ8" s="1" t="n">
+        <v>158.8</v>
+      </c>
     </row>
     <row r="9" ht="20" customHeight="1">
       <c r="A9" s="1" t="n">
@@ -2768,6 +2795,9 @@
       <c r="BY9" s="3" t="n">
         <v>130.9</v>
       </c>
+      <c r="BZ9" s="1" t="n">
+        <v>159.3</v>
+      </c>
     </row>
     <row r="10" ht="20" customHeight="1">
       <c r="A10" s="1" t="n">
@@ -3001,6 +3031,9 @@
       <c r="BY10" s="1" t="n">
         <v>147.6</v>
       </c>
+      <c r="BZ10" s="3" t="n">
+        <v>127.3</v>
+      </c>
     </row>
     <row r="11" ht="20" customHeight="1">
       <c r="A11" s="1" t="n">
@@ -3234,6 +3267,9 @@
       <c r="BY11" s="1" t="n">
         <v>201.3</v>
       </c>
+      <c r="BZ11" s="1" t="n">
+        <v>313.9</v>
+      </c>
     </row>
     <row r="12" ht="20" customHeight="1">
       <c r="A12" s="1" t="n">
@@ -3467,6 +3503,9 @@
       <c r="BY12" s="1" t="n">
         <v>163.8</v>
       </c>
+      <c r="BZ12" s="1" t="n">
+        <v>162.4</v>
+      </c>
     </row>
     <row r="13" ht="20" customHeight="1">
       <c r="A13" s="1" t="n">
@@ -3700,6 +3739,9 @@
       <c r="BY13" s="1" t="n">
         <v>175.2</v>
       </c>
+      <c r="BZ13" s="2" t="n">
+        <v>117.1</v>
+      </c>
     </row>
     <row r="14" ht="20" customHeight="1">
       <c r="A14" s="1" t="n">
@@ -3933,6 +3975,9 @@
       <c r="BY14" s="1" t="n">
         <v>141.1</v>
       </c>
+      <c r="BZ14" s="1" t="n">
+        <v>144.3</v>
+      </c>
     </row>
     <row r="15" ht="20" customHeight="1">
       <c r="A15" s="1" t="n">
@@ -4166,6 +4211,9 @@
       <c r="BY15" s="1" t="n">
         <v>196.2</v>
       </c>
+      <c r="BZ15" s="1" t="n">
+        <v>156.1</v>
+      </c>
     </row>
     <row r="16" ht="20" customHeight="1">
       <c r="A16" s="1" t="n">
@@ -4399,6 +4447,9 @@
       <c r="BY16" s="2" t="n">
         <v>124.3</v>
       </c>
+      <c r="BZ16" s="2" t="n">
+        <v>121.6</v>
+      </c>
     </row>
     <row r="17" ht="20" customHeight="1">
       <c r="A17" s="1" t="n">
@@ -4632,6 +4683,9 @@
       <c r="BY17" s="1" t="n">
         <v>207.1</v>
       </c>
+      <c r="BZ17" s="3" t="n">
+        <v>130.1</v>
+      </c>
     </row>
     <row r="18" ht="20" customHeight="1">
       <c r="A18" s="1" t="n">
@@ -4865,6 +4919,9 @@
       <c r="BY18" s="1" t="n">
         <v>170.9</v>
       </c>
+      <c r="BZ18" s="1" t="n">
+        <v>290.9</v>
+      </c>
     </row>
     <row r="19" ht="20" customHeight="1">
       <c r="A19" s="1" t="n">
@@ -5098,6 +5155,9 @@
       <c r="BY19" s="2" t="n">
         <v>123.4</v>
       </c>
+      <c r="BZ19" s="2" t="n">
+        <v>114.3</v>
+      </c>
     </row>
     <row r="20" ht="20" customHeight="1">
       <c r="A20" s="1" t="n">
@@ -5331,6 +5391,9 @@
       <c r="BY20" s="1" t="n">
         <v>149.9</v>
       </c>
+      <c r="BZ20" s="1" t="n">
+        <v>187.7</v>
+      </c>
     </row>
     <row r="21" ht="20" customHeight="1">
       <c r="A21" s="1" t="n">
@@ -5564,6 +5627,9 @@
       <c r="BY21" s="1" t="n">
         <v>215.3</v>
       </c>
+      <c r="BZ21" s="2" t="n">
+        <v>120.1</v>
+      </c>
     </row>
     <row r="22" ht="20" customHeight="1">
       <c r="A22" s="1" t="n">
@@ -5797,6 +5863,9 @@
       <c r="BY22" s="3" t="n">
         <v>125.8</v>
       </c>
+      <c r="BZ22" s="3" t="n">
+        <v>134.3</v>
+      </c>
     </row>
     <row r="23" ht="20" customHeight="1">
       <c r="A23" s="1" t="n">
@@ -6030,6 +6099,9 @@
       <c r="BY23" s="3" t="n">
         <v>133.1</v>
       </c>
+      <c r="BZ23" s="1" t="n">
+        <v>179.8</v>
+      </c>
     </row>
     <row r="24" ht="20" customHeight="1">
       <c r="A24" s="1" t="n">
@@ -6263,6 +6335,9 @@
       <c r="BY24" s="3" t="n">
         <v>128.9</v>
       </c>
+      <c r="BZ24" s="1" t="n">
+        <v>167.4</v>
+      </c>
     </row>
     <row r="25" ht="20" customHeight="1">
       <c r="A25" s="1" t="n">
@@ -6496,6 +6571,9 @@
       <c r="BY25" s="2" t="n">
         <v>124.9</v>
       </c>
+      <c r="BZ25" s="3" t="n">
+        <v>133.2</v>
+      </c>
     </row>
     <row r="26" ht="20" customHeight="1">
       <c r="A26" s="1" t="n">
@@ -6729,6 +6807,9 @@
       <c r="BY26" s="1" t="n">
         <v>164.2</v>
       </c>
+      <c r="BZ26" s="1" t="n">
+        <v>147</v>
+      </c>
     </row>
     <row r="27" ht="20" customHeight="1">
       <c r="A27" s="1" t="n">
@@ -6962,6 +7043,9 @@
       <c r="BY27" s="1" t="n">
         <v>186.1</v>
       </c>
+      <c r="BZ27" s="1" t="n">
+        <v>180.7</v>
+      </c>
     </row>
     <row r="28" ht="20" customHeight="1">
       <c r="A28" s="1" t="n">
@@ -7195,6 +7279,9 @@
       <c r="BY28" s="1" t="n">
         <v>163</v>
       </c>
+      <c r="BZ28" s="1" t="n">
+        <v>155.4</v>
+      </c>
     </row>
     <row r="29" ht="20" customHeight="1">
       <c r="A29" s="1" t="n">
@@ -7428,6 +7515,9 @@
       <c r="BY29" s="1" t="n">
         <v>237.6</v>
       </c>
+      <c r="BZ29" s="1" t="n">
+        <v>144.6</v>
+      </c>
     </row>
     <row r="30" ht="20" customHeight="1">
       <c r="A30" s="1" t="n">
@@ -7661,6 +7751,9 @@
       <c r="BY30" s="1" t="n">
         <v>175.4</v>
       </c>
+      <c r="BZ30" s="1" t="n">
+        <v>155.5</v>
+      </c>
     </row>
     <row r="31" ht="20" customHeight="1">
       <c r="A31" s="1" t="n">
@@ -7894,6 +7987,9 @@
       <c r="BY31" s="1" t="n">
         <v>175.2</v>
       </c>
+      <c r="BZ31" s="1" t="n">
+        <v>147.4</v>
+      </c>
     </row>
     <row r="32" ht="20" customHeight="1">
       <c r="A32" s="1" t="n">
@@ -8127,6 +8223,9 @@
       <c r="BY32" s="3" t="n">
         <v>133.2</v>
       </c>
+      <c r="BZ32" s="1" t="n">
+        <v>150.6</v>
+      </c>
     </row>
     <row r="33" ht="20" customHeight="1">
       <c r="A33" s="1" t="n">
@@ -8360,6 +8459,9 @@
       <c r="BY33" s="1" t="n">
         <v>144.4</v>
       </c>
+      <c r="BZ33" s="1" t="n">
+        <v>155.1</v>
+      </c>
     </row>
     <row r="34" ht="20" customHeight="1">
       <c r="A34" s="1" t="n">
@@ -8593,6 +8695,9 @@
       <c r="BY34" s="1" t="n">
         <v>156.2</v>
       </c>
+      <c r="BZ34" s="1" t="n">
+        <v>146.6</v>
+      </c>
     </row>
     <row r="35" ht="20" customHeight="1">
       <c r="A35" s="1" t="n">
@@ -8826,6 +8931,9 @@
       <c r="BY35" s="2" t="n">
         <v>113</v>
       </c>
+      <c r="BZ35" s="1" t="n">
+        <v>141.9</v>
+      </c>
     </row>
     <row r="36" ht="20" customHeight="1">
       <c r="A36" s="1" t="n">
@@ -9059,6 +9167,9 @@
       <c r="BY36" s="1" t="n">
         <v>181.1</v>
       </c>
+      <c r="BZ36" s="1" t="n">
+        <v>141.6</v>
+      </c>
     </row>
     <row r="37" ht="20" customHeight="1">
       <c r="A37" s="1" t="n">
@@ -9292,6 +9403,9 @@
       <c r="BY37" s="1" t="n">
         <v>168.9</v>
       </c>
+      <c r="BZ37" s="2" t="n">
+        <v>119.4</v>
+      </c>
     </row>
     <row r="38" ht="20" customHeight="1">
       <c r="A38" s="1" t="n">
@@ -9525,6 +9639,9 @@
       <c r="BY38" s="1" t="n">
         <v>152.7</v>
       </c>
+      <c r="BZ38" s="1" t="n">
+        <v>193.4</v>
+      </c>
     </row>
     <row r="39" ht="20" customHeight="1">
       <c r="A39" s="1" t="n">
@@ -9758,6 +9875,9 @@
       <c r="BY39" s="1" t="n">
         <v>185.1</v>
       </c>
+      <c r="BZ39" s="3" t="n">
+        <v>132.5</v>
+      </c>
     </row>
     <row r="40" ht="20" customHeight="1">
       <c r="A40" s="1" t="n">
@@ -9991,6 +10111,9 @@
       <c r="BY40" s="1" t="n">
         <v>232.8</v>
       </c>
+      <c r="BZ40" s="3" t="n">
+        <v>132.4</v>
+      </c>
     </row>
     <row r="41" ht="20" customHeight="1">
       <c r="A41" s="1" t="n">
@@ -10224,6 +10347,9 @@
       <c r="BY41" s="3" t="n">
         <v>136.6</v>
       </c>
+      <c r="BZ41" s="3" t="n">
+        <v>135.5</v>
+      </c>
     </row>
     <row r="42" ht="20" customHeight="1">
       <c r="A42" s="1" t="n">
@@ -10457,6 +10583,9 @@
       <c r="BY42" s="1" t="n">
         <v>151.6</v>
       </c>
+      <c r="BZ42" s="3" t="n">
+        <v>134.7</v>
+      </c>
     </row>
     <row r="43" ht="20" customHeight="1">
       <c r="A43" s="1" t="n">
@@ -10690,6 +10819,9 @@
       <c r="BY43" s="1" t="n">
         <v>140.1</v>
       </c>
+      <c r="BZ43" s="1" t="n">
+        <v>220.8</v>
+      </c>
     </row>
     <row r="44" ht="20" customHeight="1">
       <c r="A44" s="1" t="n">
@@ -10923,6 +11055,9 @@
       <c r="BY44" s="3" t="n">
         <v>139.6</v>
       </c>
+      <c r="BZ44" s="2" t="n">
+        <v>118.7</v>
+      </c>
     </row>
     <row r="45" ht="20" customHeight="1">
       <c r="A45" s="1" t="n">
@@ -11156,6 +11291,9 @@
       <c r="BY45" s="1" t="n">
         <v>180.3</v>
       </c>
+      <c r="BZ45" s="1" t="n">
+        <v>232.6</v>
+      </c>
     </row>
     <row r="46" ht="20" customHeight="1">
       <c r="A46" s="1" t="n">
@@ -11389,6 +11527,9 @@
       <c r="BY46" s="1" t="n">
         <v>149</v>
       </c>
+      <c r="BZ46" s="1" t="n">
+        <v>175.4</v>
+      </c>
     </row>
     <row r="47" ht="20" customHeight="1">
       <c r="A47" s="1" t="n">
@@ -11622,6 +11763,9 @@
       <c r="BY47" s="1" t="n">
         <v>164.2</v>
       </c>
+      <c r="BZ47" s="1" t="n">
+        <v>156</v>
+      </c>
     </row>
     <row r="48" ht="20" customHeight="1">
       <c r="A48" s="1" t="n">
@@ -11855,6 +11999,9 @@
       <c r="BY48" s="1" t="n">
         <v>181.7</v>
       </c>
+      <c r="BZ48" s="3" t="n">
+        <v>133.5</v>
+      </c>
     </row>
     <row r="49" ht="20" customHeight="1">
       <c r="A49" s="1" t="n">
@@ -12088,6 +12235,9 @@
       <c r="BY49" s="1" t="n">
         <v>163</v>
       </c>
+      <c r="BZ49" s="2" t="n">
+        <v>114.7</v>
+      </c>
     </row>
     <row r="50" ht="20" customHeight="1">
       <c r="A50" s="1" t="n">
@@ -12321,6 +12471,9 @@
       <c r="BY50" s="2" t="n">
         <v>111.8</v>
       </c>
+      <c r="BZ50" s="1" t="n">
+        <v>163.7</v>
+      </c>
     </row>
     <row r="51" ht="20" customHeight="1">
       <c r="A51" s="1" t="n">
@@ -12554,6 +12707,9 @@
       <c r="BY51" s="3" t="n">
         <v>139.2</v>
       </c>
+      <c r="BZ51" s="3" t="n">
+        <v>136.7</v>
+      </c>
     </row>
     <row r="52" ht="20" customHeight="1">
       <c r="A52" s="1" t="n">
@@ -12787,6 +12943,9 @@
       <c r="BY52" s="2" t="n">
         <v>122.9</v>
       </c>
+      <c r="BZ52" s="1" t="n">
+        <v>174.4</v>
+      </c>
     </row>
     <row r="53" ht="20" customHeight="1">
       <c r="A53" s="1" t="n">
@@ -13019,6 +13178,9 @@
       </c>
       <c r="BY53" s="1" t="n">
         <v>159.9</v>
+      </c>
+      <c r="BZ53" s="2" t="n">
+        <v>95.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2024-12-06
</commit_message>
<xml_diff>
--- a/マイジャグラーV_塗りつぶし済み.xlsx
+++ b/マイジャグラーV_塗りつぶし済み.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:CJ53"/>
+  <dimension ref="A1:CK53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -527,6 +527,7 @@
     <col width="12" customWidth="1" min="86" max="86"/>
     <col width="12" customWidth="1" min="87" max="87"/>
     <col width="12" customWidth="1" min="88" max="88"/>
+    <col width="12" customWidth="1" min="89" max="89"/>
   </cols>
   <sheetData>
     <row r="1" ht="20" customHeight="1">
@@ -970,6 +971,11 @@
           <t>2024/12/05</t>
         </is>
       </c>
+      <c r="CK1" s="1" t="inlineStr">
+        <is>
+          <t>2024/12/06</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="20" customHeight="1">
       <c r="A2" s="1" t="n">
@@ -1236,6 +1242,9 @@
       <c r="CJ2" s="3" t="n">
         <v>134.8</v>
       </c>
+      <c r="CK2" s="1" t="n">
+        <v>152.3</v>
+      </c>
     </row>
     <row r="3" ht="20" customHeight="1">
       <c r="A3" s="1" t="n">
@@ -1502,6 +1511,9 @@
       <c r="CJ3" s="1" t="n">
         <v>217.6</v>
       </c>
+      <c r="CK3" s="1" t="n">
+        <v>177.1</v>
+      </c>
     </row>
     <row r="4" ht="20" customHeight="1">
       <c r="A4" s="1" t="n">
@@ -1768,6 +1780,9 @@
       <c r="CJ4" s="3" t="n">
         <v>136.9</v>
       </c>
+      <c r="CK4" s="1" t="n">
+        <v>153.3</v>
+      </c>
     </row>
     <row r="5" ht="20" customHeight="1">
       <c r="A5" s="1" t="n">
@@ -2034,6 +2049,9 @@
       <c r="CJ5" s="1" t="n">
         <v>143.3</v>
       </c>
+      <c r="CK5" s="1" t="n">
+        <v>163</v>
+      </c>
     </row>
     <row r="6" ht="20" customHeight="1">
       <c r="A6" s="1" t="n">
@@ -2300,6 +2318,9 @@
       <c r="CJ6" s="2" t="n">
         <v>113.5</v>
       </c>
+      <c r="CK6" s="3" t="n">
+        <v>127.2</v>
+      </c>
     </row>
     <row r="7" ht="20" customHeight="1">
       <c r="A7" s="1" t="n">
@@ -2566,6 +2587,9 @@
       <c r="CJ7" s="1" t="n">
         <v>183.1</v>
       </c>
+      <c r="CK7" s="1" t="n">
+        <v>191.7</v>
+      </c>
     </row>
     <row r="8" ht="20" customHeight="1">
       <c r="A8" s="1" t="n">
@@ -2832,6 +2856,9 @@
       <c r="CJ8" s="2" t="n">
         <v>109.6</v>
       </c>
+      <c r="CK8" s="3" t="n">
+        <v>136.9</v>
+      </c>
     </row>
     <row r="9" ht="20" customHeight="1">
       <c r="A9" s="1" t="n">
@@ -3098,6 +3125,9 @@
       <c r="CJ9" s="1" t="n">
         <v>212.5</v>
       </c>
+      <c r="CK9" s="1" t="n">
+        <v>143.1</v>
+      </c>
     </row>
     <row r="10" ht="20" customHeight="1">
       <c r="A10" s="1" t="n">
@@ -3364,6 +3394,9 @@
       <c r="CJ10" s="1" t="n">
         <v>151</v>
       </c>
+      <c r="CK10" s="1" t="n">
+        <v>163.2</v>
+      </c>
     </row>
     <row r="11" ht="20" customHeight="1">
       <c r="A11" s="1" t="n">
@@ -3630,6 +3663,9 @@
       <c r="CJ11" s="2" t="n">
         <v>123.3</v>
       </c>
+      <c r="CK11" s="1" t="n">
+        <v>480.3</v>
+      </c>
     </row>
     <row r="12" ht="20" customHeight="1">
       <c r="A12" s="1" t="n">
@@ -3896,6 +3932,9 @@
       <c r="CJ12" s="2" t="n">
         <v>119</v>
       </c>
+      <c r="CK12" s="1" t="n">
+        <v>166.8</v>
+      </c>
     </row>
     <row r="13" ht="20" customHeight="1">
       <c r="A13" s="1" t="n">
@@ -4162,6 +4201,9 @@
       <c r="CJ13" s="3" t="n">
         <v>127.3</v>
       </c>
+      <c r="CK13" s="1" t="n">
+        <v>154.5</v>
+      </c>
     </row>
     <row r="14" ht="20" customHeight="1">
       <c r="A14" s="1" t="n">
@@ -4428,6 +4470,9 @@
       <c r="CJ14" s="2" t="n">
         <v>124.9</v>
       </c>
+      <c r="CK14" s="2" t="n">
+        <v>123.9</v>
+      </c>
     </row>
     <row r="15" ht="20" customHeight="1">
       <c r="A15" s="1" t="n">
@@ -4694,6 +4739,9 @@
       <c r="CJ15" s="1" t="n">
         <v>161.9</v>
       </c>
+      <c r="CK15" s="3" t="n">
+        <v>136.5</v>
+      </c>
     </row>
     <row r="16" ht="20" customHeight="1">
       <c r="A16" s="1" t="n">
@@ -4960,6 +5008,9 @@
       <c r="CJ16" s="1" t="n">
         <v>173</v>
       </c>
+      <c r="CK16" s="3" t="n">
+        <v>133.2</v>
+      </c>
     </row>
     <row r="17" ht="20" customHeight="1">
       <c r="A17" s="1" t="n">
@@ -5226,6 +5277,9 @@
       <c r="CJ17" s="1" t="n">
         <v>141</v>
       </c>
+      <c r="CK17" s="1" t="n">
+        <v>236.6</v>
+      </c>
     </row>
     <row r="18" ht="20" customHeight="1">
       <c r="A18" s="1" t="n">
@@ -5492,6 +5546,9 @@
       <c r="CJ18" s="1" t="n">
         <v>154.9</v>
       </c>
+      <c r="CK18" s="2" t="n">
+        <v>106.5</v>
+      </c>
     </row>
     <row r="19" ht="20" customHeight="1">
       <c r="A19" s="1" t="n">
@@ -5758,6 +5815,9 @@
       <c r="CJ19" s="1" t="n">
         <v>161.5</v>
       </c>
+      <c r="CK19" s="1" t="n">
+        <v>154.2</v>
+      </c>
     </row>
     <row r="20" ht="20" customHeight="1">
       <c r="A20" s="1" t="n">
@@ -6024,6 +6084,9 @@
       <c r="CJ20" s="1" t="n">
         <v>148.6</v>
       </c>
+      <c r="CK20" s="1" t="n">
+        <v>201</v>
+      </c>
     </row>
     <row r="21" ht="20" customHeight="1">
       <c r="A21" s="1" t="n">
@@ -6290,6 +6353,9 @@
       <c r="CJ21" s="1" t="n">
         <v>141.8</v>
       </c>
+      <c r="CK21" s="1" t="n">
+        <v>156.7</v>
+      </c>
     </row>
     <row r="22" ht="20" customHeight="1">
       <c r="A22" s="1" t="n">
@@ -6556,6 +6622,9 @@
       <c r="CJ22" s="1" t="n">
         <v>154.7</v>
       </c>
+      <c r="CK22" s="1" t="n">
+        <v>158.5</v>
+      </c>
     </row>
     <row r="23" ht="20" customHeight="1">
       <c r="A23" s="1" t="n">
@@ -6822,6 +6891,9 @@
       <c r="CJ23" s="1" t="n">
         <v>188.7</v>
       </c>
+      <c r="CK23" s="1" t="n">
+        <v>224.1</v>
+      </c>
     </row>
     <row r="24" ht="20" customHeight="1">
       <c r="A24" s="1" t="n">
@@ -7088,6 +7160,9 @@
       <c r="CJ24" s="2" t="n">
         <v>114.8</v>
       </c>
+      <c r="CK24" s="1" t="n">
+        <v>147.9</v>
+      </c>
     </row>
     <row r="25" ht="20" customHeight="1">
       <c r="A25" s="1" t="n">
@@ -7354,6 +7429,9 @@
       <c r="CJ25" s="1" t="n">
         <v>163.4</v>
       </c>
+      <c r="CK25" s="1" t="n">
+        <v>189.4</v>
+      </c>
     </row>
     <row r="26" ht="20" customHeight="1">
       <c r="A26" s="1" t="n">
@@ -7620,6 +7698,9 @@
       <c r="CJ26" s="1" t="n">
         <v>146.3</v>
       </c>
+      <c r="CK26" s="1" t="n">
+        <v>162.5</v>
+      </c>
     </row>
     <row r="27" ht="20" customHeight="1">
       <c r="A27" s="1" t="n">
@@ -7886,6 +7967,9 @@
       <c r="CJ27" s="3" t="n">
         <v>138.8</v>
       </c>
+      <c r="CK27" s="1" t="n">
+        <v>261.3</v>
+      </c>
     </row>
     <row r="28" ht="20" customHeight="1">
       <c r="A28" s="1" t="n">
@@ -8152,6 +8236,9 @@
       <c r="CJ28" s="1" t="n">
         <v>151.7</v>
       </c>
+      <c r="CK28" s="1" t="n">
+        <v>140.9</v>
+      </c>
     </row>
     <row r="29" ht="20" customHeight="1">
       <c r="A29" s="1" t="n">
@@ -8418,6 +8505,9 @@
       <c r="CJ29" s="1" t="n">
         <v>150.1</v>
       </c>
+      <c r="CK29" s="2" t="n">
+        <v>108.7</v>
+      </c>
     </row>
     <row r="30" ht="20" customHeight="1">
       <c r="A30" s="1" t="n">
@@ -8684,6 +8774,9 @@
       <c r="CJ30" s="1" t="n">
         <v>151.3</v>
       </c>
+      <c r="CK30" s="1" t="n">
+        <v>164.5</v>
+      </c>
     </row>
     <row r="31" ht="20" customHeight="1">
       <c r="A31" s="1" t="n">
@@ -8950,6 +9043,9 @@
       <c r="CJ31" s="1" t="n">
         <v>140.3</v>
       </c>
+      <c r="CK31" s="1" t="n">
+        <v>144.4</v>
+      </c>
     </row>
     <row r="32" ht="20" customHeight="1">
       <c r="A32" s="1" t="n">
@@ -9216,6 +9312,9 @@
       <c r="CJ32" s="2" t="n">
         <v>122.3</v>
       </c>
+      <c r="CK32" s="1" t="n">
+        <v>209.3</v>
+      </c>
     </row>
     <row r="33" ht="20" customHeight="1">
       <c r="A33" s="1" t="n">
@@ -9482,6 +9581,9 @@
       <c r="CJ33" s="1" t="n">
         <v>143.4</v>
       </c>
+      <c r="CK33" s="1" t="n">
+        <v>158.2</v>
+      </c>
     </row>
     <row r="34" ht="20" customHeight="1">
       <c r="A34" s="1" t="n">
@@ -9748,6 +9850,9 @@
       <c r="CJ34" s="1" t="n">
         <v>155.9</v>
       </c>
+      <c r="CK34" s="2" t="n">
+        <v>118.2</v>
+      </c>
     </row>
     <row r="35" ht="20" customHeight="1">
       <c r="A35" s="1" t="n">
@@ -10014,6 +10119,9 @@
       <c r="CJ35" s="1" t="n">
         <v>160.4</v>
       </c>
+      <c r="CK35" s="1" t="n">
+        <v>247</v>
+      </c>
     </row>
     <row r="36" ht="20" customHeight="1">
       <c r="A36" s="1" t="n">
@@ -10280,6 +10388,9 @@
       <c r="CJ36" s="2" t="n">
         <v>118.8</v>
       </c>
+      <c r="CK36" s="2" t="n">
+        <v>113</v>
+      </c>
     </row>
     <row r="37" ht="20" customHeight="1">
       <c r="A37" s="1" t="n">
@@ -10546,6 +10657,9 @@
       <c r="CJ37" s="1" t="n">
         <v>178.7</v>
       </c>
+      <c r="CK37" s="1" t="n">
+        <v>249</v>
+      </c>
     </row>
     <row r="38" ht="20" customHeight="1">
       <c r="A38" s="1" t="n">
@@ -10812,6 +10926,9 @@
       <c r="CJ38" s="3" t="n">
         <v>130.5</v>
       </c>
+      <c r="CK38" s="1" t="n">
+        <v>168.9</v>
+      </c>
     </row>
     <row r="39" ht="20" customHeight="1">
       <c r="A39" s="1" t="n">
@@ -11078,6 +11195,9 @@
       <c r="CJ39" s="1" t="n">
         <v>162.7</v>
       </c>
+      <c r="CK39" s="3" t="n">
+        <v>127.3</v>
+      </c>
     </row>
     <row r="40" ht="20" customHeight="1">
       <c r="A40" s="1" t="n">
@@ -11344,6 +11464,9 @@
       <c r="CJ40" s="1" t="n">
         <v>150.9</v>
       </c>
+      <c r="CK40" s="3" t="n">
+        <v>138.4</v>
+      </c>
     </row>
     <row r="41" ht="20" customHeight="1">
       <c r="A41" s="1" t="n">
@@ -11610,6 +11733,9 @@
       <c r="CJ41" s="3" t="n">
         <v>134.4</v>
       </c>
+      <c r="CK41" s="1" t="n">
+        <v>170.4</v>
+      </c>
     </row>
     <row r="42" ht="20" customHeight="1">
       <c r="A42" s="1" t="n">
@@ -11876,6 +12002,9 @@
       <c r="CJ42" s="1" t="n">
         <v>171.1</v>
       </c>
+      <c r="CK42" s="1" t="n">
+        <v>240.5</v>
+      </c>
     </row>
     <row r="43" ht="20" customHeight="1">
       <c r="A43" s="1" t="n">
@@ -12142,6 +12271,9 @@
       <c r="CJ43" s="1" t="n">
         <v>156</v>
       </c>
+      <c r="CK43" s="3" t="n">
+        <v>138.5</v>
+      </c>
     </row>
     <row r="44" ht="20" customHeight="1">
       <c r="A44" s="1" t="n">
@@ -12408,6 +12540,9 @@
       <c r="CJ44" s="3" t="n">
         <v>128.1</v>
       </c>
+      <c r="CK44" s="3" t="n">
+        <v>128.4</v>
+      </c>
     </row>
     <row r="45" ht="20" customHeight="1">
       <c r="A45" s="1" t="n">
@@ -12674,6 +12809,9 @@
       <c r="CJ45" s="1" t="n">
         <v>170.6</v>
       </c>
+      <c r="CK45" s="3" t="n">
+        <v>128.9</v>
+      </c>
     </row>
     <row r="46" ht="20" customHeight="1">
       <c r="A46" s="1" t="n">
@@ -12940,6 +13078,9 @@
       <c r="CJ46" s="1" t="n">
         <v>207.1</v>
       </c>
+      <c r="CK46" s="1" t="n">
+        <v>207.4</v>
+      </c>
     </row>
     <row r="47" ht="20" customHeight="1">
       <c r="A47" s="1" t="n">
@@ -13206,6 +13347,9 @@
       <c r="CJ47" s="1" t="n">
         <v>158.9</v>
       </c>
+      <c r="CK47" s="1" t="n">
+        <v>174.1</v>
+      </c>
     </row>
     <row r="48" ht="20" customHeight="1">
       <c r="A48" s="1" t="n">
@@ -13472,6 +13616,9 @@
       <c r="CJ48" s="1" t="n">
         <v>148</v>
       </c>
+      <c r="CK48" s="1" t="n">
+        <v>251.2</v>
+      </c>
     </row>
     <row r="49" ht="20" customHeight="1">
       <c r="A49" s="1" t="n">
@@ -13738,6 +13885,9 @@
       <c r="CJ49" s="1" t="n">
         <v>152.2</v>
       </c>
+      <c r="CK49" s="1" t="n">
+        <v>164.8</v>
+      </c>
     </row>
     <row r="50" ht="20" customHeight="1">
       <c r="A50" s="1" t="n">
@@ -14004,6 +14154,9 @@
       <c r="CJ50" s="1" t="n">
         <v>169.7</v>
       </c>
+      <c r="CK50" s="1" t="n">
+        <v>179.3</v>
+      </c>
     </row>
     <row r="51" ht="20" customHeight="1">
       <c r="A51" s="1" t="n">
@@ -14270,6 +14423,9 @@
       <c r="CJ51" s="2" t="n">
         <v>120.3</v>
       </c>
+      <c r="CK51" s="3" t="n">
+        <v>125</v>
+      </c>
     </row>
     <row r="52" ht="20" customHeight="1">
       <c r="A52" s="1" t="n">
@@ -14536,6 +14692,9 @@
       <c r="CJ52" s="1" t="n">
         <v>144</v>
       </c>
+      <c r="CK52" s="1" t="n">
+        <v>153.7</v>
+      </c>
     </row>
     <row r="53" ht="20" customHeight="1">
       <c r="A53" s="1" t="n">
@@ -14801,6 +14960,9 @@
       </c>
       <c r="CJ53" s="2" t="n">
         <v>112.4</v>
+      </c>
+      <c r="CK53" s="1" t="n">
+        <v>157.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2024-12-07
</commit_message>
<xml_diff>
--- a/マイジャグラーV_塗りつぶし済み.xlsx
+++ b/マイジャグラーV_塗りつぶし済み.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:CK53"/>
+  <dimension ref="A1:CL53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -528,6 +528,7 @@
     <col width="12" customWidth="1" min="87" max="87"/>
     <col width="12" customWidth="1" min="88" max="88"/>
     <col width="12" customWidth="1" min="89" max="89"/>
+    <col width="12" customWidth="1" min="90" max="90"/>
   </cols>
   <sheetData>
     <row r="1" ht="20" customHeight="1">
@@ -976,6 +977,11 @@
           <t>2024/12/06</t>
         </is>
       </c>
+      <c r="CL1" s="1" t="inlineStr">
+        <is>
+          <t>2024/12/07</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="20" customHeight="1">
       <c r="A2" s="1" t="n">
@@ -1245,6 +1251,9 @@
       <c r="CK2" s="1" t="n">
         <v>152.3</v>
       </c>
+      <c r="CL2" s="1" t="n">
+        <v>153</v>
+      </c>
     </row>
     <row r="3" ht="20" customHeight="1">
       <c r="A3" s="1" t="n">
@@ -1514,6 +1523,9 @@
       <c r="CK3" s="1" t="n">
         <v>177.1</v>
       </c>
+      <c r="CL3" s="3" t="n">
+        <v>128</v>
+      </c>
     </row>
     <row r="4" ht="20" customHeight="1">
       <c r="A4" s="1" t="n">
@@ -1783,6 +1795,9 @@
       <c r="CK4" s="1" t="n">
         <v>153.3</v>
       </c>
+      <c r="CL4" s="1" t="n">
+        <v>160.4</v>
+      </c>
     </row>
     <row r="5" ht="20" customHeight="1">
       <c r="A5" s="1" t="n">
@@ -2052,6 +2067,9 @@
       <c r="CK5" s="1" t="n">
         <v>163</v>
       </c>
+      <c r="CL5" s="3" t="n">
+        <v>133.8</v>
+      </c>
     </row>
     <row r="6" ht="20" customHeight="1">
       <c r="A6" s="1" t="n">
@@ -2321,6 +2339,9 @@
       <c r="CK6" s="3" t="n">
         <v>127.2</v>
       </c>
+      <c r="CL6" s="1" t="n">
+        <v>170.7</v>
+      </c>
     </row>
     <row r="7" ht="20" customHeight="1">
       <c r="A7" s="1" t="n">
@@ -2590,6 +2611,9 @@
       <c r="CK7" s="1" t="n">
         <v>191.7</v>
       </c>
+      <c r="CL7" s="2" t="n">
+        <v>112</v>
+      </c>
     </row>
     <row r="8" ht="20" customHeight="1">
       <c r="A8" s="1" t="n">
@@ -2859,6 +2883,9 @@
       <c r="CK8" s="3" t="n">
         <v>136.9</v>
       </c>
+      <c r="CL8" s="1" t="n">
+        <v>155.6</v>
+      </c>
     </row>
     <row r="9" ht="20" customHeight="1">
       <c r="A9" s="1" t="n">
@@ -3128,6 +3155,9 @@
       <c r="CK9" s="1" t="n">
         <v>143.1</v>
       </c>
+      <c r="CL9" s="1" t="n">
+        <v>178.3</v>
+      </c>
     </row>
     <row r="10" ht="20" customHeight="1">
       <c r="A10" s="1" t="n">
@@ -3397,6 +3427,9 @@
       <c r="CK10" s="1" t="n">
         <v>163.2</v>
       </c>
+      <c r="CL10" s="1" t="n">
+        <v>158.4</v>
+      </c>
     </row>
     <row r="11" ht="20" customHeight="1">
       <c r="A11" s="1" t="n">
@@ -3666,6 +3699,9 @@
       <c r="CK11" s="1" t="n">
         <v>480.3</v>
       </c>
+      <c r="CL11" s="3" t="n">
+        <v>129.8</v>
+      </c>
     </row>
     <row r="12" ht="20" customHeight="1">
       <c r="A12" s="1" t="n">
@@ -3935,6 +3971,9 @@
       <c r="CK12" s="1" t="n">
         <v>166.8</v>
       </c>
+      <c r="CL12" s="1" t="n">
+        <v>174.4</v>
+      </c>
     </row>
     <row r="13" ht="20" customHeight="1">
       <c r="A13" s="1" t="n">
@@ -4204,6 +4243,9 @@
       <c r="CK13" s="1" t="n">
         <v>154.5</v>
       </c>
+      <c r="CL13" s="1" t="n">
+        <v>165.9</v>
+      </c>
     </row>
     <row r="14" ht="20" customHeight="1">
       <c r="A14" s="1" t="n">
@@ -4473,6 +4515,9 @@
       <c r="CK14" s="2" t="n">
         <v>123.9</v>
       </c>
+      <c r="CL14" s="1" t="n">
+        <v>142.9</v>
+      </c>
     </row>
     <row r="15" ht="20" customHeight="1">
       <c r="A15" s="1" t="n">
@@ -4742,6 +4787,9 @@
       <c r="CK15" s="3" t="n">
         <v>136.5</v>
       </c>
+      <c r="CL15" s="1" t="n">
+        <v>163.4</v>
+      </c>
     </row>
     <row r="16" ht="20" customHeight="1">
       <c r="A16" s="1" t="n">
@@ -5011,6 +5059,9 @@
       <c r="CK16" s="3" t="n">
         <v>133.2</v>
       </c>
+      <c r="CL16" s="1" t="n">
+        <v>190.2</v>
+      </c>
     </row>
     <row r="17" ht="20" customHeight="1">
       <c r="A17" s="1" t="n">
@@ -5280,6 +5331,9 @@
       <c r="CK17" s="1" t="n">
         <v>236.6</v>
       </c>
+      <c r="CL17" s="1" t="n">
+        <v>141.5</v>
+      </c>
     </row>
     <row r="18" ht="20" customHeight="1">
       <c r="A18" s="1" t="n">
@@ -5549,6 +5603,9 @@
       <c r="CK18" s="2" t="n">
         <v>106.5</v>
       </c>
+      <c r="CL18" s="1" t="n">
+        <v>145.6</v>
+      </c>
     </row>
     <row r="19" ht="20" customHeight="1">
       <c r="A19" s="1" t="n">
@@ -5818,6 +5875,9 @@
       <c r="CK19" s="1" t="n">
         <v>154.2</v>
       </c>
+      <c r="CL19" s="1" t="n">
+        <v>150.9</v>
+      </c>
     </row>
     <row r="20" ht="20" customHeight="1">
       <c r="A20" s="1" t="n">
@@ -6087,6 +6147,9 @@
       <c r="CK20" s="1" t="n">
         <v>201</v>
       </c>
+      <c r="CL20" s="1" t="n">
+        <v>159.9</v>
+      </c>
     </row>
     <row r="21" ht="20" customHeight="1">
       <c r="A21" s="1" t="n">
@@ -6356,6 +6419,9 @@
       <c r="CK21" s="1" t="n">
         <v>156.7</v>
       </c>
+      <c r="CL21" s="1" t="n">
+        <v>170.7</v>
+      </c>
     </row>
     <row r="22" ht="20" customHeight="1">
       <c r="A22" s="1" t="n">
@@ -6625,6 +6691,9 @@
       <c r="CK22" s="1" t="n">
         <v>158.5</v>
       </c>
+      <c r="CL22" s="3" t="n">
+        <v>132.5</v>
+      </c>
     </row>
     <row r="23" ht="20" customHeight="1">
       <c r="A23" s="1" t="n">
@@ -6894,6 +6963,9 @@
       <c r="CK23" s="1" t="n">
         <v>224.1</v>
       </c>
+      <c r="CL23" s="3" t="n">
+        <v>127.6</v>
+      </c>
     </row>
     <row r="24" ht="20" customHeight="1">
       <c r="A24" s="1" t="n">
@@ -7163,6 +7235,9 @@
       <c r="CK24" s="1" t="n">
         <v>147.9</v>
       </c>
+      <c r="CL24" s="1" t="n">
+        <v>160.7</v>
+      </c>
     </row>
     <row r="25" ht="20" customHeight="1">
       <c r="A25" s="1" t="n">
@@ -7432,6 +7507,9 @@
       <c r="CK25" s="1" t="n">
         <v>189.4</v>
       </c>
+      <c r="CL25" s="3" t="n">
+        <v>126.6</v>
+      </c>
     </row>
     <row r="26" ht="20" customHeight="1">
       <c r="A26" s="1" t="n">
@@ -7701,6 +7779,9 @@
       <c r="CK26" s="1" t="n">
         <v>162.5</v>
       </c>
+      <c r="CL26" s="1" t="n">
+        <v>145</v>
+      </c>
     </row>
     <row r="27" ht="20" customHeight="1">
       <c r="A27" s="1" t="n">
@@ -7970,6 +8051,9 @@
       <c r="CK27" s="1" t="n">
         <v>261.3</v>
       </c>
+      <c r="CL27" s="1" t="n">
+        <v>149.4</v>
+      </c>
     </row>
     <row r="28" ht="20" customHeight="1">
       <c r="A28" s="1" t="n">
@@ -8239,6 +8323,9 @@
       <c r="CK28" s="1" t="n">
         <v>140.9</v>
       </c>
+      <c r="CL28" s="2" t="n">
+        <v>119.6</v>
+      </c>
     </row>
     <row r="29" ht="20" customHeight="1">
       <c r="A29" s="1" t="n">
@@ -8508,6 +8595,9 @@
       <c r="CK29" s="2" t="n">
         <v>108.7</v>
       </c>
+      <c r="CL29" s="3" t="n">
+        <v>139.6</v>
+      </c>
     </row>
     <row r="30" ht="20" customHeight="1">
       <c r="A30" s="1" t="n">
@@ -8777,6 +8867,9 @@
       <c r="CK30" s="1" t="n">
         <v>164.5</v>
       </c>
+      <c r="CL30" s="3" t="n">
+        <v>131.6</v>
+      </c>
     </row>
     <row r="31" ht="20" customHeight="1">
       <c r="A31" s="1" t="n">
@@ -9046,6 +9139,9 @@
       <c r="CK31" s="1" t="n">
         <v>144.4</v>
       </c>
+      <c r="CL31" s="1" t="n">
+        <v>145.3</v>
+      </c>
     </row>
     <row r="32" ht="20" customHeight="1">
       <c r="A32" s="1" t="n">
@@ -9315,6 +9411,9 @@
       <c r="CK32" s="1" t="n">
         <v>209.3</v>
       </c>
+      <c r="CL32" s="2" t="n">
+        <v>123.4</v>
+      </c>
     </row>
     <row r="33" ht="20" customHeight="1">
       <c r="A33" s="1" t="n">
@@ -9584,6 +9683,9 @@
       <c r="CK33" s="1" t="n">
         <v>158.2</v>
       </c>
+      <c r="CL33" s="1" t="n">
+        <v>140</v>
+      </c>
     </row>
     <row r="34" ht="20" customHeight="1">
       <c r="A34" s="1" t="n">
@@ -9853,6 +9955,9 @@
       <c r="CK34" s="2" t="n">
         <v>118.2</v>
       </c>
+      <c r="CL34" s="1" t="n">
+        <v>163.9</v>
+      </c>
     </row>
     <row r="35" ht="20" customHeight="1">
       <c r="A35" s="1" t="n">
@@ -10122,6 +10227,9 @@
       <c r="CK35" s="1" t="n">
         <v>247</v>
       </c>
+      <c r="CL35" s="1" t="n">
+        <v>145.4</v>
+      </c>
     </row>
     <row r="36" ht="20" customHeight="1">
       <c r="A36" s="1" t="n">
@@ -10391,6 +10499,9 @@
       <c r="CK36" s="2" t="n">
         <v>113</v>
       </c>
+      <c r="CL36" s="3" t="n">
+        <v>135.1</v>
+      </c>
     </row>
     <row r="37" ht="20" customHeight="1">
       <c r="A37" s="1" t="n">
@@ -10660,6 +10771,9 @@
       <c r="CK37" s="1" t="n">
         <v>249</v>
       </c>
+      <c r="CL37" s="1" t="n">
+        <v>145.6</v>
+      </c>
     </row>
     <row r="38" ht="20" customHeight="1">
       <c r="A38" s="1" t="n">
@@ -10929,6 +11043,9 @@
       <c r="CK38" s="1" t="n">
         <v>168.9</v>
       </c>
+      <c r="CL38" s="1" t="n">
+        <v>151.6</v>
+      </c>
     </row>
     <row r="39" ht="20" customHeight="1">
       <c r="A39" s="1" t="n">
@@ -11198,6 +11315,9 @@
       <c r="CK39" s="3" t="n">
         <v>127.3</v>
       </c>
+      <c r="CL39" s="1" t="n">
+        <v>160</v>
+      </c>
     </row>
     <row r="40" ht="20" customHeight="1">
       <c r="A40" s="1" t="n">
@@ -11467,6 +11587,9 @@
       <c r="CK40" s="3" t="n">
         <v>138.4</v>
       </c>
+      <c r="CL40" s="3" t="n">
+        <v>129.4</v>
+      </c>
     </row>
     <row r="41" ht="20" customHeight="1">
       <c r="A41" s="1" t="n">
@@ -11736,6 +11859,9 @@
       <c r="CK41" s="1" t="n">
         <v>170.4</v>
       </c>
+      <c r="CL41" s="1" t="n">
+        <v>157.4</v>
+      </c>
     </row>
     <row r="42" ht="20" customHeight="1">
       <c r="A42" s="1" t="n">
@@ -12005,6 +12131,9 @@
       <c r="CK42" s="1" t="n">
         <v>240.5</v>
       </c>
+      <c r="CL42" s="1" t="n">
+        <v>178.6</v>
+      </c>
     </row>
     <row r="43" ht="20" customHeight="1">
       <c r="A43" s="1" t="n">
@@ -12274,6 +12403,9 @@
       <c r="CK43" s="3" t="n">
         <v>138.5</v>
       </c>
+      <c r="CL43" s="1" t="n">
+        <v>186</v>
+      </c>
     </row>
     <row r="44" ht="20" customHeight="1">
       <c r="A44" s="1" t="n">
@@ -12543,6 +12675,9 @@
       <c r="CK44" s="3" t="n">
         <v>128.4</v>
       </c>
+      <c r="CL44" s="1" t="n">
+        <v>144.5</v>
+      </c>
     </row>
     <row r="45" ht="20" customHeight="1">
       <c r="A45" s="1" t="n">
@@ -12812,6 +12947,9 @@
       <c r="CK45" s="3" t="n">
         <v>128.9</v>
       </c>
+      <c r="CL45" s="1" t="n">
+        <v>145.7</v>
+      </c>
     </row>
     <row r="46" ht="20" customHeight="1">
       <c r="A46" s="1" t="n">
@@ -13081,6 +13219,9 @@
       <c r="CK46" s="1" t="n">
         <v>207.4</v>
       </c>
+      <c r="CL46" s="3" t="n">
+        <v>132.5</v>
+      </c>
     </row>
     <row r="47" ht="20" customHeight="1">
       <c r="A47" s="1" t="n">
@@ -13350,6 +13491,9 @@
       <c r="CK47" s="1" t="n">
         <v>174.1</v>
       </c>
+      <c r="CL47" s="2" t="n">
+        <v>123.5</v>
+      </c>
     </row>
     <row r="48" ht="20" customHeight="1">
       <c r="A48" s="1" t="n">
@@ -13619,6 +13763,9 @@
       <c r="CK48" s="1" t="n">
         <v>251.2</v>
       </c>
+      <c r="CL48" s="1" t="n">
+        <v>174.6</v>
+      </c>
     </row>
     <row r="49" ht="20" customHeight="1">
       <c r="A49" s="1" t="n">
@@ -13888,6 +14035,9 @@
       <c r="CK49" s="1" t="n">
         <v>164.8</v>
       </c>
+      <c r="CL49" s="1" t="n">
+        <v>187.5</v>
+      </c>
     </row>
     <row r="50" ht="20" customHeight="1">
       <c r="A50" s="1" t="n">
@@ -14157,6 +14307,9 @@
       <c r="CK50" s="1" t="n">
         <v>179.3</v>
       </c>
+      <c r="CL50" s="1" t="n">
+        <v>150.8</v>
+      </c>
     </row>
     <row r="51" ht="20" customHeight="1">
       <c r="A51" s="1" t="n">
@@ -14426,6 +14579,9 @@
       <c r="CK51" s="3" t="n">
         <v>125</v>
       </c>
+      <c r="CL51" s="1" t="n">
+        <v>225.3</v>
+      </c>
     </row>
     <row r="52" ht="20" customHeight="1">
       <c r="A52" s="1" t="n">
@@ -14695,6 +14851,9 @@
       <c r="CK52" s="1" t="n">
         <v>153.7</v>
       </c>
+      <c r="CL52" s="1" t="n">
+        <v>151.1</v>
+      </c>
     </row>
     <row r="53" ht="20" customHeight="1">
       <c r="A53" s="1" t="n">
@@ -14963,6 +15122,9 @@
       </c>
       <c r="CK53" s="1" t="n">
         <v>157.5</v>
+      </c>
+      <c r="CL53" s="1" t="n">
+        <v>144.6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2024-12-08
</commit_message>
<xml_diff>
--- a/マイジャグラーV_塗りつぶし済み.xlsx
+++ b/マイジャグラーV_塗りつぶし済み.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:CL53"/>
+  <dimension ref="A1:CM53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -529,6 +529,7 @@
     <col width="12" customWidth="1" min="88" max="88"/>
     <col width="12" customWidth="1" min="89" max="89"/>
     <col width="12" customWidth="1" min="90" max="90"/>
+    <col width="12" customWidth="1" min="91" max="91"/>
   </cols>
   <sheetData>
     <row r="1" ht="20" customHeight="1">
@@ -982,6 +983,11 @@
           <t>2024/12/07</t>
         </is>
       </c>
+      <c r="CM1" s="1" t="inlineStr">
+        <is>
+          <t>2024/12/08</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="20" customHeight="1">
       <c r="A2" s="1" t="n">
@@ -1254,6 +1260,9 @@
       <c r="CL2" s="1" t="n">
         <v>153</v>
       </c>
+      <c r="CM2" s="1" t="n">
+        <v>142.7</v>
+      </c>
     </row>
     <row r="3" ht="20" customHeight="1">
       <c r="A3" s="1" t="n">
@@ -1526,6 +1535,9 @@
       <c r="CL3" s="3" t="n">
         <v>128</v>
       </c>
+      <c r="CM3" s="1" t="n">
+        <v>170.7</v>
+      </c>
     </row>
     <row r="4" ht="20" customHeight="1">
       <c r="A4" s="1" t="n">
@@ -1798,6 +1810,9 @@
       <c r="CL4" s="1" t="n">
         <v>160.4</v>
       </c>
+      <c r="CM4" s="1" t="n">
+        <v>164.3</v>
+      </c>
     </row>
     <row r="5" ht="20" customHeight="1">
       <c r="A5" s="1" t="n">
@@ -2070,6 +2085,9 @@
       <c r="CL5" s="3" t="n">
         <v>133.8</v>
       </c>
+      <c r="CM5" s="1" t="n">
+        <v>145.1</v>
+      </c>
     </row>
     <row r="6" ht="20" customHeight="1">
       <c r="A6" s="1" t="n">
@@ -2342,6 +2360,9 @@
       <c r="CL6" s="1" t="n">
         <v>170.7</v>
       </c>
+      <c r="CM6" s="1" t="n">
+        <v>165.1</v>
+      </c>
     </row>
     <row r="7" ht="20" customHeight="1">
       <c r="A7" s="1" t="n">
@@ -2614,6 +2635,9 @@
       <c r="CL7" s="2" t="n">
         <v>112</v>
       </c>
+      <c r="CM7" s="2" t="n">
+        <v>95.90000000000001</v>
+      </c>
     </row>
     <row r="8" ht="20" customHeight="1">
       <c r="A8" s="1" t="n">
@@ -2886,6 +2910,9 @@
       <c r="CL8" s="1" t="n">
         <v>155.6</v>
       </c>
+      <c r="CM8" s="1" t="n">
+        <v>177.2</v>
+      </c>
     </row>
     <row r="9" ht="20" customHeight="1">
       <c r="A9" s="1" t="n">
@@ -3158,6 +3185,9 @@
       <c r="CL9" s="1" t="n">
         <v>178.3</v>
       </c>
+      <c r="CM9" s="1" t="n">
+        <v>146.8</v>
+      </c>
     </row>
     <row r="10" ht="20" customHeight="1">
       <c r="A10" s="1" t="n">
@@ -3430,6 +3460,9 @@
       <c r="CL10" s="1" t="n">
         <v>158.4</v>
       </c>
+      <c r="CM10" s="1" t="n">
+        <v>151.5</v>
+      </c>
     </row>
     <row r="11" ht="20" customHeight="1">
       <c r="A11" s="1" t="n">
@@ -3702,6 +3735,9 @@
       <c r="CL11" s="3" t="n">
         <v>129.8</v>
       </c>
+      <c r="CM11" s="1" t="n">
+        <v>141.2</v>
+      </c>
     </row>
     <row r="12" ht="20" customHeight="1">
       <c r="A12" s="1" t="n">
@@ -3974,6 +4010,9 @@
       <c r="CL12" s="1" t="n">
         <v>174.4</v>
       </c>
+      <c r="CM12" s="1" t="n">
+        <v>147.6</v>
+      </c>
     </row>
     <row r="13" ht="20" customHeight="1">
       <c r="A13" s="1" t="n">
@@ -4246,6 +4285,9 @@
       <c r="CL13" s="1" t="n">
         <v>165.9</v>
       </c>
+      <c r="CM13" s="1" t="n">
+        <v>176.8</v>
+      </c>
     </row>
     <row r="14" ht="20" customHeight="1">
       <c r="A14" s="1" t="n">
@@ -4518,6 +4560,9 @@
       <c r="CL14" s="1" t="n">
         <v>142.9</v>
       </c>
+      <c r="CM14" s="1" t="n">
+        <v>143.6</v>
+      </c>
     </row>
     <row r="15" ht="20" customHeight="1">
       <c r="A15" s="1" t="n">
@@ -4790,6 +4835,9 @@
       <c r="CL15" s="1" t="n">
         <v>163.4</v>
       </c>
+      <c r="CM15" s="1" t="n">
+        <v>166.2</v>
+      </c>
     </row>
     <row r="16" ht="20" customHeight="1">
       <c r="A16" s="1" t="n">
@@ -5062,6 +5110,9 @@
       <c r="CL16" s="1" t="n">
         <v>190.2</v>
       </c>
+      <c r="CM16" s="3" t="n">
+        <v>132</v>
+      </c>
     </row>
     <row r="17" ht="20" customHeight="1">
       <c r="A17" s="1" t="n">
@@ -5334,6 +5385,9 @@
       <c r="CL17" s="1" t="n">
         <v>141.5</v>
       </c>
+      <c r="CM17" s="1" t="n">
+        <v>225.8</v>
+      </c>
     </row>
     <row r="18" ht="20" customHeight="1">
       <c r="A18" s="1" t="n">
@@ -5606,6 +5660,9 @@
       <c r="CL18" s="1" t="n">
         <v>145.6</v>
       </c>
+      <c r="CM18" s="1" t="n">
+        <v>146.5</v>
+      </c>
     </row>
     <row r="19" ht="20" customHeight="1">
       <c r="A19" s="1" t="n">
@@ -5878,6 +5935,9 @@
       <c r="CL19" s="1" t="n">
         <v>150.9</v>
       </c>
+      <c r="CM19" s="2" t="n">
+        <v>121.7</v>
+      </c>
     </row>
     <row r="20" ht="20" customHeight="1">
       <c r="A20" s="1" t="n">
@@ -6150,6 +6210,9 @@
       <c r="CL20" s="1" t="n">
         <v>159.9</v>
       </c>
+      <c r="CM20" s="1" t="n">
+        <v>146.9</v>
+      </c>
     </row>
     <row r="21" ht="20" customHeight="1">
       <c r="A21" s="1" t="n">
@@ -6422,6 +6485,9 @@
       <c r="CL21" s="1" t="n">
         <v>170.7</v>
       </c>
+      <c r="CM21" s="1" t="n">
+        <v>164</v>
+      </c>
     </row>
     <row r="22" ht="20" customHeight="1">
       <c r="A22" s="1" t="n">
@@ -6694,6 +6760,9 @@
       <c r="CL22" s="3" t="n">
         <v>132.5</v>
       </c>
+      <c r="CM22" s="1" t="n">
+        <v>180.4</v>
+      </c>
     </row>
     <row r="23" ht="20" customHeight="1">
       <c r="A23" s="1" t="n">
@@ -6966,6 +7035,9 @@
       <c r="CL23" s="3" t="n">
         <v>127.6</v>
       </c>
+      <c r="CM23" s="1" t="n">
+        <v>140.2</v>
+      </c>
     </row>
     <row r="24" ht="20" customHeight="1">
       <c r="A24" s="1" t="n">
@@ -7238,6 +7310,9 @@
       <c r="CL24" s="1" t="n">
         <v>160.7</v>
       </c>
+      <c r="CM24" s="1" t="n">
+        <v>195.5</v>
+      </c>
     </row>
     <row r="25" ht="20" customHeight="1">
       <c r="A25" s="1" t="n">
@@ -7510,6 +7585,9 @@
       <c r="CL25" s="3" t="n">
         <v>126.6</v>
       </c>
+      <c r="CM25" s="2" t="n">
+        <v>123.4</v>
+      </c>
     </row>
     <row r="26" ht="20" customHeight="1">
       <c r="A26" s="1" t="n">
@@ -7782,6 +7860,9 @@
       <c r="CL26" s="1" t="n">
         <v>145</v>
       </c>
+      <c r="CM26" s="3" t="n">
+        <v>126.1</v>
+      </c>
     </row>
     <row r="27" ht="20" customHeight="1">
       <c r="A27" s="1" t="n">
@@ -8054,6 +8135,9 @@
       <c r="CL27" s="1" t="n">
         <v>149.4</v>
       </c>
+      <c r="CM27" s="1" t="n">
+        <v>300.3</v>
+      </c>
     </row>
     <row r="28" ht="20" customHeight="1">
       <c r="A28" s="1" t="n">
@@ -8326,6 +8410,9 @@
       <c r="CL28" s="2" t="n">
         <v>119.6</v>
       </c>
+      <c r="CM28" s="1" t="n">
+        <v>168.8</v>
+      </c>
     </row>
     <row r="29" ht="20" customHeight="1">
       <c r="A29" s="1" t="n">
@@ -8598,6 +8685,9 @@
       <c r="CL29" s="3" t="n">
         <v>139.6</v>
       </c>
+      <c r="CM29" s="1" t="n">
+        <v>173.3</v>
+      </c>
     </row>
     <row r="30" ht="20" customHeight="1">
       <c r="A30" s="1" t="n">
@@ -8870,6 +8960,9 @@
       <c r="CL30" s="3" t="n">
         <v>131.6</v>
       </c>
+      <c r="CM30" s="1" t="n">
+        <v>144.7</v>
+      </c>
     </row>
     <row r="31" ht="20" customHeight="1">
       <c r="A31" s="1" t="n">
@@ -9142,6 +9235,9 @@
       <c r="CL31" s="1" t="n">
         <v>145.3</v>
       </c>
+      <c r="CM31" s="1" t="n">
+        <v>186.9</v>
+      </c>
     </row>
     <row r="32" ht="20" customHeight="1">
       <c r="A32" s="1" t="n">
@@ -9414,6 +9510,9 @@
       <c r="CL32" s="2" t="n">
         <v>123.4</v>
       </c>
+      <c r="CM32" s="3" t="n">
+        <v>136.8</v>
+      </c>
     </row>
     <row r="33" ht="20" customHeight="1">
       <c r="A33" s="1" t="n">
@@ -9686,6 +9785,9 @@
       <c r="CL33" s="1" t="n">
         <v>140</v>
       </c>
+      <c r="CM33" s="1" t="n">
+        <v>194.4</v>
+      </c>
     </row>
     <row r="34" ht="20" customHeight="1">
       <c r="A34" s="1" t="n">
@@ -9958,6 +10060,9 @@
       <c r="CL34" s="1" t="n">
         <v>163.9</v>
       </c>
+      <c r="CM34" s="1" t="n">
+        <v>175.2</v>
+      </c>
     </row>
     <row r="35" ht="20" customHeight="1">
       <c r="A35" s="1" t="n">
@@ -10230,6 +10335,9 @@
       <c r="CL35" s="1" t="n">
         <v>145.4</v>
       </c>
+      <c r="CM35" s="1" t="n">
+        <v>140.3</v>
+      </c>
     </row>
     <row r="36" ht="20" customHeight="1">
       <c r="A36" s="1" t="n">
@@ -10502,6 +10610,9 @@
       <c r="CL36" s="3" t="n">
         <v>135.1</v>
       </c>
+      <c r="CM36" s="1" t="n">
+        <v>174.2</v>
+      </c>
     </row>
     <row r="37" ht="20" customHeight="1">
       <c r="A37" s="1" t="n">
@@ -10774,6 +10885,9 @@
       <c r="CL37" s="1" t="n">
         <v>145.6</v>
       </c>
+      <c r="CM37" s="1" t="n">
+        <v>174.5</v>
+      </c>
     </row>
     <row r="38" ht="20" customHeight="1">
       <c r="A38" s="1" t="n">
@@ -11046,6 +11160,9 @@
       <c r="CL38" s="1" t="n">
         <v>151.6</v>
       </c>
+      <c r="CM38" s="1" t="n">
+        <v>145.7</v>
+      </c>
     </row>
     <row r="39" ht="20" customHeight="1">
       <c r="A39" s="1" t="n">
@@ -11318,6 +11435,9 @@
       <c r="CL39" s="1" t="n">
         <v>160</v>
       </c>
+      <c r="CM39" s="1" t="n">
+        <v>198.3</v>
+      </c>
     </row>
     <row r="40" ht="20" customHeight="1">
       <c r="A40" s="1" t="n">
@@ -11590,6 +11710,9 @@
       <c r="CL40" s="3" t="n">
         <v>129.4</v>
       </c>
+      <c r="CM40" s="1" t="n">
+        <v>187.7</v>
+      </c>
     </row>
     <row r="41" ht="20" customHeight="1">
       <c r="A41" s="1" t="n">
@@ -11862,6 +11985,9 @@
       <c r="CL41" s="1" t="n">
         <v>157.4</v>
       </c>
+      <c r="CM41" s="2" t="n">
+        <v>116.5</v>
+      </c>
     </row>
     <row r="42" ht="20" customHeight="1">
       <c r="A42" s="1" t="n">
@@ -12134,6 +12260,9 @@
       <c r="CL42" s="1" t="n">
         <v>178.6</v>
       </c>
+      <c r="CM42" s="1" t="n">
+        <v>179</v>
+      </c>
     </row>
     <row r="43" ht="20" customHeight="1">
       <c r="A43" s="1" t="n">
@@ -12406,6 +12535,9 @@
       <c r="CL43" s="1" t="n">
         <v>186</v>
       </c>
+      <c r="CM43" s="1" t="n">
+        <v>158.5</v>
+      </c>
     </row>
     <row r="44" ht="20" customHeight="1">
       <c r="A44" s="1" t="n">
@@ -12678,6 +12810,9 @@
       <c r="CL44" s="1" t="n">
         <v>144.5</v>
       </c>
+      <c r="CM44" s="3" t="n">
+        <v>132.3</v>
+      </c>
     </row>
     <row r="45" ht="20" customHeight="1">
       <c r="A45" s="1" t="n">
@@ -12950,6 +13085,9 @@
       <c r="CL45" s="1" t="n">
         <v>145.7</v>
       </c>
+      <c r="CM45" s="1" t="n">
+        <v>409.8</v>
+      </c>
     </row>
     <row r="46" ht="20" customHeight="1">
       <c r="A46" s="1" t="n">
@@ -13222,6 +13360,9 @@
       <c r="CL46" s="3" t="n">
         <v>132.5</v>
       </c>
+      <c r="CM46" s="1" t="n">
+        <v>152.5</v>
+      </c>
     </row>
     <row r="47" ht="20" customHeight="1">
       <c r="A47" s="1" t="n">
@@ -13494,6 +13635,9 @@
       <c r="CL47" s="2" t="n">
         <v>123.5</v>
       </c>
+      <c r="CM47" s="1" t="n">
+        <v>152.3</v>
+      </c>
     </row>
     <row r="48" ht="20" customHeight="1">
       <c r="A48" s="1" t="n">
@@ -13766,6 +13910,9 @@
       <c r="CL48" s="1" t="n">
         <v>174.6</v>
       </c>
+      <c r="CM48" s="1" t="n">
+        <v>197.4</v>
+      </c>
     </row>
     <row r="49" ht="20" customHeight="1">
       <c r="A49" s="1" t="n">
@@ -14038,6 +14185,9 @@
       <c r="CL49" s="1" t="n">
         <v>187.5</v>
       </c>
+      <c r="CM49" s="1" t="n">
+        <v>158.4</v>
+      </c>
     </row>
     <row r="50" ht="20" customHeight="1">
       <c r="A50" s="1" t="n">
@@ -14310,6 +14460,9 @@
       <c r="CL50" s="1" t="n">
         <v>150.8</v>
       </c>
+      <c r="CM50" s="1" t="n">
+        <v>209.8</v>
+      </c>
     </row>
     <row r="51" ht="20" customHeight="1">
       <c r="A51" s="1" t="n">
@@ -14582,6 +14735,9 @@
       <c r="CL51" s="1" t="n">
         <v>225.3</v>
       </c>
+      <c r="CM51" s="3" t="n">
+        <v>127.3</v>
+      </c>
     </row>
     <row r="52" ht="20" customHeight="1">
       <c r="A52" s="1" t="n">
@@ -14854,6 +15010,9 @@
       <c r="CL52" s="1" t="n">
         <v>151.1</v>
       </c>
+      <c r="CM52" s="1" t="n">
+        <v>160.5</v>
+      </c>
     </row>
     <row r="53" ht="20" customHeight="1">
       <c r="A53" s="1" t="n">
@@ -15125,6 +15284,9 @@
       </c>
       <c r="CL53" s="1" t="n">
         <v>144.6</v>
+      </c>
+      <c r="CM53" s="1" t="n">
+        <v>154.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2024-12-09
</commit_message>
<xml_diff>
--- a/マイジャグラーV_塗りつぶし済み.xlsx
+++ b/マイジャグラーV_塗りつぶし済み.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:CM53"/>
+  <dimension ref="A1:CN53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -530,6 +530,7 @@
     <col width="12" customWidth="1" min="89" max="89"/>
     <col width="12" customWidth="1" min="90" max="90"/>
     <col width="12" customWidth="1" min="91" max="91"/>
+    <col width="12" customWidth="1" min="92" max="92"/>
   </cols>
   <sheetData>
     <row r="1" ht="20" customHeight="1">
@@ -988,6 +989,11 @@
           <t>2024/12/08</t>
         </is>
       </c>
+      <c r="CN1" s="1" t="inlineStr">
+        <is>
+          <t>2024/12/09</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="20" customHeight="1">
       <c r="A2" s="1" t="n">
@@ -1263,6 +1269,9 @@
       <c r="CM2" s="1" t="n">
         <v>142.7</v>
       </c>
+      <c r="CN2" s="3" t="n">
+        <v>138</v>
+      </c>
     </row>
     <row r="3" ht="20" customHeight="1">
       <c r="A3" s="1" t="n">
@@ -1538,6 +1547,9 @@
       <c r="CM3" s="1" t="n">
         <v>170.7</v>
       </c>
+      <c r="CN3" s="1" t="n">
+        <v>266.4</v>
+      </c>
     </row>
     <row r="4" ht="20" customHeight="1">
       <c r="A4" s="1" t="n">
@@ -1813,6 +1825,9 @@
       <c r="CM4" s="1" t="n">
         <v>164.3</v>
       </c>
+      <c r="CN4" s="1" t="n">
+        <v>188.6</v>
+      </c>
     </row>
     <row r="5" ht="20" customHeight="1">
       <c r="A5" s="1" t="n">
@@ -2088,6 +2103,9 @@
       <c r="CM5" s="1" t="n">
         <v>145.1</v>
       </c>
+      <c r="CN5" s="1" t="n">
+        <v>170.8</v>
+      </c>
     </row>
     <row r="6" ht="20" customHeight="1">
       <c r="A6" s="1" t="n">
@@ -2363,6 +2381,9 @@
       <c r="CM6" s="1" t="n">
         <v>165.1</v>
       </c>
+      <c r="CN6" s="1" t="n">
+        <v>197.6</v>
+      </c>
     </row>
     <row r="7" ht="20" customHeight="1">
       <c r="A7" s="1" t="n">
@@ -2638,6 +2659,9 @@
       <c r="CM7" s="2" t="n">
         <v>95.90000000000001</v>
       </c>
+      <c r="CN7" s="1" t="n">
+        <v>143.5</v>
+      </c>
     </row>
     <row r="8" ht="20" customHeight="1">
       <c r="A8" s="1" t="n">
@@ -2913,6 +2937,9 @@
       <c r="CM8" s="1" t="n">
         <v>177.2</v>
       </c>
+      <c r="CN8" s="1" t="n">
+        <v>266.7</v>
+      </c>
     </row>
     <row r="9" ht="20" customHeight="1">
       <c r="A9" s="1" t="n">
@@ -3188,6 +3215,9 @@
       <c r="CM9" s="1" t="n">
         <v>146.8</v>
       </c>
+      <c r="CN9" s="1" t="n">
+        <v>232.2</v>
+      </c>
     </row>
     <row r="10" ht="20" customHeight="1">
       <c r="A10" s="1" t="n">
@@ -3463,6 +3493,9 @@
       <c r="CM10" s="1" t="n">
         <v>151.5</v>
       </c>
+      <c r="CN10" s="3" t="n">
+        <v>136.9</v>
+      </c>
     </row>
     <row r="11" ht="20" customHeight="1">
       <c r="A11" s="1" t="n">
@@ -3738,6 +3771,9 @@
       <c r="CM11" s="1" t="n">
         <v>141.2</v>
       </c>
+      <c r="CN11" s="1" t="n">
+        <v>165.3</v>
+      </c>
     </row>
     <row r="12" ht="20" customHeight="1">
       <c r="A12" s="1" t="n">
@@ -4013,6 +4049,9 @@
       <c r="CM12" s="1" t="n">
         <v>147.6</v>
       </c>
+      <c r="CN12" s="1" t="n">
+        <v>186.1</v>
+      </c>
     </row>
     <row r="13" ht="20" customHeight="1">
       <c r="A13" s="1" t="n">
@@ -4288,6 +4327,9 @@
       <c r="CM13" s="1" t="n">
         <v>176.8</v>
       </c>
+      <c r="CN13" s="1" t="n">
+        <v>159.2</v>
+      </c>
     </row>
     <row r="14" ht="20" customHeight="1">
       <c r="A14" s="1" t="n">
@@ -4563,6 +4605,9 @@
       <c r="CM14" s="1" t="n">
         <v>143.6</v>
       </c>
+      <c r="CN14" s="2" t="n">
+        <v>122.6</v>
+      </c>
     </row>
     <row r="15" ht="20" customHeight="1">
       <c r="A15" s="1" t="n">
@@ -4838,6 +4883,9 @@
       <c r="CM15" s="1" t="n">
         <v>166.2</v>
       </c>
+      <c r="CN15" s="1" t="n">
+        <v>146.4</v>
+      </c>
     </row>
     <row r="16" ht="20" customHeight="1">
       <c r="A16" s="1" t="n">
@@ -5113,6 +5161,9 @@
       <c r="CM16" s="3" t="n">
         <v>132</v>
       </c>
+      <c r="CN16" s="1" t="n">
+        <v>192.5</v>
+      </c>
     </row>
     <row r="17" ht="20" customHeight="1">
       <c r="A17" s="1" t="n">
@@ -5388,6 +5439,9 @@
       <c r="CM17" s="1" t="n">
         <v>225.8</v>
       </c>
+      <c r="CN17" s="1" t="n">
+        <v>163.8</v>
+      </c>
     </row>
     <row r="18" ht="20" customHeight="1">
       <c r="A18" s="1" t="n">
@@ -5663,6 +5717,9 @@
       <c r="CM18" s="1" t="n">
         <v>146.5</v>
       </c>
+      <c r="CN18" s="1" t="n">
+        <v>153.9</v>
+      </c>
     </row>
     <row r="19" ht="20" customHeight="1">
       <c r="A19" s="1" t="n">
@@ -5938,6 +5995,9 @@
       <c r="CM19" s="2" t="n">
         <v>121.7</v>
       </c>
+      <c r="CN19" s="3" t="n">
+        <v>136.3</v>
+      </c>
     </row>
     <row r="20" ht="20" customHeight="1">
       <c r="A20" s="1" t="n">
@@ -6213,6 +6273,9 @@
       <c r="CM20" s="1" t="n">
         <v>146.9</v>
       </c>
+      <c r="CN20" s="1" t="n">
+        <v>178</v>
+      </c>
     </row>
     <row r="21" ht="20" customHeight="1">
       <c r="A21" s="1" t="n">
@@ -6488,6 +6551,9 @@
       <c r="CM21" s="1" t="n">
         <v>164</v>
       </c>
+      <c r="CN21" s="1" t="n">
+        <v>161.3</v>
+      </c>
     </row>
     <row r="22" ht="20" customHeight="1">
       <c r="A22" s="1" t="n">
@@ -6763,6 +6829,9 @@
       <c r="CM22" s="1" t="n">
         <v>180.4</v>
       </c>
+      <c r="CN22" s="1" t="n">
+        <v>257</v>
+      </c>
     </row>
     <row r="23" ht="20" customHeight="1">
       <c r="A23" s="1" t="n">
@@ -7038,6 +7107,9 @@
       <c r="CM23" s="1" t="n">
         <v>140.2</v>
       </c>
+      <c r="CN23" s="3" t="n">
+        <v>134.6</v>
+      </c>
     </row>
     <row r="24" ht="20" customHeight="1">
       <c r="A24" s="1" t="n">
@@ -7313,6 +7385,9 @@
       <c r="CM24" s="1" t="n">
         <v>195.5</v>
       </c>
+      <c r="CN24" s="1" t="n">
+        <v>176.4</v>
+      </c>
     </row>
     <row r="25" ht="20" customHeight="1">
       <c r="A25" s="1" t="n">
@@ -7588,6 +7663,9 @@
       <c r="CM25" s="2" t="n">
         <v>123.4</v>
       </c>
+      <c r="CN25" s="2" t="n">
+        <v>124.6</v>
+      </c>
     </row>
     <row r="26" ht="20" customHeight="1">
       <c r="A26" s="1" t="n">
@@ -7863,6 +7941,9 @@
       <c r="CM26" s="3" t="n">
         <v>126.1</v>
       </c>
+      <c r="CN26" s="1" t="n">
+        <v>164.6</v>
+      </c>
     </row>
     <row r="27" ht="20" customHeight="1">
       <c r="A27" s="1" t="n">
@@ -8138,6 +8219,9 @@
       <c r="CM27" s="1" t="n">
         <v>300.3</v>
       </c>
+      <c r="CN27" s="1" t="n">
+        <v>148.1</v>
+      </c>
     </row>
     <row r="28" ht="20" customHeight="1">
       <c r="A28" s="1" t="n">
@@ -8413,6 +8497,9 @@
       <c r="CM28" s="1" t="n">
         <v>168.8</v>
       </c>
+      <c r="CN28" s="1" t="n">
+        <v>337.7</v>
+      </c>
     </row>
     <row r="29" ht="20" customHeight="1">
       <c r="A29" s="1" t="n">
@@ -8688,6 +8775,9 @@
       <c r="CM29" s="1" t="n">
         <v>173.3</v>
       </c>
+      <c r="CN29" s="1" t="n">
+        <v>184.3</v>
+      </c>
     </row>
     <row r="30" ht="20" customHeight="1">
       <c r="A30" s="1" t="n">
@@ -8963,6 +9053,9 @@
       <c r="CM30" s="1" t="n">
         <v>144.7</v>
       </c>
+      <c r="CN30" s="1" t="n">
+        <v>220.1</v>
+      </c>
     </row>
     <row r="31" ht="20" customHeight="1">
       <c r="A31" s="1" t="n">
@@ -9238,6 +9331,9 @@
       <c r="CM31" s="1" t="n">
         <v>186.9</v>
       </c>
+      <c r="CN31" s="3" t="n">
+        <v>125.1</v>
+      </c>
     </row>
     <row r="32" ht="20" customHeight="1">
       <c r="A32" s="1" t="n">
@@ -9513,6 +9609,9 @@
       <c r="CM32" s="3" t="n">
         <v>136.8</v>
       </c>
+      <c r="CN32" s="1" t="n">
+        <v>142.1</v>
+      </c>
     </row>
     <row r="33" ht="20" customHeight="1">
       <c r="A33" s="1" t="n">
@@ -9788,6 +9887,9 @@
       <c r="CM33" s="1" t="n">
         <v>194.4</v>
       </c>
+      <c r="CN33" s="1" t="n">
+        <v>217.3</v>
+      </c>
     </row>
     <row r="34" ht="20" customHeight="1">
       <c r="A34" s="1" t="n">
@@ -10063,6 +10165,9 @@
       <c r="CM34" s="1" t="n">
         <v>175.2</v>
       </c>
+      <c r="CN34" s="3" t="n">
+        <v>130.7</v>
+      </c>
     </row>
     <row r="35" ht="20" customHeight="1">
       <c r="A35" s="1" t="n">
@@ -10338,6 +10443,9 @@
       <c r="CM35" s="1" t="n">
         <v>140.3</v>
       </c>
+      <c r="CN35" s="1" t="n">
+        <v>150.5</v>
+      </c>
     </row>
     <row r="36" ht="20" customHeight="1">
       <c r="A36" s="1" t="n">
@@ -10613,6 +10721,9 @@
       <c r="CM36" s="1" t="n">
         <v>174.2</v>
       </c>
+      <c r="CN36" s="3" t="n">
+        <v>133.4</v>
+      </c>
     </row>
     <row r="37" ht="20" customHeight="1">
       <c r="A37" s="1" t="n">
@@ -10888,6 +10999,9 @@
       <c r="CM37" s="1" t="n">
         <v>174.5</v>
       </c>
+      <c r="CN37" s="2" t="n">
+        <v>124.4</v>
+      </c>
     </row>
     <row r="38" ht="20" customHeight="1">
       <c r="A38" s="1" t="n">
@@ -11163,6 +11277,9 @@
       <c r="CM38" s="1" t="n">
         <v>145.7</v>
       </c>
+      <c r="CN38" s="1" t="n">
+        <v>221.2</v>
+      </c>
     </row>
     <row r="39" ht="20" customHeight="1">
       <c r="A39" s="1" t="n">
@@ -11438,6 +11555,9 @@
       <c r="CM39" s="1" t="n">
         <v>198.3</v>
       </c>
+      <c r="CN39" s="1" t="n">
+        <v>159.4</v>
+      </c>
     </row>
     <row r="40" ht="20" customHeight="1">
       <c r="A40" s="1" t="n">
@@ -11713,6 +11833,9 @@
       <c r="CM40" s="1" t="n">
         <v>187.7</v>
       </c>
+      <c r="CN40" s="2" t="n">
+        <v>119.8</v>
+      </c>
     </row>
     <row r="41" ht="20" customHeight="1">
       <c r="A41" s="1" t="n">
@@ -11988,6 +12111,9 @@
       <c r="CM41" s="2" t="n">
         <v>116.5</v>
       </c>
+      <c r="CN41" s="1" t="n">
+        <v>145.6</v>
+      </c>
     </row>
     <row r="42" ht="20" customHeight="1">
       <c r="A42" s="1" t="n">
@@ -12263,6 +12389,9 @@
       <c r="CM42" s="1" t="n">
         <v>179</v>
       </c>
+      <c r="CN42" s="1" t="n">
+        <v>147.2</v>
+      </c>
     </row>
     <row r="43" ht="20" customHeight="1">
       <c r="A43" s="1" t="n">
@@ -12538,6 +12667,9 @@
       <c r="CM43" s="1" t="n">
         <v>158.5</v>
       </c>
+      <c r="CN43" s="1" t="n">
+        <v>163.8</v>
+      </c>
     </row>
     <row r="44" ht="20" customHeight="1">
       <c r="A44" s="1" t="n">
@@ -12813,6 +12945,9 @@
       <c r="CM44" s="3" t="n">
         <v>132.3</v>
       </c>
+      <c r="CN44" s="1" t="n">
+        <v>150.4</v>
+      </c>
     </row>
     <row r="45" ht="20" customHeight="1">
       <c r="A45" s="1" t="n">
@@ -13088,6 +13223,9 @@
       <c r="CM45" s="1" t="n">
         <v>409.8</v>
       </c>
+      <c r="CN45" s="3" t="n">
+        <v>136.6</v>
+      </c>
     </row>
     <row r="46" ht="20" customHeight="1">
       <c r="A46" s="1" t="n">
@@ -13363,6 +13501,9 @@
       <c r="CM46" s="1" t="n">
         <v>152.5</v>
       </c>
+      <c r="CN46" s="1" t="n">
+        <v>171.8</v>
+      </c>
     </row>
     <row r="47" ht="20" customHeight="1">
       <c r="A47" s="1" t="n">
@@ -13638,6 +13779,9 @@
       <c r="CM47" s="1" t="n">
         <v>152.3</v>
       </c>
+      <c r="CN47" s="1" t="n">
+        <v>151.7</v>
+      </c>
     </row>
     <row r="48" ht="20" customHeight="1">
       <c r="A48" s="1" t="n">
@@ -13913,6 +14057,9 @@
       <c r="CM48" s="1" t="n">
         <v>197.4</v>
       </c>
+      <c r="CN48" s="1" t="n">
+        <v>218.6</v>
+      </c>
     </row>
     <row r="49" ht="20" customHeight="1">
       <c r="A49" s="1" t="n">
@@ -14188,6 +14335,9 @@
       <c r="CM49" s="1" t="n">
         <v>158.4</v>
       </c>
+      <c r="CN49" s="1" t="n">
+        <v>163.3</v>
+      </c>
     </row>
     <row r="50" ht="20" customHeight="1">
       <c r="A50" s="1" t="n">
@@ -14463,6 +14613,9 @@
       <c r="CM50" s="1" t="n">
         <v>209.8</v>
       </c>
+      <c r="CN50" s="1" t="n">
+        <v>159.9</v>
+      </c>
     </row>
     <row r="51" ht="20" customHeight="1">
       <c r="A51" s="1" t="n">
@@ -14738,6 +14891,9 @@
       <c r="CM51" s="3" t="n">
         <v>127.3</v>
       </c>
+      <c r="CN51" s="1" t="n">
+        <v>161.2</v>
+      </c>
     </row>
     <row r="52" ht="20" customHeight="1">
       <c r="A52" s="1" t="n">
@@ -15013,6 +15169,9 @@
       <c r="CM52" s="1" t="n">
         <v>160.5</v>
       </c>
+      <c r="CN52" s="1" t="n">
+        <v>145.4</v>
+      </c>
     </row>
     <row r="53" ht="20" customHeight="1">
       <c r="A53" s="1" t="n">
@@ -15287,6 +15446,9 @@
       </c>
       <c r="CM53" s="1" t="n">
         <v>154.1</v>
+      </c>
+      <c r="CN53" s="1" t="n">
+        <v>143.9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2024-12-10
</commit_message>
<xml_diff>
--- a/マイジャグラーV_塗りつぶし済み.xlsx
+++ b/マイジャグラーV_塗りつぶし済み.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:CN53"/>
+  <dimension ref="A1:CO53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -531,6 +531,7 @@
     <col width="12" customWidth="1" min="90" max="90"/>
     <col width="12" customWidth="1" min="91" max="91"/>
     <col width="12" customWidth="1" min="92" max="92"/>
+    <col width="12" customWidth="1" min="93" max="93"/>
   </cols>
   <sheetData>
     <row r="1" ht="20" customHeight="1">
@@ -994,6 +995,11 @@
           <t>2024/12/09</t>
         </is>
       </c>
+      <c r="CO1" s="1" t="inlineStr">
+        <is>
+          <t>2024/12/10</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="20" customHeight="1">
       <c r="A2" s="1" t="n">
@@ -1272,6 +1278,9 @@
       <c r="CN2" s="3" t="n">
         <v>138</v>
       </c>
+      <c r="CO2" s="3" t="n">
+        <v>136.8</v>
+      </c>
     </row>
     <row r="3" ht="20" customHeight="1">
       <c r="A3" s="1" t="n">
@@ -1550,6 +1559,9 @@
       <c r="CN3" s="1" t="n">
         <v>266.4</v>
       </c>
+      <c r="CO3" s="1" t="n">
+        <v>153.7</v>
+      </c>
     </row>
     <row r="4" ht="20" customHeight="1">
       <c r="A4" s="1" t="n">
@@ -1828,6 +1840,9 @@
       <c r="CN4" s="1" t="n">
         <v>188.6</v>
       </c>
+      <c r="CO4" s="3" t="n">
+        <v>133</v>
+      </c>
     </row>
     <row r="5" ht="20" customHeight="1">
       <c r="A5" s="1" t="n">
@@ -2106,6 +2121,9 @@
       <c r="CN5" s="1" t="n">
         <v>170.8</v>
       </c>
+      <c r="CO5" s="1" t="n">
+        <v>149.8</v>
+      </c>
     </row>
     <row r="6" ht="20" customHeight="1">
       <c r="A6" s="1" t="n">
@@ -2384,6 +2402,9 @@
       <c r="CN6" s="1" t="n">
         <v>197.6</v>
       </c>
+      <c r="CO6" s="2" t="n">
+        <v>124.1</v>
+      </c>
     </row>
     <row r="7" ht="20" customHeight="1">
       <c r="A7" s="1" t="n">
@@ -2662,6 +2683,9 @@
       <c r="CN7" s="1" t="n">
         <v>143.5</v>
       </c>
+      <c r="CO7" s="2" t="n">
+        <v>121.5</v>
+      </c>
     </row>
     <row r="8" ht="20" customHeight="1">
       <c r="A8" s="1" t="n">
@@ -2940,6 +2964,9 @@
       <c r="CN8" s="1" t="n">
         <v>266.7</v>
       </c>
+      <c r="CO8" s="1" t="n">
+        <v>197.1</v>
+      </c>
     </row>
     <row r="9" ht="20" customHeight="1">
       <c r="A9" s="1" t="n">
@@ -3218,6 +3245,9 @@
       <c r="CN9" s="1" t="n">
         <v>232.2</v>
       </c>
+      <c r="CO9" s="1" t="n">
+        <v>151</v>
+      </c>
     </row>
     <row r="10" ht="20" customHeight="1">
       <c r="A10" s="1" t="n">
@@ -3496,6 +3526,9 @@
       <c r="CN10" s="3" t="n">
         <v>136.9</v>
       </c>
+      <c r="CO10" s="1" t="n">
+        <v>224.8</v>
+      </c>
     </row>
     <row r="11" ht="20" customHeight="1">
       <c r="A11" s="1" t="n">
@@ -3774,6 +3807,9 @@
       <c r="CN11" s="1" t="n">
         <v>165.3</v>
       </c>
+      <c r="CO11" s="1" t="n">
+        <v>178.6</v>
+      </c>
     </row>
     <row r="12" ht="20" customHeight="1">
       <c r="A12" s="1" t="n">
@@ -4052,6 +4088,9 @@
       <c r="CN12" s="1" t="n">
         <v>186.1</v>
       </c>
+      <c r="CO12" s="1" t="n">
+        <v>182.3</v>
+      </c>
     </row>
     <row r="13" ht="20" customHeight="1">
       <c r="A13" s="1" t="n">
@@ -4330,6 +4369,9 @@
       <c r="CN13" s="1" t="n">
         <v>159.2</v>
       </c>
+      <c r="CO13" s="1" t="n">
+        <v>149.7</v>
+      </c>
     </row>
     <row r="14" ht="20" customHeight="1">
       <c r="A14" s="1" t="n">
@@ -4608,6 +4650,9 @@
       <c r="CN14" s="2" t="n">
         <v>122.6</v>
       </c>
+      <c r="CO14" s="1" t="n">
+        <v>184.4</v>
+      </c>
     </row>
     <row r="15" ht="20" customHeight="1">
       <c r="A15" s="1" t="n">
@@ -4886,6 +4931,9 @@
       <c r="CN15" s="1" t="n">
         <v>146.4</v>
       </c>
+      <c r="CO15" s="3" t="n">
+        <v>136.8</v>
+      </c>
     </row>
     <row r="16" ht="20" customHeight="1">
       <c r="A16" s="1" t="n">
@@ -5164,6 +5212,9 @@
       <c r="CN16" s="1" t="n">
         <v>192.5</v>
       </c>
+      <c r="CO16" s="1" t="n">
+        <v>160.1</v>
+      </c>
     </row>
     <row r="17" ht="20" customHeight="1">
       <c r="A17" s="1" t="n">
@@ -5442,6 +5493,9 @@
       <c r="CN17" s="1" t="n">
         <v>163.8</v>
       </c>
+      <c r="CO17" s="1" t="n">
+        <v>179.8</v>
+      </c>
     </row>
     <row r="18" ht="20" customHeight="1">
       <c r="A18" s="1" t="n">
@@ -5720,6 +5774,9 @@
       <c r="CN18" s="1" t="n">
         <v>153.9</v>
       </c>
+      <c r="CO18" s="1" t="n">
+        <v>220.8</v>
+      </c>
     </row>
     <row r="19" ht="20" customHeight="1">
       <c r="A19" s="1" t="n">
@@ -5998,6 +6055,9 @@
       <c r="CN19" s="3" t="n">
         <v>136.3</v>
       </c>
+      <c r="CO19" s="1" t="n">
+        <v>153.8</v>
+      </c>
     </row>
     <row r="20" ht="20" customHeight="1">
       <c r="A20" s="1" t="n">
@@ -6276,6 +6336,9 @@
       <c r="CN20" s="1" t="n">
         <v>178</v>
       </c>
+      <c r="CO20" s="1" t="n">
+        <v>160.7</v>
+      </c>
     </row>
     <row r="21" ht="20" customHeight="1">
       <c r="A21" s="1" t="n">
@@ -6554,6 +6617,9 @@
       <c r="CN21" s="1" t="n">
         <v>161.3</v>
       </c>
+      <c r="CO21" s="3" t="n">
+        <v>136.7</v>
+      </c>
     </row>
     <row r="22" ht="20" customHeight="1">
       <c r="A22" s="1" t="n">
@@ -6832,6 +6898,9 @@
       <c r="CN22" s="1" t="n">
         <v>257</v>
       </c>
+      <c r="CO22" s="1" t="n">
+        <v>149</v>
+      </c>
     </row>
     <row r="23" ht="20" customHeight="1">
       <c r="A23" s="1" t="n">
@@ -7110,6 +7179,9 @@
       <c r="CN23" s="3" t="n">
         <v>134.6</v>
       </c>
+      <c r="CO23" s="1" t="n">
+        <v>175.6</v>
+      </c>
     </row>
     <row r="24" ht="20" customHeight="1">
       <c r="A24" s="1" t="n">
@@ -7388,6 +7460,9 @@
       <c r="CN24" s="1" t="n">
         <v>176.4</v>
       </c>
+      <c r="CO24" s="1" t="n">
+        <v>174.4</v>
+      </c>
     </row>
     <row r="25" ht="20" customHeight="1">
       <c r="A25" s="1" t="n">
@@ -7666,6 +7741,9 @@
       <c r="CN25" s="2" t="n">
         <v>124.6</v>
       </c>
+      <c r="CO25" s="1" t="n">
+        <v>178.5</v>
+      </c>
     </row>
     <row r="26" ht="20" customHeight="1">
       <c r="A26" s="1" t="n">
@@ -7944,6 +8022,9 @@
       <c r="CN26" s="1" t="n">
         <v>164.6</v>
       </c>
+      <c r="CO26" s="1" t="n">
+        <v>204.2</v>
+      </c>
     </row>
     <row r="27" ht="20" customHeight="1">
       <c r="A27" s="1" t="n">
@@ -8222,6 +8303,9 @@
       <c r="CN27" s="1" t="n">
         <v>148.1</v>
       </c>
+      <c r="CO27" s="3" t="n">
+        <v>136.9</v>
+      </c>
     </row>
     <row r="28" ht="20" customHeight="1">
       <c r="A28" s="1" t="n">
@@ -8500,6 +8584,9 @@
       <c r="CN28" s="1" t="n">
         <v>337.7</v>
       </c>
+      <c r="CO28" s="1" t="n">
+        <v>154.3</v>
+      </c>
     </row>
     <row r="29" ht="20" customHeight="1">
       <c r="A29" s="1" t="n">
@@ -8778,6 +8865,9 @@
       <c r="CN29" s="1" t="n">
         <v>184.3</v>
       </c>
+      <c r="CO29" s="1" t="n">
+        <v>168</v>
+      </c>
     </row>
     <row r="30" ht="20" customHeight="1">
       <c r="A30" s="1" t="n">
@@ -9056,6 +9146,9 @@
       <c r="CN30" s="1" t="n">
         <v>220.1</v>
       </c>
+      <c r="CO30" s="3" t="n">
+        <v>132.1</v>
+      </c>
     </row>
     <row r="31" ht="20" customHeight="1">
       <c r="A31" s="1" t="n">
@@ -9334,6 +9427,9 @@
       <c r="CN31" s="3" t="n">
         <v>125.1</v>
       </c>
+      <c r="CO31" s="1" t="n">
+        <v>155.6</v>
+      </c>
     </row>
     <row r="32" ht="20" customHeight="1">
       <c r="A32" s="1" t="n">
@@ -9612,6 +9708,9 @@
       <c r="CN32" s="1" t="n">
         <v>142.1</v>
       </c>
+      <c r="CO32" s="1" t="n">
+        <v>170.5</v>
+      </c>
     </row>
     <row r="33" ht="20" customHeight="1">
       <c r="A33" s="1" t="n">
@@ -9890,6 +9989,9 @@
       <c r="CN33" s="1" t="n">
         <v>217.3</v>
       </c>
+      <c r="CO33" s="1" t="n">
+        <v>143.8</v>
+      </c>
     </row>
     <row r="34" ht="20" customHeight="1">
       <c r="A34" s="1" t="n">
@@ -10168,6 +10270,9 @@
       <c r="CN34" s="3" t="n">
         <v>130.7</v>
       </c>
+      <c r="CO34" s="1" t="n">
+        <v>142.6</v>
+      </c>
     </row>
     <row r="35" ht="20" customHeight="1">
       <c r="A35" s="1" t="n">
@@ -10446,6 +10551,9 @@
       <c r="CN35" s="1" t="n">
         <v>150.5</v>
       </c>
+      <c r="CO35" s="2" t="n">
+        <v>119.4</v>
+      </c>
     </row>
     <row r="36" ht="20" customHeight="1">
       <c r="A36" s="1" t="n">
@@ -10724,6 +10832,9 @@
       <c r="CN36" s="3" t="n">
         <v>133.4</v>
       </c>
+      <c r="CO36" s="1" t="n">
+        <v>171.5</v>
+      </c>
     </row>
     <row r="37" ht="20" customHeight="1">
       <c r="A37" s="1" t="n">
@@ -11002,6 +11113,9 @@
       <c r="CN37" s="2" t="n">
         <v>124.4</v>
       </c>
+      <c r="CO37" s="1" t="n">
+        <v>192.7</v>
+      </c>
     </row>
     <row r="38" ht="20" customHeight="1">
       <c r="A38" s="1" t="n">
@@ -11280,6 +11394,9 @@
       <c r="CN38" s="1" t="n">
         <v>221.2</v>
       </c>
+      <c r="CO38" s="1" t="n">
+        <v>193</v>
+      </c>
     </row>
     <row r="39" ht="20" customHeight="1">
       <c r="A39" s="1" t="n">
@@ -11558,6 +11675,9 @@
       <c r="CN39" s="1" t="n">
         <v>159.4</v>
       </c>
+      <c r="CO39" s="1" t="n">
+        <v>340.6</v>
+      </c>
     </row>
     <row r="40" ht="20" customHeight="1">
       <c r="A40" s="1" t="n">
@@ -11836,6 +11956,9 @@
       <c r="CN40" s="2" t="n">
         <v>119.8</v>
       </c>
+      <c r="CO40" s="1" t="n">
+        <v>215.4</v>
+      </c>
     </row>
     <row r="41" ht="20" customHeight="1">
       <c r="A41" s="1" t="n">
@@ -12114,6 +12237,9 @@
       <c r="CN41" s="1" t="n">
         <v>145.6</v>
       </c>
+      <c r="CO41" s="3" t="n">
+        <v>130</v>
+      </c>
     </row>
     <row r="42" ht="20" customHeight="1">
       <c r="A42" s="1" t="n">
@@ -12392,6 +12518,9 @@
       <c r="CN42" s="1" t="n">
         <v>147.2</v>
       </c>
+      <c r="CO42" s="3" t="n">
+        <v>137.7</v>
+      </c>
     </row>
     <row r="43" ht="20" customHeight="1">
       <c r="A43" s="1" t="n">
@@ -12670,6 +12799,9 @@
       <c r="CN43" s="1" t="n">
         <v>163.8</v>
       </c>
+      <c r="CO43" s="1" t="n">
+        <v>153.1</v>
+      </c>
     </row>
     <row r="44" ht="20" customHeight="1">
       <c r="A44" s="1" t="n">
@@ -12948,6 +13080,9 @@
       <c r="CN44" s="1" t="n">
         <v>150.4</v>
       </c>
+      <c r="CO44" s="1" t="n">
+        <v>140.6</v>
+      </c>
     </row>
     <row r="45" ht="20" customHeight="1">
       <c r="A45" s="1" t="n">
@@ -13226,6 +13361,9 @@
       <c r="CN45" s="3" t="n">
         <v>136.6</v>
       </c>
+      <c r="CO45" s="1" t="n">
+        <v>178.3</v>
+      </c>
     </row>
     <row r="46" ht="20" customHeight="1">
       <c r="A46" s="1" t="n">
@@ -13504,6 +13642,9 @@
       <c r="CN46" s="1" t="n">
         <v>171.8</v>
       </c>
+      <c r="CO46" s="3" t="n">
+        <v>131.3</v>
+      </c>
     </row>
     <row r="47" ht="20" customHeight="1">
       <c r="A47" s="1" t="n">
@@ -13782,6 +13923,9 @@
       <c r="CN47" s="1" t="n">
         <v>151.7</v>
       </c>
+      <c r="CO47" s="2" t="n">
+        <v>110.4</v>
+      </c>
     </row>
     <row r="48" ht="20" customHeight="1">
       <c r="A48" s="1" t="n">
@@ -14060,6 +14204,9 @@
       <c r="CN48" s="1" t="n">
         <v>218.6</v>
       </c>
+      <c r="CO48" s="2" t="n">
+        <v>114.4</v>
+      </c>
     </row>
     <row r="49" ht="20" customHeight="1">
       <c r="A49" s="1" t="n">
@@ -14338,6 +14485,9 @@
       <c r="CN49" s="1" t="n">
         <v>163.3</v>
       </c>
+      <c r="CO49" s="1" t="n">
+        <v>181.8</v>
+      </c>
     </row>
     <row r="50" ht="20" customHeight="1">
       <c r="A50" s="1" t="n">
@@ -14616,6 +14766,9 @@
       <c r="CN50" s="1" t="n">
         <v>159.9</v>
       </c>
+      <c r="CO50" s="1" t="n">
+        <v>163.1</v>
+      </c>
     </row>
     <row r="51" ht="20" customHeight="1">
       <c r="A51" s="1" t="n">
@@ -14894,6 +15047,9 @@
       <c r="CN51" s="1" t="n">
         <v>161.2</v>
       </c>
+      <c r="CO51" s="1" t="n">
+        <v>154.4</v>
+      </c>
     </row>
     <row r="52" ht="20" customHeight="1">
       <c r="A52" s="1" t="n">
@@ -15172,6 +15328,9 @@
       <c r="CN52" s="1" t="n">
         <v>145.4</v>
       </c>
+      <c r="CO52" s="1" t="n">
+        <v>222.2</v>
+      </c>
     </row>
     <row r="53" ht="20" customHeight="1">
       <c r="A53" s="1" t="n">
@@ -15449,6 +15608,9 @@
       </c>
       <c r="CN53" s="1" t="n">
         <v>143.9</v>
+      </c>
+      <c r="CO53" s="3" t="n">
+        <v>136.7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2024-12-11
</commit_message>
<xml_diff>
--- a/マイジャグラーV_塗りつぶし済み.xlsx
+++ b/マイジャグラーV_塗りつぶし済み.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:CO53"/>
+  <dimension ref="A1:CP53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -532,6 +532,7 @@
     <col width="12" customWidth="1" min="91" max="91"/>
     <col width="12" customWidth="1" min="92" max="92"/>
     <col width="12" customWidth="1" min="93" max="93"/>
+    <col width="12" customWidth="1" min="94" max="94"/>
   </cols>
   <sheetData>
     <row r="1" ht="20" customHeight="1">
@@ -1000,6 +1001,11 @@
           <t>2024/12/10</t>
         </is>
       </c>
+      <c r="CP1" s="1" t="inlineStr">
+        <is>
+          <t>2024/12/11</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="20" customHeight="1">
       <c r="A2" s="1" t="n">
@@ -1281,6 +1287,9 @@
       <c r="CO2" s="3" t="n">
         <v>136.8</v>
       </c>
+      <c r="CP2" s="1" t="n">
+        <v>195.6</v>
+      </c>
     </row>
     <row r="3" ht="20" customHeight="1">
       <c r="A3" s="1" t="n">
@@ -1562,6 +1571,9 @@
       <c r="CO3" s="1" t="n">
         <v>153.7</v>
       </c>
+      <c r="CP3" s="2" t="n">
+        <v>119.7</v>
+      </c>
     </row>
     <row r="4" ht="20" customHeight="1">
       <c r="A4" s="1" t="n">
@@ -1843,6 +1855,9 @@
       <c r="CO4" s="3" t="n">
         <v>133</v>
       </c>
+      <c r="CP4" s="1" t="n">
+        <v>140</v>
+      </c>
     </row>
     <row r="5" ht="20" customHeight="1">
       <c r="A5" s="1" t="n">
@@ -2124,6 +2139,9 @@
       <c r="CO5" s="1" t="n">
         <v>149.8</v>
       </c>
+      <c r="CP5" s="1" t="n">
+        <v>249</v>
+      </c>
     </row>
     <row r="6" ht="20" customHeight="1">
       <c r="A6" s="1" t="n">
@@ -2405,6 +2423,9 @@
       <c r="CO6" s="2" t="n">
         <v>124.1</v>
       </c>
+      <c r="CP6" s="1" t="n">
+        <v>162.9</v>
+      </c>
     </row>
     <row r="7" ht="20" customHeight="1">
       <c r="A7" s="1" t="n">
@@ -2686,6 +2707,9 @@
       <c r="CO7" s="2" t="n">
         <v>121.5</v>
       </c>
+      <c r="CP7" s="1" t="n">
+        <v>216.1</v>
+      </c>
     </row>
     <row r="8" ht="20" customHeight="1">
       <c r="A8" s="1" t="n">
@@ -2967,6 +2991,9 @@
       <c r="CO8" s="1" t="n">
         <v>197.1</v>
       </c>
+      <c r="CP8" s="1" t="n">
+        <v>170.2</v>
+      </c>
     </row>
     <row r="9" ht="20" customHeight="1">
       <c r="A9" s="1" t="n">
@@ -3248,6 +3275,9 @@
       <c r="CO9" s="1" t="n">
         <v>151</v>
       </c>
+      <c r="CP9" s="2" t="n">
+        <v>123.8</v>
+      </c>
     </row>
     <row r="10" ht="20" customHeight="1">
       <c r="A10" s="1" t="n">
@@ -3529,6 +3559,9 @@
       <c r="CO10" s="1" t="n">
         <v>224.8</v>
       </c>
+      <c r="CP10" s="1" t="n">
+        <v>145.3</v>
+      </c>
     </row>
     <row r="11" ht="20" customHeight="1">
       <c r="A11" s="1" t="n">
@@ -3810,6 +3843,9 @@
       <c r="CO11" s="1" t="n">
         <v>178.6</v>
       </c>
+      <c r="CP11" s="1" t="n">
+        <v>175.8</v>
+      </c>
     </row>
     <row r="12" ht="20" customHeight="1">
       <c r="A12" s="1" t="n">
@@ -4091,6 +4127,9 @@
       <c r="CO12" s="1" t="n">
         <v>182.3</v>
       </c>
+      <c r="CP12" s="3" t="n">
+        <v>138.6</v>
+      </c>
     </row>
     <row r="13" ht="20" customHeight="1">
       <c r="A13" s="1" t="n">
@@ -4372,6 +4411,9 @@
       <c r="CO13" s="1" t="n">
         <v>149.7</v>
       </c>
+      <c r="CP13" s="1" t="n">
+        <v>145.9</v>
+      </c>
     </row>
     <row r="14" ht="20" customHeight="1">
       <c r="A14" s="1" t="n">
@@ -4653,6 +4695,9 @@
       <c r="CO14" s="1" t="n">
         <v>184.4</v>
       </c>
+      <c r="CP14" s="1" t="n">
+        <v>203.5</v>
+      </c>
     </row>
     <row r="15" ht="20" customHeight="1">
       <c r="A15" s="1" t="n">
@@ -4934,6 +4979,9 @@
       <c r="CO15" s="3" t="n">
         <v>136.8</v>
       </c>
+      <c r="CP15" s="1" t="n">
+        <v>147.7</v>
+      </c>
     </row>
     <row r="16" ht="20" customHeight="1">
       <c r="A16" s="1" t="n">
@@ -5215,6 +5263,9 @@
       <c r="CO16" s="1" t="n">
         <v>160.1</v>
       </c>
+      <c r="CP16" s="3" t="n">
+        <v>137.4</v>
+      </c>
     </row>
     <row r="17" ht="20" customHeight="1">
       <c r="A17" s="1" t="n">
@@ -5496,6 +5547,9 @@
       <c r="CO17" s="1" t="n">
         <v>179.8</v>
       </c>
+      <c r="CP17" s="3" t="n">
+        <v>128.8</v>
+      </c>
     </row>
     <row r="18" ht="20" customHeight="1">
       <c r="A18" s="1" t="n">
@@ -5777,6 +5831,9 @@
       <c r="CO18" s="1" t="n">
         <v>220.8</v>
       </c>
+      <c r="CP18" s="1" t="n">
+        <v>164.6</v>
+      </c>
     </row>
     <row r="19" ht="20" customHeight="1">
       <c r="A19" s="1" t="n">
@@ -6058,6 +6115,9 @@
       <c r="CO19" s="1" t="n">
         <v>153.8</v>
       </c>
+      <c r="CP19" s="1" t="n">
+        <v>249.8</v>
+      </c>
     </row>
     <row r="20" ht="20" customHeight="1">
       <c r="A20" s="1" t="n">
@@ -6339,6 +6399,9 @@
       <c r="CO20" s="1" t="n">
         <v>160.7</v>
       </c>
+      <c r="CP20" s="3" t="n">
+        <v>130.6</v>
+      </c>
     </row>
     <row r="21" ht="20" customHeight="1">
       <c r="A21" s="1" t="n">
@@ -6620,6 +6683,9 @@
       <c r="CO21" s="3" t="n">
         <v>136.7</v>
       </c>
+      <c r="CP21" s="2" t="n">
+        <v>116.8</v>
+      </c>
     </row>
     <row r="22" ht="20" customHeight="1">
       <c r="A22" s="1" t="n">
@@ -6901,6 +6967,9 @@
       <c r="CO22" s="1" t="n">
         <v>149</v>
       </c>
+      <c r="CP22" s="3" t="n">
+        <v>131</v>
+      </c>
     </row>
     <row r="23" ht="20" customHeight="1">
       <c r="A23" s="1" t="n">
@@ -7182,6 +7251,9 @@
       <c r="CO23" s="1" t="n">
         <v>175.6</v>
       </c>
+      <c r="CP23" s="2" t="n">
+        <v>109.9</v>
+      </c>
     </row>
     <row r="24" ht="20" customHeight="1">
       <c r="A24" s="1" t="n">
@@ -7463,6 +7535,9 @@
       <c r="CO24" s="1" t="n">
         <v>174.4</v>
       </c>
+      <c r="CP24" s="1" t="n">
+        <v>206.1</v>
+      </c>
     </row>
     <row r="25" ht="20" customHeight="1">
       <c r="A25" s="1" t="n">
@@ -7744,6 +7819,9 @@
       <c r="CO25" s="1" t="n">
         <v>178.5</v>
       </c>
+      <c r="CP25" s="3" t="n">
+        <v>130.8</v>
+      </c>
     </row>
     <row r="26" ht="20" customHeight="1">
       <c r="A26" s="1" t="n">
@@ -8025,6 +8103,9 @@
       <c r="CO26" s="1" t="n">
         <v>204.2</v>
       </c>
+      <c r="CP26" s="3" t="n">
+        <v>126.9</v>
+      </c>
     </row>
     <row r="27" ht="20" customHeight="1">
       <c r="A27" s="1" t="n">
@@ -8306,6 +8387,9 @@
       <c r="CO27" s="3" t="n">
         <v>136.9</v>
       </c>
+      <c r="CP27" s="1" t="n">
+        <v>191.9</v>
+      </c>
     </row>
     <row r="28" ht="20" customHeight="1">
       <c r="A28" s="1" t="n">
@@ -8587,6 +8671,9 @@
       <c r="CO28" s="1" t="n">
         <v>154.3</v>
       </c>
+      <c r="CP28" s="3" t="n">
+        <v>132.6</v>
+      </c>
     </row>
     <row r="29" ht="20" customHeight="1">
       <c r="A29" s="1" t="n">
@@ -8868,6 +8955,9 @@
       <c r="CO29" s="1" t="n">
         <v>168</v>
       </c>
+      <c r="CP29" s="2" t="n">
+        <v>124</v>
+      </c>
     </row>
     <row r="30" ht="20" customHeight="1">
       <c r="A30" s="1" t="n">
@@ -9149,6 +9239,9 @@
       <c r="CO30" s="3" t="n">
         <v>132.1</v>
       </c>
+      <c r="CP30" s="1" t="n">
+        <v>159.8</v>
+      </c>
     </row>
     <row r="31" ht="20" customHeight="1">
       <c r="A31" s="1" t="n">
@@ -9430,6 +9523,9 @@
       <c r="CO31" s="1" t="n">
         <v>155.6</v>
       </c>
+      <c r="CP31" s="1" t="n">
+        <v>157.5</v>
+      </c>
     </row>
     <row r="32" ht="20" customHeight="1">
       <c r="A32" s="1" t="n">
@@ -9711,6 +9807,9 @@
       <c r="CO32" s="1" t="n">
         <v>170.5</v>
       </c>
+      <c r="CP32" s="1" t="n">
+        <v>141.2</v>
+      </c>
     </row>
     <row r="33" ht="20" customHeight="1">
       <c r="A33" s="1" t="n">
@@ -9992,6 +10091,9 @@
       <c r="CO33" s="1" t="n">
         <v>143.8</v>
       </c>
+      <c r="CP33" s="3" t="n">
+        <v>129.9</v>
+      </c>
     </row>
     <row r="34" ht="20" customHeight="1">
       <c r="A34" s="1" t="n">
@@ -10273,6 +10375,9 @@
       <c r="CO34" s="1" t="n">
         <v>142.6</v>
       </c>
+      <c r="CP34" s="1" t="n">
+        <v>422.3</v>
+      </c>
     </row>
     <row r="35" ht="20" customHeight="1">
       <c r="A35" s="1" t="n">
@@ -10554,6 +10659,9 @@
       <c r="CO35" s="2" t="n">
         <v>119.4</v>
       </c>
+      <c r="CP35" s="1" t="n">
+        <v>171.4</v>
+      </c>
     </row>
     <row r="36" ht="20" customHeight="1">
       <c r="A36" s="1" t="n">
@@ -10835,6 +10943,9 @@
       <c r="CO36" s="1" t="n">
         <v>171.5</v>
       </c>
+      <c r="CP36" s="3" t="n">
+        <v>127.8</v>
+      </c>
     </row>
     <row r="37" ht="20" customHeight="1">
       <c r="A37" s="1" t="n">
@@ -11116,6 +11227,9 @@
       <c r="CO37" s="1" t="n">
         <v>192.7</v>
       </c>
+      <c r="CP37" s="1" t="n">
+        <v>141.2</v>
+      </c>
     </row>
     <row r="38" ht="20" customHeight="1">
       <c r="A38" s="1" t="n">
@@ -11397,6 +11511,9 @@
       <c r="CO38" s="1" t="n">
         <v>193</v>
       </c>
+      <c r="CP38" s="1" t="n">
+        <v>174.1</v>
+      </c>
     </row>
     <row r="39" ht="20" customHeight="1">
       <c r="A39" s="1" t="n">
@@ -11678,6 +11795,9 @@
       <c r="CO39" s="1" t="n">
         <v>340.6</v>
       </c>
+      <c r="CP39" s="3" t="n">
+        <v>125.7</v>
+      </c>
     </row>
     <row r="40" ht="20" customHeight="1">
       <c r="A40" s="1" t="n">
@@ -11959,6 +12079,9 @@
       <c r="CO40" s="1" t="n">
         <v>215.4</v>
       </c>
+      <c r="CP40" s="1" t="n">
+        <v>149.8</v>
+      </c>
     </row>
     <row r="41" ht="20" customHeight="1">
       <c r="A41" s="1" t="n">
@@ -12240,6 +12363,9 @@
       <c r="CO41" s="3" t="n">
         <v>130</v>
       </c>
+      <c r="CP41" s="3" t="n">
+        <v>129.8</v>
+      </c>
     </row>
     <row r="42" ht="20" customHeight="1">
       <c r="A42" s="1" t="n">
@@ -12521,6 +12647,9 @@
       <c r="CO42" s="3" t="n">
         <v>137.7</v>
       </c>
+      <c r="CP42" s="2" t="n">
+        <v>122.1</v>
+      </c>
     </row>
     <row r="43" ht="20" customHeight="1">
       <c r="A43" s="1" t="n">
@@ -12802,6 +12931,9 @@
       <c r="CO43" s="1" t="n">
         <v>153.1</v>
       </c>
+      <c r="CP43" s="1" t="n">
+        <v>171.8</v>
+      </c>
     </row>
     <row r="44" ht="20" customHeight="1">
       <c r="A44" s="1" t="n">
@@ -13083,6 +13215,9 @@
       <c r="CO44" s="1" t="n">
         <v>140.6</v>
       </c>
+      <c r="CP44" s="1" t="n">
+        <v>175.9</v>
+      </c>
     </row>
     <row r="45" ht="20" customHeight="1">
       <c r="A45" s="1" t="n">
@@ -13364,6 +13499,9 @@
       <c r="CO45" s="1" t="n">
         <v>178.3</v>
       </c>
+      <c r="CP45" s="1" t="n">
+        <v>162.5</v>
+      </c>
     </row>
     <row r="46" ht="20" customHeight="1">
       <c r="A46" s="1" t="n">
@@ -13645,6 +13783,9 @@
       <c r="CO46" s="3" t="n">
         <v>131.3</v>
       </c>
+      <c r="CP46" s="1" t="n">
+        <v>302.8</v>
+      </c>
     </row>
     <row r="47" ht="20" customHeight="1">
       <c r="A47" s="1" t="n">
@@ -13926,6 +14067,9 @@
       <c r="CO47" s="2" t="n">
         <v>110.4</v>
       </c>
+      <c r="CP47" s="3" t="n">
+        <v>136.6</v>
+      </c>
     </row>
     <row r="48" ht="20" customHeight="1">
       <c r="A48" s="1" t="n">
@@ -14207,6 +14351,9 @@
       <c r="CO48" s="2" t="n">
         <v>114.4</v>
       </c>
+      <c r="CP48" s="1" t="n">
+        <v>168.4</v>
+      </c>
     </row>
     <row r="49" ht="20" customHeight="1">
       <c r="A49" s="1" t="n">
@@ -14488,6 +14635,9 @@
       <c r="CO49" s="1" t="n">
         <v>181.8</v>
       </c>
+      <c r="CP49" s="1" t="n">
+        <v>141.1</v>
+      </c>
     </row>
     <row r="50" ht="20" customHeight="1">
       <c r="A50" s="1" t="n">
@@ -14769,6 +14919,9 @@
       <c r="CO50" s="1" t="n">
         <v>163.1</v>
       </c>
+      <c r="CP50" s="3" t="n">
+        <v>129.3</v>
+      </c>
     </row>
     <row r="51" ht="20" customHeight="1">
       <c r="A51" s="1" t="n">
@@ -15050,6 +15203,9 @@
       <c r="CO51" s="1" t="n">
         <v>154.4</v>
       </c>
+      <c r="CP51" s="1" t="n">
+        <v>213.5</v>
+      </c>
     </row>
     <row r="52" ht="20" customHeight="1">
       <c r="A52" s="1" t="n">
@@ -15331,6 +15487,9 @@
       <c r="CO52" s="1" t="n">
         <v>222.2</v>
       </c>
+      <c r="CP52" s="1" t="n">
+        <v>165.3</v>
+      </c>
     </row>
     <row r="53" ht="20" customHeight="1">
       <c r="A53" s="1" t="n">
@@ -15611,6 +15770,9 @@
       </c>
       <c r="CO53" s="3" t="n">
         <v>136.7</v>
+      </c>
+      <c r="CP53" s="3" t="n">
+        <v>127.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2024-12-12
</commit_message>
<xml_diff>
--- a/マイジャグラーV_塗りつぶし済み.xlsx
+++ b/マイジャグラーV_塗りつぶし済み.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:CP53"/>
+  <dimension ref="A1:CQ53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -533,6 +533,7 @@
     <col width="12" customWidth="1" min="92" max="92"/>
     <col width="12" customWidth="1" min="93" max="93"/>
     <col width="12" customWidth="1" min="94" max="94"/>
+    <col width="12" customWidth="1" min="95" max="95"/>
   </cols>
   <sheetData>
     <row r="1" ht="20" customHeight="1">
@@ -1006,6 +1007,11 @@
           <t>2024/12/11</t>
         </is>
       </c>
+      <c r="CQ1" s="1" t="inlineStr">
+        <is>
+          <t>2024/12/12</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="20" customHeight="1">
       <c r="A2" s="1" t="n">
@@ -1290,6 +1296,9 @@
       <c r="CP2" s="1" t="n">
         <v>195.6</v>
       </c>
+      <c r="CQ2" s="1" t="n">
+        <v>186.3</v>
+      </c>
     </row>
     <row r="3" ht="20" customHeight="1">
       <c r="A3" s="1" t="n">
@@ -1574,6 +1583,9 @@
       <c r="CP3" s="2" t="n">
         <v>119.7</v>
       </c>
+      <c r="CQ3" s="1" t="n">
+        <v>192.4</v>
+      </c>
     </row>
     <row r="4" ht="20" customHeight="1">
       <c r="A4" s="1" t="n">
@@ -1858,6 +1870,9 @@
       <c r="CP4" s="1" t="n">
         <v>140</v>
       </c>
+      <c r="CQ4" s="1" t="n">
+        <v>188.2</v>
+      </c>
     </row>
     <row r="5" ht="20" customHeight="1">
       <c r="A5" s="1" t="n">
@@ -2142,6 +2157,9 @@
       <c r="CP5" s="1" t="n">
         <v>249</v>
       </c>
+      <c r="CQ5" s="3" t="n">
+        <v>136.9</v>
+      </c>
     </row>
     <row r="6" ht="20" customHeight="1">
       <c r="A6" s="1" t="n">
@@ -2426,6 +2444,9 @@
       <c r="CP6" s="1" t="n">
         <v>162.9</v>
       </c>
+      <c r="CQ6" s="3" t="n">
+        <v>128.7</v>
+      </c>
     </row>
     <row r="7" ht="20" customHeight="1">
       <c r="A7" s="1" t="n">
@@ -2710,6 +2731,9 @@
       <c r="CP7" s="1" t="n">
         <v>216.1</v>
       </c>
+      <c r="CQ7" s="2" t="n">
+        <v>114</v>
+      </c>
     </row>
     <row r="8" ht="20" customHeight="1">
       <c r="A8" s="1" t="n">
@@ -2994,6 +3018,9 @@
       <c r="CP8" s="1" t="n">
         <v>170.2</v>
       </c>
+      <c r="CQ8" s="3" t="n">
+        <v>127.6</v>
+      </c>
     </row>
     <row r="9" ht="20" customHeight="1">
       <c r="A9" s="1" t="n">
@@ -3278,6 +3305,9 @@
       <c r="CP9" s="2" t="n">
         <v>123.8</v>
       </c>
+      <c r="CQ9" s="2" t="n">
+        <v>124</v>
+      </c>
     </row>
     <row r="10" ht="20" customHeight="1">
       <c r="A10" s="1" t="n">
@@ -3562,6 +3592,9 @@
       <c r="CP10" s="1" t="n">
         <v>145.3</v>
       </c>
+      <c r="CQ10" s="1" t="n">
+        <v>226.2</v>
+      </c>
     </row>
     <row r="11" ht="20" customHeight="1">
       <c r="A11" s="1" t="n">
@@ -3846,6 +3879,9 @@
       <c r="CP11" s="1" t="n">
         <v>175.8</v>
       </c>
+      <c r="CQ11" s="1" t="n">
+        <v>176.1</v>
+      </c>
     </row>
     <row r="12" ht="20" customHeight="1">
       <c r="A12" s="1" t="n">
@@ -4130,6 +4166,9 @@
       <c r="CP12" s="3" t="n">
         <v>138.6</v>
       </c>
+      <c r="CQ12" s="1" t="n">
+        <v>143.6</v>
+      </c>
     </row>
     <row r="13" ht="20" customHeight="1">
       <c r="A13" s="1" t="n">
@@ -4414,6 +4453,9 @@
       <c r="CP13" s="1" t="n">
         <v>145.9</v>
       </c>
+      <c r="CQ13" s="2" t="n">
+        <v>124.4</v>
+      </c>
     </row>
     <row r="14" ht="20" customHeight="1">
       <c r="A14" s="1" t="n">
@@ -4698,6 +4740,9 @@
       <c r="CP14" s="1" t="n">
         <v>203.5</v>
       </c>
+      <c r="CQ14" s="3" t="n">
+        <v>136.7</v>
+      </c>
     </row>
     <row r="15" ht="20" customHeight="1">
       <c r="A15" s="1" t="n">
@@ -4982,6 +5027,9 @@
       <c r="CP15" s="1" t="n">
         <v>147.7</v>
       </c>
+      <c r="CQ15" s="1" t="n">
+        <v>157.2</v>
+      </c>
     </row>
     <row r="16" ht="20" customHeight="1">
       <c r="A16" s="1" t="n">
@@ -5266,6 +5314,9 @@
       <c r="CP16" s="3" t="n">
         <v>137.4</v>
       </c>
+      <c r="CQ16" s="1" t="n">
+        <v>158.5</v>
+      </c>
     </row>
     <row r="17" ht="20" customHeight="1">
       <c r="A17" s="1" t="n">
@@ -5550,6 +5601,9 @@
       <c r="CP17" s="3" t="n">
         <v>128.8</v>
       </c>
+      <c r="CQ17" s="1" t="n">
+        <v>157.2</v>
+      </c>
     </row>
     <row r="18" ht="20" customHeight="1">
       <c r="A18" s="1" t="n">
@@ -5834,6 +5888,9 @@
       <c r="CP18" s="1" t="n">
         <v>164.6</v>
       </c>
+      <c r="CQ18" s="3" t="n">
+        <v>137.7</v>
+      </c>
     </row>
     <row r="19" ht="20" customHeight="1">
       <c r="A19" s="1" t="n">
@@ -6118,6 +6175,9 @@
       <c r="CP19" s="1" t="n">
         <v>249.8</v>
       </c>
+      <c r="CQ19" s="3" t="n">
+        <v>139.8</v>
+      </c>
     </row>
     <row r="20" ht="20" customHeight="1">
       <c r="A20" s="1" t="n">
@@ -6402,6 +6462,9 @@
       <c r="CP20" s="3" t="n">
         <v>130.6</v>
       </c>
+      <c r="CQ20" s="1" t="n">
+        <v>150.5</v>
+      </c>
     </row>
     <row r="21" ht="20" customHeight="1">
       <c r="A21" s="1" t="n">
@@ -6686,6 +6749,9 @@
       <c r="CP21" s="2" t="n">
         <v>116.8</v>
       </c>
+      <c r="CQ21" s="3" t="n">
+        <v>136.9</v>
+      </c>
     </row>
     <row r="22" ht="20" customHeight="1">
       <c r="A22" s="1" t="n">
@@ -6970,6 +7036,9 @@
       <c r="CP22" s="3" t="n">
         <v>131</v>
       </c>
+      <c r="CQ22" s="1" t="n">
+        <v>168.5</v>
+      </c>
     </row>
     <row r="23" ht="20" customHeight="1">
       <c r="A23" s="1" t="n">
@@ -7254,6 +7323,9 @@
       <c r="CP23" s="2" t="n">
         <v>109.9</v>
       </c>
+      <c r="CQ23" s="1" t="n">
+        <v>148.1</v>
+      </c>
     </row>
     <row r="24" ht="20" customHeight="1">
       <c r="A24" s="1" t="n">
@@ -7538,6 +7610,9 @@
       <c r="CP24" s="1" t="n">
         <v>206.1</v>
       </c>
+      <c r="CQ24" s="1" t="n">
+        <v>152.8</v>
+      </c>
     </row>
     <row r="25" ht="20" customHeight="1">
       <c r="A25" s="1" t="n">
@@ -7822,6 +7897,9 @@
       <c r="CP25" s="3" t="n">
         <v>130.8</v>
       </c>
+      <c r="CQ25" s="2" t="n">
+        <v>111.2</v>
+      </c>
     </row>
     <row r="26" ht="20" customHeight="1">
       <c r="A26" s="1" t="n">
@@ -8106,6 +8184,9 @@
       <c r="CP26" s="3" t="n">
         <v>126.9</v>
       </c>
+      <c r="CQ26" s="1" t="n">
+        <v>186.9</v>
+      </c>
     </row>
     <row r="27" ht="20" customHeight="1">
       <c r="A27" s="1" t="n">
@@ -8390,6 +8471,9 @@
       <c r="CP27" s="1" t="n">
         <v>191.9</v>
       </c>
+      <c r="CQ27" s="1" t="n">
+        <v>160.3</v>
+      </c>
     </row>
     <row r="28" ht="20" customHeight="1">
       <c r="A28" s="1" t="n">
@@ -8674,6 +8758,9 @@
       <c r="CP28" s="3" t="n">
         <v>132.6</v>
       </c>
+      <c r="CQ28" s="1" t="n">
+        <v>178.9</v>
+      </c>
     </row>
     <row r="29" ht="20" customHeight="1">
       <c r="A29" s="1" t="n">
@@ -8958,6 +9045,9 @@
       <c r="CP29" s="2" t="n">
         <v>124</v>
       </c>
+      <c r="CQ29" s="1" t="n">
+        <v>162.3</v>
+      </c>
     </row>
     <row r="30" ht="20" customHeight="1">
       <c r="A30" s="1" t="n">
@@ -9242,6 +9332,9 @@
       <c r="CP30" s="1" t="n">
         <v>159.8</v>
       </c>
+      <c r="CQ30" s="3" t="n">
+        <v>132.4</v>
+      </c>
     </row>
     <row r="31" ht="20" customHeight="1">
       <c r="A31" s="1" t="n">
@@ -9526,6 +9619,9 @@
       <c r="CP31" s="1" t="n">
         <v>157.5</v>
       </c>
+      <c r="CQ31" s="1" t="n">
+        <v>183.6</v>
+      </c>
     </row>
     <row r="32" ht="20" customHeight="1">
       <c r="A32" s="1" t="n">
@@ -9810,6 +9906,9 @@
       <c r="CP32" s="1" t="n">
         <v>141.2</v>
       </c>
+      <c r="CQ32" s="1" t="n">
+        <v>200.5</v>
+      </c>
     </row>
     <row r="33" ht="20" customHeight="1">
       <c r="A33" s="1" t="n">
@@ -10094,6 +10193,9 @@
       <c r="CP33" s="3" t="n">
         <v>129.9</v>
       </c>
+      <c r="CQ33" s="3" t="n">
+        <v>128.8</v>
+      </c>
     </row>
     <row r="34" ht="20" customHeight="1">
       <c r="A34" s="1" t="n">
@@ -10378,6 +10480,9 @@
       <c r="CP34" s="1" t="n">
         <v>422.3</v>
       </c>
+      <c r="CQ34" s="1" t="n">
+        <v>219.8</v>
+      </c>
     </row>
     <row r="35" ht="20" customHeight="1">
       <c r="A35" s="1" t="n">
@@ -10662,6 +10767,9 @@
       <c r="CP35" s="1" t="n">
         <v>171.4</v>
       </c>
+      <c r="CQ35" s="3" t="n">
+        <v>132</v>
+      </c>
     </row>
     <row r="36" ht="20" customHeight="1">
       <c r="A36" s="1" t="n">
@@ -10946,6 +11054,9 @@
       <c r="CP36" s="3" t="n">
         <v>127.8</v>
       </c>
+      <c r="CQ36" s="1" t="n">
+        <v>173.8</v>
+      </c>
     </row>
     <row r="37" ht="20" customHeight="1">
       <c r="A37" s="1" t="n">
@@ -11230,6 +11341,9 @@
       <c r="CP37" s="1" t="n">
         <v>141.2</v>
       </c>
+      <c r="CQ37" s="1" t="n">
+        <v>165.2</v>
+      </c>
     </row>
     <row r="38" ht="20" customHeight="1">
       <c r="A38" s="1" t="n">
@@ -11514,6 +11628,9 @@
       <c r="CP38" s="1" t="n">
         <v>174.1</v>
       </c>
+      <c r="CQ38" s="3" t="n">
+        <v>135.2</v>
+      </c>
     </row>
     <row r="39" ht="20" customHeight="1">
       <c r="A39" s="1" t="n">
@@ -11798,6 +11915,9 @@
       <c r="CP39" s="3" t="n">
         <v>125.7</v>
       </c>
+      <c r="CQ39" s="1" t="n">
+        <v>214.4</v>
+      </c>
     </row>
     <row r="40" ht="20" customHeight="1">
       <c r="A40" s="1" t="n">
@@ -12082,6 +12202,9 @@
       <c r="CP40" s="1" t="n">
         <v>149.8</v>
       </c>
+      <c r="CQ40" s="1" t="n">
+        <v>140.9</v>
+      </c>
     </row>
     <row r="41" ht="20" customHeight="1">
       <c r="A41" s="1" t="n">
@@ -12366,6 +12489,9 @@
       <c r="CP41" s="3" t="n">
         <v>129.8</v>
       </c>
+      <c r="CQ41" s="3" t="n">
+        <v>130.1</v>
+      </c>
     </row>
     <row r="42" ht="20" customHeight="1">
       <c r="A42" s="1" t="n">
@@ -12650,6 +12776,9 @@
       <c r="CP42" s="2" t="n">
         <v>122.1</v>
       </c>
+      <c r="CQ42" s="1" t="n">
+        <v>162.1</v>
+      </c>
     </row>
     <row r="43" ht="20" customHeight="1">
       <c r="A43" s="1" t="n">
@@ -12934,6 +13063,9 @@
       <c r="CP43" s="1" t="n">
         <v>171.8</v>
       </c>
+      <c r="CQ43" s="1" t="n">
+        <v>141.4</v>
+      </c>
     </row>
     <row r="44" ht="20" customHeight="1">
       <c r="A44" s="1" t="n">
@@ -13218,6 +13350,9 @@
       <c r="CP44" s="1" t="n">
         <v>175.9</v>
       </c>
+      <c r="CQ44" s="1" t="n">
+        <v>147.1</v>
+      </c>
     </row>
     <row r="45" ht="20" customHeight="1">
       <c r="A45" s="1" t="n">
@@ -13502,6 +13637,9 @@
       <c r="CP45" s="1" t="n">
         <v>162.5</v>
       </c>
+      <c r="CQ45" s="3" t="n">
+        <v>131.8</v>
+      </c>
     </row>
     <row r="46" ht="20" customHeight="1">
       <c r="A46" s="1" t="n">
@@ -13786,6 +13924,9 @@
       <c r="CP46" s="1" t="n">
         <v>302.8</v>
       </c>
+      <c r="CQ46" s="1" t="n">
+        <v>146.8</v>
+      </c>
     </row>
     <row r="47" ht="20" customHeight="1">
       <c r="A47" s="1" t="n">
@@ -14070,6 +14211,9 @@
       <c r="CP47" s="3" t="n">
         <v>136.6</v>
       </c>
+      <c r="CQ47" s="3" t="n">
+        <v>131.6</v>
+      </c>
     </row>
     <row r="48" ht="20" customHeight="1">
       <c r="A48" s="1" t="n">
@@ -14354,6 +14498,9 @@
       <c r="CP48" s="1" t="n">
         <v>168.4</v>
       </c>
+      <c r="CQ48" s="1" t="n">
+        <v>162.3</v>
+      </c>
     </row>
     <row r="49" ht="20" customHeight="1">
       <c r="A49" s="1" t="n">
@@ -14638,6 +14785,9 @@
       <c r="CP49" s="1" t="n">
         <v>141.1</v>
       </c>
+      <c r="CQ49" s="1" t="n">
+        <v>248.2</v>
+      </c>
     </row>
     <row r="50" ht="20" customHeight="1">
       <c r="A50" s="1" t="n">
@@ -14922,6 +15072,9 @@
       <c r="CP50" s="3" t="n">
         <v>129.3</v>
       </c>
+      <c r="CQ50" s="1" t="n">
+        <v>183.4</v>
+      </c>
     </row>
     <row r="51" ht="20" customHeight="1">
       <c r="A51" s="1" t="n">
@@ -15206,6 +15359,9 @@
       <c r="CP51" s="1" t="n">
         <v>213.5</v>
       </c>
+      <c r="CQ51" s="1" t="n">
+        <v>221.4</v>
+      </c>
     </row>
     <row r="52" ht="20" customHeight="1">
       <c r="A52" s="1" t="n">
@@ -15490,6 +15646,9 @@
       <c r="CP52" s="1" t="n">
         <v>165.3</v>
       </c>
+      <c r="CQ52" s="3" t="n">
+        <v>134.9</v>
+      </c>
     </row>
     <row r="53" ht="20" customHeight="1">
       <c r="A53" s="1" t="n">
@@ -15773,6 +15932,9 @@
       </c>
       <c r="CP53" s="3" t="n">
         <v>127.5</v>
+      </c>
+      <c r="CQ53" s="1" t="n">
+        <v>142.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2024-12-13
</commit_message>
<xml_diff>
--- a/マイジャグラーV_塗りつぶし済み.xlsx
+++ b/マイジャグラーV_塗りつぶし済み.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:CQ53"/>
+  <dimension ref="A1:CR53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -534,6 +534,7 @@
     <col width="12" customWidth="1" min="93" max="93"/>
     <col width="12" customWidth="1" min="94" max="94"/>
     <col width="12" customWidth="1" min="95" max="95"/>
+    <col width="12" customWidth="1" min="96" max="96"/>
   </cols>
   <sheetData>
     <row r="1" ht="20" customHeight="1">
@@ -1012,6 +1013,11 @@
           <t>2024/12/12</t>
         </is>
       </c>
+      <c r="CR1" s="1" t="inlineStr">
+        <is>
+          <t>2024/12/13</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="20" customHeight="1">
       <c r="A2" s="1" t="n">
@@ -1299,6 +1305,9 @@
       <c r="CQ2" s="1" t="n">
         <v>186.3</v>
       </c>
+      <c r="CR2" s="3" t="n">
+        <v>134.9</v>
+      </c>
     </row>
     <row r="3" ht="20" customHeight="1">
       <c r="A3" s="1" t="n">
@@ -1586,6 +1595,9 @@
       <c r="CQ3" s="1" t="n">
         <v>192.4</v>
       </c>
+      <c r="CR3" s="3" t="n">
+        <v>131.6</v>
+      </c>
     </row>
     <row r="4" ht="20" customHeight="1">
       <c r="A4" s="1" t="n">
@@ -1873,6 +1885,9 @@
       <c r="CQ4" s="1" t="n">
         <v>188.2</v>
       </c>
+      <c r="CR4" s="1" t="n">
+        <v>140.6</v>
+      </c>
     </row>
     <row r="5" ht="20" customHeight="1">
       <c r="A5" s="1" t="n">
@@ -2160,6 +2175,9 @@
       <c r="CQ5" s="3" t="n">
         <v>136.9</v>
       </c>
+      <c r="CR5" s="3" t="n">
+        <v>131.5</v>
+      </c>
     </row>
     <row r="6" ht="20" customHeight="1">
       <c r="A6" s="1" t="n">
@@ -2447,6 +2465,9 @@
       <c r="CQ6" s="3" t="n">
         <v>128.7</v>
       </c>
+      <c r="CR6" s="1" t="n">
+        <v>164.1</v>
+      </c>
     </row>
     <row r="7" ht="20" customHeight="1">
       <c r="A7" s="1" t="n">
@@ -2734,6 +2755,9 @@
       <c r="CQ7" s="2" t="n">
         <v>114</v>
       </c>
+      <c r="CR7" s="1" t="n">
+        <v>255.3</v>
+      </c>
     </row>
     <row r="8" ht="20" customHeight="1">
       <c r="A8" s="1" t="n">
@@ -3021,6 +3045,9 @@
       <c r="CQ8" s="3" t="n">
         <v>127.6</v>
       </c>
+      <c r="CR8" s="1" t="n">
+        <v>156.4</v>
+      </c>
     </row>
     <row r="9" ht="20" customHeight="1">
       <c r="A9" s="1" t="n">
@@ -3308,6 +3335,9 @@
       <c r="CQ9" s="2" t="n">
         <v>124</v>
       </c>
+      <c r="CR9" s="3" t="n">
+        <v>137.2</v>
+      </c>
     </row>
     <row r="10" ht="20" customHeight="1">
       <c r="A10" s="1" t="n">
@@ -3595,6 +3625,9 @@
       <c r="CQ10" s="1" t="n">
         <v>226.2</v>
       </c>
+      <c r="CR10" s="1" t="n">
+        <v>177.5</v>
+      </c>
     </row>
     <row r="11" ht="20" customHeight="1">
       <c r="A11" s="1" t="n">
@@ -3882,6 +3915,9 @@
       <c r="CQ11" s="1" t="n">
         <v>176.1</v>
       </c>
+      <c r="CR11" s="1" t="n">
+        <v>173.8</v>
+      </c>
     </row>
     <row r="12" ht="20" customHeight="1">
       <c r="A12" s="1" t="n">
@@ -4169,6 +4205,9 @@
       <c r="CQ12" s="1" t="n">
         <v>143.6</v>
       </c>
+      <c r="CR12" s="1" t="n">
+        <v>151.1</v>
+      </c>
     </row>
     <row r="13" ht="20" customHeight="1">
       <c r="A13" s="1" t="n">
@@ -4456,6 +4495,9 @@
       <c r="CQ13" s="2" t="n">
         <v>124.4</v>
       </c>
+      <c r="CR13" s="1" t="n">
+        <v>200</v>
+      </c>
     </row>
     <row r="14" ht="20" customHeight="1">
       <c r="A14" s="1" t="n">
@@ -4743,6 +4785,9 @@
       <c r="CQ14" s="3" t="n">
         <v>136.7</v>
       </c>
+      <c r="CR14" s="1" t="n">
+        <v>165.1</v>
+      </c>
     </row>
     <row r="15" ht="20" customHeight="1">
       <c r="A15" s="1" t="n">
@@ -5030,6 +5075,9 @@
       <c r="CQ15" s="1" t="n">
         <v>157.2</v>
       </c>
+      <c r="CR15" s="1" t="n">
+        <v>146.3</v>
+      </c>
     </row>
     <row r="16" ht="20" customHeight="1">
       <c r="A16" s="1" t="n">
@@ -5317,6 +5365,9 @@
       <c r="CQ16" s="1" t="n">
         <v>158.5</v>
       </c>
+      <c r="CR16" s="3" t="n">
+        <v>139.9</v>
+      </c>
     </row>
     <row r="17" ht="20" customHeight="1">
       <c r="A17" s="1" t="n">
@@ -5604,6 +5655,9 @@
       <c r="CQ17" s="1" t="n">
         <v>157.2</v>
       </c>
+      <c r="CR17" s="1" t="n">
+        <v>152.5</v>
+      </c>
     </row>
     <row r="18" ht="20" customHeight="1">
       <c r="A18" s="1" t="n">
@@ -5891,6 +5945,9 @@
       <c r="CQ18" s="3" t="n">
         <v>137.7</v>
       </c>
+      <c r="CR18" s="1" t="n">
+        <v>167.3</v>
+      </c>
     </row>
     <row r="19" ht="20" customHeight="1">
       <c r="A19" s="1" t="n">
@@ -6178,6 +6235,9 @@
       <c r="CQ19" s="3" t="n">
         <v>139.8</v>
       </c>
+      <c r="CR19" s="1" t="n">
+        <v>162.5</v>
+      </c>
     </row>
     <row r="20" ht="20" customHeight="1">
       <c r="A20" s="1" t="n">
@@ -6465,6 +6525,9 @@
       <c r="CQ20" s="1" t="n">
         <v>150.5</v>
       </c>
+      <c r="CR20" s="1" t="n">
+        <v>140</v>
+      </c>
     </row>
     <row r="21" ht="20" customHeight="1">
       <c r="A21" s="1" t="n">
@@ -6752,6 +6815,9 @@
       <c r="CQ21" s="3" t="n">
         <v>136.9</v>
       </c>
+      <c r="CR21" s="1" t="n">
+        <v>259.2</v>
+      </c>
     </row>
     <row r="22" ht="20" customHeight="1">
       <c r="A22" s="1" t="n">
@@ -7039,6 +7105,9 @@
       <c r="CQ22" s="1" t="n">
         <v>168.5</v>
       </c>
+      <c r="CR22" s="1" t="n">
+        <v>171.5</v>
+      </c>
     </row>
     <row r="23" ht="20" customHeight="1">
       <c r="A23" s="1" t="n">
@@ -7326,6 +7395,9 @@
       <c r="CQ23" s="1" t="n">
         <v>148.1</v>
       </c>
+      <c r="CR23" s="1" t="n">
+        <v>166.5</v>
+      </c>
     </row>
     <row r="24" ht="20" customHeight="1">
       <c r="A24" s="1" t="n">
@@ -7613,6 +7685,9 @@
       <c r="CQ24" s="1" t="n">
         <v>152.8</v>
       </c>
+      <c r="CR24" s="1" t="n">
+        <v>142.3</v>
+      </c>
     </row>
     <row r="25" ht="20" customHeight="1">
       <c r="A25" s="1" t="n">
@@ -7900,6 +7975,9 @@
       <c r="CQ25" s="2" t="n">
         <v>111.2</v>
       </c>
+      <c r="CR25" s="1" t="n">
+        <v>214.4</v>
+      </c>
     </row>
     <row r="26" ht="20" customHeight="1">
       <c r="A26" s="1" t="n">
@@ -8187,6 +8265,9 @@
       <c r="CQ26" s="1" t="n">
         <v>186.9</v>
       </c>
+      <c r="CR26" s="1" t="n">
+        <v>152.2</v>
+      </c>
     </row>
     <row r="27" ht="20" customHeight="1">
       <c r="A27" s="1" t="n">
@@ -8474,6 +8555,9 @@
       <c r="CQ27" s="1" t="n">
         <v>160.3</v>
       </c>
+      <c r="CR27" s="1" t="n">
+        <v>140.9</v>
+      </c>
     </row>
     <row r="28" ht="20" customHeight="1">
       <c r="A28" s="1" t="n">
@@ -8761,6 +8845,9 @@
       <c r="CQ28" s="1" t="n">
         <v>178.9</v>
       </c>
+      <c r="CR28" s="1" t="n">
+        <v>464.3</v>
+      </c>
     </row>
     <row r="29" ht="20" customHeight="1">
       <c r="A29" s="1" t="n">
@@ -9048,6 +9135,9 @@
       <c r="CQ29" s="1" t="n">
         <v>162.3</v>
       </c>
+      <c r="CR29" s="1" t="n">
+        <v>162</v>
+      </c>
     </row>
     <row r="30" ht="20" customHeight="1">
       <c r="A30" s="1" t="n">
@@ -9335,6 +9425,9 @@
       <c r="CQ30" s="3" t="n">
         <v>132.4</v>
       </c>
+      <c r="CR30" s="3" t="n">
+        <v>132</v>
+      </c>
     </row>
     <row r="31" ht="20" customHeight="1">
       <c r="A31" s="1" t="n">
@@ -9622,6 +9715,9 @@
       <c r="CQ31" s="1" t="n">
         <v>183.6</v>
       </c>
+      <c r="CR31" s="1" t="n">
+        <v>195.3</v>
+      </c>
     </row>
     <row r="32" ht="20" customHeight="1">
       <c r="A32" s="1" t="n">
@@ -9909,6 +10005,9 @@
       <c r="CQ32" s="1" t="n">
         <v>200.5</v>
       </c>
+      <c r="CR32" s="1" t="n">
+        <v>140.3</v>
+      </c>
     </row>
     <row r="33" ht="20" customHeight="1">
       <c r="A33" s="1" t="n">
@@ -10196,6 +10295,9 @@
       <c r="CQ33" s="3" t="n">
         <v>128.8</v>
       </c>
+      <c r="CR33" s="1" t="n">
+        <v>201</v>
+      </c>
     </row>
     <row r="34" ht="20" customHeight="1">
       <c r="A34" s="1" t="n">
@@ -10483,6 +10585,9 @@
       <c r="CQ34" s="1" t="n">
         <v>219.8</v>
       </c>
+      <c r="CR34" s="1" t="n">
+        <v>152.5</v>
+      </c>
     </row>
     <row r="35" ht="20" customHeight="1">
       <c r="A35" s="1" t="n">
@@ -10770,6 +10875,9 @@
       <c r="CQ35" s="3" t="n">
         <v>132</v>
       </c>
+      <c r="CR35" s="1" t="n">
+        <v>164.1</v>
+      </c>
     </row>
     <row r="36" ht="20" customHeight="1">
       <c r="A36" s="1" t="n">
@@ -11057,6 +11165,9 @@
       <c r="CQ36" s="1" t="n">
         <v>173.8</v>
       </c>
+      <c r="CR36" s="1" t="n">
+        <v>141.9</v>
+      </c>
     </row>
     <row r="37" ht="20" customHeight="1">
       <c r="A37" s="1" t="n">
@@ -11344,6 +11455,9 @@
       <c r="CQ37" s="1" t="n">
         <v>165.2</v>
       </c>
+      <c r="CR37" s="1" t="n">
+        <v>194.1</v>
+      </c>
     </row>
     <row r="38" ht="20" customHeight="1">
       <c r="A38" s="1" t="n">
@@ -11631,6 +11745,9 @@
       <c r="CQ38" s="3" t="n">
         <v>135.2</v>
       </c>
+      <c r="CR38" s="3" t="n">
+        <v>131.4</v>
+      </c>
     </row>
     <row r="39" ht="20" customHeight="1">
       <c r="A39" s="1" t="n">
@@ -11918,6 +12035,9 @@
       <c r="CQ39" s="1" t="n">
         <v>214.4</v>
       </c>
+      <c r="CR39" s="1" t="n">
+        <v>254.6</v>
+      </c>
     </row>
     <row r="40" ht="20" customHeight="1">
       <c r="A40" s="1" t="n">
@@ -12205,6 +12325,9 @@
       <c r="CQ40" s="1" t="n">
         <v>140.9</v>
       </c>
+      <c r="CR40" s="1" t="n">
+        <v>159.4</v>
+      </c>
     </row>
     <row r="41" ht="20" customHeight="1">
       <c r="A41" s="1" t="n">
@@ -12492,6 +12615,9 @@
       <c r="CQ41" s="3" t="n">
         <v>130.1</v>
       </c>
+      <c r="CR41" s="1" t="n">
+        <v>244.9</v>
+      </c>
     </row>
     <row r="42" ht="20" customHeight="1">
       <c r="A42" s="1" t="n">
@@ -12779,6 +12905,9 @@
       <c r="CQ42" s="1" t="n">
         <v>162.1</v>
       </c>
+      <c r="CR42" s="1" t="n">
+        <v>151.9</v>
+      </c>
     </row>
     <row r="43" ht="20" customHeight="1">
       <c r="A43" s="1" t="n">
@@ -13066,6 +13195,9 @@
       <c r="CQ43" s="1" t="n">
         <v>141.4</v>
       </c>
+      <c r="CR43" s="1" t="n">
+        <v>175.4</v>
+      </c>
     </row>
     <row r="44" ht="20" customHeight="1">
       <c r="A44" s="1" t="n">
@@ -13353,6 +13485,9 @@
       <c r="CQ44" s="1" t="n">
         <v>147.1</v>
       </c>
+      <c r="CR44" s="1" t="n">
+        <v>142.4</v>
+      </c>
     </row>
     <row r="45" ht="20" customHeight="1">
       <c r="A45" s="1" t="n">
@@ -13640,6 +13775,9 @@
       <c r="CQ45" s="3" t="n">
         <v>131.8</v>
       </c>
+      <c r="CR45" s="1" t="n">
+        <v>187.5</v>
+      </c>
     </row>
     <row r="46" ht="20" customHeight="1">
       <c r="A46" s="1" t="n">
@@ -13927,6 +14065,9 @@
       <c r="CQ46" s="1" t="n">
         <v>146.8</v>
       </c>
+      <c r="CR46" s="1" t="n">
+        <v>261.6</v>
+      </c>
     </row>
     <row r="47" ht="20" customHeight="1">
       <c r="A47" s="1" t="n">
@@ -14214,6 +14355,9 @@
       <c r="CQ47" s="3" t="n">
         <v>131.6</v>
       </c>
+      <c r="CR47" s="2" t="n">
+        <v>123.4</v>
+      </c>
     </row>
     <row r="48" ht="20" customHeight="1">
       <c r="A48" s="1" t="n">
@@ -14501,6 +14645,9 @@
       <c r="CQ48" s="1" t="n">
         <v>162.3</v>
       </c>
+      <c r="CR48" s="1" t="n">
+        <v>236.4</v>
+      </c>
     </row>
     <row r="49" ht="20" customHeight="1">
       <c r="A49" s="1" t="n">
@@ -14788,6 +14935,9 @@
       <c r="CQ49" s="1" t="n">
         <v>248.2</v>
       </c>
+      <c r="CR49" s="1" t="n">
+        <v>202.2</v>
+      </c>
     </row>
     <row r="50" ht="20" customHeight="1">
       <c r="A50" s="1" t="n">
@@ -15075,6 +15225,9 @@
       <c r="CQ50" s="1" t="n">
         <v>183.4</v>
       </c>
+      <c r="CR50" s="1" t="n">
+        <v>142</v>
+      </c>
     </row>
     <row r="51" ht="20" customHeight="1">
       <c r="A51" s="1" t="n">
@@ -15362,6 +15515,9 @@
       <c r="CQ51" s="1" t="n">
         <v>221.4</v>
       </c>
+      <c r="CR51" s="2" t="n">
+        <v>123.5</v>
+      </c>
     </row>
     <row r="52" ht="20" customHeight="1">
       <c r="A52" s="1" t="n">
@@ -15649,6 +15805,9 @@
       <c r="CQ52" s="3" t="n">
         <v>134.9</v>
       </c>
+      <c r="CR52" s="1" t="n">
+        <v>179.5</v>
+      </c>
     </row>
     <row r="53" ht="20" customHeight="1">
       <c r="A53" s="1" t="n">
@@ -15935,6 +16094,9 @@
       </c>
       <c r="CQ53" s="1" t="n">
         <v>142.8</v>
+      </c>
+      <c r="CR53" s="1" t="n">
+        <v>140.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2024-12-14
</commit_message>
<xml_diff>
--- a/マイジャグラーV_塗りつぶし済み.xlsx
+++ b/マイジャグラーV_塗りつぶし済み.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:CR53"/>
+  <dimension ref="A1:CS53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -535,6 +535,7 @@
     <col width="12" customWidth="1" min="94" max="94"/>
     <col width="12" customWidth="1" min="95" max="95"/>
     <col width="12" customWidth="1" min="96" max="96"/>
+    <col width="12" customWidth="1" min="97" max="97"/>
   </cols>
   <sheetData>
     <row r="1" ht="20" customHeight="1">
@@ -1018,6 +1019,11 @@
           <t>2024/12/13</t>
         </is>
       </c>
+      <c r="CS1" s="1" t="inlineStr">
+        <is>
+          <t>2024/12/14</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="20" customHeight="1">
       <c r="A2" s="1" t="n">
@@ -1308,6 +1314,9 @@
       <c r="CR2" s="3" t="n">
         <v>134.9</v>
       </c>
+      <c r="CS2" s="3" t="n">
+        <v>125</v>
+      </c>
     </row>
     <row r="3" ht="20" customHeight="1">
       <c r="A3" s="1" t="n">
@@ -1598,6 +1607,9 @@
       <c r="CR3" s="3" t="n">
         <v>131.6</v>
       </c>
+      <c r="CS3" s="3" t="n">
+        <v>137.7</v>
+      </c>
     </row>
     <row r="4" ht="20" customHeight="1">
       <c r="A4" s="1" t="n">
@@ -1888,6 +1900,9 @@
       <c r="CR4" s="1" t="n">
         <v>140.6</v>
       </c>
+      <c r="CS4" s="1" t="n">
+        <v>173.5</v>
+      </c>
     </row>
     <row r="5" ht="20" customHeight="1">
       <c r="A5" s="1" t="n">
@@ -2178,6 +2193,9 @@
       <c r="CR5" s="3" t="n">
         <v>131.5</v>
       </c>
+      <c r="CS5" s="1" t="n">
+        <v>163.4</v>
+      </c>
     </row>
     <row r="6" ht="20" customHeight="1">
       <c r="A6" s="1" t="n">
@@ -2468,6 +2486,9 @@
       <c r="CR6" s="1" t="n">
         <v>164.1</v>
       </c>
+      <c r="CS6" s="3" t="n">
+        <v>135.9</v>
+      </c>
     </row>
     <row r="7" ht="20" customHeight="1">
       <c r="A7" s="1" t="n">
@@ -2758,6 +2779,9 @@
       <c r="CR7" s="1" t="n">
         <v>255.3</v>
       </c>
+      <c r="CS7" s="1" t="n">
+        <v>204.2</v>
+      </c>
     </row>
     <row r="8" ht="20" customHeight="1">
       <c r="A8" s="1" t="n">
@@ -3048,6 +3072,9 @@
       <c r="CR8" s="1" t="n">
         <v>156.4</v>
       </c>
+      <c r="CS8" s="1" t="n">
+        <v>157.1</v>
+      </c>
     </row>
     <row r="9" ht="20" customHeight="1">
       <c r="A9" s="1" t="n">
@@ -3338,6 +3365,9 @@
       <c r="CR9" s="3" t="n">
         <v>137.2</v>
       </c>
+      <c r="CS9" s="1" t="n">
+        <v>171.4</v>
+      </c>
     </row>
     <row r="10" ht="20" customHeight="1">
       <c r="A10" s="1" t="n">
@@ -3628,6 +3658,9 @@
       <c r="CR10" s="1" t="n">
         <v>177.5</v>
       </c>
+      <c r="CS10" s="1" t="n">
+        <v>165.6</v>
+      </c>
     </row>
     <row r="11" ht="20" customHeight="1">
       <c r="A11" s="1" t="n">
@@ -3918,6 +3951,9 @@
       <c r="CR11" s="1" t="n">
         <v>173.8</v>
       </c>
+      <c r="CS11" s="1" t="n">
+        <v>184.1</v>
+      </c>
     </row>
     <row r="12" ht="20" customHeight="1">
       <c r="A12" s="1" t="n">
@@ -4208,6 +4244,9 @@
       <c r="CR12" s="1" t="n">
         <v>151.1</v>
       </c>
+      <c r="CS12" s="1" t="n">
+        <v>164.9</v>
+      </c>
     </row>
     <row r="13" ht="20" customHeight="1">
       <c r="A13" s="1" t="n">
@@ -4498,6 +4537,9 @@
       <c r="CR13" s="1" t="n">
         <v>200</v>
       </c>
+      <c r="CS13" s="1" t="n">
+        <v>147.5</v>
+      </c>
     </row>
     <row r="14" ht="20" customHeight="1">
       <c r="A14" s="1" t="n">
@@ -4788,6 +4830,9 @@
       <c r="CR14" s="1" t="n">
         <v>165.1</v>
       </c>
+      <c r="CS14" s="2" t="n">
+        <v>116.5</v>
+      </c>
     </row>
     <row r="15" ht="20" customHeight="1">
       <c r="A15" s="1" t="n">
@@ -5078,6 +5123,9 @@
       <c r="CR15" s="1" t="n">
         <v>146.3</v>
       </c>
+      <c r="CS15" s="3" t="n">
+        <v>133.3</v>
+      </c>
     </row>
     <row r="16" ht="20" customHeight="1">
       <c r="A16" s="1" t="n">
@@ -5368,6 +5416,9 @@
       <c r="CR16" s="3" t="n">
         <v>139.9</v>
       </c>
+      <c r="CS16" s="1" t="n">
+        <v>158.5</v>
+      </c>
     </row>
     <row r="17" ht="20" customHeight="1">
       <c r="A17" s="1" t="n">
@@ -5658,6 +5709,9 @@
       <c r="CR17" s="1" t="n">
         <v>152.5</v>
       </c>
+      <c r="CS17" s="2" t="n">
+        <v>116.4</v>
+      </c>
     </row>
     <row r="18" ht="20" customHeight="1">
       <c r="A18" s="1" t="n">
@@ -5948,6 +6002,9 @@
       <c r="CR18" s="1" t="n">
         <v>167.3</v>
       </c>
+      <c r="CS18" s="2" t="n">
+        <v>124.5</v>
+      </c>
     </row>
     <row r="19" ht="20" customHeight="1">
       <c r="A19" s="1" t="n">
@@ -6238,6 +6295,9 @@
       <c r="CR19" s="1" t="n">
         <v>162.5</v>
       </c>
+      <c r="CS19" s="1" t="n">
+        <v>220.1</v>
+      </c>
     </row>
     <row r="20" ht="20" customHeight="1">
       <c r="A20" s="1" t="n">
@@ -6528,6 +6588,9 @@
       <c r="CR20" s="1" t="n">
         <v>140</v>
       </c>
+      <c r="CS20" s="1" t="n">
+        <v>153.2</v>
+      </c>
     </row>
     <row r="21" ht="20" customHeight="1">
       <c r="A21" s="1" t="n">
@@ -6818,6 +6881,9 @@
       <c r="CR21" s="1" t="n">
         <v>259.2</v>
       </c>
+      <c r="CS21" s="3" t="n">
+        <v>139.4</v>
+      </c>
     </row>
     <row r="22" ht="20" customHeight="1">
       <c r="A22" s="1" t="n">
@@ -7108,6 +7174,9 @@
       <c r="CR22" s="1" t="n">
         <v>171.5</v>
       </c>
+      <c r="CS22" s="1" t="n">
+        <v>177</v>
+      </c>
     </row>
     <row r="23" ht="20" customHeight="1">
       <c r="A23" s="1" t="n">
@@ -7398,6 +7467,9 @@
       <c r="CR23" s="1" t="n">
         <v>166.5</v>
       </c>
+      <c r="CS23" s="1" t="n">
+        <v>277.6</v>
+      </c>
     </row>
     <row r="24" ht="20" customHeight="1">
       <c r="A24" s="1" t="n">
@@ -7688,6 +7760,9 @@
       <c r="CR24" s="1" t="n">
         <v>142.3</v>
       </c>
+      <c r="CS24" s="2" t="n">
+        <v>115.2</v>
+      </c>
     </row>
     <row r="25" ht="20" customHeight="1">
       <c r="A25" s="1" t="n">
@@ -7978,6 +8053,9 @@
       <c r="CR25" s="1" t="n">
         <v>214.4</v>
       </c>
+      <c r="CS25" s="1" t="n">
+        <v>145.2</v>
+      </c>
     </row>
     <row r="26" ht="20" customHeight="1">
       <c r="A26" s="1" t="n">
@@ -8268,6 +8346,9 @@
       <c r="CR26" s="1" t="n">
         <v>152.2</v>
       </c>
+      <c r="CS26" s="3" t="n">
+        <v>134.1</v>
+      </c>
     </row>
     <row r="27" ht="20" customHeight="1">
       <c r="A27" s="1" t="n">
@@ -8558,6 +8639,9 @@
       <c r="CR27" s="1" t="n">
         <v>140.9</v>
       </c>
+      <c r="CS27" s="1" t="n">
+        <v>202.6</v>
+      </c>
     </row>
     <row r="28" ht="20" customHeight="1">
       <c r="A28" s="1" t="n">
@@ -8848,6 +8932,9 @@
       <c r="CR28" s="1" t="n">
         <v>464.3</v>
       </c>
+      <c r="CS28" s="1" t="n">
+        <v>159</v>
+      </c>
     </row>
     <row r="29" ht="20" customHeight="1">
       <c r="A29" s="1" t="n">
@@ -9138,6 +9225,9 @@
       <c r="CR29" s="1" t="n">
         <v>162</v>
       </c>
+      <c r="CS29" s="1" t="n">
+        <v>149.9</v>
+      </c>
     </row>
     <row r="30" ht="20" customHeight="1">
       <c r="A30" s="1" t="n">
@@ -9428,6 +9518,9 @@
       <c r="CR30" s="3" t="n">
         <v>132</v>
       </c>
+      <c r="CS30" s="1" t="n">
+        <v>150.1</v>
+      </c>
     </row>
     <row r="31" ht="20" customHeight="1">
       <c r="A31" s="1" t="n">
@@ -9718,6 +9811,9 @@
       <c r="CR31" s="1" t="n">
         <v>195.3</v>
       </c>
+      <c r="CS31" s="1" t="n">
+        <v>181.3</v>
+      </c>
     </row>
     <row r="32" ht="20" customHeight="1">
       <c r="A32" s="1" t="n">
@@ -10008,6 +10104,9 @@
       <c r="CR32" s="1" t="n">
         <v>140.3</v>
       </c>
+      <c r="CS32" s="1" t="n">
+        <v>194</v>
+      </c>
     </row>
     <row r="33" ht="20" customHeight="1">
       <c r="A33" s="1" t="n">
@@ -10298,6 +10397,9 @@
       <c r="CR33" s="1" t="n">
         <v>201</v>
       </c>
+      <c r="CS33" s="3" t="n">
+        <v>138.7</v>
+      </c>
     </row>
     <row r="34" ht="20" customHeight="1">
       <c r="A34" s="1" t="n">
@@ -10588,6 +10690,9 @@
       <c r="CR34" s="1" t="n">
         <v>152.5</v>
       </c>
+      <c r="CS34" s="1" t="n">
+        <v>221.6</v>
+      </c>
     </row>
     <row r="35" ht="20" customHeight="1">
       <c r="A35" s="1" t="n">
@@ -10878,6 +10983,9 @@
       <c r="CR35" s="1" t="n">
         <v>164.1</v>
       </c>
+      <c r="CS35" s="1" t="n">
+        <v>261.4</v>
+      </c>
     </row>
     <row r="36" ht="20" customHeight="1">
       <c r="A36" s="1" t="n">
@@ -11168,6 +11276,9 @@
       <c r="CR36" s="1" t="n">
         <v>141.9</v>
       </c>
+      <c r="CS36" s="1" t="n">
+        <v>154.3</v>
+      </c>
     </row>
     <row r="37" ht="20" customHeight="1">
       <c r="A37" s="1" t="n">
@@ -11458,6 +11569,9 @@
       <c r="CR37" s="1" t="n">
         <v>194.1</v>
       </c>
+      <c r="CS37" s="1" t="n">
+        <v>151.7</v>
+      </c>
     </row>
     <row r="38" ht="20" customHeight="1">
       <c r="A38" s="1" t="n">
@@ -11748,6 +11862,9 @@
       <c r="CR38" s="3" t="n">
         <v>131.4</v>
       </c>
+      <c r="CS38" s="1" t="n">
+        <v>179.6</v>
+      </c>
     </row>
     <row r="39" ht="20" customHeight="1">
       <c r="A39" s="1" t="n">
@@ -12038,6 +12155,9 @@
       <c r="CR39" s="1" t="n">
         <v>254.6</v>
       </c>
+      <c r="CS39" s="1" t="n">
+        <v>161.2</v>
+      </c>
     </row>
     <row r="40" ht="20" customHeight="1">
       <c r="A40" s="1" t="n">
@@ -12328,6 +12448,9 @@
       <c r="CR40" s="1" t="n">
         <v>159.4</v>
       </c>
+      <c r="CS40" s="1" t="n">
+        <v>142.9</v>
+      </c>
     </row>
     <row r="41" ht="20" customHeight="1">
       <c r="A41" s="1" t="n">
@@ -12618,6 +12741,9 @@
       <c r="CR41" s="1" t="n">
         <v>244.9</v>
       </c>
+      <c r="CS41" s="1" t="n">
+        <v>149.4</v>
+      </c>
     </row>
     <row r="42" ht="20" customHeight="1">
       <c r="A42" s="1" t="n">
@@ -12908,6 +13034,9 @@
       <c r="CR42" s="1" t="n">
         <v>151.9</v>
       </c>
+      <c r="CS42" s="1" t="n">
+        <v>145.4</v>
+      </c>
     </row>
     <row r="43" ht="20" customHeight="1">
       <c r="A43" s="1" t="n">
@@ -13198,6 +13327,9 @@
       <c r="CR43" s="1" t="n">
         <v>175.4</v>
       </c>
+      <c r="CS43" s="1" t="n">
+        <v>152.4</v>
+      </c>
     </row>
     <row r="44" ht="20" customHeight="1">
       <c r="A44" s="1" t="n">
@@ -13488,6 +13620,9 @@
       <c r="CR44" s="1" t="n">
         <v>142.4</v>
       </c>
+      <c r="CS44" s="3" t="n">
+        <v>133.4</v>
+      </c>
     </row>
     <row r="45" ht="20" customHeight="1">
       <c r="A45" s="1" t="n">
@@ -13778,6 +13913,9 @@
       <c r="CR45" s="1" t="n">
         <v>187.5</v>
       </c>
+      <c r="CS45" s="1" t="n">
+        <v>211.4</v>
+      </c>
     </row>
     <row r="46" ht="20" customHeight="1">
       <c r="A46" s="1" t="n">
@@ -14068,6 +14206,9 @@
       <c r="CR46" s="1" t="n">
         <v>261.6</v>
       </c>
+      <c r="CS46" s="1" t="n">
+        <v>150</v>
+      </c>
     </row>
     <row r="47" ht="20" customHeight="1">
       <c r="A47" s="1" t="n">
@@ -14358,6 +14499,9 @@
       <c r="CR47" s="2" t="n">
         <v>123.4</v>
       </c>
+      <c r="CS47" s="1" t="n">
+        <v>188.7</v>
+      </c>
     </row>
     <row r="48" ht="20" customHeight="1">
       <c r="A48" s="1" t="n">
@@ -14648,6 +14792,9 @@
       <c r="CR48" s="1" t="n">
         <v>236.4</v>
       </c>
+      <c r="CS48" s="3" t="n">
+        <v>137.6</v>
+      </c>
     </row>
     <row r="49" ht="20" customHeight="1">
       <c r="A49" s="1" t="n">
@@ -14938,6 +15085,9 @@
       <c r="CR49" s="1" t="n">
         <v>202.2</v>
       </c>
+      <c r="CS49" s="2" t="n">
+        <v>110.8</v>
+      </c>
     </row>
     <row r="50" ht="20" customHeight="1">
       <c r="A50" s="1" t="n">
@@ -15228,6 +15378,9 @@
       <c r="CR50" s="1" t="n">
         <v>142</v>
       </c>
+      <c r="CS50" s="1" t="n">
+        <v>234.7</v>
+      </c>
     </row>
     <row r="51" ht="20" customHeight="1">
       <c r="A51" s="1" t="n">
@@ -15518,6 +15671,9 @@
       <c r="CR51" s="2" t="n">
         <v>123.5</v>
       </c>
+      <c r="CS51" s="1" t="n">
+        <v>181.5</v>
+      </c>
     </row>
     <row r="52" ht="20" customHeight="1">
       <c r="A52" s="1" t="n">
@@ -15808,6 +15964,9 @@
       <c r="CR52" s="1" t="n">
         <v>179.5</v>
       </c>
+      <c r="CS52" s="1" t="n">
+        <v>167.3</v>
+      </c>
     </row>
     <row r="53" ht="20" customHeight="1">
       <c r="A53" s="1" t="n">
@@ -16097,6 +16256,9 @@
       </c>
       <c r="CR53" s="1" t="n">
         <v>140.4</v>
+      </c>
+      <c r="CS53" s="1" t="n">
+        <v>186.3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2024-12-15
</commit_message>
<xml_diff>
--- a/マイジャグラーV_塗りつぶし済み.xlsx
+++ b/マイジャグラーV_塗りつぶし済み.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:CS53"/>
+  <dimension ref="A1:CT53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -536,6 +536,7 @@
     <col width="12" customWidth="1" min="95" max="95"/>
     <col width="12" customWidth="1" min="96" max="96"/>
     <col width="12" customWidth="1" min="97" max="97"/>
+    <col width="12" customWidth="1" min="98" max="98"/>
   </cols>
   <sheetData>
     <row r="1" ht="20" customHeight="1">
@@ -1024,6 +1025,11 @@
           <t>2024/12/14</t>
         </is>
       </c>
+      <c r="CT1" s="1" t="inlineStr">
+        <is>
+          <t>2024/12/15</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="20" customHeight="1">
       <c r="A2" s="1" t="n">
@@ -1317,6 +1323,9 @@
       <c r="CS2" s="3" t="n">
         <v>125</v>
       </c>
+      <c r="CT2" s="1" t="n">
+        <v>145.4</v>
+      </c>
     </row>
     <row r="3" ht="20" customHeight="1">
       <c r="A3" s="1" t="n">
@@ -1610,6 +1619,9 @@
       <c r="CS3" s="3" t="n">
         <v>137.7</v>
       </c>
+      <c r="CT3" s="1" t="n">
+        <v>147.1</v>
+      </c>
     </row>
     <row r="4" ht="20" customHeight="1">
       <c r="A4" s="1" t="n">
@@ -1903,6 +1915,9 @@
       <c r="CS4" s="1" t="n">
         <v>173.5</v>
       </c>
+      <c r="CT4" s="1" t="n">
+        <v>145.8</v>
+      </c>
     </row>
     <row r="5" ht="20" customHeight="1">
       <c r="A5" s="1" t="n">
@@ -2196,6 +2211,9 @@
       <c r="CS5" s="1" t="n">
         <v>163.4</v>
       </c>
+      <c r="CT5" s="1" t="n">
+        <v>140.4</v>
+      </c>
     </row>
     <row r="6" ht="20" customHeight="1">
       <c r="A6" s="1" t="n">
@@ -2489,6 +2507,9 @@
       <c r="CS6" s="3" t="n">
         <v>135.9</v>
       </c>
+      <c r="CT6" s="1" t="n">
+        <v>163.6</v>
+      </c>
     </row>
     <row r="7" ht="20" customHeight="1">
       <c r="A7" s="1" t="n">
@@ -2782,6 +2803,9 @@
       <c r="CS7" s="1" t="n">
         <v>204.2</v>
       </c>
+      <c r="CT7" s="2" t="n">
+        <v>118.9</v>
+      </c>
     </row>
     <row r="8" ht="20" customHeight="1">
       <c r="A8" s="1" t="n">
@@ -3075,6 +3099,9 @@
       <c r="CS8" s="1" t="n">
         <v>157.1</v>
       </c>
+      <c r="CT8" s="1" t="n">
+        <v>161</v>
+      </c>
     </row>
     <row r="9" ht="20" customHeight="1">
       <c r="A9" s="1" t="n">
@@ -3368,6 +3395,9 @@
       <c r="CS9" s="1" t="n">
         <v>171.4</v>
       </c>
+      <c r="CT9" s="1" t="n">
+        <v>161.2</v>
+      </c>
     </row>
     <row r="10" ht="20" customHeight="1">
       <c r="A10" s="1" t="n">
@@ -3661,6 +3691,9 @@
       <c r="CS10" s="1" t="n">
         <v>165.6</v>
       </c>
+      <c r="CT10" s="1" t="n">
+        <v>177.6</v>
+      </c>
     </row>
     <row r="11" ht="20" customHeight="1">
       <c r="A11" s="1" t="n">
@@ -3954,6 +3987,9 @@
       <c r="CS11" s="1" t="n">
         <v>184.1</v>
       </c>
+      <c r="CT11" s="3" t="n">
+        <v>125.8</v>
+      </c>
     </row>
     <row r="12" ht="20" customHeight="1">
       <c r="A12" s="1" t="n">
@@ -4247,6 +4283,9 @@
       <c r="CS12" s="1" t="n">
         <v>164.9</v>
       </c>
+      <c r="CT12" s="1" t="n">
+        <v>149.8</v>
+      </c>
     </row>
     <row r="13" ht="20" customHeight="1">
       <c r="A13" s="1" t="n">
@@ -4540,6 +4579,9 @@
       <c r="CS13" s="1" t="n">
         <v>147.5</v>
       </c>
+      <c r="CT13" s="1" t="n">
+        <v>154.8</v>
+      </c>
     </row>
     <row r="14" ht="20" customHeight="1">
       <c r="A14" s="1" t="n">
@@ -4833,6 +4875,9 @@
       <c r="CS14" s="2" t="n">
         <v>116.5</v>
       </c>
+      <c r="CT14" s="2" t="n">
+        <v>117.4</v>
+      </c>
     </row>
     <row r="15" ht="20" customHeight="1">
       <c r="A15" s="1" t="n">
@@ -5126,6 +5171,9 @@
       <c r="CS15" s="3" t="n">
         <v>133.3</v>
       </c>
+      <c r="CT15" s="2" t="n">
+        <v>124.9</v>
+      </c>
     </row>
     <row r="16" ht="20" customHeight="1">
       <c r="A16" s="1" t="n">
@@ -5419,6 +5467,9 @@
       <c r="CS16" s="1" t="n">
         <v>158.5</v>
       </c>
+      <c r="CT16" s="1" t="n">
+        <v>190.7</v>
+      </c>
     </row>
     <row r="17" ht="20" customHeight="1">
       <c r="A17" s="1" t="n">
@@ -5712,6 +5763,9 @@
       <c r="CS17" s="2" t="n">
         <v>116.4</v>
       </c>
+      <c r="CT17" s="1" t="n">
+        <v>165.3</v>
+      </c>
     </row>
     <row r="18" ht="20" customHeight="1">
       <c r="A18" s="1" t="n">
@@ -6005,6 +6059,9 @@
       <c r="CS18" s="2" t="n">
         <v>124.5</v>
       </c>
+      <c r="CT18" s="2" t="n">
+        <v>124</v>
+      </c>
     </row>
     <row r="19" ht="20" customHeight="1">
       <c r="A19" s="1" t="n">
@@ -6298,6 +6355,9 @@
       <c r="CS19" s="1" t="n">
         <v>220.1</v>
       </c>
+      <c r="CT19" s="1" t="n">
+        <v>167.4</v>
+      </c>
     </row>
     <row r="20" ht="20" customHeight="1">
       <c r="A20" s="1" t="n">
@@ -6591,6 +6651,9 @@
       <c r="CS20" s="1" t="n">
         <v>153.2</v>
       </c>
+      <c r="CT20" s="1" t="n">
+        <v>185.9</v>
+      </c>
     </row>
     <row r="21" ht="20" customHeight="1">
       <c r="A21" s="1" t="n">
@@ -6884,6 +6947,9 @@
       <c r="CS21" s="3" t="n">
         <v>139.4</v>
       </c>
+      <c r="CT21" s="1" t="n">
+        <v>165.8</v>
+      </c>
     </row>
     <row r="22" ht="20" customHeight="1">
       <c r="A22" s="1" t="n">
@@ -7177,6 +7243,9 @@
       <c r="CS22" s="1" t="n">
         <v>177</v>
       </c>
+      <c r="CT22" s="1" t="n">
+        <v>157.7</v>
+      </c>
     </row>
     <row r="23" ht="20" customHeight="1">
       <c r="A23" s="1" t="n">
@@ -7470,6 +7539,9 @@
       <c r="CS23" s="1" t="n">
         <v>277.6</v>
       </c>
+      <c r="CT23" s="3" t="n">
+        <v>126.9</v>
+      </c>
     </row>
     <row r="24" ht="20" customHeight="1">
       <c r="A24" s="1" t="n">
@@ -7763,6 +7835,9 @@
       <c r="CS24" s="2" t="n">
         <v>115.2</v>
       </c>
+      <c r="CT24" s="1" t="n">
+        <v>191.5</v>
+      </c>
     </row>
     <row r="25" ht="20" customHeight="1">
       <c r="A25" s="1" t="n">
@@ -8056,6 +8131,9 @@
       <c r="CS25" s="1" t="n">
         <v>145.2</v>
       </c>
+      <c r="CT25" s="2" t="n">
+        <v>92.09999999999999</v>
+      </c>
     </row>
     <row r="26" ht="20" customHeight="1">
       <c r="A26" s="1" t="n">
@@ -8349,6 +8427,9 @@
       <c r="CS26" s="3" t="n">
         <v>134.1</v>
       </c>
+      <c r="CT26" s="1" t="n">
+        <v>159.2</v>
+      </c>
     </row>
     <row r="27" ht="20" customHeight="1">
       <c r="A27" s="1" t="n">
@@ -8642,6 +8723,9 @@
       <c r="CS27" s="1" t="n">
         <v>202.6</v>
       </c>
+      <c r="CT27" s="2" t="n">
+        <v>106.9</v>
+      </c>
     </row>
     <row r="28" ht="20" customHeight="1">
       <c r="A28" s="1" t="n">
@@ -8935,6 +9019,9 @@
       <c r="CS28" s="1" t="n">
         <v>159</v>
       </c>
+      <c r="CT28" s="1" t="n">
+        <v>146</v>
+      </c>
     </row>
     <row r="29" ht="20" customHeight="1">
       <c r="A29" s="1" t="n">
@@ -9228,6 +9315,9 @@
       <c r="CS29" s="1" t="n">
         <v>149.9</v>
       </c>
+      <c r="CT29" s="1" t="n">
+        <v>148</v>
+      </c>
     </row>
     <row r="30" ht="20" customHeight="1">
       <c r="A30" s="1" t="n">
@@ -9521,6 +9611,9 @@
       <c r="CS30" s="1" t="n">
         <v>150.1</v>
       </c>
+      <c r="CT30" s="3" t="n">
+        <v>134.2</v>
+      </c>
     </row>
     <row r="31" ht="20" customHeight="1">
       <c r="A31" s="1" t="n">
@@ -9814,6 +9907,9 @@
       <c r="CS31" s="1" t="n">
         <v>181.3</v>
       </c>
+      <c r="CT31" s="1" t="n">
+        <v>158</v>
+      </c>
     </row>
     <row r="32" ht="20" customHeight="1">
       <c r="A32" s="1" t="n">
@@ -10107,6 +10203,9 @@
       <c r="CS32" s="1" t="n">
         <v>194</v>
       </c>
+      <c r="CT32" s="1" t="n">
+        <v>148.6</v>
+      </c>
     </row>
     <row r="33" ht="20" customHeight="1">
       <c r="A33" s="1" t="n">
@@ -10400,6 +10499,9 @@
       <c r="CS33" s="3" t="n">
         <v>138.7</v>
       </c>
+      <c r="CT33" s="1" t="n">
+        <v>157.2</v>
+      </c>
     </row>
     <row r="34" ht="20" customHeight="1">
       <c r="A34" s="1" t="n">
@@ -10693,6 +10795,9 @@
       <c r="CS34" s="1" t="n">
         <v>221.6</v>
       </c>
+      <c r="CT34" s="1" t="n">
+        <v>165.1</v>
+      </c>
     </row>
     <row r="35" ht="20" customHeight="1">
       <c r="A35" s="1" t="n">
@@ -10986,6 +11091,9 @@
       <c r="CS35" s="1" t="n">
         <v>261.4</v>
       </c>
+      <c r="CT35" s="3" t="n">
+        <v>136.2</v>
+      </c>
     </row>
     <row r="36" ht="20" customHeight="1">
       <c r="A36" s="1" t="n">
@@ -11279,6 +11387,9 @@
       <c r="CS36" s="1" t="n">
         <v>154.3</v>
       </c>
+      <c r="CT36" s="1" t="n">
+        <v>161.3</v>
+      </c>
     </row>
     <row r="37" ht="20" customHeight="1">
       <c r="A37" s="1" t="n">
@@ -11572,6 +11683,9 @@
       <c r="CS37" s="1" t="n">
         <v>151.7</v>
       </c>
+      <c r="CT37" s="1" t="n">
+        <v>166.3</v>
+      </c>
     </row>
     <row r="38" ht="20" customHeight="1">
       <c r="A38" s="1" t="n">
@@ -11865,6 +11979,9 @@
       <c r="CS38" s="1" t="n">
         <v>179.6</v>
       </c>
+      <c r="CT38" s="3" t="n">
+        <v>127.6</v>
+      </c>
     </row>
     <row r="39" ht="20" customHeight="1">
       <c r="A39" s="1" t="n">
@@ -12158,6 +12275,9 @@
       <c r="CS39" s="1" t="n">
         <v>161.2</v>
       </c>
+      <c r="CT39" s="1" t="n">
+        <v>172.4</v>
+      </c>
     </row>
     <row r="40" ht="20" customHeight="1">
       <c r="A40" s="1" t="n">
@@ -12451,6 +12571,9 @@
       <c r="CS40" s="1" t="n">
         <v>142.9</v>
       </c>
+      <c r="CT40" s="3" t="n">
+        <v>131.5</v>
+      </c>
     </row>
     <row r="41" ht="20" customHeight="1">
       <c r="A41" s="1" t="n">
@@ -12744,6 +12867,9 @@
       <c r="CS41" s="1" t="n">
         <v>149.4</v>
       </c>
+      <c r="CT41" s="3" t="n">
+        <v>135.7</v>
+      </c>
     </row>
     <row r="42" ht="20" customHeight="1">
       <c r="A42" s="1" t="n">
@@ -13037,6 +13163,9 @@
       <c r="CS42" s="1" t="n">
         <v>145.4</v>
       </c>
+      <c r="CT42" s="1" t="n">
+        <v>174.4</v>
+      </c>
     </row>
     <row r="43" ht="20" customHeight="1">
       <c r="A43" s="1" t="n">
@@ -13330,6 +13459,9 @@
       <c r="CS43" s="1" t="n">
         <v>152.4</v>
       </c>
+      <c r="CT43" s="1" t="n">
+        <v>174.6</v>
+      </c>
     </row>
     <row r="44" ht="20" customHeight="1">
       <c r="A44" s="1" t="n">
@@ -13623,6 +13755,9 @@
       <c r="CS44" s="3" t="n">
         <v>133.4</v>
       </c>
+      <c r="CT44" s="3" t="n">
+        <v>131.5</v>
+      </c>
     </row>
     <row r="45" ht="20" customHeight="1">
       <c r="A45" s="1" t="n">
@@ -13916,6 +14051,9 @@
       <c r="CS45" s="1" t="n">
         <v>211.4</v>
       </c>
+      <c r="CT45" s="1" t="n">
+        <v>187</v>
+      </c>
     </row>
     <row r="46" ht="20" customHeight="1">
       <c r="A46" s="1" t="n">
@@ -14209,6 +14347,9 @@
       <c r="CS46" s="1" t="n">
         <v>150</v>
       </c>
+      <c r="CT46" s="1" t="n">
+        <v>156.3</v>
+      </c>
     </row>
     <row r="47" ht="20" customHeight="1">
       <c r="A47" s="1" t="n">
@@ -14502,6 +14643,9 @@
       <c r="CS47" s="1" t="n">
         <v>188.7</v>
       </c>
+      <c r="CT47" s="1" t="n">
+        <v>175.2</v>
+      </c>
     </row>
     <row r="48" ht="20" customHeight="1">
       <c r="A48" s="1" t="n">
@@ -14795,6 +14939,9 @@
       <c r="CS48" s="3" t="n">
         <v>137.6</v>
       </c>
+      <c r="CT48" s="3" t="n">
+        <v>128.4</v>
+      </c>
     </row>
     <row r="49" ht="20" customHeight="1">
       <c r="A49" s="1" t="n">
@@ -15088,6 +15235,9 @@
       <c r="CS49" s="2" t="n">
         <v>110.8</v>
       </c>
+      <c r="CT49" s="1" t="n">
+        <v>168.9</v>
+      </c>
     </row>
     <row r="50" ht="20" customHeight="1">
       <c r="A50" s="1" t="n">
@@ -15381,6 +15531,9 @@
       <c r="CS50" s="1" t="n">
         <v>234.7</v>
       </c>
+      <c r="CT50" s="1" t="n">
+        <v>156.3</v>
+      </c>
     </row>
     <row r="51" ht="20" customHeight="1">
       <c r="A51" s="1" t="n">
@@ -15674,6 +15827,9 @@
       <c r="CS51" s="1" t="n">
         <v>181.5</v>
       </c>
+      <c r="CT51" s="1" t="n">
+        <v>146.9</v>
+      </c>
     </row>
     <row r="52" ht="20" customHeight="1">
       <c r="A52" s="1" t="n">
@@ -15967,6 +16123,9 @@
       <c r="CS52" s="1" t="n">
         <v>167.3</v>
       </c>
+      <c r="CT52" s="2" t="n">
+        <v>118.6</v>
+      </c>
     </row>
     <row r="53" ht="20" customHeight="1">
       <c r="A53" s="1" t="n">
@@ -16259,6 +16418,9 @@
       </c>
       <c r="CS53" s="1" t="n">
         <v>186.3</v>
+      </c>
+      <c r="CT53" s="2" t="n">
+        <v>124.9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2024-12-16
</commit_message>
<xml_diff>
--- a/マイジャグラーV_塗りつぶし済み.xlsx
+++ b/マイジャグラーV_塗りつぶし済み.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:CT53"/>
+  <dimension ref="A1:CU53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -537,6 +537,7 @@
     <col width="12" customWidth="1" min="96" max="96"/>
     <col width="12" customWidth="1" min="97" max="97"/>
     <col width="12" customWidth="1" min="98" max="98"/>
+    <col width="12" customWidth="1" min="99" max="99"/>
   </cols>
   <sheetData>
     <row r="1" ht="20" customHeight="1">
@@ -1030,6 +1031,11 @@
           <t>2024/12/15</t>
         </is>
       </c>
+      <c r="CU1" s="1" t="inlineStr">
+        <is>
+          <t>2024/12/16</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="20" customHeight="1">
       <c r="A2" s="1" t="n">
@@ -1326,6 +1332,9 @@
       <c r="CT2" s="1" t="n">
         <v>145.4</v>
       </c>
+      <c r="CU2" s="3" t="n">
+        <v>130.8</v>
+      </c>
     </row>
     <row r="3" ht="20" customHeight="1">
       <c r="A3" s="1" t="n">
@@ -1622,6 +1631,9 @@
       <c r="CT3" s="1" t="n">
         <v>147.1</v>
       </c>
+      <c r="CU3" s="1" t="n">
+        <v>192.3</v>
+      </c>
     </row>
     <row r="4" ht="20" customHeight="1">
       <c r="A4" s="1" t="n">
@@ -1918,6 +1930,9 @@
       <c r="CT4" s="1" t="n">
         <v>145.8</v>
       </c>
+      <c r="CU4" s="1" t="n">
+        <v>140</v>
+      </c>
     </row>
     <row r="5" ht="20" customHeight="1">
       <c r="A5" s="1" t="n">
@@ -2214,6 +2229,9 @@
       <c r="CT5" s="1" t="n">
         <v>140.4</v>
       </c>
+      <c r="CU5" s="1" t="n">
+        <v>211</v>
+      </c>
     </row>
     <row r="6" ht="20" customHeight="1">
       <c r="A6" s="1" t="n">
@@ -2510,6 +2528,9 @@
       <c r="CT6" s="1" t="n">
         <v>163.6</v>
       </c>
+      <c r="CU6" s="1" t="n">
+        <v>173.1</v>
+      </c>
     </row>
     <row r="7" ht="20" customHeight="1">
       <c r="A7" s="1" t="n">
@@ -2806,6 +2827,9 @@
       <c r="CT7" s="2" t="n">
         <v>118.9</v>
       </c>
+      <c r="CU7" s="1" t="n">
+        <v>144.9</v>
+      </c>
     </row>
     <row r="8" ht="20" customHeight="1">
       <c r="A8" s="1" t="n">
@@ -3102,6 +3126,9 @@
       <c r="CT8" s="1" t="n">
         <v>161</v>
       </c>
+      <c r="CU8" s="3" t="n">
+        <v>127.8</v>
+      </c>
     </row>
     <row r="9" ht="20" customHeight="1">
       <c r="A9" s="1" t="n">
@@ -3398,6 +3425,9 @@
       <c r="CT9" s="1" t="n">
         <v>161.2</v>
       </c>
+      <c r="CU9" s="1" t="n">
+        <v>183.5</v>
+      </c>
     </row>
     <row r="10" ht="20" customHeight="1">
       <c r="A10" s="1" t="n">
@@ -3694,6 +3724,9 @@
       <c r="CT10" s="1" t="n">
         <v>177.6</v>
       </c>
+      <c r="CU10" s="1" t="n">
+        <v>160.4</v>
+      </c>
     </row>
     <row r="11" ht="20" customHeight="1">
       <c r="A11" s="1" t="n">
@@ -3990,6 +4023,9 @@
       <c r="CT11" s="3" t="n">
         <v>125.8</v>
       </c>
+      <c r="CU11" s="1" t="n">
+        <v>154</v>
+      </c>
     </row>
     <row r="12" ht="20" customHeight="1">
       <c r="A12" s="1" t="n">
@@ -4286,6 +4322,9 @@
       <c r="CT12" s="1" t="n">
         <v>149.8</v>
       </c>
+      <c r="CU12" s="3" t="n">
+        <v>129.4</v>
+      </c>
     </row>
     <row r="13" ht="20" customHeight="1">
       <c r="A13" s="1" t="n">
@@ -4582,6 +4621,9 @@
       <c r="CT13" s="1" t="n">
         <v>154.8</v>
       </c>
+      <c r="CU13" s="3" t="n">
+        <v>136.2</v>
+      </c>
     </row>
     <row r="14" ht="20" customHeight="1">
       <c r="A14" s="1" t="n">
@@ -4878,6 +4920,9 @@
       <c r="CT14" s="2" t="n">
         <v>117.4</v>
       </c>
+      <c r="CU14" s="1" t="n">
+        <v>465.5</v>
+      </c>
     </row>
     <row r="15" ht="20" customHeight="1">
       <c r="A15" s="1" t="n">
@@ -5174,6 +5219,9 @@
       <c r="CT15" s="2" t="n">
         <v>124.9</v>
       </c>
+      <c r="CU15" s="1" t="n">
+        <v>146.7</v>
+      </c>
     </row>
     <row r="16" ht="20" customHeight="1">
       <c r="A16" s="1" t="n">
@@ -5470,6 +5518,9 @@
       <c r="CT16" s="1" t="n">
         <v>190.7</v>
       </c>
+      <c r="CU16" s="2" t="n">
+        <v>117.7</v>
+      </c>
     </row>
     <row r="17" ht="20" customHeight="1">
       <c r="A17" s="1" t="n">
@@ -5766,6 +5817,9 @@
       <c r="CT17" s="1" t="n">
         <v>165.3</v>
       </c>
+      <c r="CU17" s="1" t="n">
+        <v>173.3</v>
+      </c>
     </row>
     <row r="18" ht="20" customHeight="1">
       <c r="A18" s="1" t="n">
@@ -6062,6 +6116,9 @@
       <c r="CT18" s="2" t="n">
         <v>124</v>
       </c>
+      <c r="CU18" s="1" t="n">
+        <v>170.8</v>
+      </c>
     </row>
     <row r="19" ht="20" customHeight="1">
       <c r="A19" s="1" t="n">
@@ -6358,6 +6415,9 @@
       <c r="CT19" s="1" t="n">
         <v>167.4</v>
       </c>
+      <c r="CU19" s="1" t="n">
+        <v>170.8</v>
+      </c>
     </row>
     <row r="20" ht="20" customHeight="1">
       <c r="A20" s="1" t="n">
@@ -6654,6 +6714,9 @@
       <c r="CT20" s="1" t="n">
         <v>185.9</v>
       </c>
+      <c r="CU20" s="1" t="n">
+        <v>148.1</v>
+      </c>
     </row>
     <row r="21" ht="20" customHeight="1">
       <c r="A21" s="1" t="n">
@@ -6950,6 +7013,9 @@
       <c r="CT21" s="1" t="n">
         <v>165.8</v>
       </c>
+      <c r="CU21" s="3" t="n">
+        <v>138.7</v>
+      </c>
     </row>
     <row r="22" ht="20" customHeight="1">
       <c r="A22" s="1" t="n">
@@ -7246,6 +7312,9 @@
       <c r="CT22" s="1" t="n">
         <v>157.7</v>
       </c>
+      <c r="CU22" s="1" t="n">
+        <v>156</v>
+      </c>
     </row>
     <row r="23" ht="20" customHeight="1">
       <c r="A23" s="1" t="n">
@@ -7542,6 +7611,9 @@
       <c r="CT23" s="3" t="n">
         <v>126.9</v>
       </c>
+      <c r="CU23" s="1" t="n">
+        <v>393.5</v>
+      </c>
     </row>
     <row r="24" ht="20" customHeight="1">
       <c r="A24" s="1" t="n">
@@ -7838,6 +7910,9 @@
       <c r="CT24" s="1" t="n">
         <v>191.5</v>
       </c>
+      <c r="CU24" s="1" t="n">
+        <v>168.2</v>
+      </c>
     </row>
     <row r="25" ht="20" customHeight="1">
       <c r="A25" s="1" t="n">
@@ -8134,6 +8209,9 @@
       <c r="CT25" s="2" t="n">
         <v>92.09999999999999</v>
       </c>
+      <c r="CU25" s="3" t="n">
+        <v>133.5</v>
+      </c>
     </row>
     <row r="26" ht="20" customHeight="1">
       <c r="A26" s="1" t="n">
@@ -8430,6 +8508,9 @@
       <c r="CT26" s="1" t="n">
         <v>159.2</v>
       </c>
+      <c r="CU26" s="1" t="n">
+        <v>204</v>
+      </c>
     </row>
     <row r="27" ht="20" customHeight="1">
       <c r="A27" s="1" t="n">
@@ -8726,6 +8807,9 @@
       <c r="CT27" s="2" t="n">
         <v>106.9</v>
       </c>
+      <c r="CU27" s="1" t="n">
+        <v>152.2</v>
+      </c>
     </row>
     <row r="28" ht="20" customHeight="1">
       <c r="A28" s="1" t="n">
@@ -9022,6 +9106,9 @@
       <c r="CT28" s="1" t="n">
         <v>146</v>
       </c>
+      <c r="CU28" s="3" t="n">
+        <v>131.8</v>
+      </c>
     </row>
     <row r="29" ht="20" customHeight="1">
       <c r="A29" s="1" t="n">
@@ -9318,6 +9405,9 @@
       <c r="CT29" s="1" t="n">
         <v>148</v>
       </c>
+      <c r="CU29" s="1" t="n">
+        <v>173.4</v>
+      </c>
     </row>
     <row r="30" ht="20" customHeight="1">
       <c r="A30" s="1" t="n">
@@ -9614,6 +9704,9 @@
       <c r="CT30" s="3" t="n">
         <v>134.2</v>
       </c>
+      <c r="CU30" s="1" t="n">
+        <v>177.8</v>
+      </c>
     </row>
     <row r="31" ht="20" customHeight="1">
       <c r="A31" s="1" t="n">
@@ -9910,6 +10003,9 @@
       <c r="CT31" s="1" t="n">
         <v>158</v>
       </c>
+      <c r="CU31" s="1" t="n">
+        <v>163.6</v>
+      </c>
     </row>
     <row r="32" ht="20" customHeight="1">
       <c r="A32" s="1" t="n">
@@ -10206,6 +10302,9 @@
       <c r="CT32" s="1" t="n">
         <v>148.6</v>
       </c>
+      <c r="CU32" s="1" t="n">
+        <v>195</v>
+      </c>
     </row>
     <row r="33" ht="20" customHeight="1">
       <c r="A33" s="1" t="n">
@@ -10502,6 +10601,9 @@
       <c r="CT33" s="1" t="n">
         <v>157.2</v>
       </c>
+      <c r="CU33" s="1" t="n">
+        <v>161.7</v>
+      </c>
     </row>
     <row r="34" ht="20" customHeight="1">
       <c r="A34" s="1" t="n">
@@ -10798,6 +10900,9 @@
       <c r="CT34" s="1" t="n">
         <v>165.1</v>
       </c>
+      <c r="CU34" s="3" t="n">
+        <v>136.5</v>
+      </c>
     </row>
     <row r="35" ht="20" customHeight="1">
       <c r="A35" s="1" t="n">
@@ -11094,6 +11199,9 @@
       <c r="CT35" s="3" t="n">
         <v>136.2</v>
       </c>
+      <c r="CU35" s="1" t="n">
+        <v>164.7</v>
+      </c>
     </row>
     <row r="36" ht="20" customHeight="1">
       <c r="A36" s="1" t="n">
@@ -11390,6 +11498,9 @@
       <c r="CT36" s="1" t="n">
         <v>161.3</v>
       </c>
+      <c r="CU36" s="2" t="n">
+        <v>114.6</v>
+      </c>
     </row>
     <row r="37" ht="20" customHeight="1">
       <c r="A37" s="1" t="n">
@@ -11686,6 +11797,9 @@
       <c r="CT37" s="1" t="n">
         <v>166.3</v>
       </c>
+      <c r="CU37" s="1" t="n">
+        <v>206.8</v>
+      </c>
     </row>
     <row r="38" ht="20" customHeight="1">
       <c r="A38" s="1" t="n">
@@ -11982,6 +12096,9 @@
       <c r="CT38" s="3" t="n">
         <v>127.6</v>
       </c>
+      <c r="CU38" s="3" t="n">
+        <v>132.7</v>
+      </c>
     </row>
     <row r="39" ht="20" customHeight="1">
       <c r="A39" s="1" t="n">
@@ -12278,6 +12395,9 @@
       <c r="CT39" s="1" t="n">
         <v>172.4</v>
       </c>
+      <c r="CU39" s="1" t="n">
+        <v>153.9</v>
+      </c>
     </row>
     <row r="40" ht="20" customHeight="1">
       <c r="A40" s="1" t="n">
@@ -12574,6 +12694,9 @@
       <c r="CT40" s="3" t="n">
         <v>131.5</v>
       </c>
+      <c r="CU40" s="1" t="n">
+        <v>180.9</v>
+      </c>
     </row>
     <row r="41" ht="20" customHeight="1">
       <c r="A41" s="1" t="n">
@@ -12870,6 +12993,9 @@
       <c r="CT41" s="3" t="n">
         <v>135.7</v>
       </c>
+      <c r="CU41" s="1" t="n">
+        <v>188.9</v>
+      </c>
     </row>
     <row r="42" ht="20" customHeight="1">
       <c r="A42" s="1" t="n">
@@ -13166,6 +13292,9 @@
       <c r="CT42" s="1" t="n">
         <v>174.4</v>
       </c>
+      <c r="CU42" s="3" t="n">
+        <v>133.9</v>
+      </c>
     </row>
     <row r="43" ht="20" customHeight="1">
       <c r="A43" s="1" t="n">
@@ -13462,6 +13591,9 @@
       <c r="CT43" s="1" t="n">
         <v>174.6</v>
       </c>
+      <c r="CU43" s="1" t="n">
+        <v>165.5</v>
+      </c>
     </row>
     <row r="44" ht="20" customHeight="1">
       <c r="A44" s="1" t="n">
@@ -13758,6 +13890,9 @@
       <c r="CT44" s="3" t="n">
         <v>131.5</v>
       </c>
+      <c r="CU44" s="1" t="n">
+        <v>206.4</v>
+      </c>
     </row>
     <row r="45" ht="20" customHeight="1">
       <c r="A45" s="1" t="n">
@@ -14054,6 +14189,9 @@
       <c r="CT45" s="1" t="n">
         <v>187</v>
       </c>
+      <c r="CU45" s="1" t="n">
+        <v>141.8</v>
+      </c>
     </row>
     <row r="46" ht="20" customHeight="1">
       <c r="A46" s="1" t="n">
@@ -14350,6 +14488,9 @@
       <c r="CT46" s="1" t="n">
         <v>156.3</v>
       </c>
+      <c r="CU46" s="1" t="n">
+        <v>143.1</v>
+      </c>
     </row>
     <row r="47" ht="20" customHeight="1">
       <c r="A47" s="1" t="n">
@@ -14646,6 +14787,9 @@
       <c r="CT47" s="1" t="n">
         <v>175.2</v>
       </c>
+      <c r="CU47" s="1" t="n">
+        <v>170.7</v>
+      </c>
     </row>
     <row r="48" ht="20" customHeight="1">
       <c r="A48" s="1" t="n">
@@ -14942,6 +15086,9 @@
       <c r="CT48" s="3" t="n">
         <v>128.4</v>
       </c>
+      <c r="CU48" s="3" t="n">
+        <v>133.6</v>
+      </c>
     </row>
     <row r="49" ht="20" customHeight="1">
       <c r="A49" s="1" t="n">
@@ -15238,6 +15385,9 @@
       <c r="CT49" s="1" t="n">
         <v>168.9</v>
       </c>
+      <c r="CU49" s="1" t="n">
+        <v>163.6</v>
+      </c>
     </row>
     <row r="50" ht="20" customHeight="1">
       <c r="A50" s="1" t="n">
@@ -15534,6 +15684,9 @@
       <c r="CT50" s="1" t="n">
         <v>156.3</v>
       </c>
+      <c r="CU50" s="1" t="n">
+        <v>417</v>
+      </c>
     </row>
     <row r="51" ht="20" customHeight="1">
       <c r="A51" s="1" t="n">
@@ -15830,6 +15983,9 @@
       <c r="CT51" s="1" t="n">
         <v>146.9</v>
       </c>
+      <c r="CU51" s="1" t="n">
+        <v>146</v>
+      </c>
     </row>
     <row r="52" ht="20" customHeight="1">
       <c r="A52" s="1" t="n">
@@ -16126,6 +16282,9 @@
       <c r="CT52" s="2" t="n">
         <v>118.6</v>
       </c>
+      <c r="CU52" s="1" t="n">
+        <v>238.1</v>
+      </c>
     </row>
     <row r="53" ht="20" customHeight="1">
       <c r="A53" s="1" t="n">
@@ -16421,6 +16580,9 @@
       </c>
       <c r="CT53" s="2" t="n">
         <v>124.9</v>
+      </c>
+      <c r="CU53" s="1" t="n">
+        <v>146.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2024-12-17
</commit_message>
<xml_diff>
--- a/マイジャグラーV_塗りつぶし済み.xlsx
+++ b/マイジャグラーV_塗りつぶし済み.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:CU53"/>
+  <dimension ref="A1:CV53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -538,6 +538,7 @@
     <col width="12" customWidth="1" min="97" max="97"/>
     <col width="12" customWidth="1" min="98" max="98"/>
     <col width="12" customWidth="1" min="99" max="99"/>
+    <col width="12" customWidth="1" min="100" max="100"/>
   </cols>
   <sheetData>
     <row r="1" ht="20" customHeight="1">
@@ -1036,6 +1037,11 @@
           <t>2024/12/16</t>
         </is>
       </c>
+      <c r="CV1" s="1" t="inlineStr">
+        <is>
+          <t>2024/12/17</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="20" customHeight="1">
       <c r="A2" s="1" t="n">
@@ -1335,6 +1341,9 @@
       <c r="CU2" s="3" t="n">
         <v>130.8</v>
       </c>
+      <c r="CV2" s="2" t="n">
+        <v>114.3</v>
+      </c>
     </row>
     <row r="3" ht="20" customHeight="1">
       <c r="A3" s="1" t="n">
@@ -1634,6 +1643,9 @@
       <c r="CU3" s="1" t="n">
         <v>192.3</v>
       </c>
+      <c r="CV3" s="3" t="n">
+        <v>138.3</v>
+      </c>
     </row>
     <row r="4" ht="20" customHeight="1">
       <c r="A4" s="1" t="n">
@@ -1933,6 +1945,9 @@
       <c r="CU4" s="1" t="n">
         <v>140</v>
       </c>
+      <c r="CV4" s="1" t="n">
+        <v>145.7</v>
+      </c>
     </row>
     <row r="5" ht="20" customHeight="1">
       <c r="A5" s="1" t="n">
@@ -2232,6 +2247,9 @@
       <c r="CU5" s="1" t="n">
         <v>211</v>
       </c>
+      <c r="CV5" s="3" t="n">
+        <v>126.4</v>
+      </c>
     </row>
     <row r="6" ht="20" customHeight="1">
       <c r="A6" s="1" t="n">
@@ -2531,6 +2549,9 @@
       <c r="CU6" s="1" t="n">
         <v>173.1</v>
       </c>
+      <c r="CV6" s="3" t="n">
+        <v>138.6</v>
+      </c>
     </row>
     <row r="7" ht="20" customHeight="1">
       <c r="A7" s="1" t="n">
@@ -2830,6 +2851,9 @@
       <c r="CU7" s="1" t="n">
         <v>144.9</v>
       </c>
+      <c r="CV7" s="1" t="n">
+        <v>177</v>
+      </c>
     </row>
     <row r="8" ht="20" customHeight="1">
       <c r="A8" s="1" t="n">
@@ -3129,6 +3153,9 @@
       <c r="CU8" s="3" t="n">
         <v>127.8</v>
       </c>
+      <c r="CV8" s="1" t="n">
+        <v>151.8</v>
+      </c>
     </row>
     <row r="9" ht="20" customHeight="1">
       <c r="A9" s="1" t="n">
@@ -3428,6 +3455,9 @@
       <c r="CU9" s="1" t="n">
         <v>183.5</v>
       </c>
+      <c r="CV9" s="3" t="n">
+        <v>138.6</v>
+      </c>
     </row>
     <row r="10" ht="20" customHeight="1">
       <c r="A10" s="1" t="n">
@@ -3727,6 +3757,9 @@
       <c r="CU10" s="1" t="n">
         <v>160.4</v>
       </c>
+      <c r="CV10" s="2" t="n">
+        <v>108.4</v>
+      </c>
     </row>
     <row r="11" ht="20" customHeight="1">
       <c r="A11" s="1" t="n">
@@ -4026,6 +4059,9 @@
       <c r="CU11" s="1" t="n">
         <v>154</v>
       </c>
+      <c r="CV11" s="1" t="n">
+        <v>150.6</v>
+      </c>
     </row>
     <row r="12" ht="20" customHeight="1">
       <c r="A12" s="1" t="n">
@@ -4325,6 +4361,9 @@
       <c r="CU12" s="3" t="n">
         <v>129.4</v>
       </c>
+      <c r="CV12" s="1" t="n">
+        <v>171.4</v>
+      </c>
     </row>
     <row r="13" ht="20" customHeight="1">
       <c r="A13" s="1" t="n">
@@ -4624,6 +4663,9 @@
       <c r="CU13" s="3" t="n">
         <v>136.2</v>
       </c>
+      <c r="CV13" s="2" t="n">
+        <v>122.7</v>
+      </c>
     </row>
     <row r="14" ht="20" customHeight="1">
       <c r="A14" s="1" t="n">
@@ -4923,6 +4965,9 @@
       <c r="CU14" s="1" t="n">
         <v>465.5</v>
       </c>
+      <c r="CV14" s="1" t="n">
+        <v>149.5</v>
+      </c>
     </row>
     <row r="15" ht="20" customHeight="1">
       <c r="A15" s="1" t="n">
@@ -5222,6 +5267,9 @@
       <c r="CU15" s="1" t="n">
         <v>146.7</v>
       </c>
+      <c r="CV15" s="1" t="n">
+        <v>156.1</v>
+      </c>
     </row>
     <row r="16" ht="20" customHeight="1">
       <c r="A16" s="1" t="n">
@@ -5521,6 +5569,9 @@
       <c r="CU16" s="2" t="n">
         <v>117.7</v>
       </c>
+      <c r="CV16" s="1" t="n">
+        <v>195.9</v>
+      </c>
     </row>
     <row r="17" ht="20" customHeight="1">
       <c r="A17" s="1" t="n">
@@ -5820,6 +5871,9 @@
       <c r="CU17" s="1" t="n">
         <v>173.3</v>
       </c>
+      <c r="CV17" s="1" t="n">
+        <v>161.1</v>
+      </c>
     </row>
     <row r="18" ht="20" customHeight="1">
       <c r="A18" s="1" t="n">
@@ -6119,6 +6173,9 @@
       <c r="CU18" s="1" t="n">
         <v>170.8</v>
       </c>
+      <c r="CV18" s="1" t="n">
+        <v>164.9</v>
+      </c>
     </row>
     <row r="19" ht="20" customHeight="1">
       <c r="A19" s="1" t="n">
@@ -6418,6 +6475,9 @@
       <c r="CU19" s="1" t="n">
         <v>170.8</v>
       </c>
+      <c r="CV19" s="1" t="n">
+        <v>159.4</v>
+      </c>
     </row>
     <row r="20" ht="20" customHeight="1">
       <c r="A20" s="1" t="n">
@@ -6717,6 +6777,9 @@
       <c r="CU20" s="1" t="n">
         <v>148.1</v>
       </c>
+      <c r="CV20" s="3" t="n">
+        <v>137.2</v>
+      </c>
     </row>
     <row r="21" ht="20" customHeight="1">
       <c r="A21" s="1" t="n">
@@ -7016,6 +7079,9 @@
       <c r="CU21" s="3" t="n">
         <v>138.7</v>
       </c>
+      <c r="CV21" s="1" t="n">
+        <v>141.8</v>
+      </c>
     </row>
     <row r="22" ht="20" customHeight="1">
       <c r="A22" s="1" t="n">
@@ -7315,6 +7381,9 @@
       <c r="CU22" s="1" t="n">
         <v>156</v>
       </c>
+      <c r="CV22" s="1" t="n">
+        <v>147.6</v>
+      </c>
     </row>
     <row r="23" ht="20" customHeight="1">
       <c r="A23" s="1" t="n">
@@ -7614,6 +7683,9 @@
       <c r="CU23" s="1" t="n">
         <v>393.5</v>
       </c>
+      <c r="CV23" s="1" t="n">
+        <v>256</v>
+      </c>
     </row>
     <row r="24" ht="20" customHeight="1">
       <c r="A24" s="1" t="n">
@@ -7913,6 +7985,9 @@
       <c r="CU24" s="1" t="n">
         <v>168.2</v>
       </c>
+      <c r="CV24" s="3" t="n">
+        <v>136.2</v>
+      </c>
     </row>
     <row r="25" ht="20" customHeight="1">
       <c r="A25" s="1" t="n">
@@ -8212,6 +8287,9 @@
       <c r="CU25" s="3" t="n">
         <v>133.5</v>
       </c>
+      <c r="CV25" s="1" t="n">
+        <v>150.1</v>
+      </c>
     </row>
     <row r="26" ht="20" customHeight="1">
       <c r="A26" s="1" t="n">
@@ -8511,6 +8589,9 @@
       <c r="CU26" s="1" t="n">
         <v>204</v>
       </c>
+      <c r="CV26" s="3" t="n">
+        <v>127.3</v>
+      </c>
     </row>
     <row r="27" ht="20" customHeight="1">
       <c r="A27" s="1" t="n">
@@ -8810,6 +8891,9 @@
       <c r="CU27" s="1" t="n">
         <v>152.2</v>
       </c>
+      <c r="CV27" s="1" t="n">
+        <v>156.5</v>
+      </c>
     </row>
     <row r="28" ht="20" customHeight="1">
       <c r="A28" s="1" t="n">
@@ -9109,6 +9193,9 @@
       <c r="CU28" s="3" t="n">
         <v>131.8</v>
       </c>
+      <c r="CV28" s="1" t="n">
+        <v>190.3</v>
+      </c>
     </row>
     <row r="29" ht="20" customHeight="1">
       <c r="A29" s="1" t="n">
@@ -9408,6 +9495,9 @@
       <c r="CU29" s="1" t="n">
         <v>173.4</v>
       </c>
+      <c r="CV29" s="1" t="n">
+        <v>168</v>
+      </c>
     </row>
     <row r="30" ht="20" customHeight="1">
       <c r="A30" s="1" t="n">
@@ -9707,6 +9797,9 @@
       <c r="CU30" s="1" t="n">
         <v>177.8</v>
       </c>
+      <c r="CV30" s="3" t="n">
+        <v>125.4</v>
+      </c>
     </row>
     <row r="31" ht="20" customHeight="1">
       <c r="A31" s="1" t="n">
@@ -10006,6 +10099,9 @@
       <c r="CU31" s="1" t="n">
         <v>163.6</v>
       </c>
+      <c r="CV31" s="1" t="n">
+        <v>173.6</v>
+      </c>
     </row>
     <row r="32" ht="20" customHeight="1">
       <c r="A32" s="1" t="n">
@@ -10305,6 +10401,9 @@
       <c r="CU32" s="1" t="n">
         <v>195</v>
       </c>
+      <c r="CV32" s="1" t="n">
+        <v>181.2</v>
+      </c>
     </row>
     <row r="33" ht="20" customHeight="1">
       <c r="A33" s="1" t="n">
@@ -10604,6 +10703,9 @@
       <c r="CU33" s="1" t="n">
         <v>161.7</v>
       </c>
+      <c r="CV33" s="3" t="n">
+        <v>134.5</v>
+      </c>
     </row>
     <row r="34" ht="20" customHeight="1">
       <c r="A34" s="1" t="n">
@@ -10903,6 +11005,9 @@
       <c r="CU34" s="3" t="n">
         <v>136.5</v>
       </c>
+      <c r="CV34" s="1" t="n">
+        <v>160.8</v>
+      </c>
     </row>
     <row r="35" ht="20" customHeight="1">
       <c r="A35" s="1" t="n">
@@ -11202,6 +11307,9 @@
       <c r="CU35" s="1" t="n">
         <v>164.7</v>
       </c>
+      <c r="CV35" s="3" t="n">
+        <v>131</v>
+      </c>
     </row>
     <row r="36" ht="20" customHeight="1">
       <c r="A36" s="1" t="n">
@@ -11501,6 +11609,9 @@
       <c r="CU36" s="2" t="n">
         <v>114.6</v>
       </c>
+      <c r="CV36" s="1" t="n">
+        <v>172.4</v>
+      </c>
     </row>
     <row r="37" ht="20" customHeight="1">
       <c r="A37" s="1" t="n">
@@ -11800,6 +11911,9 @@
       <c r="CU37" s="1" t="n">
         <v>206.8</v>
       </c>
+      <c r="CV37" s="1" t="n">
+        <v>151.7</v>
+      </c>
     </row>
     <row r="38" ht="20" customHeight="1">
       <c r="A38" s="1" t="n">
@@ -12099,6 +12213,9 @@
       <c r="CU38" s="3" t="n">
         <v>132.7</v>
       </c>
+      <c r="CV38" s="3" t="n">
+        <v>128</v>
+      </c>
     </row>
     <row r="39" ht="20" customHeight="1">
       <c r="A39" s="1" t="n">
@@ -12398,6 +12515,9 @@
       <c r="CU39" s="1" t="n">
         <v>153.9</v>
       </c>
+      <c r="CV39" s="1" t="n">
+        <v>168.2</v>
+      </c>
     </row>
     <row r="40" ht="20" customHeight="1">
       <c r="A40" s="1" t="n">
@@ -12697,6 +12817,9 @@
       <c r="CU40" s="1" t="n">
         <v>180.9</v>
       </c>
+      <c r="CV40" s="2" t="n">
+        <v>117.4</v>
+      </c>
     </row>
     <row r="41" ht="20" customHeight="1">
       <c r="A41" s="1" t="n">
@@ -12996,6 +13119,9 @@
       <c r="CU41" s="1" t="n">
         <v>188.9</v>
       </c>
+      <c r="CV41" s="1" t="n">
+        <v>185.9</v>
+      </c>
     </row>
     <row r="42" ht="20" customHeight="1">
       <c r="A42" s="1" t="n">
@@ -13295,6 +13421,9 @@
       <c r="CU42" s="3" t="n">
         <v>133.9</v>
       </c>
+      <c r="CV42" s="1" t="n">
+        <v>145.8</v>
+      </c>
     </row>
     <row r="43" ht="20" customHeight="1">
       <c r="A43" s="1" t="n">
@@ -13594,6 +13723,9 @@
       <c r="CU43" s="1" t="n">
         <v>165.5</v>
       </c>
+      <c r="CV43" s="2" t="n">
+        <v>118.6</v>
+      </c>
     </row>
     <row r="44" ht="20" customHeight="1">
       <c r="A44" s="1" t="n">
@@ -13893,6 +14025,9 @@
       <c r="CU44" s="1" t="n">
         <v>206.4</v>
       </c>
+      <c r="CV44" s="3" t="n">
+        <v>134.5</v>
+      </c>
     </row>
     <row r="45" ht="20" customHeight="1">
       <c r="A45" s="1" t="n">
@@ -14192,6 +14327,9 @@
       <c r="CU45" s="1" t="n">
         <v>141.8</v>
       </c>
+      <c r="CV45" s="3" t="n">
+        <v>126</v>
+      </c>
     </row>
     <row r="46" ht="20" customHeight="1">
       <c r="A46" s="1" t="n">
@@ -14491,6 +14629,9 @@
       <c r="CU46" s="1" t="n">
         <v>143.1</v>
       </c>
+      <c r="CV46" s="1" t="n">
+        <v>156.5</v>
+      </c>
     </row>
     <row r="47" ht="20" customHeight="1">
       <c r="A47" s="1" t="n">
@@ -14790,6 +14931,9 @@
       <c r="CU47" s="1" t="n">
         <v>170.7</v>
       </c>
+      <c r="CV47" s="1" t="n">
+        <v>165.7</v>
+      </c>
     </row>
     <row r="48" ht="20" customHeight="1">
       <c r="A48" s="1" t="n">
@@ -15089,6 +15233,9 @@
       <c r="CU48" s="3" t="n">
         <v>133.6</v>
       </c>
+      <c r="CV48" s="1" t="n">
+        <v>164.7</v>
+      </c>
     </row>
     <row r="49" ht="20" customHeight="1">
       <c r="A49" s="1" t="n">
@@ -15388,6 +15535,9 @@
       <c r="CU49" s="1" t="n">
         <v>163.6</v>
       </c>
+      <c r="CV49" s="3" t="n">
+        <v>130.6</v>
+      </c>
     </row>
     <row r="50" ht="20" customHeight="1">
       <c r="A50" s="1" t="n">
@@ -15687,6 +15837,9 @@
       <c r="CU50" s="1" t="n">
         <v>417</v>
       </c>
+      <c r="CV50" s="1" t="n">
+        <v>152.8</v>
+      </c>
     </row>
     <row r="51" ht="20" customHeight="1">
       <c r="A51" s="1" t="n">
@@ -15986,6 +16139,9 @@
       <c r="CU51" s="1" t="n">
         <v>146</v>
       </c>
+      <c r="CV51" s="1" t="n">
+        <v>250.1</v>
+      </c>
     </row>
     <row r="52" ht="20" customHeight="1">
       <c r="A52" s="1" t="n">
@@ -16285,6 +16441,9 @@
       <c r="CU52" s="1" t="n">
         <v>238.1</v>
       </c>
+      <c r="CV52" s="3" t="n">
+        <v>132.4</v>
+      </c>
     </row>
     <row r="53" ht="20" customHeight="1">
       <c r="A53" s="1" t="n">
@@ -16583,6 +16742,9 @@
       </c>
       <c r="CU53" s="1" t="n">
         <v>146.2</v>
+      </c>
+      <c r="CV53" s="1" t="n">
+        <v>235.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2024-12-18
</commit_message>
<xml_diff>
--- a/マイジャグラーV_塗りつぶし済み.xlsx
+++ b/マイジャグラーV_塗りつぶし済み.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:CV53"/>
+  <dimension ref="A1:CW53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -539,6 +539,7 @@
     <col width="12" customWidth="1" min="98" max="98"/>
     <col width="12" customWidth="1" min="99" max="99"/>
     <col width="12" customWidth="1" min="100" max="100"/>
+    <col width="12" customWidth="1" min="101" max="101"/>
   </cols>
   <sheetData>
     <row r="1" ht="20" customHeight="1">
@@ -1042,6 +1043,11 @@
           <t>2024/12/17</t>
         </is>
       </c>
+      <c r="CW1" s="1" t="inlineStr">
+        <is>
+          <t>2024/12/18</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="20" customHeight="1">
       <c r="A2" s="1" t="n">
@@ -1344,6 +1350,9 @@
       <c r="CV2" s="2" t="n">
         <v>114.3</v>
       </c>
+      <c r="CW2" s="1" t="n">
+        <v>191.9</v>
+      </c>
     </row>
     <row r="3" ht="20" customHeight="1">
       <c r="A3" s="1" t="n">
@@ -1646,6 +1655,9 @@
       <c r="CV3" s="3" t="n">
         <v>138.3</v>
       </c>
+      <c r="CW3" s="2" t="n">
+        <v>110</v>
+      </c>
     </row>
     <row r="4" ht="20" customHeight="1">
       <c r="A4" s="1" t="n">
@@ -1948,6 +1960,9 @@
       <c r="CV4" s="1" t="n">
         <v>145.7</v>
       </c>
+      <c r="CW4" s="1" t="n">
+        <v>156.4</v>
+      </c>
     </row>
     <row r="5" ht="20" customHeight="1">
       <c r="A5" s="1" t="n">
@@ -2250,6 +2265,9 @@
       <c r="CV5" s="3" t="n">
         <v>126.4</v>
       </c>
+      <c r="CW5" s="1" t="n">
+        <v>201.2</v>
+      </c>
     </row>
     <row r="6" ht="20" customHeight="1">
       <c r="A6" s="1" t="n">
@@ -2552,6 +2570,9 @@
       <c r="CV6" s="3" t="n">
         <v>138.6</v>
       </c>
+      <c r="CW6" s="3" t="n">
+        <v>125.1</v>
+      </c>
     </row>
     <row r="7" ht="20" customHeight="1">
       <c r="A7" s="1" t="n">
@@ -2854,6 +2875,9 @@
       <c r="CV7" s="1" t="n">
         <v>177</v>
       </c>
+      <c r="CW7" s="1" t="n">
+        <v>224.5</v>
+      </c>
     </row>
     <row r="8" ht="20" customHeight="1">
       <c r="A8" s="1" t="n">
@@ -3156,6 +3180,9 @@
       <c r="CV8" s="1" t="n">
         <v>151.8</v>
       </c>
+      <c r="CW8" s="3" t="n">
+        <v>138.3</v>
+      </c>
     </row>
     <row r="9" ht="20" customHeight="1">
       <c r="A9" s="1" t="n">
@@ -3458,6 +3485,9 @@
       <c r="CV9" s="3" t="n">
         <v>138.6</v>
       </c>
+      <c r="CW9" s="1" t="n">
+        <v>190.3</v>
+      </c>
     </row>
     <row r="10" ht="20" customHeight="1">
       <c r="A10" s="1" t="n">
@@ -3760,6 +3790,9 @@
       <c r="CV10" s="2" t="n">
         <v>108.4</v>
       </c>
+      <c r="CW10" s="1" t="n">
+        <v>239.9</v>
+      </c>
     </row>
     <row r="11" ht="20" customHeight="1">
       <c r="A11" s="1" t="n">
@@ -4062,6 +4095,9 @@
       <c r="CV11" s="1" t="n">
         <v>150.6</v>
       </c>
+      <c r="CW11" s="3" t="n">
+        <v>132.5</v>
+      </c>
     </row>
     <row r="12" ht="20" customHeight="1">
       <c r="A12" s="1" t="n">
@@ -4364,6 +4400,9 @@
       <c r="CV12" s="1" t="n">
         <v>171.4</v>
       </c>
+      <c r="CW12" s="3" t="n">
+        <v>133.1</v>
+      </c>
     </row>
     <row r="13" ht="20" customHeight="1">
       <c r="A13" s="1" t="n">
@@ -4666,6 +4705,9 @@
       <c r="CV13" s="2" t="n">
         <v>122.7</v>
       </c>
+      <c r="CW13" s="1" t="n">
+        <v>163.5</v>
+      </c>
     </row>
     <row r="14" ht="20" customHeight="1">
       <c r="A14" s="1" t="n">
@@ -4968,6 +5010,9 @@
       <c r="CV14" s="1" t="n">
         <v>149.5</v>
       </c>
+      <c r="CW14" s="1" t="n">
+        <v>243.6</v>
+      </c>
     </row>
     <row r="15" ht="20" customHeight="1">
       <c r="A15" s="1" t="n">
@@ -5270,6 +5315,9 @@
       <c r="CV15" s="1" t="n">
         <v>156.1</v>
       </c>
+      <c r="CW15" s="1" t="n">
+        <v>140.6</v>
+      </c>
     </row>
     <row r="16" ht="20" customHeight="1">
       <c r="A16" s="1" t="n">
@@ -5572,6 +5620,9 @@
       <c r="CV16" s="1" t="n">
         <v>195.9</v>
       </c>
+      <c r="CW16" s="1" t="n">
+        <v>164.8</v>
+      </c>
     </row>
     <row r="17" ht="20" customHeight="1">
       <c r="A17" s="1" t="n">
@@ -5874,6 +5925,9 @@
       <c r="CV17" s="1" t="n">
         <v>161.1</v>
       </c>
+      <c r="CW17" s="1" t="n">
+        <v>178.5</v>
+      </c>
     </row>
     <row r="18" ht="20" customHeight="1">
       <c r="A18" s="1" t="n">
@@ -6176,6 +6230,9 @@
       <c r="CV18" s="1" t="n">
         <v>164.9</v>
       </c>
+      <c r="CW18" s="1" t="n">
+        <v>312.9</v>
+      </c>
     </row>
     <row r="19" ht="20" customHeight="1">
       <c r="A19" s="1" t="n">
@@ -6478,6 +6535,9 @@
       <c r="CV19" s="1" t="n">
         <v>159.4</v>
       </c>
+      <c r="CW19" s="1" t="n">
+        <v>153.6</v>
+      </c>
     </row>
     <row r="20" ht="20" customHeight="1">
       <c r="A20" s="1" t="n">
@@ -6780,6 +6840,9 @@
       <c r="CV20" s="3" t="n">
         <v>137.2</v>
       </c>
+      <c r="CW20" s="1" t="n">
+        <v>188.5</v>
+      </c>
     </row>
     <row r="21" ht="20" customHeight="1">
       <c r="A21" s="1" t="n">
@@ -7082,6 +7145,9 @@
       <c r="CV21" s="1" t="n">
         <v>141.8</v>
       </c>
+      <c r="CW21" s="3" t="n">
+        <v>128.2</v>
+      </c>
     </row>
     <row r="22" ht="20" customHeight="1">
       <c r="A22" s="1" t="n">
@@ -7384,6 +7450,9 @@
       <c r="CV22" s="1" t="n">
         <v>147.6</v>
       </c>
+      <c r="CW22" s="1" t="n">
+        <v>148</v>
+      </c>
     </row>
     <row r="23" ht="20" customHeight="1">
       <c r="A23" s="1" t="n">
@@ -7686,6 +7755,9 @@
       <c r="CV23" s="1" t="n">
         <v>256</v>
       </c>
+      <c r="CW23" s="1" t="n">
+        <v>149.1</v>
+      </c>
     </row>
     <row r="24" ht="20" customHeight="1">
       <c r="A24" s="1" t="n">
@@ -7988,6 +8060,9 @@
       <c r="CV24" s="3" t="n">
         <v>136.2</v>
       </c>
+      <c r="CW24" s="1" t="n">
+        <v>145.6</v>
+      </c>
     </row>
     <row r="25" ht="20" customHeight="1">
       <c r="A25" s="1" t="n">
@@ -8290,6 +8365,9 @@
       <c r="CV25" s="1" t="n">
         <v>150.1</v>
       </c>
+      <c r="CW25" s="1" t="n">
+        <v>218.6</v>
+      </c>
     </row>
     <row r="26" ht="20" customHeight="1">
       <c r="A26" s="1" t="n">
@@ -8592,6 +8670,9 @@
       <c r="CV26" s="3" t="n">
         <v>127.3</v>
       </c>
+      <c r="CW26" s="3" t="n">
+        <v>135.7</v>
+      </c>
     </row>
     <row r="27" ht="20" customHeight="1">
       <c r="A27" s="1" t="n">
@@ -8894,6 +8975,9 @@
       <c r="CV27" s="1" t="n">
         <v>156.5</v>
       </c>
+      <c r="CW27" s="1" t="n">
+        <v>191</v>
+      </c>
     </row>
     <row r="28" ht="20" customHeight="1">
       <c r="A28" s="1" t="n">
@@ -9196,6 +9280,9 @@
       <c r="CV28" s="1" t="n">
         <v>190.3</v>
       </c>
+      <c r="CW28" s="1" t="n">
+        <v>145.9</v>
+      </c>
     </row>
     <row r="29" ht="20" customHeight="1">
       <c r="A29" s="1" t="n">
@@ -9498,6 +9585,9 @@
       <c r="CV29" s="1" t="n">
         <v>168</v>
       </c>
+      <c r="CW29" s="1" t="n">
+        <v>263.9</v>
+      </c>
     </row>
     <row r="30" ht="20" customHeight="1">
       <c r="A30" s="1" t="n">
@@ -9800,6 +9890,9 @@
       <c r="CV30" s="3" t="n">
         <v>125.4</v>
       </c>
+      <c r="CW30" s="1" t="n">
+        <v>150.9</v>
+      </c>
     </row>
     <row r="31" ht="20" customHeight="1">
       <c r="A31" s="1" t="n">
@@ -10102,6 +10195,9 @@
       <c r="CV31" s="1" t="n">
         <v>173.6</v>
       </c>
+      <c r="CW31" s="1" t="n">
+        <v>154.4</v>
+      </c>
     </row>
     <row r="32" ht="20" customHeight="1">
       <c r="A32" s="1" t="n">
@@ -10404,6 +10500,9 @@
       <c r="CV32" s="1" t="n">
         <v>181.2</v>
       </c>
+      <c r="CW32" s="1" t="n">
+        <v>144.1</v>
+      </c>
     </row>
     <row r="33" ht="20" customHeight="1">
       <c r="A33" s="1" t="n">
@@ -10706,6 +10805,9 @@
       <c r="CV33" s="3" t="n">
         <v>134.5</v>
       </c>
+      <c r="CW33" s="1" t="n">
+        <v>200.5</v>
+      </c>
     </row>
     <row r="34" ht="20" customHeight="1">
       <c r="A34" s="1" t="n">
@@ -11008,6 +11110,9 @@
       <c r="CV34" s="1" t="n">
         <v>160.8</v>
       </c>
+      <c r="CW34" s="2" t="n">
+        <v>117.2</v>
+      </c>
     </row>
     <row r="35" ht="20" customHeight="1">
       <c r="A35" s="1" t="n">
@@ -11310,6 +11415,9 @@
       <c r="CV35" s="3" t="n">
         <v>131</v>
       </c>
+      <c r="CW35" s="3" t="n">
+        <v>132.9</v>
+      </c>
     </row>
     <row r="36" ht="20" customHeight="1">
       <c r="A36" s="1" t="n">
@@ -11612,6 +11720,9 @@
       <c r="CV36" s="1" t="n">
         <v>172.4</v>
       </c>
+      <c r="CW36" s="1" t="n">
+        <v>227</v>
+      </c>
     </row>
     <row r="37" ht="20" customHeight="1">
       <c r="A37" s="1" t="n">
@@ -11914,6 +12025,9 @@
       <c r="CV37" s="1" t="n">
         <v>151.7</v>
       </c>
+      <c r="CW37" s="1" t="n">
+        <v>170.5</v>
+      </c>
     </row>
     <row r="38" ht="20" customHeight="1">
       <c r="A38" s="1" t="n">
@@ -12216,6 +12330,9 @@
       <c r="CV38" s="3" t="n">
         <v>128</v>
       </c>
+      <c r="CW38" s="3" t="n">
+        <v>134</v>
+      </c>
     </row>
     <row r="39" ht="20" customHeight="1">
       <c r="A39" s="1" t="n">
@@ -12518,6 +12635,9 @@
       <c r="CV39" s="1" t="n">
         <v>168.2</v>
       </c>
+      <c r="CW39" s="1" t="n">
+        <v>159.7</v>
+      </c>
     </row>
     <row r="40" ht="20" customHeight="1">
       <c r="A40" s="1" t="n">
@@ -12820,6 +12940,9 @@
       <c r="CV40" s="2" t="n">
         <v>117.4</v>
       </c>
+      <c r="CW40" s="1" t="n">
+        <v>194.7</v>
+      </c>
     </row>
     <row r="41" ht="20" customHeight="1">
       <c r="A41" s="1" t="n">
@@ -13122,6 +13245,9 @@
       <c r="CV41" s="1" t="n">
         <v>185.9</v>
       </c>
+      <c r="CW41" s="1" t="n">
+        <v>164.1</v>
+      </c>
     </row>
     <row r="42" ht="20" customHeight="1">
       <c r="A42" s="1" t="n">
@@ -13424,6 +13550,9 @@
       <c r="CV42" s="1" t="n">
         <v>145.8</v>
       </c>
+      <c r="CW42" s="1" t="n">
+        <v>160.3</v>
+      </c>
     </row>
     <row r="43" ht="20" customHeight="1">
       <c r="A43" s="1" t="n">
@@ -13726,6 +13855,9 @@
       <c r="CV43" s="2" t="n">
         <v>118.6</v>
       </c>
+      <c r="CW43" s="1" t="n">
+        <v>214.1</v>
+      </c>
     </row>
     <row r="44" ht="20" customHeight="1">
       <c r="A44" s="1" t="n">
@@ -14028,6 +14160,9 @@
       <c r="CV44" s="3" t="n">
         <v>134.5</v>
       </c>
+      <c r="CW44" s="1" t="n">
+        <v>234</v>
+      </c>
     </row>
     <row r="45" ht="20" customHeight="1">
       <c r="A45" s="1" t="n">
@@ -14330,6 +14465,9 @@
       <c r="CV45" s="3" t="n">
         <v>126</v>
       </c>
+      <c r="CW45" s="3" t="n">
+        <v>127.5</v>
+      </c>
     </row>
     <row r="46" ht="20" customHeight="1">
       <c r="A46" s="1" t="n">
@@ -14632,6 +14770,9 @@
       <c r="CV46" s="1" t="n">
         <v>156.5</v>
       </c>
+      <c r="CW46" s="1" t="n">
+        <v>246.4</v>
+      </c>
     </row>
     <row r="47" ht="20" customHeight="1">
       <c r="A47" s="1" t="n">
@@ -14934,6 +15075,9 @@
       <c r="CV47" s="1" t="n">
         <v>165.7</v>
       </c>
+      <c r="CW47" s="1" t="n">
+        <v>175.9</v>
+      </c>
     </row>
     <row r="48" ht="20" customHeight="1">
       <c r="A48" s="1" t="n">
@@ -15236,6 +15380,9 @@
       <c r="CV48" s="1" t="n">
         <v>164.7</v>
       </c>
+      <c r="CW48" s="3" t="n">
+        <v>137.9</v>
+      </c>
     </row>
     <row r="49" ht="20" customHeight="1">
       <c r="A49" s="1" t="n">
@@ -15538,6 +15685,9 @@
       <c r="CV49" s="3" t="n">
         <v>130.6</v>
       </c>
+      <c r="CW49" s="1" t="n">
+        <v>512.3</v>
+      </c>
     </row>
     <row r="50" ht="20" customHeight="1">
       <c r="A50" s="1" t="n">
@@ -15840,6 +15990,9 @@
       <c r="CV50" s="1" t="n">
         <v>152.8</v>
       </c>
+      <c r="CW50" s="1" t="n">
+        <v>147.8</v>
+      </c>
     </row>
     <row r="51" ht="20" customHeight="1">
       <c r="A51" s="1" t="n">
@@ -16142,6 +16295,9 @@
       <c r="CV51" s="1" t="n">
         <v>250.1</v>
       </c>
+      <c r="CW51" s="1" t="n">
+        <v>157.3</v>
+      </c>
     </row>
     <row r="52" ht="20" customHeight="1">
       <c r="A52" s="1" t="n">
@@ -16444,6 +16600,9 @@
       <c r="CV52" s="3" t="n">
         <v>132.4</v>
       </c>
+      <c r="CW52" s="1" t="n">
+        <v>155.6</v>
+      </c>
     </row>
     <row r="53" ht="20" customHeight="1">
       <c r="A53" s="1" t="n">
@@ -16745,6 +16904,9 @@
       </c>
       <c r="CV53" s="1" t="n">
         <v>235.1</v>
+      </c>
+      <c r="CW53" s="1" t="n">
+        <v>143.6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2024-12-19
</commit_message>
<xml_diff>
--- a/マイジャグラーV_塗りつぶし済み.xlsx
+++ b/マイジャグラーV_塗りつぶし済み.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:CW53"/>
+  <dimension ref="A1:CX53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -540,6 +540,7 @@
     <col width="12" customWidth="1" min="99" max="99"/>
     <col width="12" customWidth="1" min="100" max="100"/>
     <col width="12" customWidth="1" min="101" max="101"/>
+    <col width="12" customWidth="1" min="102" max="102"/>
   </cols>
   <sheetData>
     <row r="1" ht="20" customHeight="1">
@@ -1048,6 +1049,11 @@
           <t>2024/12/18</t>
         </is>
       </c>
+      <c r="CX1" s="1" t="inlineStr">
+        <is>
+          <t>2024/12/19</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="20" customHeight="1">
       <c r="A2" s="1" t="n">
@@ -1353,6 +1359,9 @@
       <c r="CW2" s="1" t="n">
         <v>191.9</v>
       </c>
+      <c r="CX2" s="1" t="n">
+        <v>140.8</v>
+      </c>
     </row>
     <row r="3" ht="20" customHeight="1">
       <c r="A3" s="1" t="n">
@@ -1658,6 +1667,9 @@
       <c r="CW3" s="2" t="n">
         <v>110</v>
       </c>
+      <c r="CX3" s="1" t="n">
+        <v>217.5</v>
+      </c>
     </row>
     <row r="4" ht="20" customHeight="1">
       <c r="A4" s="1" t="n">
@@ -1963,6 +1975,9 @@
       <c r="CW4" s="1" t="n">
         <v>156.4</v>
       </c>
+      <c r="CX4" s="1" t="n">
+        <v>182.4</v>
+      </c>
     </row>
     <row r="5" ht="20" customHeight="1">
       <c r="A5" s="1" t="n">
@@ -2268,6 +2283,9 @@
       <c r="CW5" s="1" t="n">
         <v>201.2</v>
       </c>
+      <c r="CX5" s="1" t="n">
+        <v>171.2</v>
+      </c>
     </row>
     <row r="6" ht="20" customHeight="1">
       <c r="A6" s="1" t="n">
@@ -2573,6 +2591,9 @@
       <c r="CW6" s="3" t="n">
         <v>125.1</v>
       </c>
+      <c r="CX6" s="1" t="n">
+        <v>176.2</v>
+      </c>
     </row>
     <row r="7" ht="20" customHeight="1">
       <c r="A7" s="1" t="n">
@@ -2878,6 +2899,9 @@
       <c r="CW7" s="1" t="n">
         <v>224.5</v>
       </c>
+      <c r="CX7" s="1" t="n">
+        <v>241</v>
+      </c>
     </row>
     <row r="8" ht="20" customHeight="1">
       <c r="A8" s="1" t="n">
@@ -3183,6 +3207,9 @@
       <c r="CW8" s="3" t="n">
         <v>138.3</v>
       </c>
+      <c r="CX8" s="2" t="n">
+        <v>111.6</v>
+      </c>
     </row>
     <row r="9" ht="20" customHeight="1">
       <c r="A9" s="1" t="n">
@@ -3488,6 +3515,9 @@
       <c r="CW9" s="1" t="n">
         <v>190.3</v>
       </c>
+      <c r="CX9" s="3" t="n">
+        <v>128.5</v>
+      </c>
     </row>
     <row r="10" ht="20" customHeight="1">
       <c r="A10" s="1" t="n">
@@ -3793,6 +3823,9 @@
       <c r="CW10" s="1" t="n">
         <v>239.9</v>
       </c>
+      <c r="CX10" s="1" t="n">
+        <v>143.6</v>
+      </c>
     </row>
     <row r="11" ht="20" customHeight="1">
       <c r="A11" s="1" t="n">
@@ -4098,6 +4131,9 @@
       <c r="CW11" s="3" t="n">
         <v>132.5</v>
       </c>
+      <c r="CX11" s="1" t="n">
+        <v>190.1</v>
+      </c>
     </row>
     <row r="12" ht="20" customHeight="1">
       <c r="A12" s="1" t="n">
@@ -4403,6 +4439,9 @@
       <c r="CW12" s="3" t="n">
         <v>133.1</v>
       </c>
+      <c r="CX12" s="3" t="n">
+        <v>138</v>
+      </c>
     </row>
     <row r="13" ht="20" customHeight="1">
       <c r="A13" s="1" t="n">
@@ -4708,6 +4747,9 @@
       <c r="CW13" s="1" t="n">
         <v>163.5</v>
       </c>
+      <c r="CX13" s="1" t="n">
+        <v>145.6</v>
+      </c>
     </row>
     <row r="14" ht="20" customHeight="1">
       <c r="A14" s="1" t="n">
@@ -5013,6 +5055,9 @@
       <c r="CW14" s="1" t="n">
         <v>243.6</v>
       </c>
+      <c r="CX14" s="1" t="n">
+        <v>253.4</v>
+      </c>
     </row>
     <row r="15" ht="20" customHeight="1">
       <c r="A15" s="1" t="n">
@@ -5318,6 +5363,9 @@
       <c r="CW15" s="1" t="n">
         <v>140.6</v>
       </c>
+      <c r="CX15" s="2" t="n">
+        <v>121.4</v>
+      </c>
     </row>
     <row r="16" ht="20" customHeight="1">
       <c r="A16" s="1" t="n">
@@ -5623,6 +5671,9 @@
       <c r="CW16" s="1" t="n">
         <v>164.8</v>
       </c>
+      <c r="CX16" s="1" t="n">
+        <v>164.3</v>
+      </c>
     </row>
     <row r="17" ht="20" customHeight="1">
       <c r="A17" s="1" t="n">
@@ -5928,6 +5979,9 @@
       <c r="CW17" s="1" t="n">
         <v>178.5</v>
       </c>
+      <c r="CX17" s="1" t="n">
+        <v>149.9</v>
+      </c>
     </row>
     <row r="18" ht="20" customHeight="1">
       <c r="A18" s="1" t="n">
@@ -6233,6 +6287,9 @@
       <c r="CW18" s="1" t="n">
         <v>312.9</v>
       </c>
+      <c r="CX18" s="1" t="n">
+        <v>170.7</v>
+      </c>
     </row>
     <row r="19" ht="20" customHeight="1">
       <c r="A19" s="1" t="n">
@@ -6538,6 +6595,9 @@
       <c r="CW19" s="1" t="n">
         <v>153.6</v>
       </c>
+      <c r="CX19" s="1" t="n">
+        <v>190</v>
+      </c>
     </row>
     <row r="20" ht="20" customHeight="1">
       <c r="A20" s="1" t="n">
@@ -6843,6 +6903,9 @@
       <c r="CW20" s="1" t="n">
         <v>188.5</v>
       </c>
+      <c r="CX20" s="3" t="n">
+        <v>129.8</v>
+      </c>
     </row>
     <row r="21" ht="20" customHeight="1">
       <c r="A21" s="1" t="n">
@@ -7148,6 +7211,9 @@
       <c r="CW21" s="3" t="n">
         <v>128.2</v>
       </c>
+      <c r="CX21" s="1" t="n">
+        <v>202.4</v>
+      </c>
     </row>
     <row r="22" ht="20" customHeight="1">
       <c r="A22" s="1" t="n">
@@ -7453,6 +7519,9 @@
       <c r="CW22" s="1" t="n">
         <v>148</v>
       </c>
+      <c r="CX22" s="1" t="n">
+        <v>220.3</v>
+      </c>
     </row>
     <row r="23" ht="20" customHeight="1">
       <c r="A23" s="1" t="n">
@@ -7758,6 +7827,9 @@
       <c r="CW23" s="1" t="n">
         <v>149.1</v>
       </c>
+      <c r="CX23" s="1" t="n">
+        <v>142.6</v>
+      </c>
     </row>
     <row r="24" ht="20" customHeight="1">
       <c r="A24" s="1" t="n">
@@ -8063,6 +8135,9 @@
       <c r="CW24" s="1" t="n">
         <v>145.6</v>
       </c>
+      <c r="CX24" s="1" t="n">
+        <v>211.8</v>
+      </c>
     </row>
     <row r="25" ht="20" customHeight="1">
       <c r="A25" s="1" t="n">
@@ -8368,6 +8443,9 @@
       <c r="CW25" s="1" t="n">
         <v>218.6</v>
       </c>
+      <c r="CX25" s="1" t="n">
+        <v>163.1</v>
+      </c>
     </row>
     <row r="26" ht="20" customHeight="1">
       <c r="A26" s="1" t="n">
@@ -8673,6 +8751,9 @@
       <c r="CW26" s="3" t="n">
         <v>135.7</v>
       </c>
+      <c r="CX26" s="1" t="n">
+        <v>156.6</v>
+      </c>
     </row>
     <row r="27" ht="20" customHeight="1">
       <c r="A27" s="1" t="n">
@@ -8978,6 +9059,9 @@
       <c r="CW27" s="1" t="n">
         <v>191</v>
       </c>
+      <c r="CX27" s="1" t="n">
+        <v>177.3</v>
+      </c>
     </row>
     <row r="28" ht="20" customHeight="1">
       <c r="A28" s="1" t="n">
@@ -9283,6 +9367,9 @@
       <c r="CW28" s="1" t="n">
         <v>145.9</v>
       </c>
+      <c r="CX28" s="1" t="n">
+        <v>155.6</v>
+      </c>
     </row>
     <row r="29" ht="20" customHeight="1">
       <c r="A29" s="1" t="n">
@@ -9588,6 +9675,9 @@
       <c r="CW29" s="1" t="n">
         <v>263.9</v>
       </c>
+      <c r="CX29" s="1" t="n">
+        <v>359.3</v>
+      </c>
     </row>
     <row r="30" ht="20" customHeight="1">
       <c r="A30" s="1" t="n">
@@ -9893,6 +9983,9 @@
       <c r="CW30" s="1" t="n">
         <v>150.9</v>
       </c>
+      <c r="CX30" s="1" t="n">
+        <v>152.7</v>
+      </c>
     </row>
     <row r="31" ht="20" customHeight="1">
       <c r="A31" s="1" t="n">
@@ -10198,6 +10291,9 @@
       <c r="CW31" s="1" t="n">
         <v>154.4</v>
       </c>
+      <c r="CX31" s="1" t="n">
+        <v>170.8</v>
+      </c>
     </row>
     <row r="32" ht="20" customHeight="1">
       <c r="A32" s="1" t="n">
@@ -10503,6 +10599,9 @@
       <c r="CW32" s="1" t="n">
         <v>144.1</v>
       </c>
+      <c r="CX32" s="2" t="n">
+        <v>110.6</v>
+      </c>
     </row>
     <row r="33" ht="20" customHeight="1">
       <c r="A33" s="1" t="n">
@@ -10808,6 +10907,9 @@
       <c r="CW33" s="1" t="n">
         <v>200.5</v>
       </c>
+      <c r="CX33" s="2" t="n">
+        <v>120.8</v>
+      </c>
     </row>
     <row r="34" ht="20" customHeight="1">
       <c r="A34" s="1" t="n">
@@ -11113,6 +11215,9 @@
       <c r="CW34" s="2" t="n">
         <v>117.2</v>
       </c>
+      <c r="CX34" s="1" t="n">
+        <v>142.2</v>
+      </c>
     </row>
     <row r="35" ht="20" customHeight="1">
       <c r="A35" s="1" t="n">
@@ -11418,6 +11523,9 @@
       <c r="CW35" s="3" t="n">
         <v>132.9</v>
       </c>
+      <c r="CX35" s="1" t="n">
+        <v>158.9</v>
+      </c>
     </row>
     <row r="36" ht="20" customHeight="1">
       <c r="A36" s="1" t="n">
@@ -11723,6 +11831,9 @@
       <c r="CW36" s="1" t="n">
         <v>227</v>
       </c>
+      <c r="CX36" s="1" t="n">
+        <v>140.5</v>
+      </c>
     </row>
     <row r="37" ht="20" customHeight="1">
       <c r="A37" s="1" t="n">
@@ -12028,6 +12139,9 @@
       <c r="CW37" s="1" t="n">
         <v>170.5</v>
       </c>
+      <c r="CX37" s="1" t="n">
+        <v>172</v>
+      </c>
     </row>
     <row r="38" ht="20" customHeight="1">
       <c r="A38" s="1" t="n">
@@ -12333,6 +12447,9 @@
       <c r="CW38" s="3" t="n">
         <v>134</v>
       </c>
+      <c r="CX38" s="3" t="n">
+        <v>138.9</v>
+      </c>
     </row>
     <row r="39" ht="20" customHeight="1">
       <c r="A39" s="1" t="n">
@@ -12638,6 +12755,9 @@
       <c r="CW39" s="1" t="n">
         <v>159.7</v>
       </c>
+      <c r="CX39" s="1" t="n">
+        <v>207.2</v>
+      </c>
     </row>
     <row r="40" ht="20" customHeight="1">
       <c r="A40" s="1" t="n">
@@ -12943,6 +13063,9 @@
       <c r="CW40" s="1" t="n">
         <v>194.7</v>
       </c>
+      <c r="CX40" s="1" t="n">
+        <v>204.8</v>
+      </c>
     </row>
     <row r="41" ht="20" customHeight="1">
       <c r="A41" s="1" t="n">
@@ -13248,6 +13371,9 @@
       <c r="CW41" s="1" t="n">
         <v>164.1</v>
       </c>
+      <c r="CX41" s="1" t="n">
+        <v>169.6</v>
+      </c>
     </row>
     <row r="42" ht="20" customHeight="1">
       <c r="A42" s="1" t="n">
@@ -13553,6 +13679,9 @@
       <c r="CW42" s="1" t="n">
         <v>160.3</v>
       </c>
+      <c r="CX42" s="1" t="n">
+        <v>270.3</v>
+      </c>
     </row>
     <row r="43" ht="20" customHeight="1">
       <c r="A43" s="1" t="n">
@@ -13858,6 +13987,9 @@
       <c r="CW43" s="1" t="n">
         <v>214.1</v>
       </c>
+      <c r="CX43" s="3" t="n">
+        <v>136.8</v>
+      </c>
     </row>
     <row r="44" ht="20" customHeight="1">
       <c r="A44" s="1" t="n">
@@ -14163,6 +14295,9 @@
       <c r="CW44" s="1" t="n">
         <v>234</v>
       </c>
+      <c r="CX44" s="1" t="n">
+        <v>212.6</v>
+      </c>
     </row>
     <row r="45" ht="20" customHeight="1">
       <c r="A45" s="1" t="n">
@@ -14468,6 +14603,9 @@
       <c r="CW45" s="3" t="n">
         <v>127.5</v>
       </c>
+      <c r="CX45" s="1" t="n">
+        <v>237.5</v>
+      </c>
     </row>
     <row r="46" ht="20" customHeight="1">
       <c r="A46" s="1" t="n">
@@ -14773,6 +14911,9 @@
       <c r="CW46" s="1" t="n">
         <v>246.4</v>
       </c>
+      <c r="CX46" s="1" t="n">
+        <v>303.7</v>
+      </c>
     </row>
     <row r="47" ht="20" customHeight="1">
       <c r="A47" s="1" t="n">
@@ -15078,6 +15219,9 @@
       <c r="CW47" s="1" t="n">
         <v>175.9</v>
       </c>
+      <c r="CX47" s="1" t="n">
+        <v>142.3</v>
+      </c>
     </row>
     <row r="48" ht="20" customHeight="1">
       <c r="A48" s="1" t="n">
@@ -15383,6 +15527,9 @@
       <c r="CW48" s="3" t="n">
         <v>137.9</v>
       </c>
+      <c r="CX48" s="1" t="n">
+        <v>155.2</v>
+      </c>
     </row>
     <row r="49" ht="20" customHeight="1">
       <c r="A49" s="1" t="n">
@@ -15688,6 +15835,9 @@
       <c r="CW49" s="1" t="n">
         <v>512.3</v>
       </c>
+      <c r="CX49" s="2" t="n">
+        <v>110.2</v>
+      </c>
     </row>
     <row r="50" ht="20" customHeight="1">
       <c r="A50" s="1" t="n">
@@ -15993,6 +16143,9 @@
       <c r="CW50" s="1" t="n">
         <v>147.8</v>
       </c>
+      <c r="CX50" s="1" t="n">
+        <v>148.2</v>
+      </c>
     </row>
     <row r="51" ht="20" customHeight="1">
       <c r="A51" s="1" t="n">
@@ -16298,6 +16451,9 @@
       <c r="CW51" s="1" t="n">
         <v>157.3</v>
       </c>
+      <c r="CX51" s="3" t="n">
+        <v>127.2</v>
+      </c>
     </row>
     <row r="52" ht="20" customHeight="1">
       <c r="A52" s="1" t="n">
@@ -16603,6 +16759,9 @@
       <c r="CW52" s="1" t="n">
         <v>155.6</v>
       </c>
+      <c r="CX52" s="1" t="n">
+        <v>178.1</v>
+      </c>
     </row>
     <row r="53" ht="20" customHeight="1">
       <c r="A53" s="1" t="n">
@@ -16907,6 +17066,9 @@
       </c>
       <c r="CW53" s="1" t="n">
         <v>143.6</v>
+      </c>
+      <c r="CX53" s="1" t="n">
+        <v>149.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2024-12-20
</commit_message>
<xml_diff>
--- a/マイジャグラーV_塗りつぶし済み.xlsx
+++ b/マイジャグラーV_塗りつぶし済み.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:CX53"/>
+  <dimension ref="A1:CY53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -541,6 +541,7 @@
     <col width="12" customWidth="1" min="100" max="100"/>
     <col width="12" customWidth="1" min="101" max="101"/>
     <col width="12" customWidth="1" min="102" max="102"/>
+    <col width="12" customWidth="1" min="103" max="103"/>
   </cols>
   <sheetData>
     <row r="1" ht="20" customHeight="1">
@@ -1054,6 +1055,11 @@
           <t>2024/12/19</t>
         </is>
       </c>
+      <c r="CY1" s="1" t="inlineStr">
+        <is>
+          <t>2024/12/20</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="20" customHeight="1">
       <c r="A2" s="1" t="n">
@@ -1362,6 +1368,9 @@
       <c r="CX2" s="1" t="n">
         <v>140.8</v>
       </c>
+      <c r="CY2" s="1" t="n">
+        <v>198.2</v>
+      </c>
     </row>
     <row r="3" ht="20" customHeight="1">
       <c r="A3" s="1" t="n">
@@ -1670,6 +1679,9 @@
       <c r="CX3" s="1" t="n">
         <v>217.5</v>
       </c>
+      <c r="CY3" s="3" t="n">
+        <v>133.8</v>
+      </c>
     </row>
     <row r="4" ht="20" customHeight="1">
       <c r="A4" s="1" t="n">
@@ -1978,6 +1990,9 @@
       <c r="CX4" s="1" t="n">
         <v>182.4</v>
       </c>
+      <c r="CY4" s="1" t="n">
+        <v>158.6</v>
+      </c>
     </row>
     <row r="5" ht="20" customHeight="1">
       <c r="A5" s="1" t="n">
@@ -2286,6 +2301,9 @@
       <c r="CX5" s="1" t="n">
         <v>171.2</v>
       </c>
+      <c r="CY5" s="1" t="n">
+        <v>142.2</v>
+      </c>
     </row>
     <row r="6" ht="20" customHeight="1">
       <c r="A6" s="1" t="n">
@@ -2594,6 +2612,9 @@
       <c r="CX6" s="1" t="n">
         <v>176.2</v>
       </c>
+      <c r="CY6" s="1" t="n">
+        <v>149</v>
+      </c>
     </row>
     <row r="7" ht="20" customHeight="1">
       <c r="A7" s="1" t="n">
@@ -2902,6 +2923,9 @@
       <c r="CX7" s="1" t="n">
         <v>241</v>
       </c>
+      <c r="CY7" s="1" t="n">
+        <v>245.3</v>
+      </c>
     </row>
     <row r="8" ht="20" customHeight="1">
       <c r="A8" s="1" t="n">
@@ -3210,6 +3234,9 @@
       <c r="CX8" s="2" t="n">
         <v>111.6</v>
       </c>
+      <c r="CY8" s="1" t="n">
+        <v>142.3</v>
+      </c>
     </row>
     <row r="9" ht="20" customHeight="1">
       <c r="A9" s="1" t="n">
@@ -3518,6 +3545,9 @@
       <c r="CX9" s="3" t="n">
         <v>128.5</v>
       </c>
+      <c r="CY9" s="1" t="n">
+        <v>165.9</v>
+      </c>
     </row>
     <row r="10" ht="20" customHeight="1">
       <c r="A10" s="1" t="n">
@@ -3826,6 +3856,9 @@
       <c r="CX10" s="1" t="n">
         <v>143.6</v>
       </c>
+      <c r="CY10" s="1" t="n">
+        <v>204</v>
+      </c>
     </row>
     <row r="11" ht="20" customHeight="1">
       <c r="A11" s="1" t="n">
@@ -4134,6 +4167,9 @@
       <c r="CX11" s="1" t="n">
         <v>190.1</v>
       </c>
+      <c r="CY11" s="1" t="n">
+        <v>247</v>
+      </c>
     </row>
     <row r="12" ht="20" customHeight="1">
       <c r="A12" s="1" t="n">
@@ -4442,6 +4478,9 @@
       <c r="CX12" s="3" t="n">
         <v>138</v>
       </c>
+      <c r="CY12" s="3" t="n">
+        <v>134.4</v>
+      </c>
     </row>
     <row r="13" ht="20" customHeight="1">
       <c r="A13" s="1" t="n">
@@ -4750,6 +4789,9 @@
       <c r="CX13" s="1" t="n">
         <v>145.6</v>
       </c>
+      <c r="CY13" s="1" t="n">
+        <v>295.5</v>
+      </c>
     </row>
     <row r="14" ht="20" customHeight="1">
       <c r="A14" s="1" t="n">
@@ -5058,6 +5100,9 @@
       <c r="CX14" s="1" t="n">
         <v>253.4</v>
       </c>
+      <c r="CY14" s="1" t="n">
+        <v>156.3</v>
+      </c>
     </row>
     <row r="15" ht="20" customHeight="1">
       <c r="A15" s="1" t="n">
@@ -5366,6 +5411,9 @@
       <c r="CX15" s="2" t="n">
         <v>121.4</v>
       </c>
+      <c r="CY15" s="1" t="n">
+        <v>165.2</v>
+      </c>
     </row>
     <row r="16" ht="20" customHeight="1">
       <c r="A16" s="1" t="n">
@@ -5674,6 +5722,9 @@
       <c r="CX16" s="1" t="n">
         <v>164.3</v>
       </c>
+      <c r="CY16" s="3" t="n">
+        <v>135.7</v>
+      </c>
     </row>
     <row r="17" ht="20" customHeight="1">
       <c r="A17" s="1" t="n">
@@ -5982,6 +6033,9 @@
       <c r="CX17" s="1" t="n">
         <v>149.9</v>
       </c>
+      <c r="CY17" s="1" t="n">
+        <v>242.2</v>
+      </c>
     </row>
     <row r="18" ht="20" customHeight="1">
       <c r="A18" s="1" t="n">
@@ -6290,6 +6344,9 @@
       <c r="CX18" s="1" t="n">
         <v>170.7</v>
       </c>
+      <c r="CY18" s="3" t="n">
+        <v>135.9</v>
+      </c>
     </row>
     <row r="19" ht="20" customHeight="1">
       <c r="A19" s="1" t="n">
@@ -6598,6 +6655,9 @@
       <c r="CX19" s="1" t="n">
         <v>190</v>
       </c>
+      <c r="CY19" s="1" t="n">
+        <v>141.6</v>
+      </c>
     </row>
     <row r="20" ht="20" customHeight="1">
       <c r="A20" s="1" t="n">
@@ -6906,6 +6966,9 @@
       <c r="CX20" s="3" t="n">
         <v>129.8</v>
       </c>
+      <c r="CY20" s="1" t="n">
+        <v>145.1</v>
+      </c>
     </row>
     <row r="21" ht="20" customHeight="1">
       <c r="A21" s="1" t="n">
@@ -7214,6 +7277,9 @@
       <c r="CX21" s="1" t="n">
         <v>202.4</v>
       </c>
+      <c r="CY21" s="3" t="n">
+        <v>138.5</v>
+      </c>
     </row>
     <row r="22" ht="20" customHeight="1">
       <c r="A22" s="1" t="n">
@@ -7522,6 +7588,9 @@
       <c r="CX22" s="1" t="n">
         <v>220.3</v>
       </c>
+      <c r="CY22" s="2" t="n">
+        <v>117.4</v>
+      </c>
     </row>
     <row r="23" ht="20" customHeight="1">
       <c r="A23" s="1" t="n">
@@ -7830,6 +7899,9 @@
       <c r="CX23" s="1" t="n">
         <v>142.6</v>
       </c>
+      <c r="CY23" s="1" t="n">
+        <v>155.2</v>
+      </c>
     </row>
     <row r="24" ht="20" customHeight="1">
       <c r="A24" s="1" t="n">
@@ -8138,6 +8210,9 @@
       <c r="CX24" s="1" t="n">
         <v>211.8</v>
       </c>
+      <c r="CY24" s="1" t="n">
+        <v>146.7</v>
+      </c>
     </row>
     <row r="25" ht="20" customHeight="1">
       <c r="A25" s="1" t="n">
@@ -8446,6 +8521,9 @@
       <c r="CX25" s="1" t="n">
         <v>163.1</v>
       </c>
+      <c r="CY25" s="1" t="n">
+        <v>147.4</v>
+      </c>
     </row>
     <row r="26" ht="20" customHeight="1">
       <c r="A26" s="1" t="n">
@@ -8754,6 +8832,9 @@
       <c r="CX26" s="1" t="n">
         <v>156.6</v>
       </c>
+      <c r="CY26" s="3" t="n">
+        <v>136.3</v>
+      </c>
     </row>
     <row r="27" ht="20" customHeight="1">
       <c r="A27" s="1" t="n">
@@ -9062,6 +9143,9 @@
       <c r="CX27" s="1" t="n">
         <v>177.3</v>
       </c>
+      <c r="CY27" s="1" t="n">
+        <v>168.8</v>
+      </c>
     </row>
     <row r="28" ht="20" customHeight="1">
       <c r="A28" s="1" t="n">
@@ -9370,6 +9454,9 @@
       <c r="CX28" s="1" t="n">
         <v>155.6</v>
       </c>
+      <c r="CY28" s="1" t="n">
+        <v>182.1</v>
+      </c>
     </row>
     <row r="29" ht="20" customHeight="1">
       <c r="A29" s="1" t="n">
@@ -9678,6 +9765,9 @@
       <c r="CX29" s="1" t="n">
         <v>359.3</v>
       </c>
+      <c r="CY29" s="1" t="n">
+        <v>205.9</v>
+      </c>
     </row>
     <row r="30" ht="20" customHeight="1">
       <c r="A30" s="1" t="n">
@@ -9986,6 +10076,9 @@
       <c r="CX30" s="1" t="n">
         <v>152.7</v>
       </c>
+      <c r="CY30" s="1" t="n">
+        <v>160.1</v>
+      </c>
     </row>
     <row r="31" ht="20" customHeight="1">
       <c r="A31" s="1" t="n">
@@ -10294,6 +10387,9 @@
       <c r="CX31" s="1" t="n">
         <v>170.8</v>
       </c>
+      <c r="CY31" s="1" t="n">
+        <v>143.2</v>
+      </c>
     </row>
     <row r="32" ht="20" customHeight="1">
       <c r="A32" s="1" t="n">
@@ -10602,6 +10698,9 @@
       <c r="CX32" s="2" t="n">
         <v>110.6</v>
       </c>
+      <c r="CY32" s="1" t="n">
+        <v>142.3</v>
+      </c>
     </row>
     <row r="33" ht="20" customHeight="1">
       <c r="A33" s="1" t="n">
@@ -10910,6 +11009,9 @@
       <c r="CX33" s="2" t="n">
         <v>120.8</v>
       </c>
+      <c r="CY33" s="3" t="n">
+        <v>136</v>
+      </c>
     </row>
     <row r="34" ht="20" customHeight="1">
       <c r="A34" s="1" t="n">
@@ -11218,6 +11320,9 @@
       <c r="CX34" s="1" t="n">
         <v>142.2</v>
       </c>
+      <c r="CY34" s="1" t="n">
+        <v>176</v>
+      </c>
     </row>
     <row r="35" ht="20" customHeight="1">
       <c r="A35" s="1" t="n">
@@ -11526,6 +11631,9 @@
       <c r="CX35" s="1" t="n">
         <v>158.9</v>
       </c>
+      <c r="CY35" s="3" t="n">
+        <v>125.5</v>
+      </c>
     </row>
     <row r="36" ht="20" customHeight="1">
       <c r="A36" s="1" t="n">
@@ -11834,6 +11942,9 @@
       <c r="CX36" s="1" t="n">
         <v>140.5</v>
       </c>
+      <c r="CY36" s="1" t="n">
+        <v>160.2</v>
+      </c>
     </row>
     <row r="37" ht="20" customHeight="1">
       <c r="A37" s="1" t="n">
@@ -12142,6 +12253,9 @@
       <c r="CX37" s="1" t="n">
         <v>172</v>
       </c>
+      <c r="CY37" s="1" t="n">
+        <v>173.3</v>
+      </c>
     </row>
     <row r="38" ht="20" customHeight="1">
       <c r="A38" s="1" t="n">
@@ -12450,6 +12564,9 @@
       <c r="CX38" s="3" t="n">
         <v>138.9</v>
       </c>
+      <c r="CY38" s="2" t="n">
+        <v>121.6</v>
+      </c>
     </row>
     <row r="39" ht="20" customHeight="1">
       <c r="A39" s="1" t="n">
@@ -12758,6 +12875,9 @@
       <c r="CX39" s="1" t="n">
         <v>207.2</v>
       </c>
+      <c r="CY39" s="3" t="n">
+        <v>134.3</v>
+      </c>
     </row>
     <row r="40" ht="20" customHeight="1">
       <c r="A40" s="1" t="n">
@@ -13066,6 +13186,9 @@
       <c r="CX40" s="1" t="n">
         <v>204.8</v>
       </c>
+      <c r="CY40" s="3" t="n">
+        <v>131</v>
+      </c>
     </row>
     <row r="41" ht="20" customHeight="1">
       <c r="A41" s="1" t="n">
@@ -13374,6 +13497,9 @@
       <c r="CX41" s="1" t="n">
         <v>169.6</v>
       </c>
+      <c r="CY41" s="1" t="n">
+        <v>179.1</v>
+      </c>
     </row>
     <row r="42" ht="20" customHeight="1">
       <c r="A42" s="1" t="n">
@@ -13682,6 +13808,9 @@
       <c r="CX42" s="1" t="n">
         <v>270.3</v>
       </c>
+      <c r="CY42" s="1" t="n">
+        <v>191.5</v>
+      </c>
     </row>
     <row r="43" ht="20" customHeight="1">
       <c r="A43" s="1" t="n">
@@ -13990,6 +14119,9 @@
       <c r="CX43" s="3" t="n">
         <v>136.8</v>
       </c>
+      <c r="CY43" s="3" t="n">
+        <v>129.5</v>
+      </c>
     </row>
     <row r="44" ht="20" customHeight="1">
       <c r="A44" s="1" t="n">
@@ -14298,6 +14430,9 @@
       <c r="CX44" s="1" t="n">
         <v>212.6</v>
       </c>
+      <c r="CY44" s="3" t="n">
+        <v>136.2</v>
+      </c>
     </row>
     <row r="45" ht="20" customHeight="1">
       <c r="A45" s="1" t="n">
@@ -14606,6 +14741,9 @@
       <c r="CX45" s="1" t="n">
         <v>237.5</v>
       </c>
+      <c r="CY45" s="1" t="n">
+        <v>160.6</v>
+      </c>
     </row>
     <row r="46" ht="20" customHeight="1">
       <c r="A46" s="1" t="n">
@@ -14914,6 +15052,9 @@
       <c r="CX46" s="1" t="n">
         <v>303.7</v>
       </c>
+      <c r="CY46" s="1" t="n">
+        <v>142.3</v>
+      </c>
     </row>
     <row r="47" ht="20" customHeight="1">
       <c r="A47" s="1" t="n">
@@ -15222,6 +15363,9 @@
       <c r="CX47" s="1" t="n">
         <v>142.3</v>
       </c>
+      <c r="CY47" s="3" t="n">
+        <v>133.1</v>
+      </c>
     </row>
     <row r="48" ht="20" customHeight="1">
       <c r="A48" s="1" t="n">
@@ -15530,6 +15674,9 @@
       <c r="CX48" s="1" t="n">
         <v>155.2</v>
       </c>
+      <c r="CY48" s="1" t="n">
+        <v>201.2</v>
+      </c>
     </row>
     <row r="49" ht="20" customHeight="1">
       <c r="A49" s="1" t="n">
@@ -15838,6 +15985,9 @@
       <c r="CX49" s="2" t="n">
         <v>110.2</v>
       </c>
+      <c r="CY49" s="1" t="n">
+        <v>146.8</v>
+      </c>
     </row>
     <row r="50" ht="20" customHeight="1">
       <c r="A50" s="1" t="n">
@@ -16146,6 +16296,9 @@
       <c r="CX50" s="1" t="n">
         <v>148.2</v>
       </c>
+      <c r="CY50" s="1" t="n">
+        <v>167.6</v>
+      </c>
     </row>
     <row r="51" ht="20" customHeight="1">
       <c r="A51" s="1" t="n">
@@ -16454,6 +16607,9 @@
       <c r="CX51" s="3" t="n">
         <v>127.2</v>
       </c>
+      <c r="CY51" s="1" t="n">
+        <v>173.5</v>
+      </c>
     </row>
     <row r="52" ht="20" customHeight="1">
       <c r="A52" s="1" t="n">
@@ -16762,6 +16918,9 @@
       <c r="CX52" s="1" t="n">
         <v>178.1</v>
       </c>
+      <c r="CY52" s="1" t="n">
+        <v>140.4</v>
+      </c>
     </row>
     <row r="53" ht="20" customHeight="1">
       <c r="A53" s="1" t="n">
@@ -17069,6 +17228,9 @@
       </c>
       <c r="CX53" s="1" t="n">
         <v>149.8</v>
+      </c>
+      <c r="CY53" s="1" t="n">
+        <v>177.3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2024-12-21
</commit_message>
<xml_diff>
--- a/マイジャグラーV_塗りつぶし済み.xlsx
+++ b/マイジャグラーV_塗りつぶし済み.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:CY53"/>
+  <dimension ref="A1:CZ53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -542,6 +542,7 @@
     <col width="12" customWidth="1" min="101" max="101"/>
     <col width="12" customWidth="1" min="102" max="102"/>
     <col width="12" customWidth="1" min="103" max="103"/>
+    <col width="12" customWidth="1" min="104" max="104"/>
   </cols>
   <sheetData>
     <row r="1" ht="20" customHeight="1">
@@ -1060,6 +1061,11 @@
           <t>2024/12/20</t>
         </is>
       </c>
+      <c r="CZ1" s="1" t="inlineStr">
+        <is>
+          <t>2024/12/21</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="20" customHeight="1">
       <c r="A2" s="1" t="n">
@@ -1371,6 +1377,9 @@
       <c r="CY2" s="1" t="n">
         <v>198.2</v>
       </c>
+      <c r="CZ2" s="1" t="n">
+        <v>142</v>
+      </c>
     </row>
     <row r="3" ht="20" customHeight="1">
       <c r="A3" s="1" t="n">
@@ -1682,6 +1691,9 @@
       <c r="CY3" s="3" t="n">
         <v>133.8</v>
       </c>
+      <c r="CZ3" s="1" t="n">
+        <v>166.3</v>
+      </c>
     </row>
     <row r="4" ht="20" customHeight="1">
       <c r="A4" s="1" t="n">
@@ -1993,6 +2005,9 @@
       <c r="CY4" s="1" t="n">
         <v>158.6</v>
       </c>
+      <c r="CZ4" s="1" t="n">
+        <v>240</v>
+      </c>
     </row>
     <row r="5" ht="20" customHeight="1">
       <c r="A5" s="1" t="n">
@@ -2304,6 +2319,9 @@
       <c r="CY5" s="1" t="n">
         <v>142.2</v>
       </c>
+      <c r="CZ5" s="2" t="n">
+        <v>121.8</v>
+      </c>
     </row>
     <row r="6" ht="20" customHeight="1">
       <c r="A6" s="1" t="n">
@@ -2615,6 +2633,9 @@
       <c r="CY6" s="1" t="n">
         <v>149</v>
       </c>
+      <c r="CZ6" s="1" t="n">
+        <v>142.8</v>
+      </c>
     </row>
     <row r="7" ht="20" customHeight="1">
       <c r="A7" s="1" t="n">
@@ -2926,6 +2947,9 @@
       <c r="CY7" s="1" t="n">
         <v>245.3</v>
       </c>
+      <c r="CZ7" s="1" t="n">
+        <v>161</v>
+      </c>
     </row>
     <row r="8" ht="20" customHeight="1">
       <c r="A8" s="1" t="n">
@@ -3237,6 +3261,9 @@
       <c r="CY8" s="1" t="n">
         <v>142.3</v>
       </c>
+      <c r="CZ8" s="3" t="n">
+        <v>127.7</v>
+      </c>
     </row>
     <row r="9" ht="20" customHeight="1">
       <c r="A9" s="1" t="n">
@@ -3548,6 +3575,9 @@
       <c r="CY9" s="1" t="n">
         <v>165.9</v>
       </c>
+      <c r="CZ9" s="3" t="n">
+        <v>125.4</v>
+      </c>
     </row>
     <row r="10" ht="20" customHeight="1">
       <c r="A10" s="1" t="n">
@@ -3859,6 +3889,9 @@
       <c r="CY10" s="1" t="n">
         <v>204</v>
       </c>
+      <c r="CZ10" s="1" t="n">
+        <v>150.8</v>
+      </c>
     </row>
     <row r="11" ht="20" customHeight="1">
       <c r="A11" s="1" t="n">
@@ -4170,6 +4203,9 @@
       <c r="CY11" s="1" t="n">
         <v>247</v>
       </c>
+      <c r="CZ11" s="1" t="n">
+        <v>184.3</v>
+      </c>
     </row>
     <row r="12" ht="20" customHeight="1">
       <c r="A12" s="1" t="n">
@@ -4481,6 +4517,9 @@
       <c r="CY12" s="3" t="n">
         <v>134.4</v>
       </c>
+      <c r="CZ12" s="1" t="n">
+        <v>164.2</v>
+      </c>
     </row>
     <row r="13" ht="20" customHeight="1">
       <c r="A13" s="1" t="n">
@@ -4792,6 +4831,9 @@
       <c r="CY13" s="1" t="n">
         <v>295.5</v>
       </c>
+      <c r="CZ13" s="3" t="n">
+        <v>137.7</v>
+      </c>
     </row>
     <row r="14" ht="20" customHeight="1">
       <c r="A14" s="1" t="n">
@@ -5103,6 +5145,9 @@
       <c r="CY14" s="1" t="n">
         <v>156.3</v>
       </c>
+      <c r="CZ14" s="1" t="n">
+        <v>171.4</v>
+      </c>
     </row>
     <row r="15" ht="20" customHeight="1">
       <c r="A15" s="1" t="n">
@@ -5414,6 +5459,9 @@
       <c r="CY15" s="1" t="n">
         <v>165.2</v>
       </c>
+      <c r="CZ15" s="1" t="n">
+        <v>180.8</v>
+      </c>
     </row>
     <row r="16" ht="20" customHeight="1">
       <c r="A16" s="1" t="n">
@@ -5725,6 +5773,9 @@
       <c r="CY16" s="3" t="n">
         <v>135.7</v>
       </c>
+      <c r="CZ16" s="1" t="n">
+        <v>268.6</v>
+      </c>
     </row>
     <row r="17" ht="20" customHeight="1">
       <c r="A17" s="1" t="n">
@@ -6036,6 +6087,9 @@
       <c r="CY17" s="1" t="n">
         <v>242.2</v>
       </c>
+      <c r="CZ17" s="1" t="n">
+        <v>161.3</v>
+      </c>
     </row>
     <row r="18" ht="20" customHeight="1">
       <c r="A18" s="1" t="n">
@@ -6347,6 +6401,9 @@
       <c r="CY18" s="3" t="n">
         <v>135.9</v>
       </c>
+      <c r="CZ18" s="2" t="n">
+        <v>120.5</v>
+      </c>
     </row>
     <row r="19" ht="20" customHeight="1">
       <c r="A19" s="1" t="n">
@@ -6658,6 +6715,9 @@
       <c r="CY19" s="1" t="n">
         <v>141.6</v>
       </c>
+      <c r="CZ19" s="3" t="n">
+        <v>139.9</v>
+      </c>
     </row>
     <row r="20" ht="20" customHeight="1">
       <c r="A20" s="1" t="n">
@@ -6969,6 +7029,9 @@
       <c r="CY20" s="1" t="n">
         <v>145.1</v>
       </c>
+      <c r="CZ20" s="1" t="n">
+        <v>171.4</v>
+      </c>
     </row>
     <row r="21" ht="20" customHeight="1">
       <c r="A21" s="1" t="n">
@@ -7280,6 +7343,9 @@
       <c r="CY21" s="3" t="n">
         <v>138.5</v>
       </c>
+      <c r="CZ21" s="1" t="n">
+        <v>196.7</v>
+      </c>
     </row>
     <row r="22" ht="20" customHeight="1">
       <c r="A22" s="1" t="n">
@@ -7591,6 +7657,9 @@
       <c r="CY22" s="2" t="n">
         <v>117.4</v>
       </c>
+      <c r="CZ22" s="1" t="n">
+        <v>204</v>
+      </c>
     </row>
     <row r="23" ht="20" customHeight="1">
       <c r="A23" s="1" t="n">
@@ -7902,6 +7971,9 @@
       <c r="CY23" s="1" t="n">
         <v>155.2</v>
       </c>
+      <c r="CZ23" s="3" t="n">
+        <v>139.2</v>
+      </c>
     </row>
     <row r="24" ht="20" customHeight="1">
       <c r="A24" s="1" t="n">
@@ -8213,6 +8285,9 @@
       <c r="CY24" s="1" t="n">
         <v>146.7</v>
       </c>
+      <c r="CZ24" s="1" t="n">
+        <v>164.9</v>
+      </c>
     </row>
     <row r="25" ht="20" customHeight="1">
       <c r="A25" s="1" t="n">
@@ -8524,6 +8599,9 @@
       <c r="CY25" s="1" t="n">
         <v>147.4</v>
       </c>
+      <c r="CZ25" s="1" t="n">
+        <v>174.3</v>
+      </c>
     </row>
     <row r="26" ht="20" customHeight="1">
       <c r="A26" s="1" t="n">
@@ -8835,6 +8913,9 @@
       <c r="CY26" s="3" t="n">
         <v>136.3</v>
       </c>
+      <c r="CZ26" s="1" t="n">
+        <v>207.5</v>
+      </c>
     </row>
     <row r="27" ht="20" customHeight="1">
       <c r="A27" s="1" t="n">
@@ -9146,6 +9227,9 @@
       <c r="CY27" s="1" t="n">
         <v>168.8</v>
       </c>
+      <c r="CZ27" s="1" t="n">
+        <v>150</v>
+      </c>
     </row>
     <row r="28" ht="20" customHeight="1">
       <c r="A28" s="1" t="n">
@@ -9457,6 +9541,9 @@
       <c r="CY28" s="1" t="n">
         <v>182.1</v>
       </c>
+      <c r="CZ28" s="1" t="n">
+        <v>172.7</v>
+      </c>
     </row>
     <row r="29" ht="20" customHeight="1">
       <c r="A29" s="1" t="n">
@@ -9768,6 +9855,9 @@
       <c r="CY29" s="1" t="n">
         <v>205.9</v>
       </c>
+      <c r="CZ29" s="1" t="n">
+        <v>178.9</v>
+      </c>
     </row>
     <row r="30" ht="20" customHeight="1">
       <c r="A30" s="1" t="n">
@@ -10079,6 +10169,9 @@
       <c r="CY30" s="1" t="n">
         <v>160.1</v>
       </c>
+      <c r="CZ30" s="3" t="n">
+        <v>126.4</v>
+      </c>
     </row>
     <row r="31" ht="20" customHeight="1">
       <c r="A31" s="1" t="n">
@@ -10390,6 +10483,9 @@
       <c r="CY31" s="1" t="n">
         <v>143.2</v>
       </c>
+      <c r="CZ31" s="3" t="n">
+        <v>136.3</v>
+      </c>
     </row>
     <row r="32" ht="20" customHeight="1">
       <c r="A32" s="1" t="n">
@@ -10701,6 +10797,9 @@
       <c r="CY32" s="1" t="n">
         <v>142.3</v>
       </c>
+      <c r="CZ32" s="1" t="n">
+        <v>163.6</v>
+      </c>
     </row>
     <row r="33" ht="20" customHeight="1">
       <c r="A33" s="1" t="n">
@@ -11012,6 +11111,9 @@
       <c r="CY33" s="3" t="n">
         <v>136</v>
       </c>
+      <c r="CZ33" s="1" t="n">
+        <v>143.9</v>
+      </c>
     </row>
     <row r="34" ht="20" customHeight="1">
       <c r="A34" s="1" t="n">
@@ -11323,6 +11425,9 @@
       <c r="CY34" s="1" t="n">
         <v>176</v>
       </c>
+      <c r="CZ34" s="2" t="n">
+        <v>117.7</v>
+      </c>
     </row>
     <row r="35" ht="20" customHeight="1">
       <c r="A35" s="1" t="n">
@@ -11634,6 +11739,9 @@
       <c r="CY35" s="3" t="n">
         <v>125.5</v>
       </c>
+      <c r="CZ35" s="1" t="n">
+        <v>169.3</v>
+      </c>
     </row>
     <row r="36" ht="20" customHeight="1">
       <c r="A36" s="1" t="n">
@@ -11945,6 +12053,9 @@
       <c r="CY36" s="1" t="n">
         <v>160.2</v>
       </c>
+      <c r="CZ36" s="3" t="n">
+        <v>132.5</v>
+      </c>
     </row>
     <row r="37" ht="20" customHeight="1">
       <c r="A37" s="1" t="n">
@@ -12256,6 +12367,9 @@
       <c r="CY37" s="1" t="n">
         <v>173.3</v>
       </c>
+      <c r="CZ37" s="1" t="n">
+        <v>197</v>
+      </c>
     </row>
     <row r="38" ht="20" customHeight="1">
       <c r="A38" s="1" t="n">
@@ -12567,6 +12681,9 @@
       <c r="CY38" s="2" t="n">
         <v>121.6</v>
       </c>
+      <c r="CZ38" s="1" t="n">
+        <v>218.3</v>
+      </c>
     </row>
     <row r="39" ht="20" customHeight="1">
       <c r="A39" s="1" t="n">
@@ -12878,6 +12995,9 @@
       <c r="CY39" s="3" t="n">
         <v>134.3</v>
       </c>
+      <c r="CZ39" s="1" t="n">
+        <v>296.3</v>
+      </c>
     </row>
     <row r="40" ht="20" customHeight="1">
       <c r="A40" s="1" t="n">
@@ -13189,6 +13309,9 @@
       <c r="CY40" s="3" t="n">
         <v>131</v>
       </c>
+      <c r="CZ40" s="2" t="n">
+        <v>122.7</v>
+      </c>
     </row>
     <row r="41" ht="20" customHeight="1">
       <c r="A41" s="1" t="n">
@@ -13500,6 +13623,9 @@
       <c r="CY41" s="1" t="n">
         <v>179.1</v>
       </c>
+      <c r="CZ41" s="1" t="n">
+        <v>157</v>
+      </c>
     </row>
     <row r="42" ht="20" customHeight="1">
       <c r="A42" s="1" t="n">
@@ -13811,6 +13937,9 @@
       <c r="CY42" s="1" t="n">
         <v>191.5</v>
       </c>
+      <c r="CZ42" s="1" t="n">
+        <v>175.5</v>
+      </c>
     </row>
     <row r="43" ht="20" customHeight="1">
       <c r="A43" s="1" t="n">
@@ -14122,6 +14251,9 @@
       <c r="CY43" s="3" t="n">
         <v>129.5</v>
       </c>
+      <c r="CZ43" s="1" t="n">
+        <v>187.1</v>
+      </c>
     </row>
     <row r="44" ht="20" customHeight="1">
       <c r="A44" s="1" t="n">
@@ -14433,6 +14565,9 @@
       <c r="CY44" s="3" t="n">
         <v>136.2</v>
       </c>
+      <c r="CZ44" s="1" t="n">
+        <v>150.5</v>
+      </c>
     </row>
     <row r="45" ht="20" customHeight="1">
       <c r="A45" s="1" t="n">
@@ -14744,6 +14879,9 @@
       <c r="CY45" s="1" t="n">
         <v>160.6</v>
       </c>
+      <c r="CZ45" s="1" t="n">
+        <v>228.9</v>
+      </c>
     </row>
     <row r="46" ht="20" customHeight="1">
       <c r="A46" s="1" t="n">
@@ -15055,6 +15193,9 @@
       <c r="CY46" s="1" t="n">
         <v>142.3</v>
       </c>
+      <c r="CZ46" s="1" t="n">
+        <v>153.1</v>
+      </c>
     </row>
     <row r="47" ht="20" customHeight="1">
       <c r="A47" s="1" t="n">
@@ -15366,6 +15507,9 @@
       <c r="CY47" s="3" t="n">
         <v>133.1</v>
       </c>
+      <c r="CZ47" s="1" t="n">
+        <v>165.7</v>
+      </c>
     </row>
     <row r="48" ht="20" customHeight="1">
       <c r="A48" s="1" t="n">
@@ -15677,6 +15821,9 @@
       <c r="CY48" s="1" t="n">
         <v>201.2</v>
       </c>
+      <c r="CZ48" s="1" t="n">
+        <v>155.4</v>
+      </c>
     </row>
     <row r="49" ht="20" customHeight="1">
       <c r="A49" s="1" t="n">
@@ -15988,6 +16135,9 @@
       <c r="CY49" s="1" t="n">
         <v>146.8</v>
       </c>
+      <c r="CZ49" s="1" t="n">
+        <v>149.2</v>
+      </c>
     </row>
     <row r="50" ht="20" customHeight="1">
       <c r="A50" s="1" t="n">
@@ -16299,6 +16449,9 @@
       <c r="CY50" s="1" t="n">
         <v>167.6</v>
       </c>
+      <c r="CZ50" s="3" t="n">
+        <v>127.1</v>
+      </c>
     </row>
     <row r="51" ht="20" customHeight="1">
       <c r="A51" s="1" t="n">
@@ -16610,6 +16763,9 @@
       <c r="CY51" s="1" t="n">
         <v>173.5</v>
       </c>
+      <c r="CZ51" s="3" t="n">
+        <v>127.9</v>
+      </c>
     </row>
     <row r="52" ht="20" customHeight="1">
       <c r="A52" s="1" t="n">
@@ -16921,6 +17077,9 @@
       <c r="CY52" s="1" t="n">
         <v>140.4</v>
       </c>
+      <c r="CZ52" s="1" t="n">
+        <v>189.6</v>
+      </c>
     </row>
     <row r="53" ht="20" customHeight="1">
       <c r="A53" s="1" t="n">
@@ -17231,6 +17390,9 @@
       </c>
       <c r="CY53" s="1" t="n">
         <v>177.3</v>
+      </c>
+      <c r="CZ53" s="3" t="n">
+        <v>129.9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2024-12-22
</commit_message>
<xml_diff>
--- a/マイジャグラーV_塗りつぶし済み.xlsx
+++ b/マイジャグラーV_塗りつぶし済み.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:CZ53"/>
+  <dimension ref="A1:DA53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -543,6 +543,7 @@
     <col width="12" customWidth="1" min="102" max="102"/>
     <col width="12" customWidth="1" min="103" max="103"/>
     <col width="12" customWidth="1" min="104" max="104"/>
+    <col width="12" customWidth="1" min="105" max="105"/>
   </cols>
   <sheetData>
     <row r="1" ht="20" customHeight="1">
@@ -1066,6 +1067,11 @@
           <t>2024/12/21</t>
         </is>
       </c>
+      <c r="DA1" s="1" t="inlineStr">
+        <is>
+          <t>2024/12/22</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="20" customHeight="1">
       <c r="A2" s="1" t="n">
@@ -1380,6 +1386,9 @@
       <c r="CZ2" s="1" t="n">
         <v>142</v>
       </c>
+      <c r="DA2" s="1" t="n">
+        <v>203.3</v>
+      </c>
     </row>
     <row r="3" ht="20" customHeight="1">
       <c r="A3" s="1" t="n">
@@ -1694,6 +1703,9 @@
       <c r="CZ3" s="1" t="n">
         <v>166.3</v>
       </c>
+      <c r="DA3" s="1" t="n">
+        <v>176.5</v>
+      </c>
     </row>
     <row r="4" ht="20" customHeight="1">
       <c r="A4" s="1" t="n">
@@ -2008,6 +2020,9 @@
       <c r="CZ4" s="1" t="n">
         <v>240</v>
       </c>
+      <c r="DA4" s="1" t="n">
+        <v>229.2</v>
+      </c>
     </row>
     <row r="5" ht="20" customHeight="1">
       <c r="A5" s="1" t="n">
@@ -2322,6 +2337,9 @@
       <c r="CZ5" s="2" t="n">
         <v>121.8</v>
       </c>
+      <c r="DA5" s="1" t="n">
+        <v>142.7</v>
+      </c>
     </row>
     <row r="6" ht="20" customHeight="1">
       <c r="A6" s="1" t="n">
@@ -2636,6 +2654,9 @@
       <c r="CZ6" s="1" t="n">
         <v>142.8</v>
       </c>
+      <c r="DA6" s="3" t="n">
+        <v>130.9</v>
+      </c>
     </row>
     <row r="7" ht="20" customHeight="1">
       <c r="A7" s="1" t="n">
@@ -2950,6 +2971,9 @@
       <c r="CZ7" s="1" t="n">
         <v>161</v>
       </c>
+      <c r="DA7" s="3" t="n">
+        <v>135.7</v>
+      </c>
     </row>
     <row r="8" ht="20" customHeight="1">
       <c r="A8" s="1" t="n">
@@ -3264,6 +3288,9 @@
       <c r="CZ8" s="3" t="n">
         <v>127.7</v>
       </c>
+      <c r="DA8" s="1" t="n">
+        <v>157.4</v>
+      </c>
     </row>
     <row r="9" ht="20" customHeight="1">
       <c r="A9" s="1" t="n">
@@ -3578,6 +3605,9 @@
       <c r="CZ9" s="3" t="n">
         <v>125.4</v>
       </c>
+      <c r="DA9" s="1" t="n">
+        <v>142.1</v>
+      </c>
     </row>
     <row r="10" ht="20" customHeight="1">
       <c r="A10" s="1" t="n">
@@ -3892,6 +3922,9 @@
       <c r="CZ10" s="1" t="n">
         <v>150.8</v>
       </c>
+      <c r="DA10" s="2" t="n">
+        <v>109.5</v>
+      </c>
     </row>
     <row r="11" ht="20" customHeight="1">
       <c r="A11" s="1" t="n">
@@ -4206,6 +4239,9 @@
       <c r="CZ11" s="1" t="n">
         <v>184.3</v>
       </c>
+      <c r="DA11" s="1" t="n">
+        <v>167.4</v>
+      </c>
     </row>
     <row r="12" ht="20" customHeight="1">
       <c r="A12" s="1" t="n">
@@ -4520,6 +4556,9 @@
       <c r="CZ12" s="1" t="n">
         <v>164.2</v>
       </c>
+      <c r="DA12" s="1" t="n">
+        <v>148.2</v>
+      </c>
     </row>
     <row r="13" ht="20" customHeight="1">
       <c r="A13" s="1" t="n">
@@ -4834,6 +4873,9 @@
       <c r="CZ13" s="3" t="n">
         <v>137.7</v>
       </c>
+      <c r="DA13" s="1" t="n">
+        <v>167</v>
+      </c>
     </row>
     <row r="14" ht="20" customHeight="1">
       <c r="A14" s="1" t="n">
@@ -5148,6 +5190,9 @@
       <c r="CZ14" s="1" t="n">
         <v>171.4</v>
       </c>
+      <c r="DA14" s="3" t="n">
+        <v>134.9</v>
+      </c>
     </row>
     <row r="15" ht="20" customHeight="1">
       <c r="A15" s="1" t="n">
@@ -5462,6 +5507,9 @@
       <c r="CZ15" s="1" t="n">
         <v>180.8</v>
       </c>
+      <c r="DA15" s="1" t="n">
+        <v>169.6</v>
+      </c>
     </row>
     <row r="16" ht="20" customHeight="1">
       <c r="A16" s="1" t="n">
@@ -5776,6 +5824,9 @@
       <c r="CZ16" s="1" t="n">
         <v>268.6</v>
       </c>
+      <c r="DA16" s="3" t="n">
+        <v>127</v>
+      </c>
     </row>
     <row r="17" ht="20" customHeight="1">
       <c r="A17" s="1" t="n">
@@ -6090,6 +6141,9 @@
       <c r="CZ17" s="1" t="n">
         <v>161.3</v>
       </c>
+      <c r="DA17" s="1" t="n">
+        <v>143.8</v>
+      </c>
     </row>
     <row r="18" ht="20" customHeight="1">
       <c r="A18" s="1" t="n">
@@ -6404,6 +6458,9 @@
       <c r="CZ18" s="2" t="n">
         <v>120.5</v>
       </c>
+      <c r="DA18" s="1" t="n">
+        <v>236.9</v>
+      </c>
     </row>
     <row r="19" ht="20" customHeight="1">
       <c r="A19" s="1" t="n">
@@ -6718,6 +6775,9 @@
       <c r="CZ19" s="3" t="n">
         <v>139.9</v>
       </c>
+      <c r="DA19" s="1" t="n">
+        <v>167.1</v>
+      </c>
     </row>
     <row r="20" ht="20" customHeight="1">
       <c r="A20" s="1" t="n">
@@ -7032,6 +7092,9 @@
       <c r="CZ20" s="1" t="n">
         <v>171.4</v>
       </c>
+      <c r="DA20" s="1" t="n">
+        <v>250.7</v>
+      </c>
     </row>
     <row r="21" ht="20" customHeight="1">
       <c r="A21" s="1" t="n">
@@ -7346,6 +7409,9 @@
       <c r="CZ21" s="1" t="n">
         <v>196.7</v>
       </c>
+      <c r="DA21" s="2" t="n">
+        <v>123.3</v>
+      </c>
     </row>
     <row r="22" ht="20" customHeight="1">
       <c r="A22" s="1" t="n">
@@ -7660,6 +7726,9 @@
       <c r="CZ22" s="1" t="n">
         <v>204</v>
       </c>
+      <c r="DA22" s="1" t="n">
+        <v>153.5</v>
+      </c>
     </row>
     <row r="23" ht="20" customHeight="1">
       <c r="A23" s="1" t="n">
@@ -7974,6 +8043,9 @@
       <c r="CZ23" s="3" t="n">
         <v>139.2</v>
       </c>
+      <c r="DA23" s="2" t="n">
+        <v>123.7</v>
+      </c>
     </row>
     <row r="24" ht="20" customHeight="1">
       <c r="A24" s="1" t="n">
@@ -8288,6 +8360,9 @@
       <c r="CZ24" s="1" t="n">
         <v>164.9</v>
       </c>
+      <c r="DA24" s="1" t="n">
+        <v>296.9</v>
+      </c>
     </row>
     <row r="25" ht="20" customHeight="1">
       <c r="A25" s="1" t="n">
@@ -8602,6 +8677,9 @@
       <c r="CZ25" s="1" t="n">
         <v>174.3</v>
       </c>
+      <c r="DA25" s="1" t="n">
+        <v>174.9</v>
+      </c>
     </row>
     <row r="26" ht="20" customHeight="1">
       <c r="A26" s="1" t="n">
@@ -8916,6 +8994,9 @@
       <c r="CZ26" s="1" t="n">
         <v>207.5</v>
       </c>
+      <c r="DA26" s="3" t="n">
+        <v>135.2</v>
+      </c>
     </row>
     <row r="27" ht="20" customHeight="1">
       <c r="A27" s="1" t="n">
@@ -9230,6 +9311,9 @@
       <c r="CZ27" s="1" t="n">
         <v>150</v>
       </c>
+      <c r="DA27" s="1" t="n">
+        <v>168.6</v>
+      </c>
     </row>
     <row r="28" ht="20" customHeight="1">
       <c r="A28" s="1" t="n">
@@ -9544,6 +9628,9 @@
       <c r="CZ28" s="1" t="n">
         <v>172.7</v>
       </c>
+      <c r="DA28" s="1" t="n">
+        <v>174.3</v>
+      </c>
     </row>
     <row r="29" ht="20" customHeight="1">
       <c r="A29" s="1" t="n">
@@ -9858,6 +9945,9 @@
       <c r="CZ29" s="1" t="n">
         <v>178.9</v>
       </c>
+      <c r="DA29" s="3" t="n">
+        <v>134.1</v>
+      </c>
     </row>
     <row r="30" ht="20" customHeight="1">
       <c r="A30" s="1" t="n">
@@ -10172,6 +10262,9 @@
       <c r="CZ30" s="3" t="n">
         <v>126.4</v>
       </c>
+      <c r="DA30" s="3" t="n">
+        <v>139.8</v>
+      </c>
     </row>
     <row r="31" ht="20" customHeight="1">
       <c r="A31" s="1" t="n">
@@ -10486,6 +10579,9 @@
       <c r="CZ31" s="3" t="n">
         <v>136.3</v>
       </c>
+      <c r="DA31" s="1" t="n">
+        <v>171</v>
+      </c>
     </row>
     <row r="32" ht="20" customHeight="1">
       <c r="A32" s="1" t="n">
@@ -10800,6 +10896,9 @@
       <c r="CZ32" s="1" t="n">
         <v>163.6</v>
       </c>
+      <c r="DA32" s="1" t="n">
+        <v>210.2</v>
+      </c>
     </row>
     <row r="33" ht="20" customHeight="1">
       <c r="A33" s="1" t="n">
@@ -11114,6 +11213,9 @@
       <c r="CZ33" s="1" t="n">
         <v>143.9</v>
       </c>
+      <c r="DA33" s="3" t="n">
+        <v>134.9</v>
+      </c>
     </row>
     <row r="34" ht="20" customHeight="1">
       <c r="A34" s="1" t="n">
@@ -11428,6 +11530,9 @@
       <c r="CZ34" s="2" t="n">
         <v>117.7</v>
       </c>
+      <c r="DA34" s="1" t="n">
+        <v>156.8</v>
+      </c>
     </row>
     <row r="35" ht="20" customHeight="1">
       <c r="A35" s="1" t="n">
@@ -11742,6 +11847,9 @@
       <c r="CZ35" s="1" t="n">
         <v>169.3</v>
       </c>
+      <c r="DA35" s="2" t="n">
+        <v>121.4</v>
+      </c>
     </row>
     <row r="36" ht="20" customHeight="1">
       <c r="A36" s="1" t="n">
@@ -12056,6 +12164,9 @@
       <c r="CZ36" s="3" t="n">
         <v>132.5</v>
       </c>
+      <c r="DA36" s="1" t="n">
+        <v>241.3</v>
+      </c>
     </row>
     <row r="37" ht="20" customHeight="1">
       <c r="A37" s="1" t="n">
@@ -12370,6 +12481,9 @@
       <c r="CZ37" s="1" t="n">
         <v>197</v>
       </c>
+      <c r="DA37" s="3" t="n">
+        <v>125.2</v>
+      </c>
     </row>
     <row r="38" ht="20" customHeight="1">
       <c r="A38" s="1" t="n">
@@ -12684,6 +12798,9 @@
       <c r="CZ38" s="1" t="n">
         <v>218.3</v>
       </c>
+      <c r="DA38" s="1" t="n">
+        <v>181.3</v>
+      </c>
     </row>
     <row r="39" ht="20" customHeight="1">
       <c r="A39" s="1" t="n">
@@ -12998,6 +13115,9 @@
       <c r="CZ39" s="1" t="n">
         <v>296.3</v>
       </c>
+      <c r="DA39" s="1" t="n">
+        <v>209.8</v>
+      </c>
     </row>
     <row r="40" ht="20" customHeight="1">
       <c r="A40" s="1" t="n">
@@ -13312,6 +13432,9 @@
       <c r="CZ40" s="2" t="n">
         <v>122.7</v>
       </c>
+      <c r="DA40" s="1" t="n">
+        <v>179.9</v>
+      </c>
     </row>
     <row r="41" ht="20" customHeight="1">
       <c r="A41" s="1" t="n">
@@ -13626,6 +13749,9 @@
       <c r="CZ41" s="1" t="n">
         <v>157</v>
       </c>
+      <c r="DA41" s="3" t="n">
+        <v>136.1</v>
+      </c>
     </row>
     <row r="42" ht="20" customHeight="1">
       <c r="A42" s="1" t="n">
@@ -13940,6 +14066,9 @@
       <c r="CZ42" s="1" t="n">
         <v>175.5</v>
       </c>
+      <c r="DA42" s="1" t="n">
+        <v>155.4</v>
+      </c>
     </row>
     <row r="43" ht="20" customHeight="1">
       <c r="A43" s="1" t="n">
@@ -14254,6 +14383,9 @@
       <c r="CZ43" s="1" t="n">
         <v>187.1</v>
       </c>
+      <c r="DA43" s="1" t="n">
+        <v>157.5</v>
+      </c>
     </row>
     <row r="44" ht="20" customHeight="1">
       <c r="A44" s="1" t="n">
@@ -14568,6 +14700,9 @@
       <c r="CZ44" s="1" t="n">
         <v>150.5</v>
       </c>
+      <c r="DA44" s="1" t="n">
+        <v>202.8</v>
+      </c>
     </row>
     <row r="45" ht="20" customHeight="1">
       <c r="A45" s="1" t="n">
@@ -14882,6 +15017,9 @@
       <c r="CZ45" s="1" t="n">
         <v>228.9</v>
       </c>
+      <c r="DA45" s="1" t="n">
+        <v>319.9</v>
+      </c>
     </row>
     <row r="46" ht="20" customHeight="1">
       <c r="A46" s="1" t="n">
@@ -15196,6 +15334,9 @@
       <c r="CZ46" s="1" t="n">
         <v>153.1</v>
       </c>
+      <c r="DA46" s="1" t="n">
+        <v>190.8</v>
+      </c>
     </row>
     <row r="47" ht="20" customHeight="1">
       <c r="A47" s="1" t="n">
@@ -15510,6 +15651,9 @@
       <c r="CZ47" s="1" t="n">
         <v>165.7</v>
       </c>
+      <c r="DA47" s="1" t="n">
+        <v>179.4</v>
+      </c>
     </row>
     <row r="48" ht="20" customHeight="1">
       <c r="A48" s="1" t="n">
@@ -15824,6 +15968,9 @@
       <c r="CZ48" s="1" t="n">
         <v>155.4</v>
       </c>
+      <c r="DA48" s="1" t="n">
+        <v>176.7</v>
+      </c>
     </row>
     <row r="49" ht="20" customHeight="1">
       <c r="A49" s="1" t="n">
@@ -16138,6 +16285,9 @@
       <c r="CZ49" s="1" t="n">
         <v>149.2</v>
       </c>
+      <c r="DA49" s="3" t="n">
+        <v>132.3</v>
+      </c>
     </row>
     <row r="50" ht="20" customHeight="1">
       <c r="A50" s="1" t="n">
@@ -16452,6 +16602,9 @@
       <c r="CZ50" s="3" t="n">
         <v>127.1</v>
       </c>
+      <c r="DA50" s="1" t="n">
+        <v>159.9</v>
+      </c>
     </row>
     <row r="51" ht="20" customHeight="1">
       <c r="A51" s="1" t="n">
@@ -16766,6 +16919,9 @@
       <c r="CZ51" s="3" t="n">
         <v>127.9</v>
       </c>
+      <c r="DA51" s="1" t="n">
+        <v>162.1</v>
+      </c>
     </row>
     <row r="52" ht="20" customHeight="1">
       <c r="A52" s="1" t="n">
@@ -17080,6 +17236,9 @@
       <c r="CZ52" s="1" t="n">
         <v>189.6</v>
       </c>
+      <c r="DA52" s="1" t="n">
+        <v>149.6</v>
+      </c>
     </row>
     <row r="53" ht="20" customHeight="1">
       <c r="A53" s="1" t="n">
@@ -17393,6 +17552,9 @@
       </c>
       <c r="CZ53" s="3" t="n">
         <v>129.9</v>
+      </c>
+      <c r="DA53" s="2" t="n">
+        <v>113.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2024-12-23
</commit_message>
<xml_diff>
--- a/マイジャグラーV_塗りつぶし済み.xlsx
+++ b/マイジャグラーV_塗りつぶし済み.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:DA53"/>
+  <dimension ref="A1:DB53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -544,6 +544,7 @@
     <col width="12" customWidth="1" min="103" max="103"/>
     <col width="12" customWidth="1" min="104" max="104"/>
     <col width="12" customWidth="1" min="105" max="105"/>
+    <col width="12" customWidth="1" min="106" max="106"/>
   </cols>
   <sheetData>
     <row r="1" ht="20" customHeight="1">
@@ -1072,6 +1073,11 @@
           <t>2024/12/22</t>
         </is>
       </c>
+      <c r="DB1" s="1" t="inlineStr">
+        <is>
+          <t>2024/12/23</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="20" customHeight="1">
       <c r="A2" s="1" t="n">
@@ -1389,6 +1395,9 @@
       <c r="DA2" s="1" t="n">
         <v>203.3</v>
       </c>
+      <c r="DB2" s="3" t="n">
+        <v>131</v>
+      </c>
     </row>
     <row r="3" ht="20" customHeight="1">
       <c r="A3" s="1" t="n">
@@ -1706,6 +1715,9 @@
       <c r="DA3" s="1" t="n">
         <v>176.5</v>
       </c>
+      <c r="DB3" s="1" t="n">
+        <v>260.9</v>
+      </c>
     </row>
     <row r="4" ht="20" customHeight="1">
       <c r="A4" s="1" t="n">
@@ -2023,6 +2035,9 @@
       <c r="DA4" s="1" t="n">
         <v>229.2</v>
       </c>
+      <c r="DB4" s="1" t="n">
+        <v>167.2</v>
+      </c>
     </row>
     <row r="5" ht="20" customHeight="1">
       <c r="A5" s="1" t="n">
@@ -2340,6 +2355,9 @@
       <c r="DA5" s="1" t="n">
         <v>142.7</v>
       </c>
+      <c r="DB5" s="1" t="n">
+        <v>169.2</v>
+      </c>
     </row>
     <row r="6" ht="20" customHeight="1">
       <c r="A6" s="1" t="n">
@@ -2657,6 +2675,9 @@
       <c r="DA6" s="3" t="n">
         <v>130.9</v>
       </c>
+      <c r="DB6" s="1" t="n">
+        <v>145.9</v>
+      </c>
     </row>
     <row r="7" ht="20" customHeight="1">
       <c r="A7" s="1" t="n">
@@ -2974,6 +2995,9 @@
       <c r="DA7" s="3" t="n">
         <v>135.7</v>
       </c>
+      <c r="DB7" s="1" t="n">
+        <v>147.5</v>
+      </c>
     </row>
     <row r="8" ht="20" customHeight="1">
       <c r="A8" s="1" t="n">
@@ -3291,6 +3315,9 @@
       <c r="DA8" s="1" t="n">
         <v>157.4</v>
       </c>
+      <c r="DB8" s="1" t="n">
+        <v>201.4</v>
+      </c>
     </row>
     <row r="9" ht="20" customHeight="1">
       <c r="A9" s="1" t="n">
@@ -3608,6 +3635,9 @@
       <c r="DA9" s="1" t="n">
         <v>142.1</v>
       </c>
+      <c r="DB9" s="2" t="n">
+        <v>107.2</v>
+      </c>
     </row>
     <row r="10" ht="20" customHeight="1">
       <c r="A10" s="1" t="n">
@@ -3925,6 +3955,9 @@
       <c r="DA10" s="2" t="n">
         <v>109.5</v>
       </c>
+      <c r="DB10" s="3" t="n">
+        <v>139.2</v>
+      </c>
     </row>
     <row r="11" ht="20" customHeight="1">
       <c r="A11" s="1" t="n">
@@ -4242,6 +4275,9 @@
       <c r="DA11" s="1" t="n">
         <v>167.4</v>
       </c>
+      <c r="DB11" s="1" t="n">
+        <v>261.8</v>
+      </c>
     </row>
     <row r="12" ht="20" customHeight="1">
       <c r="A12" s="1" t="n">
@@ -4559,6 +4595,9 @@
       <c r="DA12" s="1" t="n">
         <v>148.2</v>
       </c>
+      <c r="DB12" s="2" t="n">
+        <v>113.4</v>
+      </c>
     </row>
     <row r="13" ht="20" customHeight="1">
       <c r="A13" s="1" t="n">
@@ -4876,6 +4915,9 @@
       <c r="DA13" s="1" t="n">
         <v>167</v>
       </c>
+      <c r="DB13" s="1" t="n">
+        <v>148.1</v>
+      </c>
     </row>
     <row r="14" ht="20" customHeight="1">
       <c r="A14" s="1" t="n">
@@ -5193,6 +5235,9 @@
       <c r="DA14" s="3" t="n">
         <v>134.9</v>
       </c>
+      <c r="DB14" s="2" t="n">
+        <v>123.8</v>
+      </c>
     </row>
     <row r="15" ht="20" customHeight="1">
       <c r="A15" s="1" t="n">
@@ -5510,6 +5555,9 @@
       <c r="DA15" s="1" t="n">
         <v>169.6</v>
       </c>
+      <c r="DB15" s="1" t="n">
+        <v>155</v>
+      </c>
     </row>
     <row r="16" ht="20" customHeight="1">
       <c r="A16" s="1" t="n">
@@ -5827,6 +5875,9 @@
       <c r="DA16" s="3" t="n">
         <v>127</v>
       </c>
+      <c r="DB16" s="1" t="n">
+        <v>150.9</v>
+      </c>
     </row>
     <row r="17" ht="20" customHeight="1">
       <c r="A17" s="1" t="n">
@@ -6144,6 +6195,9 @@
       <c r="DA17" s="1" t="n">
         <v>143.8</v>
       </c>
+      <c r="DB17" s="2" t="n">
+        <v>123.1</v>
+      </c>
     </row>
     <row r="18" ht="20" customHeight="1">
       <c r="A18" s="1" t="n">
@@ -6461,6 +6515,9 @@
       <c r="DA18" s="1" t="n">
         <v>236.9</v>
       </c>
+      <c r="DB18" s="1" t="n">
+        <v>149.8</v>
+      </c>
     </row>
     <row r="19" ht="20" customHeight="1">
       <c r="A19" s="1" t="n">
@@ -6778,6 +6835,9 @@
       <c r="DA19" s="1" t="n">
         <v>167.1</v>
       </c>
+      <c r="DB19" s="1" t="n">
+        <v>260.3</v>
+      </c>
     </row>
     <row r="20" ht="20" customHeight="1">
       <c r="A20" s="1" t="n">
@@ -7095,6 +7155,9 @@
       <c r="DA20" s="1" t="n">
         <v>250.7</v>
       </c>
+      <c r="DB20" s="1" t="n">
+        <v>140.3</v>
+      </c>
     </row>
     <row r="21" ht="20" customHeight="1">
       <c r="A21" s="1" t="n">
@@ -7412,6 +7475,9 @@
       <c r="DA21" s="2" t="n">
         <v>123.3</v>
       </c>
+      <c r="DB21" s="1" t="n">
+        <v>153.4</v>
+      </c>
     </row>
     <row r="22" ht="20" customHeight="1">
       <c r="A22" s="1" t="n">
@@ -7729,6 +7795,9 @@
       <c r="DA22" s="1" t="n">
         <v>153.5</v>
       </c>
+      <c r="DB22" s="3" t="n">
+        <v>131.2</v>
+      </c>
     </row>
     <row r="23" ht="20" customHeight="1">
       <c r="A23" s="1" t="n">
@@ -8046,6 +8115,9 @@
       <c r="DA23" s="2" t="n">
         <v>123.7</v>
       </c>
+      <c r="DB23" s="3" t="n">
+        <v>137.5</v>
+      </c>
     </row>
     <row r="24" ht="20" customHeight="1">
       <c r="A24" s="1" t="n">
@@ -8363,6 +8435,9 @@
       <c r="DA24" s="1" t="n">
         <v>296.9</v>
       </c>
+      <c r="DB24" s="3" t="n">
+        <v>133.7</v>
+      </c>
     </row>
     <row r="25" ht="20" customHeight="1">
       <c r="A25" s="1" t="n">
@@ -8680,6 +8755,9 @@
       <c r="DA25" s="1" t="n">
         <v>174.9</v>
       </c>
+      <c r="DB25" s="1" t="n">
+        <v>155.8</v>
+      </c>
     </row>
     <row r="26" ht="20" customHeight="1">
       <c r="A26" s="1" t="n">
@@ -8997,6 +9075,9 @@
       <c r="DA26" s="3" t="n">
         <v>135.2</v>
       </c>
+      <c r="DB26" s="1" t="n">
+        <v>155.4</v>
+      </c>
     </row>
     <row r="27" ht="20" customHeight="1">
       <c r="A27" s="1" t="n">
@@ -9314,6 +9395,9 @@
       <c r="DA27" s="1" t="n">
         <v>168.6</v>
       </c>
+      <c r="DB27" s="1" t="n">
+        <v>251.1</v>
+      </c>
     </row>
     <row r="28" ht="20" customHeight="1">
       <c r="A28" s="1" t="n">
@@ -9631,6 +9715,9 @@
       <c r="DA28" s="1" t="n">
         <v>174.3</v>
       </c>
+      <c r="DB28" s="3" t="n">
+        <v>137.9</v>
+      </c>
     </row>
     <row r="29" ht="20" customHeight="1">
       <c r="A29" s="1" t="n">
@@ -9948,6 +10035,9 @@
       <c r="DA29" s="3" t="n">
         <v>134.1</v>
       </c>
+      <c r="DB29" s="3" t="n">
+        <v>128.1</v>
+      </c>
     </row>
     <row r="30" ht="20" customHeight="1">
       <c r="A30" s="1" t="n">
@@ -10265,6 +10355,9 @@
       <c r="DA30" s="3" t="n">
         <v>139.8</v>
       </c>
+      <c r="DB30" s="3" t="n">
+        <v>133.2</v>
+      </c>
     </row>
     <row r="31" ht="20" customHeight="1">
       <c r="A31" s="1" t="n">
@@ -10582,6 +10675,9 @@
       <c r="DA31" s="1" t="n">
         <v>171</v>
       </c>
+      <c r="DB31" s="1" t="n">
+        <v>196.7</v>
+      </c>
     </row>
     <row r="32" ht="20" customHeight="1">
       <c r="A32" s="1" t="n">
@@ -10899,6 +10995,9 @@
       <c r="DA32" s="1" t="n">
         <v>210.2</v>
       </c>
+      <c r="DB32" s="3" t="n">
+        <v>132.8</v>
+      </c>
     </row>
     <row r="33" ht="20" customHeight="1">
       <c r="A33" s="1" t="n">
@@ -11216,6 +11315,9 @@
       <c r="DA33" s="3" t="n">
         <v>134.9</v>
       </c>
+      <c r="DB33" s="1" t="n">
+        <v>155.8</v>
+      </c>
     </row>
     <row r="34" ht="20" customHeight="1">
       <c r="A34" s="1" t="n">
@@ -11533,6 +11635,9 @@
       <c r="DA34" s="1" t="n">
         <v>156.8</v>
       </c>
+      <c r="DB34" s="1" t="n">
+        <v>143.6</v>
+      </c>
     </row>
     <row r="35" ht="20" customHeight="1">
       <c r="A35" s="1" t="n">
@@ -11850,6 +11955,9 @@
       <c r="DA35" s="2" t="n">
         <v>121.4</v>
       </c>
+      <c r="DB35" s="1" t="n">
+        <v>151.1</v>
+      </c>
     </row>
     <row r="36" ht="20" customHeight="1">
       <c r="A36" s="1" t="n">
@@ -12167,6 +12275,9 @@
       <c r="DA36" s="1" t="n">
         <v>241.3</v>
       </c>
+      <c r="DB36" s="1" t="n">
+        <v>226.8</v>
+      </c>
     </row>
     <row r="37" ht="20" customHeight="1">
       <c r="A37" s="1" t="n">
@@ -12484,6 +12595,9 @@
       <c r="DA37" s="3" t="n">
         <v>125.2</v>
       </c>
+      <c r="DB37" s="1" t="n">
+        <v>152.1</v>
+      </c>
     </row>
     <row r="38" ht="20" customHeight="1">
       <c r="A38" s="1" t="n">
@@ -12801,6 +12915,9 @@
       <c r="DA38" s="1" t="n">
         <v>181.3</v>
       </c>
+      <c r="DB38" s="1" t="n">
+        <v>142.1</v>
+      </c>
     </row>
     <row r="39" ht="20" customHeight="1">
       <c r="A39" s="1" t="n">
@@ -13118,6 +13235,9 @@
       <c r="DA39" s="1" t="n">
         <v>209.8</v>
       </c>
+      <c r="DB39" s="2" t="n">
+        <v>108.7</v>
+      </c>
     </row>
     <row r="40" ht="20" customHeight="1">
       <c r="A40" s="1" t="n">
@@ -13435,6 +13555,9 @@
       <c r="DA40" s="1" t="n">
         <v>179.9</v>
       </c>
+      <c r="DB40" s="1" t="n">
+        <v>166.3</v>
+      </c>
     </row>
     <row r="41" ht="20" customHeight="1">
       <c r="A41" s="1" t="n">
@@ -13752,6 +13875,9 @@
       <c r="DA41" s="3" t="n">
         <v>136.1</v>
       </c>
+      <c r="DB41" s="1" t="n">
+        <v>169.9</v>
+      </c>
     </row>
     <row r="42" ht="20" customHeight="1">
       <c r="A42" s="1" t="n">
@@ -14069,6 +14195,7 @@
       <c r="DA42" s="1" t="n">
         <v>155.4</v>
       </c>
+      <c r="DB42" s="1" t="n"/>
     </row>
     <row r="43" ht="20" customHeight="1">
       <c r="A43" s="1" t="n">
@@ -14386,6 +14513,7 @@
       <c r="DA43" s="1" t="n">
         <v>157.5</v>
       </c>
+      <c r="DB43" s="1" t="n"/>
     </row>
     <row r="44" ht="20" customHeight="1">
       <c r="A44" s="1" t="n">
@@ -14703,6 +14831,9 @@
       <c r="DA44" s="1" t="n">
         <v>202.8</v>
       </c>
+      <c r="DB44" s="3" t="n">
+        <v>137.1</v>
+      </c>
     </row>
     <row r="45" ht="20" customHeight="1">
       <c r="A45" s="1" t="n">
@@ -15020,6 +15151,9 @@
       <c r="DA45" s="1" t="n">
         <v>319.9</v>
       </c>
+      <c r="DB45" s="1" t="n">
+        <v>206.8</v>
+      </c>
     </row>
     <row r="46" ht="20" customHeight="1">
       <c r="A46" s="1" t="n">
@@ -15337,6 +15471,9 @@
       <c r="DA46" s="1" t="n">
         <v>190.8</v>
       </c>
+      <c r="DB46" s="3" t="n">
+        <v>130.8</v>
+      </c>
     </row>
     <row r="47" ht="20" customHeight="1">
       <c r="A47" s="1" t="n">
@@ -15654,6 +15791,9 @@
       <c r="DA47" s="1" t="n">
         <v>179.4</v>
       </c>
+      <c r="DB47" s="3" t="n">
+        <v>131.9</v>
+      </c>
     </row>
     <row r="48" ht="20" customHeight="1">
       <c r="A48" s="1" t="n">
@@ -15971,6 +16111,9 @@
       <c r="DA48" s="1" t="n">
         <v>176.7</v>
       </c>
+      <c r="DB48" s="1" t="n">
+        <v>179.3</v>
+      </c>
     </row>
     <row r="49" ht="20" customHeight="1">
       <c r="A49" s="1" t="n">
@@ -16288,6 +16431,9 @@
       <c r="DA49" s="3" t="n">
         <v>132.3</v>
       </c>
+      <c r="DB49" s="1" t="n">
+        <v>175.8</v>
+      </c>
     </row>
     <row r="50" ht="20" customHeight="1">
       <c r="A50" s="1" t="n">
@@ -16605,6 +16751,9 @@
       <c r="DA50" s="1" t="n">
         <v>159.9</v>
       </c>
+      <c r="DB50" s="1" t="n">
+        <v>150.7</v>
+      </c>
     </row>
     <row r="51" ht="20" customHeight="1">
       <c r="A51" s="1" t="n">
@@ -16922,6 +17071,9 @@
       <c r="DA51" s="1" t="n">
         <v>162.1</v>
       </c>
+      <c r="DB51" s="1" t="n">
+        <v>155.4</v>
+      </c>
     </row>
     <row r="52" ht="20" customHeight="1">
       <c r="A52" s="1" t="n">
@@ -17239,6 +17391,9 @@
       <c r="DA52" s="1" t="n">
         <v>149.6</v>
       </c>
+      <c r="DB52" s="3" t="n">
+        <v>127</v>
+      </c>
     </row>
     <row r="53" ht="20" customHeight="1">
       <c r="A53" s="1" t="n">
@@ -17555,6 +17710,9 @@
       </c>
       <c r="DA53" s="2" t="n">
         <v>113.5</v>
+      </c>
+      <c r="DB53" s="1" t="n">
+        <v>148.3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2024-12-31
</commit_message>
<xml_diff>
--- a/マイジャグラーV_塗りつぶし済み.xlsx
+++ b/マイジャグラーV_塗りつぶし済み.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:DI53"/>
+  <dimension ref="A1:DJ53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -552,6 +552,7 @@
     <col width="12" customWidth="1" min="111" max="111"/>
     <col width="12" customWidth="1" min="112" max="112"/>
     <col width="12" customWidth="1" min="113" max="113"/>
+    <col width="12" customWidth="1" min="114" max="114"/>
   </cols>
   <sheetData>
     <row r="1" ht="20" customHeight="1">
@@ -1120,6 +1121,11 @@
           <t>2024/12/30</t>
         </is>
       </c>
+      <c r="DJ1" s="1" t="inlineStr">
+        <is>
+          <t>2024/12/31</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="20" customHeight="1">
       <c r="A2" s="1" t="n">
@@ -1461,6 +1467,9 @@
       <c r="DI2" s="1" t="n">
         <v>168.3</v>
       </c>
+      <c r="DJ2" s="3" t="n">
+        <v>137.9</v>
+      </c>
     </row>
     <row r="3" ht="20" customHeight="1">
       <c r="A3" s="1" t="n">
@@ -1802,6 +1811,9 @@
       <c r="DI3" s="1" t="n">
         <v>162.7</v>
       </c>
+      <c r="DJ3" s="1" t="n">
+        <v>161.4</v>
+      </c>
     </row>
     <row r="4" ht="20" customHeight="1">
       <c r="A4" s="1" t="n">
@@ -2143,6 +2155,9 @@
       <c r="DI4" s="1" t="n">
         <v>184.8</v>
       </c>
+      <c r="DJ4" s="1" t="n">
+        <v>158.9</v>
+      </c>
     </row>
     <row r="5" ht="20" customHeight="1">
       <c r="A5" s="1" t="n">
@@ -2484,6 +2499,9 @@
       <c r="DI5" s="3" t="n">
         <v>130.2</v>
       </c>
+      <c r="DJ5" s="1" t="n">
+        <v>190.8</v>
+      </c>
     </row>
     <row r="6" ht="20" customHeight="1">
       <c r="A6" s="1" t="n">
@@ -2825,6 +2843,9 @@
       <c r="DI6" s="1" t="n">
         <v>217.7</v>
       </c>
+      <c r="DJ6" s="1" t="n">
+        <v>197.3</v>
+      </c>
     </row>
     <row r="7" ht="20" customHeight="1">
       <c r="A7" s="1" t="n">
@@ -3166,6 +3187,9 @@
       <c r="DI7" s="1" t="n">
         <v>144.6</v>
       </c>
+      <c r="DJ7" s="2" t="n">
+        <v>113.9</v>
+      </c>
     </row>
     <row r="8" ht="20" customHeight="1">
       <c r="A8" s="1" t="n">
@@ -3507,6 +3531,9 @@
       <c r="DI8" s="1" t="n">
         <v>184.1</v>
       </c>
+      <c r="DJ8" s="1" t="n">
+        <v>148.9</v>
+      </c>
     </row>
     <row r="9" ht="20" customHeight="1">
       <c r="A9" s="1" t="n">
@@ -3848,6 +3875,9 @@
       <c r="DI9" s="1" t="n">
         <v>147.6</v>
       </c>
+      <c r="DJ9" s="1" t="n">
+        <v>140.1</v>
+      </c>
     </row>
     <row r="10" ht="20" customHeight="1">
       <c r="A10" s="1" t="n">
@@ -4189,6 +4219,9 @@
       <c r="DI10" s="1" t="n">
         <v>161.1</v>
       </c>
+      <c r="DJ10" s="1" t="n">
+        <v>254.5</v>
+      </c>
     </row>
     <row r="11" ht="20" customHeight="1">
       <c r="A11" s="1" t="n">
@@ -4530,6 +4563,9 @@
       <c r="DI11" s="1" t="n">
         <v>150.5</v>
       </c>
+      <c r="DJ11" s="3" t="n">
+        <v>136.3</v>
+      </c>
     </row>
     <row r="12" ht="20" customHeight="1">
       <c r="A12" s="1" t="n">
@@ -4871,6 +4907,9 @@
       <c r="DI12" s="1" t="n">
         <v>182.6</v>
       </c>
+      <c r="DJ12" s="1" t="n">
+        <v>182.1</v>
+      </c>
     </row>
     <row r="13" ht="20" customHeight="1">
       <c r="A13" s="1" t="n">
@@ -5212,6 +5251,9 @@
       <c r="DI13" s="1" t="n">
         <v>141.5</v>
       </c>
+      <c r="DJ13" s="3" t="n">
+        <v>129</v>
+      </c>
     </row>
     <row r="14" ht="20" customHeight="1">
       <c r="A14" s="1" t="n">
@@ -5553,6 +5595,9 @@
       <c r="DI14" s="1" t="n">
         <v>146.2</v>
       </c>
+      <c r="DJ14" s="1" t="n">
+        <v>254.2</v>
+      </c>
     </row>
     <row r="15" ht="20" customHeight="1">
       <c r="A15" s="1" t="n">
@@ -5894,6 +5939,9 @@
       <c r="DI15" s="1" t="n">
         <v>155.8</v>
       </c>
+      <c r="DJ15" s="1" t="n">
+        <v>162.1</v>
+      </c>
     </row>
     <row r="16" ht="20" customHeight="1">
       <c r="A16" s="1" t="n">
@@ -6235,6 +6283,9 @@
       <c r="DI16" s="1" t="n">
         <v>228.2</v>
       </c>
+      <c r="DJ16" s="3" t="n">
+        <v>133</v>
+      </c>
     </row>
     <row r="17" ht="20" customHeight="1">
       <c r="A17" s="1" t="n">
@@ -6576,6 +6627,9 @@
       <c r="DI17" s="1" t="n">
         <v>166.2</v>
       </c>
+      <c r="DJ17" s="1" t="n">
+        <v>144.6</v>
+      </c>
     </row>
     <row r="18" ht="20" customHeight="1">
       <c r="A18" s="1" t="n">
@@ -6917,6 +6971,9 @@
       <c r="DI18" s="1" t="n">
         <v>154.2</v>
       </c>
+      <c r="DJ18" s="1" t="n">
+        <v>144.3</v>
+      </c>
     </row>
     <row r="19" ht="20" customHeight="1">
       <c r="A19" s="1" t="n">
@@ -7258,6 +7315,9 @@
       <c r="DI19" s="1" t="n">
         <v>142.3</v>
       </c>
+      <c r="DJ19" s="1" t="n">
+        <v>146</v>
+      </c>
     </row>
     <row r="20" ht="20" customHeight="1">
       <c r="A20" s="1" t="n">
@@ -7599,6 +7659,9 @@
       <c r="DI20" s="1" t="n">
         <v>143.4</v>
       </c>
+      <c r="DJ20" s="1" t="n">
+        <v>199.6</v>
+      </c>
     </row>
     <row r="21" ht="20" customHeight="1">
       <c r="A21" s="1" t="n">
@@ -7940,6 +8003,9 @@
       <c r="DI21" s="1" t="n">
         <v>183.1</v>
       </c>
+      <c r="DJ21" s="1" t="n">
+        <v>175.2</v>
+      </c>
     </row>
     <row r="22" ht="20" customHeight="1">
       <c r="A22" s="1" t="n">
@@ -8281,6 +8347,9 @@
       <c r="DI22" s="1" t="n">
         <v>165.5</v>
       </c>
+      <c r="DJ22" s="1" t="n">
+        <v>166.6</v>
+      </c>
     </row>
     <row r="23" ht="20" customHeight="1">
       <c r="A23" s="1" t="n">
@@ -8622,6 +8691,9 @@
       <c r="DI23" s="2" t="n">
         <v>124.8</v>
       </c>
+      <c r="DJ23" s="1" t="n">
+        <v>155.3</v>
+      </c>
     </row>
     <row r="24" ht="20" customHeight="1">
       <c r="A24" s="1" t="n">
@@ -8963,6 +9035,9 @@
       <c r="DI24" s="3" t="n">
         <v>126</v>
       </c>
+      <c r="DJ24" s="1" t="n">
+        <v>171</v>
+      </c>
     </row>
     <row r="25" ht="20" customHeight="1">
       <c r="A25" s="1" t="n">
@@ -9304,6 +9379,9 @@
       <c r="DI25" s="2" t="n">
         <v>123</v>
       </c>
+      <c r="DJ25" s="3" t="n">
+        <v>135</v>
+      </c>
     </row>
     <row r="26" ht="20" customHeight="1">
       <c r="A26" s="1" t="n">
@@ -9645,6 +9723,9 @@
       <c r="DI26" s="1" t="n">
         <v>168.4</v>
       </c>
+      <c r="DJ26" s="3" t="n">
+        <v>133.2</v>
+      </c>
     </row>
     <row r="27" ht="20" customHeight="1">
       <c r="A27" s="1" t="n">
@@ -9986,6 +10067,9 @@
       <c r="DI27" s="1" t="n">
         <v>159.4</v>
       </c>
+      <c r="DJ27" s="3" t="n">
+        <v>129.2</v>
+      </c>
     </row>
     <row r="28" ht="20" customHeight="1">
       <c r="A28" s="1" t="n">
@@ -10327,6 +10411,9 @@
       <c r="DI28" s="1" t="n">
         <v>294.8</v>
       </c>
+      <c r="DJ28" s="1" t="n">
+        <v>170.5</v>
+      </c>
     </row>
     <row r="29" ht="20" customHeight="1">
       <c r="A29" s="1" t="n">
@@ -10668,6 +10755,9 @@
       <c r="DI29" s="2" t="n">
         <v>116.9</v>
       </c>
+      <c r="DJ29" s="3" t="n">
+        <v>131.8</v>
+      </c>
     </row>
     <row r="30" ht="20" customHeight="1">
       <c r="A30" s="1" t="n">
@@ -11009,6 +11099,9 @@
       <c r="DI30" s="1" t="n">
         <v>181.1</v>
       </c>
+      <c r="DJ30" s="3" t="n">
+        <v>129.8</v>
+      </c>
     </row>
     <row r="31" ht="20" customHeight="1">
       <c r="A31" s="1" t="n">
@@ -11350,6 +11443,9 @@
       <c r="DI31" s="1" t="n">
         <v>168.5</v>
       </c>
+      <c r="DJ31" s="1" t="n">
+        <v>161.8</v>
+      </c>
     </row>
     <row r="32" ht="20" customHeight="1">
       <c r="A32" s="1" t="n">
@@ -11691,6 +11787,9 @@
       <c r="DI32" s="2" t="n">
         <v>98.2</v>
       </c>
+      <c r="DJ32" s="1" t="n">
+        <v>156.5</v>
+      </c>
     </row>
     <row r="33" ht="20" customHeight="1">
       <c r="A33" s="1" t="n">
@@ -12032,6 +12131,9 @@
       <c r="DI33" s="1" t="n">
         <v>158</v>
       </c>
+      <c r="DJ33" s="1" t="n">
+        <v>153.9</v>
+      </c>
     </row>
     <row r="34" ht="20" customHeight="1">
       <c r="A34" s="1" t="n">
@@ -12373,6 +12475,9 @@
       <c r="DI34" s="1" t="n">
         <v>182.6</v>
       </c>
+      <c r="DJ34" s="3" t="n">
+        <v>132.5</v>
+      </c>
     </row>
     <row r="35" ht="20" customHeight="1">
       <c r="A35" s="1" t="n">
@@ -12714,6 +12819,9 @@
       <c r="DI35" s="3" t="n">
         <v>131.1</v>
       </c>
+      <c r="DJ35" s="2" t="n">
+        <v>111.1</v>
+      </c>
     </row>
     <row r="36" ht="20" customHeight="1">
       <c r="A36" s="1" t="n">
@@ -13055,6 +13163,9 @@
       <c r="DI36" s="1" t="n">
         <v>167.4</v>
       </c>
+      <c r="DJ36" s="1" t="n">
+        <v>188.1</v>
+      </c>
     </row>
     <row r="37" ht="20" customHeight="1">
       <c r="A37" s="1" t="n">
@@ -13396,6 +13507,9 @@
       <c r="DI37" s="1" t="n">
         <v>142.1</v>
       </c>
+      <c r="DJ37" s="1" t="n">
+        <v>160.6</v>
+      </c>
     </row>
     <row r="38" ht="20" customHeight="1">
       <c r="A38" s="1" t="n">
@@ -13737,6 +13851,9 @@
       <c r="DI38" s="1" t="n">
         <v>142.9</v>
       </c>
+      <c r="DJ38" s="1" t="n">
+        <v>160.2</v>
+      </c>
     </row>
     <row r="39" ht="20" customHeight="1">
       <c r="A39" s="1" t="n">
@@ -14078,6 +14195,9 @@
       <c r="DI39" s="1" t="n">
         <v>185.1</v>
       </c>
+      <c r="DJ39" s="1" t="n">
+        <v>195.1</v>
+      </c>
     </row>
     <row r="40" ht="20" customHeight="1">
       <c r="A40" s="1" t="n">
@@ -14419,6 +14539,9 @@
       <c r="DI40" s="3" t="n">
         <v>127.8</v>
       </c>
+      <c r="DJ40" s="1" t="n">
+        <v>159.7</v>
+      </c>
     </row>
     <row r="41" ht="20" customHeight="1">
       <c r="A41" s="1" t="n">
@@ -14759,6 +14882,9 @@
       </c>
       <c r="DI41" s="1" t="n">
         <v>179</v>
+      </c>
+      <c r="DJ41" s="1" t="n">
+        <v>164.9</v>
       </c>
     </row>
     <row r="42" ht="20" customHeight="1">
@@ -15085,6 +15211,7 @@
       <c r="DG42" s="1" t="n"/>
       <c r="DH42" s="1" t="n"/>
       <c r="DI42" s="1" t="n"/>
+      <c r="DJ42" s="1" t="n"/>
     </row>
     <row r="43" ht="20" customHeight="1">
       <c r="A43" s="1" t="n">
@@ -15410,6 +15537,7 @@
       <c r="DG43" s="1" t="n"/>
       <c r="DH43" s="1" t="n"/>
       <c r="DI43" s="1" t="n"/>
+      <c r="DJ43" s="1" t="n"/>
     </row>
     <row r="44" ht="20" customHeight="1">
       <c r="A44" s="1" t="n">
@@ -15751,6 +15879,9 @@
       <c r="DI44" s="1" t="n">
         <v>172.3</v>
       </c>
+      <c r="DJ44" s="1" t="n">
+        <v>159.6</v>
+      </c>
     </row>
     <row r="45" ht="20" customHeight="1">
       <c r="A45" s="1" t="n">
@@ -16092,6 +16223,9 @@
       <c r="DI45" s="2" t="n">
         <v>116.3</v>
       </c>
+      <c r="DJ45" s="1" t="n">
+        <v>196.7</v>
+      </c>
     </row>
     <row r="46" ht="20" customHeight="1">
       <c r="A46" s="1" t="n">
@@ -16433,6 +16567,9 @@
       <c r="DI46" s="1" t="n">
         <v>161.5</v>
       </c>
+      <c r="DJ46" s="3" t="n">
+        <v>132.2</v>
+      </c>
     </row>
     <row r="47" ht="20" customHeight="1">
       <c r="A47" s="1" t="n">
@@ -16774,6 +16911,9 @@
       <c r="DI47" s="1" t="n">
         <v>142.2</v>
       </c>
+      <c r="DJ47" s="1" t="n">
+        <v>162.9</v>
+      </c>
     </row>
     <row r="48" ht="20" customHeight="1">
       <c r="A48" s="1" t="n">
@@ -17115,6 +17255,9 @@
       <c r="DI48" s="3" t="n">
         <v>131.9</v>
       </c>
+      <c r="DJ48" s="1" t="n">
+        <v>152.8</v>
+      </c>
     </row>
     <row r="49" ht="20" customHeight="1">
       <c r="A49" s="1" t="n">
@@ -17456,6 +17599,9 @@
       <c r="DI49" s="2" t="n">
         <v>121.1</v>
       </c>
+      <c r="DJ49" s="1" t="n">
+        <v>141.1</v>
+      </c>
     </row>
     <row r="50" ht="20" customHeight="1">
       <c r="A50" s="1" t="n">
@@ -17797,6 +17943,9 @@
       <c r="DI50" s="1" t="n">
         <v>218.6</v>
       </c>
+      <c r="DJ50" s="1" t="n">
+        <v>167</v>
+      </c>
     </row>
     <row r="51" ht="20" customHeight="1">
       <c r="A51" s="1" t="n">
@@ -18138,6 +18287,9 @@
       <c r="DI51" s="1" t="n">
         <v>147.7</v>
       </c>
+      <c r="DJ51" s="1" t="n">
+        <v>147.1</v>
+      </c>
     </row>
     <row r="52" ht="20" customHeight="1">
       <c r="A52" s="1" t="n">
@@ -18479,6 +18631,9 @@
       <c r="DI52" s="3" t="n">
         <v>127.7</v>
       </c>
+      <c r="DJ52" s="3" t="n">
+        <v>126.7</v>
+      </c>
     </row>
     <row r="53" ht="20" customHeight="1">
       <c r="A53" s="1" t="n">
@@ -18819,6 +18974,9 @@
       </c>
       <c r="DI53" s="3" t="n">
         <v>139.4</v>
+      </c>
+      <c r="DJ53" s="1" t="n">
+        <v>193.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2025-01-01
</commit_message>
<xml_diff>
--- a/マイジャグラーV_塗りつぶし済み.xlsx
+++ b/マイジャグラーV_塗りつぶし済み.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:DJ53"/>
+  <dimension ref="A1:DK53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -553,6 +553,7 @@
     <col width="12" customWidth="1" min="112" max="112"/>
     <col width="12" customWidth="1" min="113" max="113"/>
     <col width="12" customWidth="1" min="114" max="114"/>
+    <col width="12" customWidth="1" min="115" max="115"/>
   </cols>
   <sheetData>
     <row r="1" ht="20" customHeight="1">
@@ -1126,6 +1127,11 @@
           <t>2024/12/31</t>
         </is>
       </c>
+      <c r="DK1" s="1" t="inlineStr">
+        <is>
+          <t>2025/01/01</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="20" customHeight="1">
       <c r="A2" s="1" t="n">
@@ -1470,6 +1476,9 @@
       <c r="DJ2" s="3" t="n">
         <v>137.9</v>
       </c>
+      <c r="DK2" s="1" t="n">
+        <v>192.1</v>
+      </c>
     </row>
     <row r="3" ht="20" customHeight="1">
       <c r="A3" s="1" t="n">
@@ -1814,6 +1823,9 @@
       <c r="DJ3" s="1" t="n">
         <v>161.4</v>
       </c>
+      <c r="DK3" s="1" t="n">
+        <v>153.9</v>
+      </c>
     </row>
     <row r="4" ht="20" customHeight="1">
       <c r="A4" s="1" t="n">
@@ -2158,6 +2170,9 @@
       <c r="DJ4" s="1" t="n">
         <v>158.9</v>
       </c>
+      <c r="DK4" s="1" t="n">
+        <v>141.4</v>
+      </c>
     </row>
     <row r="5" ht="20" customHeight="1">
       <c r="A5" s="1" t="n">
@@ -2502,6 +2517,9 @@
       <c r="DJ5" s="1" t="n">
         <v>190.8</v>
       </c>
+      <c r="DK5" s="1" t="n">
+        <v>149.1</v>
+      </c>
     </row>
     <row r="6" ht="20" customHeight="1">
       <c r="A6" s="1" t="n">
@@ -2846,6 +2864,9 @@
       <c r="DJ6" s="1" t="n">
         <v>197.3</v>
       </c>
+      <c r="DK6" s="1" t="n">
+        <v>189.9</v>
+      </c>
     </row>
     <row r="7" ht="20" customHeight="1">
       <c r="A7" s="1" t="n">
@@ -3190,6 +3211,9 @@
       <c r="DJ7" s="2" t="n">
         <v>113.9</v>
       </c>
+      <c r="DK7" s="1" t="n">
+        <v>168.9</v>
+      </c>
     </row>
     <row r="8" ht="20" customHeight="1">
       <c r="A8" s="1" t="n">
@@ -3534,6 +3558,9 @@
       <c r="DJ8" s="1" t="n">
         <v>148.9</v>
       </c>
+      <c r="DK8" s="1" t="n">
+        <v>169</v>
+      </c>
     </row>
     <row r="9" ht="20" customHeight="1">
       <c r="A9" s="1" t="n">
@@ -3878,6 +3905,9 @@
       <c r="DJ9" s="1" t="n">
         <v>140.1</v>
       </c>
+      <c r="DK9" s="1" t="n">
+        <v>166.4</v>
+      </c>
     </row>
     <row r="10" ht="20" customHeight="1">
       <c r="A10" s="1" t="n">
@@ -4222,6 +4252,9 @@
       <c r="DJ10" s="1" t="n">
         <v>254.5</v>
       </c>
+      <c r="DK10" s="1" t="n">
+        <v>183.3</v>
+      </c>
     </row>
     <row r="11" ht="20" customHeight="1">
       <c r="A11" s="1" t="n">
@@ -4566,6 +4599,9 @@
       <c r="DJ11" s="3" t="n">
         <v>136.3</v>
       </c>
+      <c r="DK11" s="1" t="n">
+        <v>171.8</v>
+      </c>
     </row>
     <row r="12" ht="20" customHeight="1">
       <c r="A12" s="1" t="n">
@@ -4910,6 +4946,9 @@
       <c r="DJ12" s="1" t="n">
         <v>182.1</v>
       </c>
+      <c r="DK12" s="3" t="n">
+        <v>135.5</v>
+      </c>
     </row>
     <row r="13" ht="20" customHeight="1">
       <c r="A13" s="1" t="n">
@@ -5254,6 +5293,9 @@
       <c r="DJ13" s="3" t="n">
         <v>129</v>
       </c>
+      <c r="DK13" s="1" t="n">
+        <v>179</v>
+      </c>
     </row>
     <row r="14" ht="20" customHeight="1">
       <c r="A14" s="1" t="n">
@@ -5598,6 +5640,9 @@
       <c r="DJ14" s="1" t="n">
         <v>254.2</v>
       </c>
+      <c r="DK14" s="3" t="n">
+        <v>135.2</v>
+      </c>
     </row>
     <row r="15" ht="20" customHeight="1">
       <c r="A15" s="1" t="n">
@@ -5942,6 +5987,9 @@
       <c r="DJ15" s="1" t="n">
         <v>162.1</v>
       </c>
+      <c r="DK15" s="1" t="n">
+        <v>158.6</v>
+      </c>
     </row>
     <row r="16" ht="20" customHeight="1">
       <c r="A16" s="1" t="n">
@@ -6286,6 +6334,9 @@
       <c r="DJ16" s="3" t="n">
         <v>133</v>
       </c>
+      <c r="DK16" s="1" t="n">
+        <v>160.3</v>
+      </c>
     </row>
     <row r="17" ht="20" customHeight="1">
       <c r="A17" s="1" t="n">
@@ -6630,6 +6681,9 @@
       <c r="DJ17" s="1" t="n">
         <v>144.6</v>
       </c>
+      <c r="DK17" s="1" t="n">
+        <v>173.3</v>
+      </c>
     </row>
     <row r="18" ht="20" customHeight="1">
       <c r="A18" s="1" t="n">
@@ -6974,6 +7028,9 @@
       <c r="DJ18" s="1" t="n">
         <v>144.3</v>
       </c>
+      <c r="DK18" s="1" t="n">
+        <v>142.5</v>
+      </c>
     </row>
     <row r="19" ht="20" customHeight="1">
       <c r="A19" s="1" t="n">
@@ -7318,6 +7375,9 @@
       <c r="DJ19" s="1" t="n">
         <v>146</v>
       </c>
+      <c r="DK19" s="1" t="n">
+        <v>207.1</v>
+      </c>
     </row>
     <row r="20" ht="20" customHeight="1">
       <c r="A20" s="1" t="n">
@@ -7662,6 +7722,9 @@
       <c r="DJ20" s="1" t="n">
         <v>199.6</v>
       </c>
+      <c r="DK20" s="1" t="n">
+        <v>192.6</v>
+      </c>
     </row>
     <row r="21" ht="20" customHeight="1">
       <c r="A21" s="1" t="n">
@@ -8006,6 +8069,9 @@
       <c r="DJ21" s="1" t="n">
         <v>175.2</v>
       </c>
+      <c r="DK21" s="3" t="n">
+        <v>138.6</v>
+      </c>
     </row>
     <row r="22" ht="20" customHeight="1">
       <c r="A22" s="1" t="n">
@@ -8350,6 +8416,9 @@
       <c r="DJ22" s="1" t="n">
         <v>166.6</v>
       </c>
+      <c r="DK22" s="1" t="n">
+        <v>142.7</v>
+      </c>
     </row>
     <row r="23" ht="20" customHeight="1">
       <c r="A23" s="1" t="n">
@@ -8694,6 +8763,9 @@
       <c r="DJ23" s="1" t="n">
         <v>155.3</v>
       </c>
+      <c r="DK23" s="2" t="n">
+        <v>114.4</v>
+      </c>
     </row>
     <row r="24" ht="20" customHeight="1">
       <c r="A24" s="1" t="n">
@@ -9038,6 +9110,9 @@
       <c r="DJ24" s="1" t="n">
         <v>171</v>
       </c>
+      <c r="DK24" s="1" t="n">
+        <v>156.9</v>
+      </c>
     </row>
     <row r="25" ht="20" customHeight="1">
       <c r="A25" s="1" t="n">
@@ -9382,6 +9457,9 @@
       <c r="DJ25" s="3" t="n">
         <v>135</v>
       </c>
+      <c r="DK25" s="1" t="n">
+        <v>172.5</v>
+      </c>
     </row>
     <row r="26" ht="20" customHeight="1">
       <c r="A26" s="1" t="n">
@@ -9726,6 +9804,9 @@
       <c r="DJ26" s="3" t="n">
         <v>133.2</v>
       </c>
+      <c r="DK26" s="2" t="n">
+        <v>115.6</v>
+      </c>
     </row>
     <row r="27" ht="20" customHeight="1">
       <c r="A27" s="1" t="n">
@@ -10070,6 +10151,9 @@
       <c r="DJ27" s="3" t="n">
         <v>129.2</v>
       </c>
+      <c r="DK27" s="2" t="n">
+        <v>124.9</v>
+      </c>
     </row>
     <row r="28" ht="20" customHeight="1">
       <c r="A28" s="1" t="n">
@@ -10414,6 +10498,9 @@
       <c r="DJ28" s="1" t="n">
         <v>170.5</v>
       </c>
+      <c r="DK28" s="1" t="n">
+        <v>184.3</v>
+      </c>
     </row>
     <row r="29" ht="20" customHeight="1">
       <c r="A29" s="1" t="n">
@@ -10758,6 +10845,9 @@
       <c r="DJ29" s="3" t="n">
         <v>131.8</v>
       </c>
+      <c r="DK29" s="1" t="n">
+        <v>202.5</v>
+      </c>
     </row>
     <row r="30" ht="20" customHeight="1">
       <c r="A30" s="1" t="n">
@@ -11102,6 +11192,9 @@
       <c r="DJ30" s="3" t="n">
         <v>129.8</v>
       </c>
+      <c r="DK30" s="1" t="n">
+        <v>140.8</v>
+      </c>
     </row>
     <row r="31" ht="20" customHeight="1">
       <c r="A31" s="1" t="n">
@@ -11446,6 +11539,9 @@
       <c r="DJ31" s="1" t="n">
         <v>161.8</v>
       </c>
+      <c r="DK31" s="3" t="n">
+        <v>125.6</v>
+      </c>
     </row>
     <row r="32" ht="20" customHeight="1">
       <c r="A32" s="1" t="n">
@@ -11790,6 +11886,9 @@
       <c r="DJ32" s="1" t="n">
         <v>156.5</v>
       </c>
+      <c r="DK32" s="1" t="n">
+        <v>173.4</v>
+      </c>
     </row>
     <row r="33" ht="20" customHeight="1">
       <c r="A33" s="1" t="n">
@@ -12134,6 +12233,9 @@
       <c r="DJ33" s="1" t="n">
         <v>153.9</v>
       </c>
+      <c r="DK33" s="3" t="n">
+        <v>130.5</v>
+      </c>
     </row>
     <row r="34" ht="20" customHeight="1">
       <c r="A34" s="1" t="n">
@@ -12478,6 +12580,9 @@
       <c r="DJ34" s="3" t="n">
         <v>132.5</v>
       </c>
+      <c r="DK34" s="1" t="n">
+        <v>225.3</v>
+      </c>
     </row>
     <row r="35" ht="20" customHeight="1">
       <c r="A35" s="1" t="n">
@@ -12822,6 +12927,9 @@
       <c r="DJ35" s="2" t="n">
         <v>111.1</v>
       </c>
+      <c r="DK35" s="1" t="n">
+        <v>178.2</v>
+      </c>
     </row>
     <row r="36" ht="20" customHeight="1">
       <c r="A36" s="1" t="n">
@@ -13166,6 +13274,9 @@
       <c r="DJ36" s="1" t="n">
         <v>188.1</v>
       </c>
+      <c r="DK36" s="1" t="n">
+        <v>174.6</v>
+      </c>
     </row>
     <row r="37" ht="20" customHeight="1">
       <c r="A37" s="1" t="n">
@@ -13510,6 +13621,9 @@
       <c r="DJ37" s="1" t="n">
         <v>160.6</v>
       </c>
+      <c r="DK37" s="1" t="n">
+        <v>176.3</v>
+      </c>
     </row>
     <row r="38" ht="20" customHeight="1">
       <c r="A38" s="1" t="n">
@@ -13854,6 +13968,9 @@
       <c r="DJ38" s="1" t="n">
         <v>160.2</v>
       </c>
+      <c r="DK38" s="1" t="n">
+        <v>228.4</v>
+      </c>
     </row>
     <row r="39" ht="20" customHeight="1">
       <c r="A39" s="1" t="n">
@@ -14198,6 +14315,9 @@
       <c r="DJ39" s="1" t="n">
         <v>195.1</v>
       </c>
+      <c r="DK39" s="1" t="n">
+        <v>143.5</v>
+      </c>
     </row>
     <row r="40" ht="20" customHeight="1">
       <c r="A40" s="1" t="n">
@@ -14542,6 +14662,9 @@
       <c r="DJ40" s="1" t="n">
         <v>159.7</v>
       </c>
+      <c r="DK40" s="1" t="n">
+        <v>186.4</v>
+      </c>
     </row>
     <row r="41" ht="20" customHeight="1">
       <c r="A41" s="1" t="n">
@@ -14885,6 +15008,9 @@
       </c>
       <c r="DJ41" s="1" t="n">
         <v>164.9</v>
+      </c>
+      <c r="DK41" s="1" t="n">
+        <v>143.7</v>
       </c>
     </row>
     <row r="42" ht="20" customHeight="1">
@@ -15212,6 +15338,7 @@
       <c r="DH42" s="1" t="n"/>
       <c r="DI42" s="1" t="n"/>
       <c r="DJ42" s="1" t="n"/>
+      <c r="DK42" s="1" t="n"/>
     </row>
     <row r="43" ht="20" customHeight="1">
       <c r="A43" s="1" t="n">
@@ -15538,6 +15665,7 @@
       <c r="DH43" s="1" t="n"/>
       <c r="DI43" s="1" t="n"/>
       <c r="DJ43" s="1" t="n"/>
+      <c r="DK43" s="1" t="n"/>
     </row>
     <row r="44" ht="20" customHeight="1">
       <c r="A44" s="1" t="n">
@@ -15882,6 +16010,9 @@
       <c r="DJ44" s="1" t="n">
         <v>159.6</v>
       </c>
+      <c r="DK44" s="1" t="n">
+        <v>142.7</v>
+      </c>
     </row>
     <row r="45" ht="20" customHeight="1">
       <c r="A45" s="1" t="n">
@@ -16226,6 +16357,9 @@
       <c r="DJ45" s="1" t="n">
         <v>196.7</v>
       </c>
+      <c r="DK45" s="2" t="n">
+        <v>109.3</v>
+      </c>
     </row>
     <row r="46" ht="20" customHeight="1">
       <c r="A46" s="1" t="n">
@@ -16570,6 +16704,9 @@
       <c r="DJ46" s="3" t="n">
         <v>132.2</v>
       </c>
+      <c r="DK46" s="1" t="n">
+        <v>168.9</v>
+      </c>
     </row>
     <row r="47" ht="20" customHeight="1">
       <c r="A47" s="1" t="n">
@@ -16914,6 +17051,9 @@
       <c r="DJ47" s="1" t="n">
         <v>162.9</v>
       </c>
+      <c r="DK47" s="1" t="n">
+        <v>156.4</v>
+      </c>
     </row>
     <row r="48" ht="20" customHeight="1">
       <c r="A48" s="1" t="n">
@@ -17258,6 +17398,9 @@
       <c r="DJ48" s="1" t="n">
         <v>152.8</v>
       </c>
+      <c r="DK48" s="1" t="n">
+        <v>158.8</v>
+      </c>
     </row>
     <row r="49" ht="20" customHeight="1">
       <c r="A49" s="1" t="n">
@@ -17602,6 +17745,9 @@
       <c r="DJ49" s="1" t="n">
         <v>141.1</v>
       </c>
+      <c r="DK49" s="1" t="n">
+        <v>296.8</v>
+      </c>
     </row>
     <row r="50" ht="20" customHeight="1">
       <c r="A50" s="1" t="n">
@@ -17946,6 +18092,9 @@
       <c r="DJ50" s="1" t="n">
         <v>167</v>
       </c>
+      <c r="DK50" s="3" t="n">
+        <v>138.8</v>
+      </c>
     </row>
     <row r="51" ht="20" customHeight="1">
       <c r="A51" s="1" t="n">
@@ -18290,6 +18439,9 @@
       <c r="DJ51" s="1" t="n">
         <v>147.1</v>
       </c>
+      <c r="DK51" s="1" t="n">
+        <v>219.5</v>
+      </c>
     </row>
     <row r="52" ht="20" customHeight="1">
       <c r="A52" s="1" t="n">
@@ -18634,6 +18786,9 @@
       <c r="DJ52" s="3" t="n">
         <v>126.7</v>
       </c>
+      <c r="DK52" s="1" t="n">
+        <v>191.9</v>
+      </c>
     </row>
     <row r="53" ht="20" customHeight="1">
       <c r="A53" s="1" t="n">
@@ -18977,6 +19132,9 @@
       </c>
       <c r="DJ53" s="1" t="n">
         <v>193.2</v>
+      </c>
+      <c r="DK53" s="1" t="n">
+        <v>141.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2025-01-02
</commit_message>
<xml_diff>
--- a/マイジャグラーV_塗りつぶし済み.xlsx
+++ b/マイジャグラーV_塗りつぶし済み.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:DK53"/>
+  <dimension ref="A1:DL53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -554,6 +554,7 @@
     <col width="12" customWidth="1" min="113" max="113"/>
     <col width="12" customWidth="1" min="114" max="114"/>
     <col width="12" customWidth="1" min="115" max="115"/>
+    <col width="12" customWidth="1" min="116" max="116"/>
   </cols>
   <sheetData>
     <row r="1" ht="20" customHeight="1">
@@ -1132,6 +1133,11 @@
           <t>2025/01/01</t>
         </is>
       </c>
+      <c r="DL1" s="1" t="inlineStr">
+        <is>
+          <t>2025/01/02</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="20" customHeight="1">
       <c r="A2" s="1" t="n">
@@ -1479,6 +1485,9 @@
       <c r="DK2" s="1" t="n">
         <v>192.1</v>
       </c>
+      <c r="DL2" s="1" t="n">
+        <v>156.6</v>
+      </c>
     </row>
     <row r="3" ht="20" customHeight="1">
       <c r="A3" s="1" t="n">
@@ -1826,6 +1835,9 @@
       <c r="DK3" s="1" t="n">
         <v>153.9</v>
       </c>
+      <c r="DL3" s="1" t="n">
+        <v>234.8</v>
+      </c>
     </row>
     <row r="4" ht="20" customHeight="1">
       <c r="A4" s="1" t="n">
@@ -2173,6 +2185,9 @@
       <c r="DK4" s="1" t="n">
         <v>141.4</v>
       </c>
+      <c r="DL4" s="1" t="n">
+        <v>150.2</v>
+      </c>
     </row>
     <row r="5" ht="20" customHeight="1">
       <c r="A5" s="1" t="n">
@@ -2520,6 +2535,9 @@
       <c r="DK5" s="1" t="n">
         <v>149.1</v>
       </c>
+      <c r="DL5" s="2" t="n">
+        <v>111.4</v>
+      </c>
     </row>
     <row r="6" ht="20" customHeight="1">
       <c r="A6" s="1" t="n">
@@ -2867,6 +2885,9 @@
       <c r="DK6" s="1" t="n">
         <v>189.9</v>
       </c>
+      <c r="DL6" s="3" t="n">
+        <v>138.3</v>
+      </c>
     </row>
     <row r="7" ht="20" customHeight="1">
       <c r="A7" s="1" t="n">
@@ -3214,6 +3235,9 @@
       <c r="DK7" s="1" t="n">
         <v>168.9</v>
       </c>
+      <c r="DL7" s="2" t="n">
+        <v>124.9</v>
+      </c>
     </row>
     <row r="8" ht="20" customHeight="1">
       <c r="A8" s="1" t="n">
@@ -3561,6 +3585,9 @@
       <c r="DK8" s="1" t="n">
         <v>169</v>
       </c>
+      <c r="DL8" s="1" t="n">
+        <v>158.1</v>
+      </c>
     </row>
     <row r="9" ht="20" customHeight="1">
       <c r="A9" s="1" t="n">
@@ -3908,6 +3935,9 @@
       <c r="DK9" s="1" t="n">
         <v>166.4</v>
       </c>
+      <c r="DL9" s="1" t="n">
+        <v>153.5</v>
+      </c>
     </row>
     <row r="10" ht="20" customHeight="1">
       <c r="A10" s="1" t="n">
@@ -4255,6 +4285,9 @@
       <c r="DK10" s="1" t="n">
         <v>183.3</v>
       </c>
+      <c r="DL10" s="1" t="n">
+        <v>163.9</v>
+      </c>
     </row>
     <row r="11" ht="20" customHeight="1">
       <c r="A11" s="1" t="n">
@@ -4602,6 +4635,9 @@
       <c r="DK11" s="1" t="n">
         <v>171.8</v>
       </c>
+      <c r="DL11" s="1" t="n">
+        <v>201.4</v>
+      </c>
     </row>
     <row r="12" ht="20" customHeight="1">
       <c r="A12" s="1" t="n">
@@ -4949,6 +4985,9 @@
       <c r="DK12" s="3" t="n">
         <v>135.5</v>
       </c>
+      <c r="DL12" s="1" t="n">
+        <v>140</v>
+      </c>
     </row>
     <row r="13" ht="20" customHeight="1">
       <c r="A13" s="1" t="n">
@@ -5296,6 +5335,9 @@
       <c r="DK13" s="1" t="n">
         <v>179</v>
       </c>
+      <c r="DL13" s="3" t="n">
+        <v>138.1</v>
+      </c>
     </row>
     <row r="14" ht="20" customHeight="1">
       <c r="A14" s="1" t="n">
@@ -5643,6 +5685,9 @@
       <c r="DK14" s="3" t="n">
         <v>135.2</v>
       </c>
+      <c r="DL14" s="1" t="n">
+        <v>179.9</v>
+      </c>
     </row>
     <row r="15" ht="20" customHeight="1">
       <c r="A15" s="1" t="n">
@@ -5990,6 +6035,9 @@
       <c r="DK15" s="1" t="n">
         <v>158.6</v>
       </c>
+      <c r="DL15" s="2" t="n">
+        <v>121.1</v>
+      </c>
     </row>
     <row r="16" ht="20" customHeight="1">
       <c r="A16" s="1" t="n">
@@ -6337,6 +6385,9 @@
       <c r="DK16" s="1" t="n">
         <v>160.3</v>
       </c>
+      <c r="DL16" s="1" t="n">
+        <v>186.7</v>
+      </c>
     </row>
     <row r="17" ht="20" customHeight="1">
       <c r="A17" s="1" t="n">
@@ -6684,6 +6735,9 @@
       <c r="DK17" s="1" t="n">
         <v>173.3</v>
       </c>
+      <c r="DL17" s="1" t="n">
+        <v>150.5</v>
+      </c>
     </row>
     <row r="18" ht="20" customHeight="1">
       <c r="A18" s="1" t="n">
@@ -7031,6 +7085,9 @@
       <c r="DK18" s="1" t="n">
         <v>142.5</v>
       </c>
+      <c r="DL18" s="1" t="n">
+        <v>151.3</v>
+      </c>
     </row>
     <row r="19" ht="20" customHeight="1">
       <c r="A19" s="1" t="n">
@@ -7378,6 +7435,9 @@
       <c r="DK19" s="1" t="n">
         <v>207.1</v>
       </c>
+      <c r="DL19" s="1" t="n">
+        <v>171.3</v>
+      </c>
     </row>
     <row r="20" ht="20" customHeight="1">
       <c r="A20" s="1" t="n">
@@ -7725,6 +7785,9 @@
       <c r="DK20" s="1" t="n">
         <v>192.6</v>
       </c>
+      <c r="DL20" s="1" t="n">
+        <v>164.2</v>
+      </c>
     </row>
     <row r="21" ht="20" customHeight="1">
       <c r="A21" s="1" t="n">
@@ -8072,6 +8135,9 @@
       <c r="DK21" s="3" t="n">
         <v>138.6</v>
       </c>
+      <c r="DL21" s="1" t="n">
+        <v>187.6</v>
+      </c>
     </row>
     <row r="22" ht="20" customHeight="1">
       <c r="A22" s="1" t="n">
@@ -8419,6 +8485,9 @@
       <c r="DK22" s="1" t="n">
         <v>142.7</v>
       </c>
+      <c r="DL22" s="1" t="n">
+        <v>150.1</v>
+      </c>
     </row>
     <row r="23" ht="20" customHeight="1">
       <c r="A23" s="1" t="n">
@@ -8766,6 +8835,9 @@
       <c r="DK23" s="2" t="n">
         <v>114.4</v>
       </c>
+      <c r="DL23" s="2" t="n">
+        <v>116.9</v>
+      </c>
     </row>
     <row r="24" ht="20" customHeight="1">
       <c r="A24" s="1" t="n">
@@ -9113,6 +9185,9 @@
       <c r="DK24" s="1" t="n">
         <v>156.9</v>
       </c>
+      <c r="DL24" s="1" t="n">
+        <v>174.9</v>
+      </c>
     </row>
     <row r="25" ht="20" customHeight="1">
       <c r="A25" s="1" t="n">
@@ -9460,6 +9535,9 @@
       <c r="DK25" s="1" t="n">
         <v>172.5</v>
       </c>
+      <c r="DL25" s="1" t="n">
+        <v>180.5</v>
+      </c>
     </row>
     <row r="26" ht="20" customHeight="1">
       <c r="A26" s="1" t="n">
@@ -9807,6 +9885,9 @@
       <c r="DK26" s="2" t="n">
         <v>115.6</v>
       </c>
+      <c r="DL26" s="1" t="n">
+        <v>191.1</v>
+      </c>
     </row>
     <row r="27" ht="20" customHeight="1">
       <c r="A27" s="1" t="n">
@@ -10154,6 +10235,9 @@
       <c r="DK27" s="2" t="n">
         <v>124.9</v>
       </c>
+      <c r="DL27" s="1" t="n">
+        <v>208.4</v>
+      </c>
     </row>
     <row r="28" ht="20" customHeight="1">
       <c r="A28" s="1" t="n">
@@ -10501,6 +10585,9 @@
       <c r="DK28" s="1" t="n">
         <v>184.3</v>
       </c>
+      <c r="DL28" s="1" t="n">
+        <v>157.9</v>
+      </c>
     </row>
     <row r="29" ht="20" customHeight="1">
       <c r="A29" s="1" t="n">
@@ -10848,6 +10935,9 @@
       <c r="DK29" s="1" t="n">
         <v>202.5</v>
       </c>
+      <c r="DL29" s="2" t="n">
+        <v>124.7</v>
+      </c>
     </row>
     <row r="30" ht="20" customHeight="1">
       <c r="A30" s="1" t="n">
@@ -11195,6 +11285,9 @@
       <c r="DK30" s="1" t="n">
         <v>140.8</v>
       </c>
+      <c r="DL30" s="1" t="n">
+        <v>141.7</v>
+      </c>
     </row>
     <row r="31" ht="20" customHeight="1">
       <c r="A31" s="1" t="n">
@@ -11542,6 +11635,9 @@
       <c r="DK31" s="3" t="n">
         <v>125.6</v>
       </c>
+      <c r="DL31" s="1" t="n">
+        <v>206.5</v>
+      </c>
     </row>
     <row r="32" ht="20" customHeight="1">
       <c r="A32" s="1" t="n">
@@ -11889,6 +11985,9 @@
       <c r="DK32" s="1" t="n">
         <v>173.4</v>
       </c>
+      <c r="DL32" s="1" t="n">
+        <v>148.2</v>
+      </c>
     </row>
     <row r="33" ht="20" customHeight="1">
       <c r="A33" s="1" t="n">
@@ -12236,6 +12335,9 @@
       <c r="DK33" s="3" t="n">
         <v>130.5</v>
       </c>
+      <c r="DL33" s="3" t="n">
+        <v>126.5</v>
+      </c>
     </row>
     <row r="34" ht="20" customHeight="1">
       <c r="A34" s="1" t="n">
@@ -12583,6 +12685,9 @@
       <c r="DK34" s="1" t="n">
         <v>225.3</v>
       </c>
+      <c r="DL34" s="1" t="n">
+        <v>142.9</v>
+      </c>
     </row>
     <row r="35" ht="20" customHeight="1">
       <c r="A35" s="1" t="n">
@@ -12930,6 +13035,9 @@
       <c r="DK35" s="1" t="n">
         <v>178.2</v>
       </c>
+      <c r="DL35" s="2" t="n">
+        <v>121.7</v>
+      </c>
     </row>
     <row r="36" ht="20" customHeight="1">
       <c r="A36" s="1" t="n">
@@ -13277,6 +13385,9 @@
       <c r="DK36" s="1" t="n">
         <v>174.6</v>
       </c>
+      <c r="DL36" s="1" t="n">
+        <v>181.9</v>
+      </c>
     </row>
     <row r="37" ht="20" customHeight="1">
       <c r="A37" s="1" t="n">
@@ -13624,6 +13735,9 @@
       <c r="DK37" s="1" t="n">
         <v>176.3</v>
       </c>
+      <c r="DL37" s="1" t="n">
+        <v>194.3</v>
+      </c>
     </row>
     <row r="38" ht="20" customHeight="1">
       <c r="A38" s="1" t="n">
@@ -13971,6 +14085,9 @@
       <c r="DK38" s="1" t="n">
         <v>228.4</v>
       </c>
+      <c r="DL38" s="3" t="n">
+        <v>130.3</v>
+      </c>
     </row>
     <row r="39" ht="20" customHeight="1">
       <c r="A39" s="1" t="n">
@@ -14318,6 +14435,9 @@
       <c r="DK39" s="1" t="n">
         <v>143.5</v>
       </c>
+      <c r="DL39" s="1" t="n">
+        <v>158</v>
+      </c>
     </row>
     <row r="40" ht="20" customHeight="1">
       <c r="A40" s="1" t="n">
@@ -14665,6 +14785,9 @@
       <c r="DK40" s="1" t="n">
         <v>186.4</v>
       </c>
+      <c r="DL40" s="2" t="n">
+        <v>124.2</v>
+      </c>
     </row>
     <row r="41" ht="20" customHeight="1">
       <c r="A41" s="1" t="n">
@@ -15011,6 +15134,9 @@
       </c>
       <c r="DK41" s="1" t="n">
         <v>143.7</v>
+      </c>
+      <c r="DL41" s="1" t="n">
+        <v>143.2</v>
       </c>
     </row>
     <row r="42" ht="20" customHeight="1">
@@ -15339,6 +15465,7 @@
       <c r="DI42" s="1" t="n"/>
       <c r="DJ42" s="1" t="n"/>
       <c r="DK42" s="1" t="n"/>
+      <c r="DL42" s="1" t="n"/>
     </row>
     <row r="43" ht="20" customHeight="1">
       <c r="A43" s="1" t="n">
@@ -15666,6 +15793,7 @@
       <c r="DI43" s="1" t="n"/>
       <c r="DJ43" s="1" t="n"/>
       <c r="DK43" s="1" t="n"/>
+      <c r="DL43" s="1" t="n"/>
     </row>
     <row r="44" ht="20" customHeight="1">
       <c r="A44" s="1" t="n">
@@ -16013,6 +16141,9 @@
       <c r="DK44" s="1" t="n">
         <v>142.7</v>
       </c>
+      <c r="DL44" s="1" t="n">
+        <v>178.5</v>
+      </c>
     </row>
     <row r="45" ht="20" customHeight="1">
       <c r="A45" s="1" t="n">
@@ -16360,6 +16491,9 @@
       <c r="DK45" s="2" t="n">
         <v>109.3</v>
       </c>
+      <c r="DL45" s="1" t="n">
+        <v>151.5</v>
+      </c>
     </row>
     <row r="46" ht="20" customHeight="1">
       <c r="A46" s="1" t="n">
@@ -16707,6 +16841,9 @@
       <c r="DK46" s="1" t="n">
         <v>168.9</v>
       </c>
+      <c r="DL46" s="3" t="n">
+        <v>135.4</v>
+      </c>
     </row>
     <row r="47" ht="20" customHeight="1">
       <c r="A47" s="1" t="n">
@@ -17054,6 +17191,9 @@
       <c r="DK47" s="1" t="n">
         <v>156.4</v>
       </c>
+      <c r="DL47" s="3" t="n">
+        <v>135.8</v>
+      </c>
     </row>
     <row r="48" ht="20" customHeight="1">
       <c r="A48" s="1" t="n">
@@ -17401,6 +17541,9 @@
       <c r="DK48" s="1" t="n">
         <v>158.8</v>
       </c>
+      <c r="DL48" s="1" t="n">
+        <v>168.3</v>
+      </c>
     </row>
     <row r="49" ht="20" customHeight="1">
       <c r="A49" s="1" t="n">
@@ -17748,6 +17891,9 @@
       <c r="DK49" s="1" t="n">
         <v>296.8</v>
       </c>
+      <c r="DL49" s="1" t="n">
+        <v>163</v>
+      </c>
     </row>
     <row r="50" ht="20" customHeight="1">
       <c r="A50" s="1" t="n">
@@ -18095,6 +18241,9 @@
       <c r="DK50" s="3" t="n">
         <v>138.8</v>
       </c>
+      <c r="DL50" s="1" t="n">
+        <v>143.2</v>
+      </c>
     </row>
     <row r="51" ht="20" customHeight="1">
       <c r="A51" s="1" t="n">
@@ -18442,6 +18591,9 @@
       <c r="DK51" s="1" t="n">
         <v>219.5</v>
       </c>
+      <c r="DL51" s="3" t="n">
+        <v>135.2</v>
+      </c>
     </row>
     <row r="52" ht="20" customHeight="1">
       <c r="A52" s="1" t="n">
@@ -18789,6 +18941,9 @@
       <c r="DK52" s="1" t="n">
         <v>191.9</v>
       </c>
+      <c r="DL52" s="1" t="n">
+        <v>186</v>
+      </c>
     </row>
     <row r="53" ht="20" customHeight="1">
       <c r="A53" s="1" t="n">
@@ -19135,6 +19290,9 @@
       </c>
       <c r="DK53" s="1" t="n">
         <v>141.1</v>
+      </c>
+      <c r="DL53" s="1" t="n">
+        <v>140.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2025-01-03
</commit_message>
<xml_diff>
--- a/マイジャグラーV_塗りつぶし済み.xlsx
+++ b/マイジャグラーV_塗りつぶし済み.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:DL53"/>
+  <dimension ref="A1:DM53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -555,6 +555,7 @@
     <col width="12" customWidth="1" min="114" max="114"/>
     <col width="12" customWidth="1" min="115" max="115"/>
     <col width="12" customWidth="1" min="116" max="116"/>
+    <col width="12" customWidth="1" min="117" max="117"/>
   </cols>
   <sheetData>
     <row r="1" ht="20" customHeight="1">
@@ -1138,6 +1139,11 @@
           <t>2025/01/02</t>
         </is>
       </c>
+      <c r="DM1" s="1" t="inlineStr">
+        <is>
+          <t>2025/01/03</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="20" customHeight="1">
       <c r="A2" s="1" t="n">
@@ -1488,6 +1494,9 @@
       <c r="DL2" s="1" t="n">
         <v>156.6</v>
       </c>
+      <c r="DM2" s="3" t="n">
+        <v>138.7</v>
+      </c>
     </row>
     <row r="3" ht="20" customHeight="1">
       <c r="A3" s="1" t="n">
@@ -1838,6 +1847,9 @@
       <c r="DL3" s="1" t="n">
         <v>234.8</v>
       </c>
+      <c r="DM3" s="1" t="n">
+        <v>252.5</v>
+      </c>
     </row>
     <row r="4" ht="20" customHeight="1">
       <c r="A4" s="1" t="n">
@@ -2188,6 +2200,9 @@
       <c r="DL4" s="1" t="n">
         <v>150.2</v>
       </c>
+      <c r="DM4" s="1" t="n">
+        <v>176.8</v>
+      </c>
     </row>
     <row r="5" ht="20" customHeight="1">
       <c r="A5" s="1" t="n">
@@ -2538,6 +2553,9 @@
       <c r="DL5" s="2" t="n">
         <v>111.4</v>
       </c>
+      <c r="DM5" s="3" t="n">
+        <v>137.5</v>
+      </c>
     </row>
     <row r="6" ht="20" customHeight="1">
       <c r="A6" s="1" t="n">
@@ -2888,6 +2906,9 @@
       <c r="DL6" s="3" t="n">
         <v>138.3</v>
       </c>
+      <c r="DM6" s="1" t="n">
+        <v>155.3</v>
+      </c>
     </row>
     <row r="7" ht="20" customHeight="1">
       <c r="A7" s="1" t="n">
@@ -3238,6 +3259,9 @@
       <c r="DL7" s="2" t="n">
         <v>124.9</v>
       </c>
+      <c r="DM7" s="3" t="n">
+        <v>137.9</v>
+      </c>
     </row>
     <row r="8" ht="20" customHeight="1">
       <c r="A8" s="1" t="n">
@@ -3588,6 +3612,9 @@
       <c r="DL8" s="1" t="n">
         <v>158.1</v>
       </c>
+      <c r="DM8" s="1" t="n">
+        <v>182.8</v>
+      </c>
     </row>
     <row r="9" ht="20" customHeight="1">
       <c r="A9" s="1" t="n">
@@ -3938,6 +3965,9 @@
       <c r="DL9" s="1" t="n">
         <v>153.5</v>
       </c>
+      <c r="DM9" s="1" t="n">
+        <v>162.7</v>
+      </c>
     </row>
     <row r="10" ht="20" customHeight="1">
       <c r="A10" s="1" t="n">
@@ -4288,6 +4318,9 @@
       <c r="DL10" s="1" t="n">
         <v>163.9</v>
       </c>
+      <c r="DM10" s="1" t="n">
+        <v>234.8</v>
+      </c>
     </row>
     <row r="11" ht="20" customHeight="1">
       <c r="A11" s="1" t="n">
@@ -4638,6 +4671,9 @@
       <c r="DL11" s="1" t="n">
         <v>201.4</v>
       </c>
+      <c r="DM11" s="2" t="n">
+        <v>118.8</v>
+      </c>
     </row>
     <row r="12" ht="20" customHeight="1">
       <c r="A12" s="1" t="n">
@@ -4988,6 +5024,9 @@
       <c r="DL12" s="1" t="n">
         <v>140</v>
       </c>
+      <c r="DM12" s="3" t="n">
+        <v>125.7</v>
+      </c>
     </row>
     <row r="13" ht="20" customHeight="1">
       <c r="A13" s="1" t="n">
@@ -5338,6 +5377,9 @@
       <c r="DL13" s="3" t="n">
         <v>138.1</v>
       </c>
+      <c r="DM13" s="1" t="n">
+        <v>156.9</v>
+      </c>
     </row>
     <row r="14" ht="20" customHeight="1">
       <c r="A14" s="1" t="n">
@@ -5688,6 +5730,9 @@
       <c r="DL14" s="1" t="n">
         <v>179.9</v>
       </c>
+      <c r="DM14" s="2" t="n">
+        <v>121.2</v>
+      </c>
     </row>
     <row r="15" ht="20" customHeight="1">
       <c r="A15" s="1" t="n">
@@ -6038,6 +6083,9 @@
       <c r="DL15" s="2" t="n">
         <v>121.1</v>
       </c>
+      <c r="DM15" s="2" t="n">
+        <v>115.6</v>
+      </c>
     </row>
     <row r="16" ht="20" customHeight="1">
       <c r="A16" s="1" t="n">
@@ -6388,6 +6436,9 @@
       <c r="DL16" s="1" t="n">
         <v>186.7</v>
       </c>
+      <c r="DM16" s="1" t="n">
+        <v>151.1</v>
+      </c>
     </row>
     <row r="17" ht="20" customHeight="1">
       <c r="A17" s="1" t="n">
@@ -6738,6 +6789,9 @@
       <c r="DL17" s="1" t="n">
         <v>150.5</v>
       </c>
+      <c r="DM17" s="1" t="n">
+        <v>140</v>
+      </c>
     </row>
     <row r="18" ht="20" customHeight="1">
       <c r="A18" s="1" t="n">
@@ -7088,6 +7142,9 @@
       <c r="DL18" s="1" t="n">
         <v>151.3</v>
       </c>
+      <c r="DM18" s="3" t="n">
+        <v>125.9</v>
+      </c>
     </row>
     <row r="19" ht="20" customHeight="1">
       <c r="A19" s="1" t="n">
@@ -7438,6 +7495,9 @@
       <c r="DL19" s="1" t="n">
         <v>171.3</v>
       </c>
+      <c r="DM19" s="1" t="n">
+        <v>141.8</v>
+      </c>
     </row>
     <row r="20" ht="20" customHeight="1">
       <c r="A20" s="1" t="n">
@@ -7788,6 +7848,9 @@
       <c r="DL20" s="1" t="n">
         <v>164.2</v>
       </c>
+      <c r="DM20" s="1" t="n">
+        <v>162.4</v>
+      </c>
     </row>
     <row r="21" ht="20" customHeight="1">
       <c r="A21" s="1" t="n">
@@ -8138,6 +8201,9 @@
       <c r="DL21" s="1" t="n">
         <v>187.6</v>
       </c>
+      <c r="DM21" s="1" t="n">
+        <v>159.2</v>
+      </c>
     </row>
     <row r="22" ht="20" customHeight="1">
       <c r="A22" s="1" t="n">
@@ -8488,6 +8554,9 @@
       <c r="DL22" s="1" t="n">
         <v>150.1</v>
       </c>
+      <c r="DM22" s="1" t="n">
+        <v>191.2</v>
+      </c>
     </row>
     <row r="23" ht="20" customHeight="1">
       <c r="A23" s="1" t="n">
@@ -8838,6 +8907,9 @@
       <c r="DL23" s="2" t="n">
         <v>116.9</v>
       </c>
+      <c r="DM23" s="1" t="n">
+        <v>141.3</v>
+      </c>
     </row>
     <row r="24" ht="20" customHeight="1">
       <c r="A24" s="1" t="n">
@@ -9188,6 +9260,9 @@
       <c r="DL24" s="1" t="n">
         <v>174.9</v>
       </c>
+      <c r="DM24" s="3" t="n">
+        <v>131.5</v>
+      </c>
     </row>
     <row r="25" ht="20" customHeight="1">
       <c r="A25" s="1" t="n">
@@ -9538,6 +9613,9 @@
       <c r="DL25" s="1" t="n">
         <v>180.5</v>
       </c>
+      <c r="DM25" s="1" t="n">
+        <v>197.5</v>
+      </c>
     </row>
     <row r="26" ht="20" customHeight="1">
       <c r="A26" s="1" t="n">
@@ -9888,6 +9966,9 @@
       <c r="DL26" s="1" t="n">
         <v>191.1</v>
       </c>
+      <c r="DM26" s="2" t="n">
+        <v>123.7</v>
+      </c>
     </row>
     <row r="27" ht="20" customHeight="1">
       <c r="A27" s="1" t="n">
@@ -10238,6 +10319,9 @@
       <c r="DL27" s="1" t="n">
         <v>208.4</v>
       </c>
+      <c r="DM27" s="1" t="n">
+        <v>169.8</v>
+      </c>
     </row>
     <row r="28" ht="20" customHeight="1">
       <c r="A28" s="1" t="n">
@@ -10588,6 +10672,9 @@
       <c r="DL28" s="1" t="n">
         <v>157.9</v>
       </c>
+      <c r="DM28" s="1" t="n">
+        <v>242</v>
+      </c>
     </row>
     <row r="29" ht="20" customHeight="1">
       <c r="A29" s="1" t="n">
@@ -10938,6 +11025,9 @@
       <c r="DL29" s="2" t="n">
         <v>124.7</v>
       </c>
+      <c r="DM29" s="1" t="n">
+        <v>171.5</v>
+      </c>
     </row>
     <row r="30" ht="20" customHeight="1">
       <c r="A30" s="1" t="n">
@@ -11288,6 +11378,9 @@
       <c r="DL30" s="1" t="n">
         <v>141.7</v>
       </c>
+      <c r="DM30" s="3" t="n">
+        <v>137.9</v>
+      </c>
     </row>
     <row r="31" ht="20" customHeight="1">
       <c r="A31" s="1" t="n">
@@ -11638,6 +11731,9 @@
       <c r="DL31" s="1" t="n">
         <v>206.5</v>
       </c>
+      <c r="DM31" s="1" t="n">
+        <v>180.3</v>
+      </c>
     </row>
     <row r="32" ht="20" customHeight="1">
       <c r="A32" s="1" t="n">
@@ -11988,6 +12084,9 @@
       <c r="DL32" s="1" t="n">
         <v>148.2</v>
       </c>
+      <c r="DM32" s="1" t="n">
+        <v>166.2</v>
+      </c>
     </row>
     <row r="33" ht="20" customHeight="1">
       <c r="A33" s="1" t="n">
@@ -12338,6 +12437,9 @@
       <c r="DL33" s="3" t="n">
         <v>126.5</v>
       </c>
+      <c r="DM33" s="1" t="n">
+        <v>245.7</v>
+      </c>
     </row>
     <row r="34" ht="20" customHeight="1">
       <c r="A34" s="1" t="n">
@@ -12688,6 +12790,9 @@
       <c r="DL34" s="1" t="n">
         <v>142.9</v>
       </c>
+      <c r="DM34" s="1" t="n">
+        <v>155.8</v>
+      </c>
     </row>
     <row r="35" ht="20" customHeight="1">
       <c r="A35" s="1" t="n">
@@ -13038,6 +13143,9 @@
       <c r="DL35" s="2" t="n">
         <v>121.7</v>
       </c>
+      <c r="DM35" s="1" t="n">
+        <v>157.5</v>
+      </c>
     </row>
     <row r="36" ht="20" customHeight="1">
       <c r="A36" s="1" t="n">
@@ -13388,6 +13496,9 @@
       <c r="DL36" s="1" t="n">
         <v>181.9</v>
       </c>
+      <c r="DM36" s="1" t="n">
+        <v>189.5</v>
+      </c>
     </row>
     <row r="37" ht="20" customHeight="1">
       <c r="A37" s="1" t="n">
@@ -13738,6 +13849,9 @@
       <c r="DL37" s="1" t="n">
         <v>194.3</v>
       </c>
+      <c r="DM37" s="3" t="n">
+        <v>135.4</v>
+      </c>
     </row>
     <row r="38" ht="20" customHeight="1">
       <c r="A38" s="1" t="n">
@@ -14088,6 +14202,9 @@
       <c r="DL38" s="3" t="n">
         <v>130.3</v>
       </c>
+      <c r="DM38" s="2" t="n">
+        <v>118.5</v>
+      </c>
     </row>
     <row r="39" ht="20" customHeight="1">
       <c r="A39" s="1" t="n">
@@ -14438,6 +14555,9 @@
       <c r="DL39" s="1" t="n">
         <v>158</v>
       </c>
+      <c r="DM39" s="3" t="n">
+        <v>134.8</v>
+      </c>
     </row>
     <row r="40" ht="20" customHeight="1">
       <c r="A40" s="1" t="n">
@@ -14788,6 +14908,9 @@
       <c r="DL40" s="2" t="n">
         <v>124.2</v>
       </c>
+      <c r="DM40" s="3" t="n">
+        <v>126</v>
+      </c>
     </row>
     <row r="41" ht="20" customHeight="1">
       <c r="A41" s="1" t="n">
@@ -15137,6 +15260,9 @@
       </c>
       <c r="DL41" s="1" t="n">
         <v>143.2</v>
+      </c>
+      <c r="DM41" s="3" t="n">
+        <v>136.3</v>
       </c>
     </row>
     <row r="42" ht="20" customHeight="1">
@@ -15466,6 +15592,7 @@
       <c r="DJ42" s="1" t="n"/>
       <c r="DK42" s="1" t="n"/>
       <c r="DL42" s="1" t="n"/>
+      <c r="DM42" s="1" t="n"/>
     </row>
     <row r="43" ht="20" customHeight="1">
       <c r="A43" s="1" t="n">
@@ -15794,6 +15921,7 @@
       <c r="DJ43" s="1" t="n"/>
       <c r="DK43" s="1" t="n"/>
       <c r="DL43" s="1" t="n"/>
+      <c r="DM43" s="1" t="n"/>
     </row>
     <row r="44" ht="20" customHeight="1">
       <c r="A44" s="1" t="n">
@@ -16144,6 +16272,9 @@
       <c r="DL44" s="1" t="n">
         <v>178.5</v>
       </c>
+      <c r="DM44" s="2" t="n">
+        <v>118.6</v>
+      </c>
     </row>
     <row r="45" ht="20" customHeight="1">
       <c r="A45" s="1" t="n">
@@ -16494,6 +16625,9 @@
       <c r="DL45" s="1" t="n">
         <v>151.5</v>
       </c>
+      <c r="DM45" s="3" t="n">
+        <v>128.8</v>
+      </c>
     </row>
     <row r="46" ht="20" customHeight="1">
       <c r="A46" s="1" t="n">
@@ -16844,6 +16978,9 @@
       <c r="DL46" s="3" t="n">
         <v>135.4</v>
       </c>
+      <c r="DM46" s="1" t="n">
+        <v>171.1</v>
+      </c>
     </row>
     <row r="47" ht="20" customHeight="1">
       <c r="A47" s="1" t="n">
@@ -17194,6 +17331,9 @@
       <c r="DL47" s="3" t="n">
         <v>135.8</v>
       </c>
+      <c r="DM47" s="1" t="n">
+        <v>164.1</v>
+      </c>
     </row>
     <row r="48" ht="20" customHeight="1">
       <c r="A48" s="1" t="n">
@@ -17544,6 +17684,9 @@
       <c r="DL48" s="1" t="n">
         <v>168.3</v>
       </c>
+      <c r="DM48" s="1" t="n">
+        <v>160.4</v>
+      </c>
     </row>
     <row r="49" ht="20" customHeight="1">
       <c r="A49" s="1" t="n">
@@ -17894,6 +18037,9 @@
       <c r="DL49" s="1" t="n">
         <v>163</v>
       </c>
+      <c r="DM49" s="1" t="n">
+        <v>195.4</v>
+      </c>
     </row>
     <row r="50" ht="20" customHeight="1">
       <c r="A50" s="1" t="n">
@@ -18244,6 +18390,9 @@
       <c r="DL50" s="1" t="n">
         <v>143.2</v>
       </c>
+      <c r="DM50" s="1" t="n">
+        <v>168.4</v>
+      </c>
     </row>
     <row r="51" ht="20" customHeight="1">
       <c r="A51" s="1" t="n">
@@ -18594,6 +18743,9 @@
       <c r="DL51" s="3" t="n">
         <v>135.2</v>
       </c>
+      <c r="DM51" s="1" t="n">
+        <v>145.3</v>
+      </c>
     </row>
     <row r="52" ht="20" customHeight="1">
       <c r="A52" s="1" t="n">
@@ -18944,6 +19096,9 @@
       <c r="DL52" s="1" t="n">
         <v>186</v>
       </c>
+      <c r="DM52" s="1" t="n">
+        <v>169.4</v>
+      </c>
     </row>
     <row r="53" ht="20" customHeight="1">
       <c r="A53" s="1" t="n">
@@ -19293,6 +19448,9 @@
       </c>
       <c r="DL53" s="1" t="n">
         <v>140.2</v>
+      </c>
+      <c r="DM53" s="1" t="n">
+        <v>188.7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2025-01-04
</commit_message>
<xml_diff>
--- a/マイジャグラーV_塗りつぶし済み.xlsx
+++ b/マイジャグラーV_塗りつぶし済み.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:DM53"/>
+  <dimension ref="A1:DN53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -556,6 +556,7 @@
     <col width="12" customWidth="1" min="115" max="115"/>
     <col width="12" customWidth="1" min="116" max="116"/>
     <col width="12" customWidth="1" min="117" max="117"/>
+    <col width="12" customWidth="1" min="118" max="118"/>
   </cols>
   <sheetData>
     <row r="1" ht="20" customHeight="1">
@@ -1144,6 +1145,11 @@
           <t>2025/01/03</t>
         </is>
       </c>
+      <c r="DN1" s="1" t="inlineStr">
+        <is>
+          <t>2025/01/04</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="20" customHeight="1">
       <c r="A2" s="1" t="n">
@@ -1497,6 +1503,9 @@
       <c r="DM2" s="3" t="n">
         <v>138.7</v>
       </c>
+      <c r="DN2" s="1" t="n">
+        <v>141.2</v>
+      </c>
     </row>
     <row r="3" ht="20" customHeight="1">
       <c r="A3" s="1" t="n">
@@ -1850,6 +1859,9 @@
       <c r="DM3" s="1" t="n">
         <v>252.5</v>
       </c>
+      <c r="DN3" s="1" t="n">
+        <v>142.3</v>
+      </c>
     </row>
     <row r="4" ht="20" customHeight="1">
       <c r="A4" s="1" t="n">
@@ -2203,6 +2215,9 @@
       <c r="DM4" s="1" t="n">
         <v>176.8</v>
       </c>
+      <c r="DN4" s="2" t="n">
+        <v>124.5</v>
+      </c>
     </row>
     <row r="5" ht="20" customHeight="1">
       <c r="A5" s="1" t="n">
@@ -2556,6 +2571,9 @@
       <c r="DM5" s="3" t="n">
         <v>137.5</v>
       </c>
+      <c r="DN5" s="1" t="n">
+        <v>295.5</v>
+      </c>
     </row>
     <row r="6" ht="20" customHeight="1">
       <c r="A6" s="1" t="n">
@@ -2909,6 +2927,9 @@
       <c r="DM6" s="1" t="n">
         <v>155.3</v>
       </c>
+      <c r="DN6" s="1" t="n">
+        <v>178.5</v>
+      </c>
     </row>
     <row r="7" ht="20" customHeight="1">
       <c r="A7" s="1" t="n">
@@ -3262,6 +3283,9 @@
       <c r="DM7" s="3" t="n">
         <v>137.9</v>
       </c>
+      <c r="DN7" s="1" t="n">
+        <v>177.5</v>
+      </c>
     </row>
     <row r="8" ht="20" customHeight="1">
       <c r="A8" s="1" t="n">
@@ -3615,6 +3639,9 @@
       <c r="DM8" s="1" t="n">
         <v>182.8</v>
       </c>
+      <c r="DN8" s="2" t="n">
+        <v>112.7</v>
+      </c>
     </row>
     <row r="9" ht="20" customHeight="1">
       <c r="A9" s="1" t="n">
@@ -3968,6 +3995,9 @@
       <c r="DM9" s="1" t="n">
         <v>162.7</v>
       </c>
+      <c r="DN9" s="1" t="n">
+        <v>218.1</v>
+      </c>
     </row>
     <row r="10" ht="20" customHeight="1">
       <c r="A10" s="1" t="n">
@@ -4321,6 +4351,9 @@
       <c r="DM10" s="1" t="n">
         <v>234.8</v>
       </c>
+      <c r="DN10" s="1" t="n">
+        <v>184.2</v>
+      </c>
     </row>
     <row r="11" ht="20" customHeight="1">
       <c r="A11" s="1" t="n">
@@ -4674,6 +4707,9 @@
       <c r="DM11" s="2" t="n">
         <v>118.8</v>
       </c>
+      <c r="DN11" s="1" t="n">
+        <v>175.2</v>
+      </c>
     </row>
     <row r="12" ht="20" customHeight="1">
       <c r="A12" s="1" t="n">
@@ -5027,6 +5063,9 @@
       <c r="DM12" s="3" t="n">
         <v>125.7</v>
       </c>
+      <c r="DN12" s="1" t="n">
+        <v>151.2</v>
+      </c>
     </row>
     <row r="13" ht="20" customHeight="1">
       <c r="A13" s="1" t="n">
@@ -5380,6 +5419,9 @@
       <c r="DM13" s="1" t="n">
         <v>156.9</v>
       </c>
+      <c r="DN13" s="1" t="n">
+        <v>160.3</v>
+      </c>
     </row>
     <row r="14" ht="20" customHeight="1">
       <c r="A14" s="1" t="n">
@@ -5733,6 +5775,9 @@
       <c r="DM14" s="2" t="n">
         <v>121.2</v>
       </c>
+      <c r="DN14" s="1" t="n">
+        <v>160</v>
+      </c>
     </row>
     <row r="15" ht="20" customHeight="1">
       <c r="A15" s="1" t="n">
@@ -6086,6 +6131,9 @@
       <c r="DM15" s="2" t="n">
         <v>115.6</v>
       </c>
+      <c r="DN15" s="1" t="n">
+        <v>175.1</v>
+      </c>
     </row>
     <row r="16" ht="20" customHeight="1">
       <c r="A16" s="1" t="n">
@@ -6439,6 +6487,9 @@
       <c r="DM16" s="1" t="n">
         <v>151.1</v>
       </c>
+      <c r="DN16" s="2" t="n">
+        <v>121.7</v>
+      </c>
     </row>
     <row r="17" ht="20" customHeight="1">
       <c r="A17" s="1" t="n">
@@ -6792,6 +6843,9 @@
       <c r="DM17" s="1" t="n">
         <v>140</v>
       </c>
+      <c r="DN17" s="1" t="n">
+        <v>160.2</v>
+      </c>
     </row>
     <row r="18" ht="20" customHeight="1">
       <c r="A18" s="1" t="n">
@@ -7145,6 +7199,9 @@
       <c r="DM18" s="3" t="n">
         <v>125.9</v>
       </c>
+      <c r="DN18" s="1" t="n">
+        <v>180</v>
+      </c>
     </row>
     <row r="19" ht="20" customHeight="1">
       <c r="A19" s="1" t="n">
@@ -7498,6 +7555,9 @@
       <c r="DM19" s="1" t="n">
         <v>141.8</v>
       </c>
+      <c r="DN19" s="1" t="n">
+        <v>170.7</v>
+      </c>
     </row>
     <row r="20" ht="20" customHeight="1">
       <c r="A20" s="1" t="n">
@@ -7851,6 +7911,9 @@
       <c r="DM20" s="1" t="n">
         <v>162.4</v>
       </c>
+      <c r="DN20" s="3" t="n">
+        <v>130.1</v>
+      </c>
     </row>
     <row r="21" ht="20" customHeight="1">
       <c r="A21" s="1" t="n">
@@ -8204,6 +8267,9 @@
       <c r="DM21" s="1" t="n">
         <v>159.2</v>
       </c>
+      <c r="DN21" s="1" t="n">
+        <v>165.2</v>
+      </c>
     </row>
     <row r="22" ht="20" customHeight="1">
       <c r="A22" s="1" t="n">
@@ -8557,6 +8623,9 @@
       <c r="DM22" s="1" t="n">
         <v>191.2</v>
       </c>
+      <c r="DN22" s="1" t="n">
+        <v>210</v>
+      </c>
     </row>
     <row r="23" ht="20" customHeight="1">
       <c r="A23" s="1" t="n">
@@ -8910,6 +8979,9 @@
       <c r="DM23" s="1" t="n">
         <v>141.3</v>
       </c>
+      <c r="DN23" s="1" t="n">
+        <v>149.3</v>
+      </c>
     </row>
     <row r="24" ht="20" customHeight="1">
       <c r="A24" s="1" t="n">
@@ -9263,6 +9335,9 @@
       <c r="DM24" s="3" t="n">
         <v>131.5</v>
       </c>
+      <c r="DN24" s="2" t="n">
+        <v>120.8</v>
+      </c>
     </row>
     <row r="25" ht="20" customHeight="1">
       <c r="A25" s="1" t="n">
@@ -9616,6 +9691,9 @@
       <c r="DM25" s="1" t="n">
         <v>197.5</v>
       </c>
+      <c r="DN25" s="1" t="n">
+        <v>175.3</v>
+      </c>
     </row>
     <row r="26" ht="20" customHeight="1">
       <c r="A26" s="1" t="n">
@@ -9969,6 +10047,9 @@
       <c r="DM26" s="2" t="n">
         <v>123.7</v>
       </c>
+      <c r="DN26" s="1" t="n">
+        <v>174.9</v>
+      </c>
     </row>
     <row r="27" ht="20" customHeight="1">
       <c r="A27" s="1" t="n">
@@ -10322,6 +10403,9 @@
       <c r="DM27" s="1" t="n">
         <v>169.8</v>
       </c>
+      <c r="DN27" s="1" t="n">
+        <v>157.6</v>
+      </c>
     </row>
     <row r="28" ht="20" customHeight="1">
       <c r="A28" s="1" t="n">
@@ -10675,6 +10759,9 @@
       <c r="DM28" s="1" t="n">
         <v>242</v>
       </c>
+      <c r="DN28" s="1" t="n">
+        <v>181.9</v>
+      </c>
     </row>
     <row r="29" ht="20" customHeight="1">
       <c r="A29" s="1" t="n">
@@ -11028,6 +11115,9 @@
       <c r="DM29" s="1" t="n">
         <v>171.5</v>
       </c>
+      <c r="DN29" s="3" t="n">
+        <v>126.5</v>
+      </c>
     </row>
     <row r="30" ht="20" customHeight="1">
       <c r="A30" s="1" t="n">
@@ -11381,6 +11471,9 @@
       <c r="DM30" s="3" t="n">
         <v>137.9</v>
       </c>
+      <c r="DN30" s="3" t="n">
+        <v>132.4</v>
+      </c>
     </row>
     <row r="31" ht="20" customHeight="1">
       <c r="A31" s="1" t="n">
@@ -11734,6 +11827,9 @@
       <c r="DM31" s="1" t="n">
         <v>180.3</v>
       </c>
+      <c r="DN31" s="1" t="n">
+        <v>159.4</v>
+      </c>
     </row>
     <row r="32" ht="20" customHeight="1">
       <c r="A32" s="1" t="n">
@@ -12087,6 +12183,9 @@
       <c r="DM32" s="1" t="n">
         <v>166.2</v>
       </c>
+      <c r="DN32" s="3" t="n">
+        <v>137.6</v>
+      </c>
     </row>
     <row r="33" ht="20" customHeight="1">
       <c r="A33" s="1" t="n">
@@ -12440,6 +12539,9 @@
       <c r="DM33" s="1" t="n">
         <v>245.7</v>
       </c>
+      <c r="DN33" s="1" t="n">
+        <v>222.6</v>
+      </c>
     </row>
     <row r="34" ht="20" customHeight="1">
       <c r="A34" s="1" t="n">
@@ -12793,6 +12895,9 @@
       <c r="DM34" s="1" t="n">
         <v>155.8</v>
       </c>
+      <c r="DN34" s="1" t="n">
+        <v>182.8</v>
+      </c>
     </row>
     <row r="35" ht="20" customHeight="1">
       <c r="A35" s="1" t="n">
@@ -13146,6 +13251,9 @@
       <c r="DM35" s="1" t="n">
         <v>157.5</v>
       </c>
+      <c r="DN35" s="1" t="n">
+        <v>158.6</v>
+      </c>
     </row>
     <row r="36" ht="20" customHeight="1">
       <c r="A36" s="1" t="n">
@@ -13499,6 +13607,9 @@
       <c r="DM36" s="1" t="n">
         <v>189.5</v>
       </c>
+      <c r="DN36" s="1" t="n">
+        <v>150.4</v>
+      </c>
     </row>
     <row r="37" ht="20" customHeight="1">
       <c r="A37" s="1" t="n">
@@ -13852,6 +13963,9 @@
       <c r="DM37" s="3" t="n">
         <v>135.4</v>
       </c>
+      <c r="DN37" s="1" t="n">
+        <v>158.3</v>
+      </c>
     </row>
     <row r="38" ht="20" customHeight="1">
       <c r="A38" s="1" t="n">
@@ -14205,6 +14319,9 @@
       <c r="DM38" s="2" t="n">
         <v>118.5</v>
       </c>
+      <c r="DN38" s="3" t="n">
+        <v>138.5</v>
+      </c>
     </row>
     <row r="39" ht="20" customHeight="1">
       <c r="A39" s="1" t="n">
@@ -14558,6 +14675,9 @@
       <c r="DM39" s="3" t="n">
         <v>134.8</v>
       </c>
+      <c r="DN39" s="1" t="n">
+        <v>189.4</v>
+      </c>
     </row>
     <row r="40" ht="20" customHeight="1">
       <c r="A40" s="1" t="n">
@@ -14911,6 +15031,9 @@
       <c r="DM40" s="3" t="n">
         <v>126</v>
       </c>
+      <c r="DN40" s="1" t="n">
+        <v>186.5</v>
+      </c>
     </row>
     <row r="41" ht="20" customHeight="1">
       <c r="A41" s="1" t="n">
@@ -15263,6 +15386,9 @@
       </c>
       <c r="DM41" s="3" t="n">
         <v>136.3</v>
+      </c>
+      <c r="DN41" s="1" t="n">
+        <v>151.3</v>
       </c>
     </row>
     <row r="42" ht="20" customHeight="1">
@@ -15593,6 +15719,7 @@
       <c r="DK42" s="1" t="n"/>
       <c r="DL42" s="1" t="n"/>
       <c r="DM42" s="1" t="n"/>
+      <c r="DN42" s="1" t="n"/>
     </row>
     <row r="43" ht="20" customHeight="1">
       <c r="A43" s="1" t="n">
@@ -15922,6 +16049,7 @@
       <c r="DK43" s="1" t="n"/>
       <c r="DL43" s="1" t="n"/>
       <c r="DM43" s="1" t="n"/>
+      <c r="DN43" s="1" t="n"/>
     </row>
     <row r="44" ht="20" customHeight="1">
       <c r="A44" s="1" t="n">
@@ -16275,6 +16403,9 @@
       <c r="DM44" s="2" t="n">
         <v>118.6</v>
       </c>
+      <c r="DN44" s="1" t="n">
+        <v>153.9</v>
+      </c>
     </row>
     <row r="45" ht="20" customHeight="1">
       <c r="A45" s="1" t="n">
@@ -16628,6 +16759,9 @@
       <c r="DM45" s="3" t="n">
         <v>128.8</v>
       </c>
+      <c r="DN45" s="1" t="n">
+        <v>203.1</v>
+      </c>
     </row>
     <row r="46" ht="20" customHeight="1">
       <c r="A46" s="1" t="n">
@@ -16981,6 +17115,9 @@
       <c r="DM46" s="1" t="n">
         <v>171.1</v>
       </c>
+      <c r="DN46" s="1" t="n">
+        <v>150.2</v>
+      </c>
     </row>
     <row r="47" ht="20" customHeight="1">
       <c r="A47" s="1" t="n">
@@ -17334,6 +17471,9 @@
       <c r="DM47" s="1" t="n">
         <v>164.1</v>
       </c>
+      <c r="DN47" s="1" t="n">
+        <v>142.9</v>
+      </c>
     </row>
     <row r="48" ht="20" customHeight="1">
       <c r="A48" s="1" t="n">
@@ -17687,6 +17827,9 @@
       <c r="DM48" s="1" t="n">
         <v>160.4</v>
       </c>
+      <c r="DN48" s="3" t="n">
+        <v>131.9</v>
+      </c>
     </row>
     <row r="49" ht="20" customHeight="1">
       <c r="A49" s="1" t="n">
@@ -18040,6 +18183,9 @@
       <c r="DM49" s="1" t="n">
         <v>195.4</v>
       </c>
+      <c r="DN49" s="1" t="n">
+        <v>146.4</v>
+      </c>
     </row>
     <row r="50" ht="20" customHeight="1">
       <c r="A50" s="1" t="n">
@@ -18393,6 +18539,9 @@
       <c r="DM50" s="1" t="n">
         <v>168.4</v>
       </c>
+      <c r="DN50" s="1" t="n">
+        <v>159.1</v>
+      </c>
     </row>
     <row r="51" ht="20" customHeight="1">
       <c r="A51" s="1" t="n">
@@ -18746,6 +18895,9 @@
       <c r="DM51" s="1" t="n">
         <v>145.3</v>
       </c>
+      <c r="DN51" s="1" t="n">
+        <v>143.7</v>
+      </c>
     </row>
     <row r="52" ht="20" customHeight="1">
       <c r="A52" s="1" t="n">
@@ -19099,6 +19251,9 @@
       <c r="DM52" s="1" t="n">
         <v>169.4</v>
       </c>
+      <c r="DN52" s="1" t="n">
+        <v>169.7</v>
+      </c>
     </row>
     <row r="53" ht="20" customHeight="1">
       <c r="A53" s="1" t="n">
@@ -19451,6 +19606,9 @@
       </c>
       <c r="DM53" s="1" t="n">
         <v>188.7</v>
+      </c>
+      <c r="DN53" s="2" t="n">
+        <v>120.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2025-01-05
</commit_message>
<xml_diff>
--- a/マイジャグラーV_塗りつぶし済み.xlsx
+++ b/マイジャグラーV_塗りつぶし済み.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:DN53"/>
+  <dimension ref="A1:DO53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -557,6 +557,7 @@
     <col width="12" customWidth="1" min="116" max="116"/>
     <col width="12" customWidth="1" min="117" max="117"/>
     <col width="12" customWidth="1" min="118" max="118"/>
+    <col width="12" customWidth="1" min="119" max="119"/>
   </cols>
   <sheetData>
     <row r="1" ht="20" customHeight="1">
@@ -1150,6 +1151,11 @@
           <t>2025/01/04</t>
         </is>
       </c>
+      <c r="DO1" s="1" t="inlineStr">
+        <is>
+          <t>2025/01/05</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="20" customHeight="1">
       <c r="A2" s="1" t="n">
@@ -1506,6 +1512,9 @@
       <c r="DN2" s="1" t="n">
         <v>141.2</v>
       </c>
+      <c r="DO2" s="1" t="n">
+        <v>169.8</v>
+      </c>
     </row>
     <row r="3" ht="20" customHeight="1">
       <c r="A3" s="1" t="n">
@@ -1862,6 +1871,9 @@
       <c r="DN3" s="1" t="n">
         <v>142.3</v>
       </c>
+      <c r="DO3" s="1" t="n">
+        <v>154.6</v>
+      </c>
     </row>
     <row r="4" ht="20" customHeight="1">
       <c r="A4" s="1" t="n">
@@ -2218,6 +2230,9 @@
       <c r="DN4" s="2" t="n">
         <v>124.5</v>
       </c>
+      <c r="DO4" s="1" t="n">
+        <v>197.2</v>
+      </c>
     </row>
     <row r="5" ht="20" customHeight="1">
       <c r="A5" s="1" t="n">
@@ -2574,6 +2589,9 @@
       <c r="DN5" s="1" t="n">
         <v>295.5</v>
       </c>
+      <c r="DO5" s="1" t="n">
+        <v>149</v>
+      </c>
     </row>
     <row r="6" ht="20" customHeight="1">
       <c r="A6" s="1" t="n">
@@ -2930,6 +2948,9 @@
       <c r="DN6" s="1" t="n">
         <v>178.5</v>
       </c>
+      <c r="DO6" s="1" t="n">
+        <v>150.4</v>
+      </c>
     </row>
     <row r="7" ht="20" customHeight="1">
       <c r="A7" s="1" t="n">
@@ -3286,6 +3307,9 @@
       <c r="DN7" s="1" t="n">
         <v>177.5</v>
       </c>
+      <c r="DO7" s="3" t="n">
+        <v>127.3</v>
+      </c>
     </row>
     <row r="8" ht="20" customHeight="1">
       <c r="A8" s="1" t="n">
@@ -3642,6 +3666,9 @@
       <c r="DN8" s="2" t="n">
         <v>112.7</v>
       </c>
+      <c r="DO8" s="1" t="n">
+        <v>143.6</v>
+      </c>
     </row>
     <row r="9" ht="20" customHeight="1">
       <c r="A9" s="1" t="n">
@@ -3998,6 +4025,9 @@
       <c r="DN9" s="1" t="n">
         <v>218.1</v>
       </c>
+      <c r="DO9" s="3" t="n">
+        <v>135.8</v>
+      </c>
     </row>
     <row r="10" ht="20" customHeight="1">
       <c r="A10" s="1" t="n">
@@ -4354,6 +4384,9 @@
       <c r="DN10" s="1" t="n">
         <v>184.2</v>
       </c>
+      <c r="DO10" s="2" t="n">
+        <v>114</v>
+      </c>
     </row>
     <row r="11" ht="20" customHeight="1">
       <c r="A11" s="1" t="n">
@@ -4710,6 +4743,9 @@
       <c r="DN11" s="1" t="n">
         <v>175.2</v>
       </c>
+      <c r="DO11" s="1" t="n">
+        <v>230.1</v>
+      </c>
     </row>
     <row r="12" ht="20" customHeight="1">
       <c r="A12" s="1" t="n">
@@ -5066,6 +5102,9 @@
       <c r="DN12" s="1" t="n">
         <v>151.2</v>
       </c>
+      <c r="DO12" s="1" t="n">
+        <v>149.2</v>
+      </c>
     </row>
     <row r="13" ht="20" customHeight="1">
       <c r="A13" s="1" t="n">
@@ -5422,6 +5461,9 @@
       <c r="DN13" s="1" t="n">
         <v>160.3</v>
       </c>
+      <c r="DO13" s="1" t="n">
+        <v>142.5</v>
+      </c>
     </row>
     <row r="14" ht="20" customHeight="1">
       <c r="A14" s="1" t="n">
@@ -5778,6 +5820,9 @@
       <c r="DN14" s="1" t="n">
         <v>160</v>
       </c>
+      <c r="DO14" s="1" t="n">
+        <v>144.9</v>
+      </c>
     </row>
     <row r="15" ht="20" customHeight="1">
       <c r="A15" s="1" t="n">
@@ -6134,6 +6179,9 @@
       <c r="DN15" s="1" t="n">
         <v>175.1</v>
       </c>
+      <c r="DO15" s="2" t="n">
+        <v>122.2</v>
+      </c>
     </row>
     <row r="16" ht="20" customHeight="1">
       <c r="A16" s="1" t="n">
@@ -6490,6 +6538,9 @@
       <c r="DN16" s="2" t="n">
         <v>121.7</v>
       </c>
+      <c r="DO16" s="1" t="n">
+        <v>161.1</v>
+      </c>
     </row>
     <row r="17" ht="20" customHeight="1">
       <c r="A17" s="1" t="n">
@@ -6846,6 +6897,9 @@
       <c r="DN17" s="1" t="n">
         <v>160.2</v>
       </c>
+      <c r="DO17" s="1" t="n">
+        <v>146.7</v>
+      </c>
     </row>
     <row r="18" ht="20" customHeight="1">
       <c r="A18" s="1" t="n">
@@ -7202,6 +7256,9 @@
       <c r="DN18" s="1" t="n">
         <v>180</v>
       </c>
+      <c r="DO18" s="2" t="n">
+        <v>105.6</v>
+      </c>
     </row>
     <row r="19" ht="20" customHeight="1">
       <c r="A19" s="1" t="n">
@@ -7558,6 +7615,9 @@
       <c r="DN19" s="1" t="n">
         <v>170.7</v>
       </c>
+      <c r="DO19" s="1" t="n">
+        <v>179.8</v>
+      </c>
     </row>
     <row r="20" ht="20" customHeight="1">
       <c r="A20" s="1" t="n">
@@ -7914,6 +7974,9 @@
       <c r="DN20" s="3" t="n">
         <v>130.1</v>
       </c>
+      <c r="DO20" s="1" t="n">
+        <v>157.2</v>
+      </c>
     </row>
     <row r="21" ht="20" customHeight="1">
       <c r="A21" s="1" t="n">
@@ -8270,6 +8333,9 @@
       <c r="DN21" s="1" t="n">
         <v>165.2</v>
       </c>
+      <c r="DO21" s="2" t="n">
+        <v>118.4</v>
+      </c>
     </row>
     <row r="22" ht="20" customHeight="1">
       <c r="A22" s="1" t="n">
@@ -8626,6 +8692,9 @@
       <c r="DN22" s="1" t="n">
         <v>210</v>
       </c>
+      <c r="DO22" s="1" t="n">
+        <v>141.4</v>
+      </c>
     </row>
     <row r="23" ht="20" customHeight="1">
       <c r="A23" s="1" t="n">
@@ -8982,6 +9051,9 @@
       <c r="DN23" s="1" t="n">
         <v>149.3</v>
       </c>
+      <c r="DO23" s="1" t="n">
+        <v>189.7</v>
+      </c>
     </row>
     <row r="24" ht="20" customHeight="1">
       <c r="A24" s="1" t="n">
@@ -9338,6 +9410,9 @@
       <c r="DN24" s="2" t="n">
         <v>120.8</v>
       </c>
+      <c r="DO24" s="3" t="n">
+        <v>131.6</v>
+      </c>
     </row>
     <row r="25" ht="20" customHeight="1">
       <c r="A25" s="1" t="n">
@@ -9694,6 +9769,9 @@
       <c r="DN25" s="1" t="n">
         <v>175.3</v>
       </c>
+      <c r="DO25" s="1" t="n">
+        <v>165.1</v>
+      </c>
     </row>
     <row r="26" ht="20" customHeight="1">
       <c r="A26" s="1" t="n">
@@ -10050,6 +10128,9 @@
       <c r="DN26" s="1" t="n">
         <v>174.9</v>
       </c>
+      <c r="DO26" s="2" t="n">
+        <v>117.8</v>
+      </c>
     </row>
     <row r="27" ht="20" customHeight="1">
       <c r="A27" s="1" t="n">
@@ -10406,6 +10487,9 @@
       <c r="DN27" s="1" t="n">
         <v>157.6</v>
       </c>
+      <c r="DO27" s="1" t="n">
+        <v>204.3</v>
+      </c>
     </row>
     <row r="28" ht="20" customHeight="1">
       <c r="A28" s="1" t="n">
@@ -10762,6 +10846,9 @@
       <c r="DN28" s="1" t="n">
         <v>181.9</v>
       </c>
+      <c r="DO28" s="3" t="n">
+        <v>131.7</v>
+      </c>
     </row>
     <row r="29" ht="20" customHeight="1">
       <c r="A29" s="1" t="n">
@@ -11118,6 +11205,9 @@
       <c r="DN29" s="3" t="n">
         <v>126.5</v>
       </c>
+      <c r="DO29" s="1" t="n">
+        <v>162.3</v>
+      </c>
     </row>
     <row r="30" ht="20" customHeight="1">
       <c r="A30" s="1" t="n">
@@ -11474,6 +11564,9 @@
       <c r="DN30" s="3" t="n">
         <v>132.4</v>
       </c>
+      <c r="DO30" s="3" t="n">
+        <v>132.6</v>
+      </c>
     </row>
     <row r="31" ht="20" customHeight="1">
       <c r="A31" s="1" t="n">
@@ -11830,6 +11923,9 @@
       <c r="DN31" s="1" t="n">
         <v>159.4</v>
       </c>
+      <c r="DO31" s="1" t="n">
+        <v>205.2</v>
+      </c>
     </row>
     <row r="32" ht="20" customHeight="1">
       <c r="A32" s="1" t="n">
@@ -12186,6 +12282,9 @@
       <c r="DN32" s="3" t="n">
         <v>137.6</v>
       </c>
+      <c r="DO32" s="1" t="n">
+        <v>195.8</v>
+      </c>
     </row>
     <row r="33" ht="20" customHeight="1">
       <c r="A33" s="1" t="n">
@@ -12542,6 +12641,9 @@
       <c r="DN33" s="1" t="n">
         <v>222.6</v>
       </c>
+      <c r="DO33" s="2" t="n">
+        <v>121.3</v>
+      </c>
     </row>
     <row r="34" ht="20" customHeight="1">
       <c r="A34" s="1" t="n">
@@ -12898,6 +13000,9 @@
       <c r="DN34" s="1" t="n">
         <v>182.8</v>
       </c>
+      <c r="DO34" s="1" t="n">
+        <v>144.7</v>
+      </c>
     </row>
     <row r="35" ht="20" customHeight="1">
       <c r="A35" s="1" t="n">
@@ -13254,6 +13359,9 @@
       <c r="DN35" s="1" t="n">
         <v>158.6</v>
       </c>
+      <c r="DO35" s="1" t="n">
+        <v>187.5</v>
+      </c>
     </row>
     <row r="36" ht="20" customHeight="1">
       <c r="A36" s="1" t="n">
@@ -13610,6 +13718,9 @@
       <c r="DN36" s="1" t="n">
         <v>150.4</v>
       </c>
+      <c r="DO36" s="1" t="n">
+        <v>171.8</v>
+      </c>
     </row>
     <row r="37" ht="20" customHeight="1">
       <c r="A37" s="1" t="n">
@@ -13966,6 +14077,9 @@
       <c r="DN37" s="1" t="n">
         <v>158.3</v>
       </c>
+      <c r="DO37" s="1" t="n">
+        <v>179.9</v>
+      </c>
     </row>
     <row r="38" ht="20" customHeight="1">
       <c r="A38" s="1" t="n">
@@ -14322,6 +14436,9 @@
       <c r="DN38" s="3" t="n">
         <v>138.5</v>
       </c>
+      <c r="DO38" s="1" t="n">
+        <v>179.6</v>
+      </c>
     </row>
     <row r="39" ht="20" customHeight="1">
       <c r="A39" s="1" t="n">
@@ -14678,6 +14795,9 @@
       <c r="DN39" s="1" t="n">
         <v>189.4</v>
       </c>
+      <c r="DO39" s="3" t="n">
+        <v>125.3</v>
+      </c>
     </row>
     <row r="40" ht="20" customHeight="1">
       <c r="A40" s="1" t="n">
@@ -15034,6 +15154,9 @@
       <c r="DN40" s="1" t="n">
         <v>186.5</v>
       </c>
+      <c r="DO40" s="1" t="n">
+        <v>155</v>
+      </c>
     </row>
     <row r="41" ht="20" customHeight="1">
       <c r="A41" s="1" t="n">
@@ -15389,6 +15512,9 @@
       </c>
       <c r="DN41" s="1" t="n">
         <v>151.3</v>
+      </c>
+      <c r="DO41" s="3" t="n">
+        <v>132.3</v>
       </c>
     </row>
     <row r="42" ht="20" customHeight="1">
@@ -15720,6 +15846,7 @@
       <c r="DL42" s="1" t="n"/>
       <c r="DM42" s="1" t="n"/>
       <c r="DN42" s="1" t="n"/>
+      <c r="DO42" s="1" t="n"/>
     </row>
     <row r="43" ht="20" customHeight="1">
       <c r="A43" s="1" t="n">
@@ -16050,6 +16177,7 @@
       <c r="DL43" s="1" t="n"/>
       <c r="DM43" s="1" t="n"/>
       <c r="DN43" s="1" t="n"/>
+      <c r="DO43" s="1" t="n"/>
     </row>
     <row r="44" ht="20" customHeight="1">
       <c r="A44" s="1" t="n">
@@ -16406,6 +16534,9 @@
       <c r="DN44" s="1" t="n">
         <v>153.9</v>
       </c>
+      <c r="DO44" s="3" t="n">
+        <v>133.2</v>
+      </c>
     </row>
     <row r="45" ht="20" customHeight="1">
       <c r="A45" s="1" t="n">
@@ -16762,6 +16893,9 @@
       <c r="DN45" s="1" t="n">
         <v>203.1</v>
       </c>
+      <c r="DO45" s="1" t="n">
+        <v>212.1</v>
+      </c>
     </row>
     <row r="46" ht="20" customHeight="1">
       <c r="A46" s="1" t="n">
@@ -17118,6 +17252,9 @@
       <c r="DN46" s="1" t="n">
         <v>150.2</v>
       </c>
+      <c r="DO46" s="1" t="n">
+        <v>145.4</v>
+      </c>
     </row>
     <row r="47" ht="20" customHeight="1">
       <c r="A47" s="1" t="n">
@@ -17474,6 +17611,9 @@
       <c r="DN47" s="1" t="n">
         <v>142.9</v>
       </c>
+      <c r="DO47" s="1" t="n">
+        <v>166.5</v>
+      </c>
     </row>
     <row r="48" ht="20" customHeight="1">
       <c r="A48" s="1" t="n">
@@ -17830,6 +17970,9 @@
       <c r="DN48" s="3" t="n">
         <v>131.9</v>
       </c>
+      <c r="DO48" s="1" t="n">
+        <v>150.7</v>
+      </c>
     </row>
     <row r="49" ht="20" customHeight="1">
       <c r="A49" s="1" t="n">
@@ -18186,6 +18329,9 @@
       <c r="DN49" s="1" t="n">
         <v>146.4</v>
       </c>
+      <c r="DO49" s="3" t="n">
+        <v>134.4</v>
+      </c>
     </row>
     <row r="50" ht="20" customHeight="1">
       <c r="A50" s="1" t="n">
@@ -18542,6 +18688,9 @@
       <c r="DN50" s="1" t="n">
         <v>159.1</v>
       </c>
+      <c r="DO50" s="1" t="n">
+        <v>166.2</v>
+      </c>
     </row>
     <row r="51" ht="20" customHeight="1">
       <c r="A51" s="1" t="n">
@@ -18898,6 +19047,9 @@
       <c r="DN51" s="1" t="n">
         <v>143.7</v>
       </c>
+      <c r="DO51" s="3" t="n">
+        <v>132.1</v>
+      </c>
     </row>
     <row r="52" ht="20" customHeight="1">
       <c r="A52" s="1" t="n">
@@ -19254,6 +19406,9 @@
       <c r="DN52" s="1" t="n">
         <v>169.7</v>
       </c>
+      <c r="DO52" s="3" t="n">
+        <v>126.6</v>
+      </c>
     </row>
     <row r="53" ht="20" customHeight="1">
       <c r="A53" s="1" t="n">
@@ -19609,6 +19764,9 @@
       </c>
       <c r="DN53" s="2" t="n">
         <v>120.2</v>
+      </c>
+      <c r="DO53" s="2" t="n">
+        <v>121.7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2025-01-06
</commit_message>
<xml_diff>
--- a/マイジャグラーV_塗りつぶし済み.xlsx
+++ b/マイジャグラーV_塗りつぶし済み.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:DO53"/>
+  <dimension ref="A1:DP53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -558,6 +558,7 @@
     <col width="12" customWidth="1" min="117" max="117"/>
     <col width="12" customWidth="1" min="118" max="118"/>
     <col width="12" customWidth="1" min="119" max="119"/>
+    <col width="12" customWidth="1" min="120" max="120"/>
   </cols>
   <sheetData>
     <row r="1" ht="20" customHeight="1">
@@ -1156,6 +1157,11 @@
           <t>2025/01/05</t>
         </is>
       </c>
+      <c r="DP1" s="1" t="inlineStr">
+        <is>
+          <t>2025/01/06</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="20" customHeight="1">
       <c r="A2" s="1" t="n">
@@ -1515,6 +1521,9 @@
       <c r="DO2" s="1" t="n">
         <v>169.8</v>
       </c>
+      <c r="DP2" s="2" t="n">
+        <v>121.3</v>
+      </c>
     </row>
     <row r="3" ht="20" customHeight="1">
       <c r="A3" s="1" t="n">
@@ -1874,6 +1883,9 @@
       <c r="DO3" s="1" t="n">
         <v>154.6</v>
       </c>
+      <c r="DP3" s="1" t="n">
+        <v>166.6</v>
+      </c>
     </row>
     <row r="4" ht="20" customHeight="1">
       <c r="A4" s="1" t="n">
@@ -2233,6 +2245,9 @@
       <c r="DO4" s="1" t="n">
         <v>197.2</v>
       </c>
+      <c r="DP4" s="1" t="n">
+        <v>144.1</v>
+      </c>
     </row>
     <row r="5" ht="20" customHeight="1">
       <c r="A5" s="1" t="n">
@@ -2592,6 +2607,9 @@
       <c r="DO5" s="1" t="n">
         <v>149</v>
       </c>
+      <c r="DP5" s="1" t="n">
+        <v>173.5</v>
+      </c>
     </row>
     <row r="6" ht="20" customHeight="1">
       <c r="A6" s="1" t="n">
@@ -2951,6 +2969,9 @@
       <c r="DO6" s="1" t="n">
         <v>150.4</v>
       </c>
+      <c r="DP6" s="1" t="n">
+        <v>152.7</v>
+      </c>
     </row>
     <row r="7" ht="20" customHeight="1">
       <c r="A7" s="1" t="n">
@@ -3310,6 +3331,9 @@
       <c r="DO7" s="3" t="n">
         <v>127.3</v>
       </c>
+      <c r="DP7" s="1" t="n">
+        <v>159.5</v>
+      </c>
     </row>
     <row r="8" ht="20" customHeight="1">
       <c r="A8" s="1" t="n">
@@ -3669,6 +3693,9 @@
       <c r="DO8" s="1" t="n">
         <v>143.6</v>
       </c>
+      <c r="DP8" s="1" t="n">
+        <v>311.9</v>
+      </c>
     </row>
     <row r="9" ht="20" customHeight="1">
       <c r="A9" s="1" t="n">
@@ -4028,6 +4055,9 @@
       <c r="DO9" s="3" t="n">
         <v>135.8</v>
       </c>
+      <c r="DP9" s="3" t="n">
+        <v>135.6</v>
+      </c>
     </row>
     <row r="10" ht="20" customHeight="1">
       <c r="A10" s="1" t="n">
@@ -4387,6 +4417,9 @@
       <c r="DO10" s="2" t="n">
         <v>114</v>
       </c>
+      <c r="DP10" s="1" t="n">
+        <v>198.4</v>
+      </c>
     </row>
     <row r="11" ht="20" customHeight="1">
       <c r="A11" s="1" t="n">
@@ -4746,6 +4779,9 @@
       <c r="DO11" s="1" t="n">
         <v>230.1</v>
       </c>
+      <c r="DP11" s="1" t="n">
+        <v>247.8</v>
+      </c>
     </row>
     <row r="12" ht="20" customHeight="1">
       <c r="A12" s="1" t="n">
@@ -5105,6 +5141,9 @@
       <c r="DO12" s="1" t="n">
         <v>149.2</v>
       </c>
+      <c r="DP12" s="1" t="n">
+        <v>209</v>
+      </c>
     </row>
     <row r="13" ht="20" customHeight="1">
       <c r="A13" s="1" t="n">
@@ -5464,6 +5503,9 @@
       <c r="DO13" s="1" t="n">
         <v>142.5</v>
       </c>
+      <c r="DP13" s="3" t="n">
+        <v>139.2</v>
+      </c>
     </row>
     <row r="14" ht="20" customHeight="1">
       <c r="A14" s="1" t="n">
@@ -5823,6 +5865,9 @@
       <c r="DO14" s="1" t="n">
         <v>144.9</v>
       </c>
+      <c r="DP14" s="1" t="n">
+        <v>146.4</v>
+      </c>
     </row>
     <row r="15" ht="20" customHeight="1">
       <c r="A15" s="1" t="n">
@@ -6182,6 +6227,9 @@
       <c r="DO15" s="2" t="n">
         <v>122.2</v>
       </c>
+      <c r="DP15" s="1" t="n">
+        <v>189.4</v>
+      </c>
     </row>
     <row r="16" ht="20" customHeight="1">
       <c r="A16" s="1" t="n">
@@ -6541,6 +6589,9 @@
       <c r="DO16" s="1" t="n">
         <v>161.1</v>
       </c>
+      <c r="DP16" s="1" t="n">
+        <v>165.6</v>
+      </c>
     </row>
     <row r="17" ht="20" customHeight="1">
       <c r="A17" s="1" t="n">
@@ -6900,6 +6951,9 @@
       <c r="DO17" s="1" t="n">
         <v>146.7</v>
       </c>
+      <c r="DP17" s="1" t="n">
+        <v>142</v>
+      </c>
     </row>
     <row r="18" ht="20" customHeight="1">
       <c r="A18" s="1" t="n">
@@ -7259,6 +7313,9 @@
       <c r="DO18" s="2" t="n">
         <v>105.6</v>
       </c>
+      <c r="DP18" s="1" t="n">
+        <v>158.4</v>
+      </c>
     </row>
     <row r="19" ht="20" customHeight="1">
       <c r="A19" s="1" t="n">
@@ -7618,6 +7675,9 @@
       <c r="DO19" s="1" t="n">
         <v>179.8</v>
       </c>
+      <c r="DP19" s="3" t="n">
+        <v>131.5</v>
+      </c>
     </row>
     <row r="20" ht="20" customHeight="1">
       <c r="A20" s="1" t="n">
@@ -7977,6 +8037,9 @@
       <c r="DO20" s="1" t="n">
         <v>157.2</v>
       </c>
+      <c r="DP20" s="1" t="n">
+        <v>308.5</v>
+      </c>
     </row>
     <row r="21" ht="20" customHeight="1">
       <c r="A21" s="1" t="n">
@@ -8336,6 +8399,9 @@
       <c r="DO21" s="2" t="n">
         <v>118.4</v>
       </c>
+      <c r="DP21" s="1" t="n">
+        <v>198.8</v>
+      </c>
     </row>
     <row r="22" ht="20" customHeight="1">
       <c r="A22" s="1" t="n">
@@ -8695,6 +8761,9 @@
       <c r="DO22" s="1" t="n">
         <v>141.4</v>
       </c>
+      <c r="DP22" s="1" t="n">
+        <v>149</v>
+      </c>
     </row>
     <row r="23" ht="20" customHeight="1">
       <c r="A23" s="1" t="n">
@@ -9054,6 +9123,9 @@
       <c r="DO23" s="1" t="n">
         <v>189.7</v>
       </c>
+      <c r="DP23" s="3" t="n">
+        <v>131.7</v>
+      </c>
     </row>
     <row r="24" ht="20" customHeight="1">
       <c r="A24" s="1" t="n">
@@ -9413,6 +9485,9 @@
       <c r="DO24" s="3" t="n">
         <v>131.6</v>
       </c>
+      <c r="DP24" s="1" t="n">
+        <v>180.7</v>
+      </c>
     </row>
     <row r="25" ht="20" customHeight="1">
       <c r="A25" s="1" t="n">
@@ -9772,6 +9847,9 @@
       <c r="DO25" s="1" t="n">
         <v>165.1</v>
       </c>
+      <c r="DP25" s="1" t="n">
+        <v>154.4</v>
+      </c>
     </row>
     <row r="26" ht="20" customHeight="1">
       <c r="A26" s="1" t="n">
@@ -10131,6 +10209,9 @@
       <c r="DO26" s="2" t="n">
         <v>117.8</v>
       </c>
+      <c r="DP26" s="3" t="n">
+        <v>137.6</v>
+      </c>
     </row>
     <row r="27" ht="20" customHeight="1">
       <c r="A27" s="1" t="n">
@@ -10490,6 +10571,9 @@
       <c r="DO27" s="1" t="n">
         <v>204.3</v>
       </c>
+      <c r="DP27" s="1" t="n">
+        <v>284.4</v>
+      </c>
     </row>
     <row r="28" ht="20" customHeight="1">
       <c r="A28" s="1" t="n">
@@ -10849,6 +10933,9 @@
       <c r="DO28" s="3" t="n">
         <v>131.7</v>
       </c>
+      <c r="DP28" s="3" t="n">
+        <v>131.2</v>
+      </c>
     </row>
     <row r="29" ht="20" customHeight="1">
       <c r="A29" s="1" t="n">
@@ -11208,6 +11295,9 @@
       <c r="DO29" s="1" t="n">
         <v>162.3</v>
       </c>
+      <c r="DP29" s="1" t="n">
+        <v>186.3</v>
+      </c>
     </row>
     <row r="30" ht="20" customHeight="1">
       <c r="A30" s="1" t="n">
@@ -11567,6 +11657,9 @@
       <c r="DO30" s="3" t="n">
         <v>132.6</v>
       </c>
+      <c r="DP30" s="1" t="n">
+        <v>440.8</v>
+      </c>
     </row>
     <row r="31" ht="20" customHeight="1">
       <c r="A31" s="1" t="n">
@@ -11926,6 +12019,9 @@
       <c r="DO31" s="1" t="n">
         <v>205.2</v>
       </c>
+      <c r="DP31" s="3" t="n">
+        <v>128.1</v>
+      </c>
     </row>
     <row r="32" ht="20" customHeight="1">
       <c r="A32" s="1" t="n">
@@ -12285,6 +12381,9 @@
       <c r="DO32" s="1" t="n">
         <v>195.8</v>
       </c>
+      <c r="DP32" s="1" t="n">
+        <v>166.4</v>
+      </c>
     </row>
     <row r="33" ht="20" customHeight="1">
       <c r="A33" s="1" t="n">
@@ -12644,6 +12743,9 @@
       <c r="DO33" s="2" t="n">
         <v>121.3</v>
       </c>
+      <c r="DP33" s="1" t="n">
+        <v>145.4</v>
+      </c>
     </row>
     <row r="34" ht="20" customHeight="1">
       <c r="A34" s="1" t="n">
@@ -13003,6 +13105,9 @@
       <c r="DO34" s="1" t="n">
         <v>144.7</v>
       </c>
+      <c r="DP34" s="1" t="n">
+        <v>153.2</v>
+      </c>
     </row>
     <row r="35" ht="20" customHeight="1">
       <c r="A35" s="1" t="n">
@@ -13362,6 +13467,9 @@
       <c r="DO35" s="1" t="n">
         <v>187.5</v>
       </c>
+      <c r="DP35" s="1" t="n">
+        <v>164</v>
+      </c>
     </row>
     <row r="36" ht="20" customHeight="1">
       <c r="A36" s="1" t="n">
@@ -13721,6 +13829,9 @@
       <c r="DO36" s="1" t="n">
         <v>171.8</v>
       </c>
+      <c r="DP36" s="1" t="n">
+        <v>207.6</v>
+      </c>
     </row>
     <row r="37" ht="20" customHeight="1">
       <c r="A37" s="1" t="n">
@@ -14080,6 +14191,9 @@
       <c r="DO37" s="1" t="n">
         <v>179.9</v>
       </c>
+      <c r="DP37" s="3" t="n">
+        <v>131.1</v>
+      </c>
     </row>
     <row r="38" ht="20" customHeight="1">
       <c r="A38" s="1" t="n">
@@ -14439,6 +14553,9 @@
       <c r="DO38" s="1" t="n">
         <v>179.6</v>
       </c>
+      <c r="DP38" s="3" t="n">
+        <v>126.7</v>
+      </c>
     </row>
     <row r="39" ht="20" customHeight="1">
       <c r="A39" s="1" t="n">
@@ -14798,6 +14915,9 @@
       <c r="DO39" s="3" t="n">
         <v>125.3</v>
       </c>
+      <c r="DP39" s="1" t="n">
+        <v>166.6</v>
+      </c>
     </row>
     <row r="40" ht="20" customHeight="1">
       <c r="A40" s="1" t="n">
@@ -15157,6 +15277,9 @@
       <c r="DO40" s="1" t="n">
         <v>155</v>
       </c>
+      <c r="DP40" s="3" t="n">
+        <v>139.1</v>
+      </c>
     </row>
     <row r="41" ht="20" customHeight="1">
       <c r="A41" s="1" t="n">
@@ -15515,6 +15638,9 @@
       </c>
       <c r="DO41" s="3" t="n">
         <v>132.3</v>
+      </c>
+      <c r="DP41" s="1" t="n">
+        <v>150.1</v>
       </c>
     </row>
     <row r="42" ht="20" customHeight="1">
@@ -15847,6 +15973,7 @@
       <c r="DM42" s="1" t="n"/>
       <c r="DN42" s="1" t="n"/>
       <c r="DO42" s="1" t="n"/>
+      <c r="DP42" s="1" t="n"/>
     </row>
     <row r="43" ht="20" customHeight="1">
       <c r="A43" s="1" t="n">
@@ -16178,6 +16305,7 @@
       <c r="DM43" s="1" t="n"/>
       <c r="DN43" s="1" t="n"/>
       <c r="DO43" s="1" t="n"/>
+      <c r="DP43" s="1" t="n"/>
     </row>
     <row r="44" ht="20" customHeight="1">
       <c r="A44" s="1" t="n">
@@ -16537,6 +16665,9 @@
       <c r="DO44" s="3" t="n">
         <v>133.2</v>
       </c>
+      <c r="DP44" s="1" t="n">
+        <v>204.8</v>
+      </c>
     </row>
     <row r="45" ht="20" customHeight="1">
       <c r="A45" s="1" t="n">
@@ -16896,6 +17027,9 @@
       <c r="DO45" s="1" t="n">
         <v>212.1</v>
       </c>
+      <c r="DP45" s="1" t="n">
+        <v>141</v>
+      </c>
     </row>
     <row r="46" ht="20" customHeight="1">
       <c r="A46" s="1" t="n">
@@ -17255,6 +17389,9 @@
       <c r="DO46" s="1" t="n">
         <v>145.4</v>
       </c>
+      <c r="DP46" s="2" t="n">
+        <v>121.7</v>
+      </c>
     </row>
     <row r="47" ht="20" customHeight="1">
       <c r="A47" s="1" t="n">
@@ -17614,6 +17751,9 @@
       <c r="DO47" s="1" t="n">
         <v>166.5</v>
       </c>
+      <c r="DP47" s="1" t="n">
+        <v>148.6</v>
+      </c>
     </row>
     <row r="48" ht="20" customHeight="1">
       <c r="A48" s="1" t="n">
@@ -17973,6 +18113,9 @@
       <c r="DO48" s="1" t="n">
         <v>150.7</v>
       </c>
+      <c r="DP48" s="1" t="n">
+        <v>167.1</v>
+      </c>
     </row>
     <row r="49" ht="20" customHeight="1">
       <c r="A49" s="1" t="n">
@@ -18332,6 +18475,9 @@
       <c r="DO49" s="3" t="n">
         <v>134.4</v>
       </c>
+      <c r="DP49" s="1" t="n">
+        <v>160.4</v>
+      </c>
     </row>
     <row r="50" ht="20" customHeight="1">
       <c r="A50" s="1" t="n">
@@ -18691,6 +18837,9 @@
       <c r="DO50" s="1" t="n">
         <v>166.2</v>
       </c>
+      <c r="DP50" s="1" t="n">
+        <v>220.7</v>
+      </c>
     </row>
     <row r="51" ht="20" customHeight="1">
       <c r="A51" s="1" t="n">
@@ -19050,6 +19199,9 @@
       <c r="DO51" s="3" t="n">
         <v>132.1</v>
       </c>
+      <c r="DP51" s="1" t="n">
+        <v>141.3</v>
+      </c>
     </row>
     <row r="52" ht="20" customHeight="1">
       <c r="A52" s="1" t="n">
@@ -19409,6 +19561,9 @@
       <c r="DO52" s="3" t="n">
         <v>126.6</v>
       </c>
+      <c r="DP52" s="1" t="n">
+        <v>194.4</v>
+      </c>
     </row>
     <row r="53" ht="20" customHeight="1">
       <c r="A53" s="1" t="n">
@@ -19767,6 +19922,9 @@
       </c>
       <c r="DO53" s="2" t="n">
         <v>121.7</v>
+      </c>
+      <c r="DP53" s="1" t="n">
+        <v>203.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2025-01-07
</commit_message>
<xml_diff>
--- a/マイジャグラーV_塗りつぶし済み.xlsx
+++ b/マイジャグラーV_塗りつぶし済み.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:DP53"/>
+  <dimension ref="A1:DQ53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -559,6 +559,7 @@
     <col width="12" customWidth="1" min="118" max="118"/>
     <col width="12" customWidth="1" min="119" max="119"/>
     <col width="12" customWidth="1" min="120" max="120"/>
+    <col width="12" customWidth="1" min="121" max="121"/>
   </cols>
   <sheetData>
     <row r="1" ht="20" customHeight="1">
@@ -1162,6 +1163,11 @@
           <t>2025/01/06</t>
         </is>
       </c>
+      <c r="DQ1" s="1" t="inlineStr">
+        <is>
+          <t>2025/01/07</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="20" customHeight="1">
       <c r="A2" s="1" t="n">
@@ -1524,6 +1530,9 @@
       <c r="DP2" s="2" t="n">
         <v>121.3</v>
       </c>
+      <c r="DQ2" s="1" t="n">
+        <v>259.3</v>
+      </c>
     </row>
     <row r="3" ht="20" customHeight="1">
       <c r="A3" s="1" t="n">
@@ -1886,6 +1895,9 @@
       <c r="DP3" s="1" t="n">
         <v>166.6</v>
       </c>
+      <c r="DQ3" s="1" t="n">
+        <v>143.3</v>
+      </c>
     </row>
     <row r="4" ht="20" customHeight="1">
       <c r="A4" s="1" t="n">
@@ -2248,6 +2260,9 @@
       <c r="DP4" s="1" t="n">
         <v>144.1</v>
       </c>
+      <c r="DQ4" s="3" t="n">
+        <v>136.6</v>
+      </c>
     </row>
     <row r="5" ht="20" customHeight="1">
       <c r="A5" s="1" t="n">
@@ -2610,6 +2625,9 @@
       <c r="DP5" s="1" t="n">
         <v>173.5</v>
       </c>
+      <c r="DQ5" s="3" t="n">
+        <v>131.1</v>
+      </c>
     </row>
     <row r="6" ht="20" customHeight="1">
       <c r="A6" s="1" t="n">
@@ -2972,6 +2990,9 @@
       <c r="DP6" s="1" t="n">
         <v>152.7</v>
       </c>
+      <c r="DQ6" s="1" t="n">
+        <v>150.9</v>
+      </c>
     </row>
     <row r="7" ht="20" customHeight="1">
       <c r="A7" s="1" t="n">
@@ -3334,6 +3355,9 @@
       <c r="DP7" s="1" t="n">
         <v>159.5</v>
       </c>
+      <c r="DQ7" s="2" t="n">
+        <v>104.1</v>
+      </c>
     </row>
     <row r="8" ht="20" customHeight="1">
       <c r="A8" s="1" t="n">
@@ -3696,6 +3720,9 @@
       <c r="DP8" s="1" t="n">
         <v>311.9</v>
       </c>
+      <c r="DQ8" s="1" t="n">
+        <v>184.6</v>
+      </c>
     </row>
     <row r="9" ht="20" customHeight="1">
       <c r="A9" s="1" t="n">
@@ -4058,6 +4085,9 @@
       <c r="DP9" s="3" t="n">
         <v>135.6</v>
       </c>
+      <c r="DQ9" s="3" t="n">
+        <v>131.2</v>
+      </c>
     </row>
     <row r="10" ht="20" customHeight="1">
       <c r="A10" s="1" t="n">
@@ -4420,6 +4450,9 @@
       <c r="DP10" s="1" t="n">
         <v>198.4</v>
       </c>
+      <c r="DQ10" s="1" t="n">
+        <v>144.4</v>
+      </c>
     </row>
     <row r="11" ht="20" customHeight="1">
       <c r="A11" s="1" t="n">
@@ -4782,6 +4815,9 @@
       <c r="DP11" s="1" t="n">
         <v>247.8</v>
       </c>
+      <c r="DQ11" s="1" t="n">
+        <v>208.9</v>
+      </c>
     </row>
     <row r="12" ht="20" customHeight="1">
       <c r="A12" s="1" t="n">
@@ -5144,6 +5180,9 @@
       <c r="DP12" s="1" t="n">
         <v>209</v>
       </c>
+      <c r="DQ12" s="1" t="n">
+        <v>188.9</v>
+      </c>
     </row>
     <row r="13" ht="20" customHeight="1">
       <c r="A13" s="1" t="n">
@@ -5506,6 +5545,9 @@
       <c r="DP13" s="3" t="n">
         <v>139.2</v>
       </c>
+      <c r="DQ13" s="2" t="n">
+        <v>124.2</v>
+      </c>
     </row>
     <row r="14" ht="20" customHeight="1">
       <c r="A14" s="1" t="n">
@@ -5868,6 +5910,9 @@
       <c r="DP14" s="1" t="n">
         <v>146.4</v>
       </c>
+      <c r="DQ14" s="3" t="n">
+        <v>133.1</v>
+      </c>
     </row>
     <row r="15" ht="20" customHeight="1">
       <c r="A15" s="1" t="n">
@@ -6230,6 +6275,9 @@
       <c r="DP15" s="1" t="n">
         <v>189.4</v>
       </c>
+      <c r="DQ15" s="1" t="n">
+        <v>161.5</v>
+      </c>
     </row>
     <row r="16" ht="20" customHeight="1">
       <c r="A16" s="1" t="n">
@@ -6592,6 +6640,9 @@
       <c r="DP16" s="1" t="n">
         <v>165.6</v>
       </c>
+      <c r="DQ16" s="1" t="n">
+        <v>171.4</v>
+      </c>
     </row>
     <row r="17" ht="20" customHeight="1">
       <c r="A17" s="1" t="n">
@@ -6954,6 +7005,9 @@
       <c r="DP17" s="1" t="n">
         <v>142</v>
       </c>
+      <c r="DQ17" s="1" t="n">
+        <v>166.8</v>
+      </c>
     </row>
     <row r="18" ht="20" customHeight="1">
       <c r="A18" s="1" t="n">
@@ -7316,6 +7370,9 @@
       <c r="DP18" s="1" t="n">
         <v>158.4</v>
       </c>
+      <c r="DQ18" s="1" t="n">
+        <v>168</v>
+      </c>
     </row>
     <row r="19" ht="20" customHeight="1">
       <c r="A19" s="1" t="n">
@@ -7678,6 +7735,9 @@
       <c r="DP19" s="3" t="n">
         <v>131.5</v>
       </c>
+      <c r="DQ19" s="1" t="n">
+        <v>191.9</v>
+      </c>
     </row>
     <row r="20" ht="20" customHeight="1">
       <c r="A20" s="1" t="n">
@@ -8040,6 +8100,9 @@
       <c r="DP20" s="1" t="n">
         <v>308.5</v>
       </c>
+      <c r="DQ20" s="1" t="n">
+        <v>168.6</v>
+      </c>
     </row>
     <row r="21" ht="20" customHeight="1">
       <c r="A21" s="1" t="n">
@@ -8402,6 +8465,9 @@
       <c r="DP21" s="1" t="n">
         <v>198.8</v>
       </c>
+      <c r="DQ21" s="1" t="n">
+        <v>140.1</v>
+      </c>
     </row>
     <row r="22" ht="20" customHeight="1">
       <c r="A22" s="1" t="n">
@@ -8764,6 +8830,9 @@
       <c r="DP22" s="1" t="n">
         <v>149</v>
       </c>
+      <c r="DQ22" s="1" t="n">
+        <v>167.8</v>
+      </c>
     </row>
     <row r="23" ht="20" customHeight="1">
       <c r="A23" s="1" t="n">
@@ -9126,6 +9195,9 @@
       <c r="DP23" s="3" t="n">
         <v>131.7</v>
       </c>
+      <c r="DQ23" s="1" t="n">
+        <v>194.3</v>
+      </c>
     </row>
     <row r="24" ht="20" customHeight="1">
       <c r="A24" s="1" t="n">
@@ -9488,6 +9560,9 @@
       <c r="DP24" s="1" t="n">
         <v>180.7</v>
       </c>
+      <c r="DQ24" s="1" t="n">
+        <v>157.8</v>
+      </c>
     </row>
     <row r="25" ht="20" customHeight="1">
       <c r="A25" s="1" t="n">
@@ -9850,6 +9925,9 @@
       <c r="DP25" s="1" t="n">
         <v>154.4</v>
       </c>
+      <c r="DQ25" s="1" t="n">
+        <v>157.4</v>
+      </c>
     </row>
     <row r="26" ht="20" customHeight="1">
       <c r="A26" s="1" t="n">
@@ -10212,6 +10290,9 @@
       <c r="DP26" s="3" t="n">
         <v>137.6</v>
       </c>
+      <c r="DQ26" s="1" t="n">
+        <v>152.5</v>
+      </c>
     </row>
     <row r="27" ht="20" customHeight="1">
       <c r="A27" s="1" t="n">
@@ -10574,6 +10655,9 @@
       <c r="DP27" s="1" t="n">
         <v>284.4</v>
       </c>
+      <c r="DQ27" s="1" t="n">
+        <v>154.1</v>
+      </c>
     </row>
     <row r="28" ht="20" customHeight="1">
       <c r="A28" s="1" t="n">
@@ -10936,6 +11020,9 @@
       <c r="DP28" s="3" t="n">
         <v>131.2</v>
       </c>
+      <c r="DQ28" s="3" t="n">
+        <v>135.3</v>
+      </c>
     </row>
     <row r="29" ht="20" customHeight="1">
       <c r="A29" s="1" t="n">
@@ -11298,6 +11385,9 @@
       <c r="DP29" s="1" t="n">
         <v>186.3</v>
       </c>
+      <c r="DQ29" s="1" t="n">
+        <v>228.9</v>
+      </c>
     </row>
     <row r="30" ht="20" customHeight="1">
       <c r="A30" s="1" t="n">
@@ -11660,6 +11750,9 @@
       <c r="DP30" s="1" t="n">
         <v>440.8</v>
       </c>
+      <c r="DQ30" s="1" t="n">
+        <v>171.7</v>
+      </c>
     </row>
     <row r="31" ht="20" customHeight="1">
       <c r="A31" s="1" t="n">
@@ -12022,6 +12115,9 @@
       <c r="DP31" s="3" t="n">
         <v>128.1</v>
       </c>
+      <c r="DQ31" s="1" t="n">
+        <v>146.4</v>
+      </c>
     </row>
     <row r="32" ht="20" customHeight="1">
       <c r="A32" s="1" t="n">
@@ -12384,6 +12480,9 @@
       <c r="DP32" s="1" t="n">
         <v>166.4</v>
       </c>
+      <c r="DQ32" s="3" t="n">
+        <v>139.7</v>
+      </c>
     </row>
     <row r="33" ht="20" customHeight="1">
       <c r="A33" s="1" t="n">
@@ -12746,6 +12845,9 @@
       <c r="DP33" s="1" t="n">
         <v>145.4</v>
       </c>
+      <c r="DQ33" s="1" t="n">
+        <v>149.8</v>
+      </c>
     </row>
     <row r="34" ht="20" customHeight="1">
       <c r="A34" s="1" t="n">
@@ -13108,6 +13210,9 @@
       <c r="DP34" s="1" t="n">
         <v>153.2</v>
       </c>
+      <c r="DQ34" s="1" t="n">
+        <v>148.7</v>
+      </c>
     </row>
     <row r="35" ht="20" customHeight="1">
       <c r="A35" s="1" t="n">
@@ -13470,6 +13575,9 @@
       <c r="DP35" s="1" t="n">
         <v>164</v>
       </c>
+      <c r="DQ35" s="1" t="n">
+        <v>150.8</v>
+      </c>
     </row>
     <row r="36" ht="20" customHeight="1">
       <c r="A36" s="1" t="n">
@@ -13832,6 +13940,9 @@
       <c r="DP36" s="1" t="n">
         <v>207.6</v>
       </c>
+      <c r="DQ36" s="1" t="n">
+        <v>167.9</v>
+      </c>
     </row>
     <row r="37" ht="20" customHeight="1">
       <c r="A37" s="1" t="n">
@@ -14194,6 +14305,9 @@
       <c r="DP37" s="3" t="n">
         <v>131.1</v>
       </c>
+      <c r="DQ37" s="1" t="n">
+        <v>212.8</v>
+      </c>
     </row>
     <row r="38" ht="20" customHeight="1">
       <c r="A38" s="1" t="n">
@@ -14556,6 +14670,9 @@
       <c r="DP38" s="3" t="n">
         <v>126.7</v>
       </c>
+      <c r="DQ38" s="3" t="n">
+        <v>133.4</v>
+      </c>
     </row>
     <row r="39" ht="20" customHeight="1">
       <c r="A39" s="1" t="n">
@@ -14918,6 +15035,9 @@
       <c r="DP39" s="1" t="n">
         <v>166.6</v>
       </c>
+      <c r="DQ39" s="1" t="n">
+        <v>148.5</v>
+      </c>
     </row>
     <row r="40" ht="20" customHeight="1">
       <c r="A40" s="1" t="n">
@@ -15280,6 +15400,9 @@
       <c r="DP40" s="3" t="n">
         <v>139.1</v>
       </c>
+      <c r="DQ40" s="1" t="n">
+        <v>168</v>
+      </c>
     </row>
     <row r="41" ht="20" customHeight="1">
       <c r="A41" s="1" t="n">
@@ -15641,6 +15764,9 @@
       </c>
       <c r="DP41" s="1" t="n">
         <v>150.1</v>
+      </c>
+      <c r="DQ41" s="1" t="n">
+        <v>169.8</v>
       </c>
     </row>
     <row r="42" ht="20" customHeight="1">
@@ -15974,6 +16100,7 @@
       <c r="DN42" s="1" t="n"/>
       <c r="DO42" s="1" t="n"/>
       <c r="DP42" s="1" t="n"/>
+      <c r="DQ42" s="1" t="n"/>
     </row>
     <row r="43" ht="20" customHeight="1">
       <c r="A43" s="1" t="n">
@@ -16306,6 +16433,7 @@
       <c r="DN43" s="1" t="n"/>
       <c r="DO43" s="1" t="n"/>
       <c r="DP43" s="1" t="n"/>
+      <c r="DQ43" s="1" t="n"/>
     </row>
     <row r="44" ht="20" customHeight="1">
       <c r="A44" s="1" t="n">
@@ -16668,6 +16796,9 @@
       <c r="DP44" s="1" t="n">
         <v>204.8</v>
       </c>
+      <c r="DQ44" s="1" t="n">
+        <v>162.4</v>
+      </c>
     </row>
     <row r="45" ht="20" customHeight="1">
       <c r="A45" s="1" t="n">
@@ -17030,6 +17161,9 @@
       <c r="DP45" s="1" t="n">
         <v>141</v>
       </c>
+      <c r="DQ45" s="2" t="n">
+        <v>118.8</v>
+      </c>
     </row>
     <row r="46" ht="20" customHeight="1">
       <c r="A46" s="1" t="n">
@@ -17392,6 +17526,9 @@
       <c r="DP46" s="2" t="n">
         <v>121.7</v>
       </c>
+      <c r="DQ46" s="1" t="n">
+        <v>215.5</v>
+      </c>
     </row>
     <row r="47" ht="20" customHeight="1">
       <c r="A47" s="1" t="n">
@@ -17754,6 +17891,9 @@
       <c r="DP47" s="1" t="n">
         <v>148.6</v>
       </c>
+      <c r="DQ47" s="2" t="n">
+        <v>120.4</v>
+      </c>
     </row>
     <row r="48" ht="20" customHeight="1">
       <c r="A48" s="1" t="n">
@@ -18116,6 +18256,9 @@
       <c r="DP48" s="1" t="n">
         <v>167.1</v>
       </c>
+      <c r="DQ48" s="1" t="n">
+        <v>158.2</v>
+      </c>
     </row>
     <row r="49" ht="20" customHeight="1">
       <c r="A49" s="1" t="n">
@@ -18478,6 +18621,9 @@
       <c r="DP49" s="1" t="n">
         <v>160.4</v>
       </c>
+      <c r="DQ49" s="1" t="n">
+        <v>157</v>
+      </c>
     </row>
     <row r="50" ht="20" customHeight="1">
       <c r="A50" s="1" t="n">
@@ -18840,6 +18986,9 @@
       <c r="DP50" s="1" t="n">
         <v>220.7</v>
       </c>
+      <c r="DQ50" s="1" t="n">
+        <v>144.5</v>
+      </c>
     </row>
     <row r="51" ht="20" customHeight="1">
       <c r="A51" s="1" t="n">
@@ -19202,6 +19351,9 @@
       <c r="DP51" s="1" t="n">
         <v>141.3</v>
       </c>
+      <c r="DQ51" s="1" t="n">
+        <v>166.1</v>
+      </c>
     </row>
     <row r="52" ht="20" customHeight="1">
       <c r="A52" s="1" t="n">
@@ -19564,6 +19716,9 @@
       <c r="DP52" s="1" t="n">
         <v>194.4</v>
       </c>
+      <c r="DQ52" s="1" t="n">
+        <v>182.8</v>
+      </c>
     </row>
     <row r="53" ht="20" customHeight="1">
       <c r="A53" s="1" t="n">
@@ -19925,6 +20080,9 @@
       </c>
       <c r="DP53" s="1" t="n">
         <v>203.5</v>
+      </c>
+      <c r="DQ53" s="1" t="n">
+        <v>163</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2025-01-08
</commit_message>
<xml_diff>
--- a/マイジャグラーV_塗りつぶし済み.xlsx
+++ b/マイジャグラーV_塗りつぶし済み.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:DQ53"/>
+  <dimension ref="A1:DR53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -560,6 +560,7 @@
     <col width="12" customWidth="1" min="119" max="119"/>
     <col width="12" customWidth="1" min="120" max="120"/>
     <col width="12" customWidth="1" min="121" max="121"/>
+    <col width="12" customWidth="1" min="122" max="122"/>
   </cols>
   <sheetData>
     <row r="1" ht="20" customHeight="1">
@@ -1168,6 +1169,11 @@
           <t>2025/01/07</t>
         </is>
       </c>
+      <c r="DR1" s="1" t="inlineStr">
+        <is>
+          <t>2025/01/08</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="20" customHeight="1">
       <c r="A2" s="1" t="n">
@@ -1533,6 +1539,9 @@
       <c r="DQ2" s="1" t="n">
         <v>259.3</v>
       </c>
+      <c r="DR2" s="1" t="n">
+        <v>162.2</v>
+      </c>
     </row>
     <row r="3" ht="20" customHeight="1">
       <c r="A3" s="1" t="n">
@@ -1898,6 +1907,9 @@
       <c r="DQ3" s="1" t="n">
         <v>143.3</v>
       </c>
+      <c r="DR3" s="3" t="n">
+        <v>130.4</v>
+      </c>
     </row>
     <row r="4" ht="20" customHeight="1">
       <c r="A4" s="1" t="n">
@@ -2263,6 +2275,9 @@
       <c r="DQ4" s="3" t="n">
         <v>136.6</v>
       </c>
+      <c r="DR4" s="1" t="n">
+        <v>202.8</v>
+      </c>
     </row>
     <row r="5" ht="20" customHeight="1">
       <c r="A5" s="1" t="n">
@@ -2628,6 +2643,9 @@
       <c r="DQ5" s="3" t="n">
         <v>131.1</v>
       </c>
+      <c r="DR5" s="1" t="n">
+        <v>159.2</v>
+      </c>
     </row>
     <row r="6" ht="20" customHeight="1">
       <c r="A6" s="1" t="n">
@@ -2993,6 +3011,9 @@
       <c r="DQ6" s="1" t="n">
         <v>150.9</v>
       </c>
+      <c r="DR6" s="1" t="n">
+        <v>149.9</v>
+      </c>
     </row>
     <row r="7" ht="20" customHeight="1">
       <c r="A7" s="1" t="n">
@@ -3358,6 +3379,9 @@
       <c r="DQ7" s="2" t="n">
         <v>104.1</v>
       </c>
+      <c r="DR7" s="1" t="n">
+        <v>180.2</v>
+      </c>
     </row>
     <row r="8" ht="20" customHeight="1">
       <c r="A8" s="1" t="n">
@@ -3723,6 +3747,9 @@
       <c r="DQ8" s="1" t="n">
         <v>184.6</v>
       </c>
+      <c r="DR8" s="1" t="n">
+        <v>154.7</v>
+      </c>
     </row>
     <row r="9" ht="20" customHeight="1">
       <c r="A9" s="1" t="n">
@@ -4088,6 +4115,9 @@
       <c r="DQ9" s="3" t="n">
         <v>131.2</v>
       </c>
+      <c r="DR9" s="2" t="n">
+        <v>113.1</v>
+      </c>
     </row>
     <row r="10" ht="20" customHeight="1">
       <c r="A10" s="1" t="n">
@@ -4453,6 +4483,9 @@
       <c r="DQ10" s="1" t="n">
         <v>144.4</v>
       </c>
+      <c r="DR10" s="1" t="n">
+        <v>257.5</v>
+      </c>
     </row>
     <row r="11" ht="20" customHeight="1">
       <c r="A11" s="1" t="n">
@@ -4818,6 +4851,9 @@
       <c r="DQ11" s="1" t="n">
         <v>208.9</v>
       </c>
+      <c r="DR11" s="1" t="n">
+        <v>220.8</v>
+      </c>
     </row>
     <row r="12" ht="20" customHeight="1">
       <c r="A12" s="1" t="n">
@@ -5183,6 +5219,9 @@
       <c r="DQ12" s="1" t="n">
         <v>188.9</v>
       </c>
+      <c r="DR12" s="3" t="n">
+        <v>133</v>
+      </c>
     </row>
     <row r="13" ht="20" customHeight="1">
       <c r="A13" s="1" t="n">
@@ -5548,6 +5587,9 @@
       <c r="DQ13" s="2" t="n">
         <v>124.2</v>
       </c>
+      <c r="DR13" s="1" t="n">
+        <v>141.9</v>
+      </c>
     </row>
     <row r="14" ht="20" customHeight="1">
       <c r="A14" s="1" t="n">
@@ -5913,6 +5955,9 @@
       <c r="DQ14" s="3" t="n">
         <v>133.1</v>
       </c>
+      <c r="DR14" s="3" t="n">
+        <v>125.8</v>
+      </c>
     </row>
     <row r="15" ht="20" customHeight="1">
       <c r="A15" s="1" t="n">
@@ -6278,6 +6323,9 @@
       <c r="DQ15" s="1" t="n">
         <v>161.5</v>
       </c>
+      <c r="DR15" s="1" t="n">
+        <v>150</v>
+      </c>
     </row>
     <row r="16" ht="20" customHeight="1">
       <c r="A16" s="1" t="n">
@@ -6643,6 +6691,9 @@
       <c r="DQ16" s="1" t="n">
         <v>171.4</v>
       </c>
+      <c r="DR16" s="3" t="n">
+        <v>138</v>
+      </c>
     </row>
     <row r="17" ht="20" customHeight="1">
       <c r="A17" s="1" t="n">
@@ -7008,6 +7059,9 @@
       <c r="DQ17" s="1" t="n">
         <v>166.8</v>
       </c>
+      <c r="DR17" s="1" t="n">
+        <v>178.7</v>
+      </c>
     </row>
     <row r="18" ht="20" customHeight="1">
       <c r="A18" s="1" t="n">
@@ -7373,6 +7427,9 @@
       <c r="DQ18" s="1" t="n">
         <v>168</v>
       </c>
+      <c r="DR18" s="3" t="n">
+        <v>136.8</v>
+      </c>
     </row>
     <row r="19" ht="20" customHeight="1">
       <c r="A19" s="1" t="n">
@@ -7738,6 +7795,9 @@
       <c r="DQ19" s="1" t="n">
         <v>191.9</v>
       </c>
+      <c r="DR19" s="1" t="n">
+        <v>182.7</v>
+      </c>
     </row>
     <row r="20" ht="20" customHeight="1">
       <c r="A20" s="1" t="n">
@@ -8103,6 +8163,9 @@
       <c r="DQ20" s="1" t="n">
         <v>168.6</v>
       </c>
+      <c r="DR20" s="1" t="n">
+        <v>154</v>
+      </c>
     </row>
     <row r="21" ht="20" customHeight="1">
       <c r="A21" s="1" t="n">
@@ -8468,6 +8531,9 @@
       <c r="DQ21" s="1" t="n">
         <v>140.1</v>
       </c>
+      <c r="DR21" s="1" t="n">
+        <v>146.8</v>
+      </c>
     </row>
     <row r="22" ht="20" customHeight="1">
       <c r="A22" s="1" t="n">
@@ -8833,6 +8899,9 @@
       <c r="DQ22" s="1" t="n">
         <v>167.8</v>
       </c>
+      <c r="DR22" s="1" t="n">
+        <v>155.5</v>
+      </c>
     </row>
     <row r="23" ht="20" customHeight="1">
       <c r="A23" s="1" t="n">
@@ -9198,6 +9267,9 @@
       <c r="DQ23" s="1" t="n">
         <v>194.3</v>
       </c>
+      <c r="DR23" s="1" t="n">
+        <v>471.6</v>
+      </c>
     </row>
     <row r="24" ht="20" customHeight="1">
       <c r="A24" s="1" t="n">
@@ -9563,6 +9635,9 @@
       <c r="DQ24" s="1" t="n">
         <v>157.8</v>
       </c>
+      <c r="DR24" s="1" t="n">
+        <v>203.4</v>
+      </c>
     </row>
     <row r="25" ht="20" customHeight="1">
       <c r="A25" s="1" t="n">
@@ -9928,6 +10003,9 @@
       <c r="DQ25" s="1" t="n">
         <v>157.4</v>
       </c>
+      <c r="DR25" s="1" t="n">
+        <v>148.2</v>
+      </c>
     </row>
     <row r="26" ht="20" customHeight="1">
       <c r="A26" s="1" t="n">
@@ -10293,6 +10371,9 @@
       <c r="DQ26" s="1" t="n">
         <v>152.5</v>
       </c>
+      <c r="DR26" s="3" t="n">
+        <v>137.2</v>
+      </c>
     </row>
     <row r="27" ht="20" customHeight="1">
       <c r="A27" s="1" t="n">
@@ -10658,6 +10739,9 @@
       <c r="DQ27" s="1" t="n">
         <v>154.1</v>
       </c>
+      <c r="DR27" s="1" t="n">
+        <v>183.1</v>
+      </c>
     </row>
     <row r="28" ht="20" customHeight="1">
       <c r="A28" s="1" t="n">
@@ -11023,6 +11107,9 @@
       <c r="DQ28" s="3" t="n">
         <v>135.3</v>
       </c>
+      <c r="DR28" s="1" t="n">
+        <v>156.2</v>
+      </c>
     </row>
     <row r="29" ht="20" customHeight="1">
       <c r="A29" s="1" t="n">
@@ -11388,6 +11475,9 @@
       <c r="DQ29" s="1" t="n">
         <v>228.9</v>
       </c>
+      <c r="DR29" s="1" t="n">
+        <v>168.4</v>
+      </c>
     </row>
     <row r="30" ht="20" customHeight="1">
       <c r="A30" s="1" t="n">
@@ -11753,6 +11843,9 @@
       <c r="DQ30" s="1" t="n">
         <v>171.7</v>
       </c>
+      <c r="DR30" s="3" t="n">
+        <v>137.3</v>
+      </c>
     </row>
     <row r="31" ht="20" customHeight="1">
       <c r="A31" s="1" t="n">
@@ -12118,6 +12211,9 @@
       <c r="DQ31" s="1" t="n">
         <v>146.4</v>
       </c>
+      <c r="DR31" s="1" t="n">
+        <v>202.4</v>
+      </c>
     </row>
     <row r="32" ht="20" customHeight="1">
       <c r="A32" s="1" t="n">
@@ -12483,6 +12579,9 @@
       <c r="DQ32" s="3" t="n">
         <v>139.7</v>
       </c>
+      <c r="DR32" s="1" t="n">
+        <v>174.3</v>
+      </c>
     </row>
     <row r="33" ht="20" customHeight="1">
       <c r="A33" s="1" t="n">
@@ -12848,6 +12947,9 @@
       <c r="DQ33" s="1" t="n">
         <v>149.8</v>
       </c>
+      <c r="DR33" s="1" t="n">
+        <v>150.5</v>
+      </c>
     </row>
     <row r="34" ht="20" customHeight="1">
       <c r="A34" s="1" t="n">
@@ -13213,6 +13315,9 @@
       <c r="DQ34" s="1" t="n">
         <v>148.7</v>
       </c>
+      <c r="DR34" s="1" t="n">
+        <v>172.8</v>
+      </c>
     </row>
     <row r="35" ht="20" customHeight="1">
       <c r="A35" s="1" t="n">
@@ -13578,6 +13683,9 @@
       <c r="DQ35" s="1" t="n">
         <v>150.8</v>
       </c>
+      <c r="DR35" s="1" t="n">
+        <v>160.4</v>
+      </c>
     </row>
     <row r="36" ht="20" customHeight="1">
       <c r="A36" s="1" t="n">
@@ -13943,6 +14051,9 @@
       <c r="DQ36" s="1" t="n">
         <v>167.9</v>
       </c>
+      <c r="DR36" s="1" t="n">
+        <v>166.9</v>
+      </c>
     </row>
     <row r="37" ht="20" customHeight="1">
       <c r="A37" s="1" t="n">
@@ -14308,6 +14419,9 @@
       <c r="DQ37" s="1" t="n">
         <v>212.8</v>
       </c>
+      <c r="DR37" s="3" t="n">
+        <v>129.4</v>
+      </c>
     </row>
     <row r="38" ht="20" customHeight="1">
       <c r="A38" s="1" t="n">
@@ -14673,6 +14787,9 @@
       <c r="DQ38" s="3" t="n">
         <v>133.4</v>
       </c>
+      <c r="DR38" s="2" t="n">
+        <v>114.5</v>
+      </c>
     </row>
     <row r="39" ht="20" customHeight="1">
       <c r="A39" s="1" t="n">
@@ -15038,6 +15155,9 @@
       <c r="DQ39" s="1" t="n">
         <v>148.5</v>
       </c>
+      <c r="DR39" s="2" t="n">
+        <v>120</v>
+      </c>
     </row>
     <row r="40" ht="20" customHeight="1">
       <c r="A40" s="1" t="n">
@@ -15403,6 +15523,9 @@
       <c r="DQ40" s="1" t="n">
         <v>168</v>
       </c>
+      <c r="DR40" s="1" t="n">
+        <v>164.1</v>
+      </c>
     </row>
     <row r="41" ht="20" customHeight="1">
       <c r="A41" s="1" t="n">
@@ -15767,6 +15890,9 @@
       </c>
       <c r="DQ41" s="1" t="n">
         <v>169.8</v>
+      </c>
+      <c r="DR41" s="1" t="n">
+        <v>161.7</v>
       </c>
     </row>
     <row r="42" ht="20" customHeight="1">
@@ -16101,6 +16227,7 @@
       <c r="DO42" s="1" t="n"/>
       <c r="DP42" s="1" t="n"/>
       <c r="DQ42" s="1" t="n"/>
+      <c r="DR42" s="1" t="n"/>
     </row>
     <row r="43" ht="20" customHeight="1">
       <c r="A43" s="1" t="n">
@@ -16434,6 +16561,7 @@
       <c r="DO43" s="1" t="n"/>
       <c r="DP43" s="1" t="n"/>
       <c r="DQ43" s="1" t="n"/>
+      <c r="DR43" s="1" t="n"/>
     </row>
     <row r="44" ht="20" customHeight="1">
       <c r="A44" s="1" t="n">
@@ -16799,6 +16927,9 @@
       <c r="DQ44" s="1" t="n">
         <v>162.4</v>
       </c>
+      <c r="DR44" s="1" t="n">
+        <v>202.4</v>
+      </c>
     </row>
     <row r="45" ht="20" customHeight="1">
       <c r="A45" s="1" t="n">
@@ -17164,6 +17295,9 @@
       <c r="DQ45" s="2" t="n">
         <v>118.8</v>
       </c>
+      <c r="DR45" s="1" t="n">
+        <v>158.3</v>
+      </c>
     </row>
     <row r="46" ht="20" customHeight="1">
       <c r="A46" s="1" t="n">
@@ -17529,6 +17663,9 @@
       <c r="DQ46" s="1" t="n">
         <v>215.5</v>
       </c>
+      <c r="DR46" s="1" t="n">
+        <v>284.5</v>
+      </c>
     </row>
     <row r="47" ht="20" customHeight="1">
       <c r="A47" s="1" t="n">
@@ -17894,6 +18031,9 @@
       <c r="DQ47" s="2" t="n">
         <v>120.4</v>
       </c>
+      <c r="DR47" s="1" t="n">
+        <v>169.9</v>
+      </c>
     </row>
     <row r="48" ht="20" customHeight="1">
       <c r="A48" s="1" t="n">
@@ -18259,6 +18399,9 @@
       <c r="DQ48" s="1" t="n">
         <v>158.2</v>
       </c>
+      <c r="DR48" s="1" t="n">
+        <v>157.1</v>
+      </c>
     </row>
     <row r="49" ht="20" customHeight="1">
       <c r="A49" s="1" t="n">
@@ -18624,6 +18767,9 @@
       <c r="DQ49" s="1" t="n">
         <v>157</v>
       </c>
+      <c r="DR49" s="3" t="n">
+        <v>132</v>
+      </c>
     </row>
     <row r="50" ht="20" customHeight="1">
       <c r="A50" s="1" t="n">
@@ -18989,6 +19135,9 @@
       <c r="DQ50" s="1" t="n">
         <v>144.5</v>
       </c>
+      <c r="DR50" s="1" t="n">
+        <v>140</v>
+      </c>
     </row>
     <row r="51" ht="20" customHeight="1">
       <c r="A51" s="1" t="n">
@@ -19354,6 +19503,9 @@
       <c r="DQ51" s="1" t="n">
         <v>166.1</v>
       </c>
+      <c r="DR51" s="1" t="n">
+        <v>150.6</v>
+      </c>
     </row>
     <row r="52" ht="20" customHeight="1">
       <c r="A52" s="1" t="n">
@@ -19719,6 +19871,9 @@
       <c r="DQ52" s="1" t="n">
         <v>182.8</v>
       </c>
+      <c r="DR52" s="3" t="n">
+        <v>138.7</v>
+      </c>
     </row>
     <row r="53" ht="20" customHeight="1">
       <c r="A53" s="1" t="n">
@@ -20083,6 +20238,9 @@
       </c>
       <c r="DQ53" s="1" t="n">
         <v>163</v>
+      </c>
+      <c r="DR53" s="1" t="n">
+        <v>140.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2025-01-09
</commit_message>
<xml_diff>
--- a/マイジャグラーV_塗りつぶし済み.xlsx
+++ b/マイジャグラーV_塗りつぶし済み.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:DR53"/>
+  <dimension ref="A1:DS53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -561,6 +561,7 @@
     <col width="12" customWidth="1" min="120" max="120"/>
     <col width="12" customWidth="1" min="121" max="121"/>
     <col width="12" customWidth="1" min="122" max="122"/>
+    <col width="12" customWidth="1" min="123" max="123"/>
   </cols>
   <sheetData>
     <row r="1" ht="20" customHeight="1">
@@ -1174,6 +1175,11 @@
           <t>2025/01/08</t>
         </is>
       </c>
+      <c r="DS1" s="1" t="inlineStr">
+        <is>
+          <t>2025/01/09</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="20" customHeight="1">
       <c r="A2" s="1" t="n">
@@ -1542,6 +1548,9 @@
       <c r="DR2" s="1" t="n">
         <v>162.2</v>
       </c>
+      <c r="DS2" s="1" t="n">
+        <v>157</v>
+      </c>
     </row>
     <row r="3" ht="20" customHeight="1">
       <c r="A3" s="1" t="n">
@@ -1910,6 +1919,9 @@
       <c r="DR3" s="3" t="n">
         <v>130.4</v>
       </c>
+      <c r="DS3" s="1" t="n">
+        <v>166</v>
+      </c>
     </row>
     <row r="4" ht="20" customHeight="1">
       <c r="A4" s="1" t="n">
@@ -2278,6 +2290,9 @@
       <c r="DR4" s="1" t="n">
         <v>202.8</v>
       </c>
+      <c r="DS4" s="1" t="n">
+        <v>153.6</v>
+      </c>
     </row>
     <row r="5" ht="20" customHeight="1">
       <c r="A5" s="1" t="n">
@@ -2646,6 +2661,9 @@
       <c r="DR5" s="1" t="n">
         <v>159.2</v>
       </c>
+      <c r="DS5" s="3" t="n">
+        <v>138.3</v>
+      </c>
     </row>
     <row r="6" ht="20" customHeight="1">
       <c r="A6" s="1" t="n">
@@ -3014,6 +3032,9 @@
       <c r="DR6" s="1" t="n">
         <v>149.9</v>
       </c>
+      <c r="DS6" s="1" t="n">
+        <v>155</v>
+      </c>
     </row>
     <row r="7" ht="20" customHeight="1">
       <c r="A7" s="1" t="n">
@@ -3382,6 +3403,9 @@
       <c r="DR7" s="1" t="n">
         <v>180.2</v>
       </c>
+      <c r="DS7" s="3" t="n">
+        <v>133.7</v>
+      </c>
     </row>
     <row r="8" ht="20" customHeight="1">
       <c r="A8" s="1" t="n">
@@ -3750,6 +3774,9 @@
       <c r="DR8" s="1" t="n">
         <v>154.7</v>
       </c>
+      <c r="DS8" s="1" t="n">
+        <v>204.6</v>
+      </c>
     </row>
     <row r="9" ht="20" customHeight="1">
       <c r="A9" s="1" t="n">
@@ -4118,6 +4145,9 @@
       <c r="DR9" s="2" t="n">
         <v>113.1</v>
       </c>
+      <c r="DS9" s="1" t="n">
+        <v>142.9</v>
+      </c>
     </row>
     <row r="10" ht="20" customHeight="1">
       <c r="A10" s="1" t="n">
@@ -4486,6 +4516,9 @@
       <c r="DR10" s="1" t="n">
         <v>257.5</v>
       </c>
+      <c r="DS10" s="2" t="n">
+        <v>120.9</v>
+      </c>
     </row>
     <row r="11" ht="20" customHeight="1">
       <c r="A11" s="1" t="n">
@@ -4854,6 +4887,9 @@
       <c r="DR11" s="1" t="n">
         <v>220.8</v>
       </c>
+      <c r="DS11" s="2" t="n">
+        <v>104.2</v>
+      </c>
     </row>
     <row r="12" ht="20" customHeight="1">
       <c r="A12" s="1" t="n">
@@ -5222,6 +5258,9 @@
       <c r="DR12" s="3" t="n">
         <v>133</v>
       </c>
+      <c r="DS12" s="1" t="n">
+        <v>149.5</v>
+      </c>
     </row>
     <row r="13" ht="20" customHeight="1">
       <c r="A13" s="1" t="n">
@@ -5590,6 +5629,9 @@
       <c r="DR13" s="1" t="n">
         <v>141.9</v>
       </c>
+      <c r="DS13" s="1" t="n">
+        <v>161</v>
+      </c>
     </row>
     <row r="14" ht="20" customHeight="1">
       <c r="A14" s="1" t="n">
@@ -5958,6 +6000,9 @@
       <c r="DR14" s="3" t="n">
         <v>125.8</v>
       </c>
+      <c r="DS14" s="2" t="n">
+        <v>122.8</v>
+      </c>
     </row>
     <row r="15" ht="20" customHeight="1">
       <c r="A15" s="1" t="n">
@@ -6326,6 +6371,9 @@
       <c r="DR15" s="1" t="n">
         <v>150</v>
       </c>
+      <c r="DS15" s="1" t="n">
+        <v>154.4</v>
+      </c>
     </row>
     <row r="16" ht="20" customHeight="1">
       <c r="A16" s="1" t="n">
@@ -6694,6 +6742,9 @@
       <c r="DR16" s="3" t="n">
         <v>138</v>
       </c>
+      <c r="DS16" s="1" t="n">
+        <v>162.2</v>
+      </c>
     </row>
     <row r="17" ht="20" customHeight="1">
       <c r="A17" s="1" t="n">
@@ -7062,6 +7113,9 @@
       <c r="DR17" s="1" t="n">
         <v>178.7</v>
       </c>
+      <c r="DS17" s="1" t="n">
+        <v>187</v>
+      </c>
     </row>
     <row r="18" ht="20" customHeight="1">
       <c r="A18" s="1" t="n">
@@ -7430,6 +7484,9 @@
       <c r="DR18" s="3" t="n">
         <v>136.8</v>
       </c>
+      <c r="DS18" s="1" t="n">
+        <v>233</v>
+      </c>
     </row>
     <row r="19" ht="20" customHeight="1">
       <c r="A19" s="1" t="n">
@@ -7798,6 +7855,9 @@
       <c r="DR19" s="1" t="n">
         <v>182.7</v>
       </c>
+      <c r="DS19" s="1" t="n">
+        <v>146.6</v>
+      </c>
     </row>
     <row r="20" ht="20" customHeight="1">
       <c r="A20" s="1" t="n">
@@ -8166,6 +8226,9 @@
       <c r="DR20" s="1" t="n">
         <v>154</v>
       </c>
+      <c r="DS20" s="1" t="n">
+        <v>184.7</v>
+      </c>
     </row>
     <row r="21" ht="20" customHeight="1">
       <c r="A21" s="1" t="n">
@@ -8534,6 +8597,9 @@
       <c r="DR21" s="1" t="n">
         <v>146.8</v>
       </c>
+      <c r="DS21" s="1" t="n">
+        <v>163</v>
+      </c>
     </row>
     <row r="22" ht="20" customHeight="1">
       <c r="A22" s="1" t="n">
@@ -8902,6 +8968,9 @@
       <c r="DR22" s="1" t="n">
         <v>155.5</v>
       </c>
+      <c r="DS22" s="1" t="n">
+        <v>217.9</v>
+      </c>
     </row>
     <row r="23" ht="20" customHeight="1">
       <c r="A23" s="1" t="n">
@@ -9270,6 +9339,9 @@
       <c r="DR23" s="1" t="n">
         <v>471.6</v>
       </c>
+      <c r="DS23" s="1" t="n">
+        <v>144.9</v>
+      </c>
     </row>
     <row r="24" ht="20" customHeight="1">
       <c r="A24" s="1" t="n">
@@ -9638,6 +9710,9 @@
       <c r="DR24" s="1" t="n">
         <v>203.4</v>
       </c>
+      <c r="DS24" s="1" t="n">
+        <v>177.6</v>
+      </c>
     </row>
     <row r="25" ht="20" customHeight="1">
       <c r="A25" s="1" t="n">
@@ -10006,6 +10081,9 @@
       <c r="DR25" s="1" t="n">
         <v>148.2</v>
       </c>
+      <c r="DS25" s="3" t="n">
+        <v>131.3</v>
+      </c>
     </row>
     <row r="26" ht="20" customHeight="1">
       <c r="A26" s="1" t="n">
@@ -10374,6 +10452,9 @@
       <c r="DR26" s="3" t="n">
         <v>137.2</v>
       </c>
+      <c r="DS26" s="1" t="n">
+        <v>189.4</v>
+      </c>
     </row>
     <row r="27" ht="20" customHeight="1">
       <c r="A27" s="1" t="n">
@@ -10742,6 +10823,9 @@
       <c r="DR27" s="1" t="n">
         <v>183.1</v>
       </c>
+      <c r="DS27" s="1" t="n">
+        <v>145.8</v>
+      </c>
     </row>
     <row r="28" ht="20" customHeight="1">
       <c r="A28" s="1" t="n">
@@ -11110,6 +11194,9 @@
       <c r="DR28" s="1" t="n">
         <v>156.2</v>
       </c>
+      <c r="DS28" s="1" t="n">
+        <v>178.6</v>
+      </c>
     </row>
     <row r="29" ht="20" customHeight="1">
       <c r="A29" s="1" t="n">
@@ -11478,6 +11565,9 @@
       <c r="DR29" s="1" t="n">
         <v>168.4</v>
       </c>
+      <c r="DS29" s="1" t="n">
+        <v>179.8</v>
+      </c>
     </row>
     <row r="30" ht="20" customHeight="1">
       <c r="A30" s="1" t="n">
@@ -11846,6 +11936,9 @@
       <c r="DR30" s="3" t="n">
         <v>137.3</v>
       </c>
+      <c r="DS30" s="1" t="n">
+        <v>149.9</v>
+      </c>
     </row>
     <row r="31" ht="20" customHeight="1">
       <c r="A31" s="1" t="n">
@@ -12214,6 +12307,9 @@
       <c r="DR31" s="1" t="n">
         <v>202.4</v>
       </c>
+      <c r="DS31" s="1" t="n">
+        <v>153.6</v>
+      </c>
     </row>
     <row r="32" ht="20" customHeight="1">
       <c r="A32" s="1" t="n">
@@ -12582,6 +12678,9 @@
       <c r="DR32" s="1" t="n">
         <v>174.3</v>
       </c>
+      <c r="DS32" s="2" t="n">
+        <v>124.2</v>
+      </c>
     </row>
     <row r="33" ht="20" customHeight="1">
       <c r="A33" s="1" t="n">
@@ -12950,6 +13049,9 @@
       <c r="DR33" s="1" t="n">
         <v>150.5</v>
       </c>
+      <c r="DS33" s="1" t="n">
+        <v>145.8</v>
+      </c>
     </row>
     <row r="34" ht="20" customHeight="1">
       <c r="A34" s="1" t="n">
@@ -13318,6 +13420,9 @@
       <c r="DR34" s="1" t="n">
         <v>172.8</v>
       </c>
+      <c r="DS34" s="1" t="n">
+        <v>333</v>
+      </c>
     </row>
     <row r="35" ht="20" customHeight="1">
       <c r="A35" s="1" t="n">
@@ -13686,6 +13791,9 @@
       <c r="DR35" s="1" t="n">
         <v>160.4</v>
       </c>
+      <c r="DS35" s="1" t="n">
+        <v>212.7</v>
+      </c>
     </row>
     <row r="36" ht="20" customHeight="1">
       <c r="A36" s="1" t="n">
@@ -14054,6 +14162,9 @@
       <c r="DR36" s="1" t="n">
         <v>166.9</v>
       </c>
+      <c r="DS36" s="1" t="n">
+        <v>173.2</v>
+      </c>
     </row>
     <row r="37" ht="20" customHeight="1">
       <c r="A37" s="1" t="n">
@@ -14422,6 +14533,9 @@
       <c r="DR37" s="3" t="n">
         <v>129.4</v>
       </c>
+      <c r="DS37" s="1" t="n">
+        <v>260.4</v>
+      </c>
     </row>
     <row r="38" ht="20" customHeight="1">
       <c r="A38" s="1" t="n">
@@ -14790,6 +14904,9 @@
       <c r="DR38" s="2" t="n">
         <v>114.5</v>
       </c>
+      <c r="DS38" s="1" t="n">
+        <v>163.6</v>
+      </c>
     </row>
     <row r="39" ht="20" customHeight="1">
       <c r="A39" s="1" t="n">
@@ -15158,6 +15275,9 @@
       <c r="DR39" s="2" t="n">
         <v>120</v>
       </c>
+      <c r="DS39" s="2" t="n">
+        <v>114.7</v>
+      </c>
     </row>
     <row r="40" ht="20" customHeight="1">
       <c r="A40" s="1" t="n">
@@ -15526,6 +15646,9 @@
       <c r="DR40" s="1" t="n">
         <v>164.1</v>
       </c>
+      <c r="DS40" s="1" t="n">
+        <v>225.5</v>
+      </c>
     </row>
     <row r="41" ht="20" customHeight="1">
       <c r="A41" s="1" t="n">
@@ -15893,6 +16016,9 @@
       </c>
       <c r="DR41" s="1" t="n">
         <v>161.7</v>
+      </c>
+      <c r="DS41" s="1" t="n">
+        <v>156.8</v>
       </c>
     </row>
     <row r="42" ht="20" customHeight="1">
@@ -16228,6 +16354,7 @@
       <c r="DP42" s="1" t="n"/>
       <c r="DQ42" s="1" t="n"/>
       <c r="DR42" s="1" t="n"/>
+      <c r="DS42" s="1" t="n"/>
     </row>
     <row r="43" ht="20" customHeight="1">
       <c r="A43" s="1" t="n">
@@ -16562,6 +16689,7 @@
       <c r="DP43" s="1" t="n"/>
       <c r="DQ43" s="1" t="n"/>
       <c r="DR43" s="1" t="n"/>
+      <c r="DS43" s="1" t="n"/>
     </row>
     <row r="44" ht="20" customHeight="1">
       <c r="A44" s="1" t="n">
@@ -16930,6 +17058,9 @@
       <c r="DR44" s="1" t="n">
         <v>202.4</v>
       </c>
+      <c r="DS44" s="1" t="n">
+        <v>177.7</v>
+      </c>
     </row>
     <row r="45" ht="20" customHeight="1">
       <c r="A45" s="1" t="n">
@@ -17298,6 +17429,9 @@
       <c r="DR45" s="1" t="n">
         <v>158.3</v>
       </c>
+      <c r="DS45" s="1" t="n">
+        <v>175</v>
+      </c>
     </row>
     <row r="46" ht="20" customHeight="1">
       <c r="A46" s="1" t="n">
@@ -17666,6 +17800,9 @@
       <c r="DR46" s="1" t="n">
         <v>284.5</v>
       </c>
+      <c r="DS46" s="1" t="n">
+        <v>164.9</v>
+      </c>
     </row>
     <row r="47" ht="20" customHeight="1">
       <c r="A47" s="1" t="n">
@@ -18034,6 +18171,9 @@
       <c r="DR47" s="1" t="n">
         <v>169.9</v>
       </c>
+      <c r="DS47" s="1" t="n">
+        <v>334.7</v>
+      </c>
     </row>
     <row r="48" ht="20" customHeight="1">
       <c r="A48" s="1" t="n">
@@ -18402,6 +18542,9 @@
       <c r="DR48" s="1" t="n">
         <v>157.1</v>
       </c>
+      <c r="DS48" s="2" t="n">
+        <v>123.2</v>
+      </c>
     </row>
     <row r="49" ht="20" customHeight="1">
       <c r="A49" s="1" t="n">
@@ -18770,6 +18913,9 @@
       <c r="DR49" s="3" t="n">
         <v>132</v>
       </c>
+      <c r="DS49" s="1" t="n">
+        <v>142.6</v>
+      </c>
     </row>
     <row r="50" ht="20" customHeight="1">
       <c r="A50" s="1" t="n">
@@ -19138,6 +19284,9 @@
       <c r="DR50" s="1" t="n">
         <v>140</v>
       </c>
+      <c r="DS50" s="1" t="n">
+        <v>186.2</v>
+      </c>
     </row>
     <row r="51" ht="20" customHeight="1">
       <c r="A51" s="1" t="n">
@@ -19506,6 +19655,9 @@
       <c r="DR51" s="1" t="n">
         <v>150.6</v>
       </c>
+      <c r="DS51" s="1" t="n">
+        <v>166.5</v>
+      </c>
     </row>
     <row r="52" ht="20" customHeight="1">
       <c r="A52" s="1" t="n">
@@ -19874,6 +20026,9 @@
       <c r="DR52" s="3" t="n">
         <v>138.7</v>
       </c>
+      <c r="DS52" s="1" t="n">
+        <v>180.8</v>
+      </c>
     </row>
     <row r="53" ht="20" customHeight="1">
       <c r="A53" s="1" t="n">
@@ -20241,6 +20396,9 @@
       </c>
       <c r="DR53" s="1" t="n">
         <v>140.1</v>
+      </c>
+      <c r="DS53" s="1" t="n">
+        <v>184.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2025-01-10
</commit_message>
<xml_diff>
--- a/マイジャグラーV_塗りつぶし済み.xlsx
+++ b/マイジャグラーV_塗りつぶし済み.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:DS53"/>
+  <dimension ref="A1:DT53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -562,6 +562,7 @@
     <col width="12" customWidth="1" min="121" max="121"/>
     <col width="12" customWidth="1" min="122" max="122"/>
     <col width="12" customWidth="1" min="123" max="123"/>
+    <col width="12" customWidth="1" min="124" max="124"/>
   </cols>
   <sheetData>
     <row r="1" ht="20" customHeight="1">
@@ -1180,6 +1181,11 @@
           <t>2025/01/09</t>
         </is>
       </c>
+      <c r="DT1" s="1" t="inlineStr">
+        <is>
+          <t>2025/01/10</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="20" customHeight="1">
       <c r="A2" s="1" t="n">
@@ -1551,6 +1557,9 @@
       <c r="DS2" s="1" t="n">
         <v>157</v>
       </c>
+      <c r="DT2" s="1" t="n">
+        <v>161.7</v>
+      </c>
     </row>
     <row r="3" ht="20" customHeight="1">
       <c r="A3" s="1" t="n">
@@ -1922,6 +1931,9 @@
       <c r="DS3" s="1" t="n">
         <v>166</v>
       </c>
+      <c r="DT3" s="2" t="n">
+        <v>119.7</v>
+      </c>
     </row>
     <row r="4" ht="20" customHeight="1">
       <c r="A4" s="1" t="n">
@@ -2293,6 +2305,9 @@
       <c r="DS4" s="1" t="n">
         <v>153.6</v>
       </c>
+      <c r="DT4" s="1" t="n">
+        <v>174.8</v>
+      </c>
     </row>
     <row r="5" ht="20" customHeight="1">
       <c r="A5" s="1" t="n">
@@ -2664,6 +2679,9 @@
       <c r="DS5" s="3" t="n">
         <v>138.3</v>
       </c>
+      <c r="DT5" s="1" t="n">
+        <v>152.5</v>
+      </c>
     </row>
     <row r="6" ht="20" customHeight="1">
       <c r="A6" s="1" t="n">
@@ -3035,6 +3053,9 @@
       <c r="DS6" s="1" t="n">
         <v>155</v>
       </c>
+      <c r="DT6" s="1" t="n">
+        <v>158.2</v>
+      </c>
     </row>
     <row r="7" ht="20" customHeight="1">
       <c r="A7" s="1" t="n">
@@ -3406,6 +3427,9 @@
       <c r="DS7" s="3" t="n">
         <v>133.7</v>
       </c>
+      <c r="DT7" s="1" t="n">
+        <v>185.2</v>
+      </c>
     </row>
     <row r="8" ht="20" customHeight="1">
       <c r="A8" s="1" t="n">
@@ -3777,6 +3801,9 @@
       <c r="DS8" s="1" t="n">
         <v>204.6</v>
       </c>
+      <c r="DT8" s="1" t="n">
+        <v>220.9</v>
+      </c>
     </row>
     <row r="9" ht="20" customHeight="1">
       <c r="A9" s="1" t="n">
@@ -4148,6 +4175,9 @@
       <c r="DS9" s="1" t="n">
         <v>142.9</v>
       </c>
+      <c r="DT9" s="1" t="n">
+        <v>158.3</v>
+      </c>
     </row>
     <row r="10" ht="20" customHeight="1">
       <c r="A10" s="1" t="n">
@@ -4519,6 +4549,9 @@
       <c r="DS10" s="2" t="n">
         <v>120.9</v>
       </c>
+      <c r="DT10" s="1" t="n">
+        <v>172.8</v>
+      </c>
     </row>
     <row r="11" ht="20" customHeight="1">
       <c r="A11" s="1" t="n">
@@ -4890,6 +4923,9 @@
       <c r="DS11" s="2" t="n">
         <v>104.2</v>
       </c>
+      <c r="DT11" s="3" t="n">
+        <v>127.6</v>
+      </c>
     </row>
     <row r="12" ht="20" customHeight="1">
       <c r="A12" s="1" t="n">
@@ -5261,6 +5297,9 @@
       <c r="DS12" s="1" t="n">
         <v>149.5</v>
       </c>
+      <c r="DT12" s="1" t="n">
+        <v>216.2</v>
+      </c>
     </row>
     <row r="13" ht="20" customHeight="1">
       <c r="A13" s="1" t="n">
@@ -5632,6 +5671,9 @@
       <c r="DS13" s="1" t="n">
         <v>161</v>
       </c>
+      <c r="DT13" s="1" t="n">
+        <v>142.8</v>
+      </c>
     </row>
     <row r="14" ht="20" customHeight="1">
       <c r="A14" s="1" t="n">
@@ -6003,6 +6045,9 @@
       <c r="DS14" s="2" t="n">
         <v>122.8</v>
       </c>
+      <c r="DT14" s="1" t="n">
+        <v>245.9</v>
+      </c>
     </row>
     <row r="15" ht="20" customHeight="1">
       <c r="A15" s="1" t="n">
@@ -6374,6 +6419,9 @@
       <c r="DS15" s="1" t="n">
         <v>154.4</v>
       </c>
+      <c r="DT15" s="3" t="n">
+        <v>134.2</v>
+      </c>
     </row>
     <row r="16" ht="20" customHeight="1">
       <c r="A16" s="1" t="n">
@@ -6745,6 +6793,9 @@
       <c r="DS16" s="1" t="n">
         <v>162.2</v>
       </c>
+      <c r="DT16" s="1" t="n">
+        <v>154.7</v>
+      </c>
     </row>
     <row r="17" ht="20" customHeight="1">
       <c r="A17" s="1" t="n">
@@ -7116,6 +7167,9 @@
       <c r="DS17" s="1" t="n">
         <v>187</v>
       </c>
+      <c r="DT17" s="1" t="n">
+        <v>232.7</v>
+      </c>
     </row>
     <row r="18" ht="20" customHeight="1">
       <c r="A18" s="1" t="n">
@@ -7487,6 +7541,9 @@
       <c r="DS18" s="1" t="n">
         <v>233</v>
       </c>
+      <c r="DT18" s="3" t="n">
+        <v>133.7</v>
+      </c>
     </row>
     <row r="19" ht="20" customHeight="1">
       <c r="A19" s="1" t="n">
@@ -7858,6 +7915,9 @@
       <c r="DS19" s="1" t="n">
         <v>146.6</v>
       </c>
+      <c r="DT19" s="1" t="n">
+        <v>162.1</v>
+      </c>
     </row>
     <row r="20" ht="20" customHeight="1">
       <c r="A20" s="1" t="n">
@@ -8229,6 +8289,9 @@
       <c r="DS20" s="1" t="n">
         <v>184.7</v>
       </c>
+      <c r="DT20" s="1" t="n">
+        <v>156.4</v>
+      </c>
     </row>
     <row r="21" ht="20" customHeight="1">
       <c r="A21" s="1" t="n">
@@ -8600,6 +8663,9 @@
       <c r="DS21" s="1" t="n">
         <v>163</v>
       </c>
+      <c r="DT21" s="1" t="n">
+        <v>147.3</v>
+      </c>
     </row>
     <row r="22" ht="20" customHeight="1">
       <c r="A22" s="1" t="n">
@@ -8971,6 +9037,9 @@
       <c r="DS22" s="1" t="n">
         <v>217.9</v>
       </c>
+      <c r="DT22" s="1" t="n">
+        <v>173.9</v>
+      </c>
     </row>
     <row r="23" ht="20" customHeight="1">
       <c r="A23" s="1" t="n">
@@ -9342,6 +9411,9 @@
       <c r="DS23" s="1" t="n">
         <v>144.9</v>
       </c>
+      <c r="DT23" s="3" t="n">
+        <v>135.4</v>
+      </c>
     </row>
     <row r="24" ht="20" customHeight="1">
       <c r="A24" s="1" t="n">
@@ -9713,6 +9785,9 @@
       <c r="DS24" s="1" t="n">
         <v>177.6</v>
       </c>
+      <c r="DT24" s="1" t="n">
+        <v>163.4</v>
+      </c>
     </row>
     <row r="25" ht="20" customHeight="1">
       <c r="A25" s="1" t="n">
@@ -10084,6 +10159,9 @@
       <c r="DS25" s="3" t="n">
         <v>131.3</v>
       </c>
+      <c r="DT25" s="1" t="n">
+        <v>178</v>
+      </c>
     </row>
     <row r="26" ht="20" customHeight="1">
       <c r="A26" s="1" t="n">
@@ -10455,6 +10533,9 @@
       <c r="DS26" s="1" t="n">
         <v>189.4</v>
       </c>
+      <c r="DT26" s="2" t="n">
+        <v>118.2</v>
+      </c>
     </row>
     <row r="27" ht="20" customHeight="1">
       <c r="A27" s="1" t="n">
@@ -10826,6 +10907,9 @@
       <c r="DS27" s="1" t="n">
         <v>145.8</v>
       </c>
+      <c r="DT27" s="1" t="n">
+        <v>177.5</v>
+      </c>
     </row>
     <row r="28" ht="20" customHeight="1">
       <c r="A28" s="1" t="n">
@@ -11197,6 +11281,9 @@
       <c r="DS28" s="1" t="n">
         <v>178.6</v>
       </c>
+      <c r="DT28" s="3" t="n">
+        <v>129</v>
+      </c>
     </row>
     <row r="29" ht="20" customHeight="1">
       <c r="A29" s="1" t="n">
@@ -11568,6 +11655,9 @@
       <c r="DS29" s="1" t="n">
         <v>179.8</v>
       </c>
+      <c r="DT29" s="1" t="n">
+        <v>209.3</v>
+      </c>
     </row>
     <row r="30" ht="20" customHeight="1">
       <c r="A30" s="1" t="n">
@@ -11939,6 +12029,9 @@
       <c r="DS30" s="1" t="n">
         <v>149.9</v>
       </c>
+      <c r="DT30" s="2" t="n">
+        <v>123.5</v>
+      </c>
     </row>
     <row r="31" ht="20" customHeight="1">
       <c r="A31" s="1" t="n">
@@ -12310,6 +12403,9 @@
       <c r="DS31" s="1" t="n">
         <v>153.6</v>
       </c>
+      <c r="DT31" s="2" t="n">
+        <v>122.3</v>
+      </c>
     </row>
     <row r="32" ht="20" customHeight="1">
       <c r="A32" s="1" t="n">
@@ -12681,6 +12777,9 @@
       <c r="DS32" s="2" t="n">
         <v>124.2</v>
       </c>
+      <c r="DT32" s="1" t="n">
+        <v>164.2</v>
+      </c>
     </row>
     <row r="33" ht="20" customHeight="1">
       <c r="A33" s="1" t="n">
@@ -13052,6 +13151,9 @@
       <c r="DS33" s="1" t="n">
         <v>145.8</v>
       </c>
+      <c r="DT33" s="1" t="n">
+        <v>146.1</v>
+      </c>
     </row>
     <row r="34" ht="20" customHeight="1">
       <c r="A34" s="1" t="n">
@@ -13423,6 +13525,9 @@
       <c r="DS34" s="1" t="n">
         <v>333</v>
       </c>
+      <c r="DT34" s="1" t="n">
+        <v>173.1</v>
+      </c>
     </row>
     <row r="35" ht="20" customHeight="1">
       <c r="A35" s="1" t="n">
@@ -13794,6 +13899,9 @@
       <c r="DS35" s="1" t="n">
         <v>212.7</v>
       </c>
+      <c r="DT35" s="1" t="n">
+        <v>140.7</v>
+      </c>
     </row>
     <row r="36" ht="20" customHeight="1">
       <c r="A36" s="1" t="n">
@@ -14165,6 +14273,9 @@
       <c r="DS36" s="1" t="n">
         <v>173.2</v>
       </c>
+      <c r="DT36" s="1" t="n">
+        <v>166.7</v>
+      </c>
     </row>
     <row r="37" ht="20" customHeight="1">
       <c r="A37" s="1" t="n">
@@ -14536,6 +14647,9 @@
       <c r="DS37" s="1" t="n">
         <v>260.4</v>
       </c>
+      <c r="DT37" s="1" t="n">
+        <v>262.8</v>
+      </c>
     </row>
     <row r="38" ht="20" customHeight="1">
       <c r="A38" s="1" t="n">
@@ -14907,6 +15021,9 @@
       <c r="DS38" s="1" t="n">
         <v>163.6</v>
       </c>
+      <c r="DT38" s="1" t="n">
+        <v>159.6</v>
+      </c>
     </row>
     <row r="39" ht="20" customHeight="1">
       <c r="A39" s="1" t="n">
@@ -15278,6 +15395,9 @@
       <c r="DS39" s="2" t="n">
         <v>114.7</v>
       </c>
+      <c r="DT39" s="3" t="n">
+        <v>128</v>
+      </c>
     </row>
     <row r="40" ht="20" customHeight="1">
       <c r="A40" s="1" t="n">
@@ -15649,6 +15769,9 @@
       <c r="DS40" s="1" t="n">
         <v>225.5</v>
       </c>
+      <c r="DT40" s="1" t="n">
+        <v>142.2</v>
+      </c>
     </row>
     <row r="41" ht="20" customHeight="1">
       <c r="A41" s="1" t="n">
@@ -16019,6 +16142,9 @@
       </c>
       <c r="DS41" s="1" t="n">
         <v>156.8</v>
+      </c>
+      <c r="DT41" s="1" t="n">
+        <v>152.5</v>
       </c>
     </row>
     <row r="42" ht="20" customHeight="1">
@@ -16355,6 +16481,7 @@
       <c r="DQ42" s="1" t="n"/>
       <c r="DR42" s="1" t="n"/>
       <c r="DS42" s="1" t="n"/>
+      <c r="DT42" s="1" t="n"/>
     </row>
     <row r="43" ht="20" customHeight="1">
       <c r="A43" s="1" t="n">
@@ -16690,6 +16817,7 @@
       <c r="DQ43" s="1" t="n"/>
       <c r="DR43" s="1" t="n"/>
       <c r="DS43" s="1" t="n"/>
+      <c r="DT43" s="1" t="n"/>
     </row>
     <row r="44" ht="20" customHeight="1">
       <c r="A44" s="1" t="n">
@@ -17061,6 +17189,9 @@
       <c r="DS44" s="1" t="n">
         <v>177.7</v>
       </c>
+      <c r="DT44" s="1" t="n">
+        <v>161.1</v>
+      </c>
     </row>
     <row r="45" ht="20" customHeight="1">
       <c r="A45" s="1" t="n">
@@ -17432,6 +17563,9 @@
       <c r="DS45" s="1" t="n">
         <v>175</v>
       </c>
+      <c r="DT45" s="1" t="n">
+        <v>181.2</v>
+      </c>
     </row>
     <row r="46" ht="20" customHeight="1">
       <c r="A46" s="1" t="n">
@@ -17803,6 +17937,9 @@
       <c r="DS46" s="1" t="n">
         <v>164.9</v>
       </c>
+      <c r="DT46" s="1" t="n">
+        <v>144.6</v>
+      </c>
     </row>
     <row r="47" ht="20" customHeight="1">
       <c r="A47" s="1" t="n">
@@ -18174,6 +18311,9 @@
       <c r="DS47" s="1" t="n">
         <v>334.7</v>
       </c>
+      <c r="DT47" s="3" t="n">
+        <v>136</v>
+      </c>
     </row>
     <row r="48" ht="20" customHeight="1">
       <c r="A48" s="1" t="n">
@@ -18545,6 +18685,9 @@
       <c r="DS48" s="2" t="n">
         <v>123.2</v>
       </c>
+      <c r="DT48" s="1" t="n">
+        <v>159.2</v>
+      </c>
     </row>
     <row r="49" ht="20" customHeight="1">
       <c r="A49" s="1" t="n">
@@ -18916,6 +19059,9 @@
       <c r="DS49" s="1" t="n">
         <v>142.6</v>
       </c>
+      <c r="DT49" s="1" t="n">
+        <v>143.6</v>
+      </c>
     </row>
     <row r="50" ht="20" customHeight="1">
       <c r="A50" s="1" t="n">
@@ -19287,6 +19433,9 @@
       <c r="DS50" s="1" t="n">
         <v>186.2</v>
       </c>
+      <c r="DT50" s="1" t="n">
+        <v>162.3</v>
+      </c>
     </row>
     <row r="51" ht="20" customHeight="1">
       <c r="A51" s="1" t="n">
@@ -19658,6 +19807,9 @@
       <c r="DS51" s="1" t="n">
         <v>166.5</v>
       </c>
+      <c r="DT51" s="1" t="n">
+        <v>145.6</v>
+      </c>
     </row>
     <row r="52" ht="20" customHeight="1">
       <c r="A52" s="1" t="n">
@@ -20029,6 +20181,9 @@
       <c r="DS52" s="1" t="n">
         <v>180.8</v>
       </c>
+      <c r="DT52" s="1" t="n">
+        <v>223.1</v>
+      </c>
     </row>
     <row r="53" ht="20" customHeight="1">
       <c r="A53" s="1" t="n">
@@ -20399,6 +20554,9 @@
       </c>
       <c r="DS53" s="1" t="n">
         <v>184.1</v>
+      </c>
+      <c r="DT53" s="3" t="n">
+        <v>132.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2025-01-11
</commit_message>
<xml_diff>
--- a/マイジャグラーV_塗りつぶし済み.xlsx
+++ b/マイジャグラーV_塗りつぶし済み.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:DT53"/>
+  <dimension ref="A1:DU53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -563,6 +563,7 @@
     <col width="12" customWidth="1" min="122" max="122"/>
     <col width="12" customWidth="1" min="123" max="123"/>
     <col width="12" customWidth="1" min="124" max="124"/>
+    <col width="12" customWidth="1" min="125" max="125"/>
   </cols>
   <sheetData>
     <row r="1" ht="20" customHeight="1">
@@ -1186,6 +1187,11 @@
           <t>2025/01/10</t>
         </is>
       </c>
+      <c r="DU1" s="1" t="inlineStr">
+        <is>
+          <t>2025/01/11</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="20" customHeight="1">
       <c r="A2" s="1" t="n">
@@ -1560,6 +1566,9 @@
       <c r="DT2" s="1" t="n">
         <v>161.7</v>
       </c>
+      <c r="DU2" s="1" t="n">
+        <v>178</v>
+      </c>
     </row>
     <row r="3" ht="20" customHeight="1">
       <c r="A3" s="1" t="n">
@@ -1934,6 +1943,9 @@
       <c r="DT3" s="2" t="n">
         <v>119.7</v>
       </c>
+      <c r="DU3" s="1" t="n">
+        <v>204.4</v>
+      </c>
     </row>
     <row r="4" ht="20" customHeight="1">
       <c r="A4" s="1" t="n">
@@ -2308,6 +2320,9 @@
       <c r="DT4" s="1" t="n">
         <v>174.8</v>
       </c>
+      <c r="DU4" s="1" t="n">
+        <v>152.8</v>
+      </c>
     </row>
     <row r="5" ht="20" customHeight="1">
       <c r="A5" s="1" t="n">
@@ -2682,6 +2697,9 @@
       <c r="DT5" s="1" t="n">
         <v>152.5</v>
       </c>
+      <c r="DU5" s="1" t="n">
+        <v>179.7</v>
+      </c>
     </row>
     <row r="6" ht="20" customHeight="1">
       <c r="A6" s="1" t="n">
@@ -3056,6 +3074,9 @@
       <c r="DT6" s="1" t="n">
         <v>158.2</v>
       </c>
+      <c r="DU6" s="3" t="n">
+        <v>131.1</v>
+      </c>
     </row>
     <row r="7" ht="20" customHeight="1">
       <c r="A7" s="1" t="n">
@@ -3430,6 +3451,9 @@
       <c r="DT7" s="1" t="n">
         <v>185.2</v>
       </c>
+      <c r="DU7" s="1" t="n">
+        <v>154.7</v>
+      </c>
     </row>
     <row r="8" ht="20" customHeight="1">
       <c r="A8" s="1" t="n">
@@ -3804,6 +3828,9 @@
       <c r="DT8" s="1" t="n">
         <v>220.9</v>
       </c>
+      <c r="DU8" s="3" t="n">
+        <v>138</v>
+      </c>
     </row>
     <row r="9" ht="20" customHeight="1">
       <c r="A9" s="1" t="n">
@@ -4178,6 +4205,9 @@
       <c r="DT9" s="1" t="n">
         <v>158.3</v>
       </c>
+      <c r="DU9" s="1" t="n">
+        <v>144.8</v>
+      </c>
     </row>
     <row r="10" ht="20" customHeight="1">
       <c r="A10" s="1" t="n">
@@ -4552,6 +4582,9 @@
       <c r="DT10" s="1" t="n">
         <v>172.8</v>
       </c>
+      <c r="DU10" s="1" t="n">
+        <v>157.2</v>
+      </c>
     </row>
     <row r="11" ht="20" customHeight="1">
       <c r="A11" s="1" t="n">
@@ -4926,6 +4959,9 @@
       <c r="DT11" s="3" t="n">
         <v>127.6</v>
       </c>
+      <c r="DU11" s="1" t="n">
+        <v>144.6</v>
+      </c>
     </row>
     <row r="12" ht="20" customHeight="1">
       <c r="A12" s="1" t="n">
@@ -5300,6 +5336,9 @@
       <c r="DT12" s="1" t="n">
         <v>216.2</v>
       </c>
+      <c r="DU12" s="1" t="n">
+        <v>175.3</v>
+      </c>
     </row>
     <row r="13" ht="20" customHeight="1">
       <c r="A13" s="1" t="n">
@@ -5674,6 +5713,9 @@
       <c r="DT13" s="1" t="n">
         <v>142.8</v>
       </c>
+      <c r="DU13" s="3" t="n">
+        <v>137.7</v>
+      </c>
     </row>
     <row r="14" ht="20" customHeight="1">
       <c r="A14" s="1" t="n">
@@ -6048,6 +6090,9 @@
       <c r="DT14" s="1" t="n">
         <v>245.9</v>
       </c>
+      <c r="DU14" s="2" t="n">
+        <v>115.2</v>
+      </c>
     </row>
     <row r="15" ht="20" customHeight="1">
       <c r="A15" s="1" t="n">
@@ -6422,6 +6467,9 @@
       <c r="DT15" s="3" t="n">
         <v>134.2</v>
       </c>
+      <c r="DU15" s="1" t="n">
+        <v>199</v>
+      </c>
     </row>
     <row r="16" ht="20" customHeight="1">
       <c r="A16" s="1" t="n">
@@ -6796,6 +6844,9 @@
       <c r="DT16" s="1" t="n">
         <v>154.7</v>
       </c>
+      <c r="DU16" s="1" t="n">
+        <v>149.5</v>
+      </c>
     </row>
     <row r="17" ht="20" customHeight="1">
       <c r="A17" s="1" t="n">
@@ -7170,6 +7221,9 @@
       <c r="DT17" s="1" t="n">
         <v>232.7</v>
       </c>
+      <c r="DU17" s="1" t="n">
+        <v>190.4</v>
+      </c>
     </row>
     <row r="18" ht="20" customHeight="1">
       <c r="A18" s="1" t="n">
@@ -7544,6 +7598,9 @@
       <c r="DT18" s="3" t="n">
         <v>133.7</v>
       </c>
+      <c r="DU18" s="1" t="n">
+        <v>162.6</v>
+      </c>
     </row>
     <row r="19" ht="20" customHeight="1">
       <c r="A19" s="1" t="n">
@@ -7918,6 +7975,9 @@
       <c r="DT19" s="1" t="n">
         <v>162.1</v>
       </c>
+      <c r="DU19" s="1" t="n">
+        <v>160.8</v>
+      </c>
     </row>
     <row r="20" ht="20" customHeight="1">
       <c r="A20" s="1" t="n">
@@ -8292,6 +8352,9 @@
       <c r="DT20" s="1" t="n">
         <v>156.4</v>
       </c>
+      <c r="DU20" s="1" t="n">
+        <v>207.5</v>
+      </c>
     </row>
     <row r="21" ht="20" customHeight="1">
       <c r="A21" s="1" t="n">
@@ -8666,6 +8729,9 @@
       <c r="DT21" s="1" t="n">
         <v>147.3</v>
       </c>
+      <c r="DU21" s="3" t="n">
+        <v>138.5</v>
+      </c>
     </row>
     <row r="22" ht="20" customHeight="1">
       <c r="A22" s="1" t="n">
@@ -9040,6 +9106,9 @@
       <c r="DT22" s="1" t="n">
         <v>173.9</v>
       </c>
+      <c r="DU22" s="2" t="n">
+        <v>117.9</v>
+      </c>
     </row>
     <row r="23" ht="20" customHeight="1">
       <c r="A23" s="1" t="n">
@@ -9414,6 +9483,9 @@
       <c r="DT23" s="3" t="n">
         <v>135.4</v>
       </c>
+      <c r="DU23" s="1" t="n">
+        <v>159.3</v>
+      </c>
     </row>
     <row r="24" ht="20" customHeight="1">
       <c r="A24" s="1" t="n">
@@ -9788,6 +9860,9 @@
       <c r="DT24" s="1" t="n">
         <v>163.4</v>
       </c>
+      <c r="DU24" s="3" t="n">
+        <v>133.8</v>
+      </c>
     </row>
     <row r="25" ht="20" customHeight="1">
       <c r="A25" s="1" t="n">
@@ -10162,6 +10237,9 @@
       <c r="DT25" s="1" t="n">
         <v>178</v>
       </c>
+      <c r="DU25" s="3" t="n">
+        <v>131.1</v>
+      </c>
     </row>
     <row r="26" ht="20" customHeight="1">
       <c r="A26" s="1" t="n">
@@ -10536,6 +10614,9 @@
       <c r="DT26" s="2" t="n">
         <v>118.2</v>
       </c>
+      <c r="DU26" s="3" t="n">
+        <v>139.8</v>
+      </c>
     </row>
     <row r="27" ht="20" customHeight="1">
       <c r="A27" s="1" t="n">
@@ -10910,6 +10991,9 @@
       <c r="DT27" s="1" t="n">
         <v>177.5</v>
       </c>
+      <c r="DU27" s="1" t="n">
+        <v>190.3</v>
+      </c>
     </row>
     <row r="28" ht="20" customHeight="1">
       <c r="A28" s="1" t="n">
@@ -11284,6 +11368,9 @@
       <c r="DT28" s="3" t="n">
         <v>129</v>
       </c>
+      <c r="DU28" s="1" t="n">
+        <v>213.6</v>
+      </c>
     </row>
     <row r="29" ht="20" customHeight="1">
       <c r="A29" s="1" t="n">
@@ -11658,6 +11745,9 @@
       <c r="DT29" s="1" t="n">
         <v>209.3</v>
       </c>
+      <c r="DU29" s="1" t="n">
+        <v>160.6</v>
+      </c>
     </row>
     <row r="30" ht="20" customHeight="1">
       <c r="A30" s="1" t="n">
@@ -12032,6 +12122,9 @@
       <c r="DT30" s="2" t="n">
         <v>123.5</v>
       </c>
+      <c r="DU30" s="1" t="n">
+        <v>176.1</v>
+      </c>
     </row>
     <row r="31" ht="20" customHeight="1">
       <c r="A31" s="1" t="n">
@@ -12406,6 +12499,9 @@
       <c r="DT31" s="2" t="n">
         <v>122.3</v>
       </c>
+      <c r="DU31" s="1" t="n">
+        <v>147.9</v>
+      </c>
     </row>
     <row r="32" ht="20" customHeight="1">
       <c r="A32" s="1" t="n">
@@ -12780,6 +12876,9 @@
       <c r="DT32" s="1" t="n">
         <v>164.2</v>
       </c>
+      <c r="DU32" s="1" t="n">
+        <v>174.9</v>
+      </c>
     </row>
     <row r="33" ht="20" customHeight="1">
       <c r="A33" s="1" t="n">
@@ -13154,6 +13253,9 @@
       <c r="DT33" s="1" t="n">
         <v>146.1</v>
       </c>
+      <c r="DU33" s="1" t="n">
+        <v>221.8</v>
+      </c>
     </row>
     <row r="34" ht="20" customHeight="1">
       <c r="A34" s="1" t="n">
@@ -13528,6 +13630,9 @@
       <c r="DT34" s="1" t="n">
         <v>173.1</v>
       </c>
+      <c r="DU34" s="1" t="n">
+        <v>175.9</v>
+      </c>
     </row>
     <row r="35" ht="20" customHeight="1">
       <c r="A35" s="1" t="n">
@@ -13902,6 +14007,9 @@
       <c r="DT35" s="1" t="n">
         <v>140.7</v>
       </c>
+      <c r="DU35" s="2" t="n">
+        <v>124.9</v>
+      </c>
     </row>
     <row r="36" ht="20" customHeight="1">
       <c r="A36" s="1" t="n">
@@ -14276,6 +14384,9 @@
       <c r="DT36" s="1" t="n">
         <v>166.7</v>
       </c>
+      <c r="DU36" s="1" t="n">
+        <v>150.1</v>
+      </c>
     </row>
     <row r="37" ht="20" customHeight="1">
       <c r="A37" s="1" t="n">
@@ -14650,6 +14761,9 @@
       <c r="DT37" s="1" t="n">
         <v>262.8</v>
       </c>
+      <c r="DU37" s="1" t="n">
+        <v>140.9</v>
+      </c>
     </row>
     <row r="38" ht="20" customHeight="1">
       <c r="A38" s="1" t="n">
@@ -15024,6 +15138,9 @@
       <c r="DT38" s="1" t="n">
         <v>159.6</v>
       </c>
+      <c r="DU38" s="2" t="n">
+        <v>118.8</v>
+      </c>
     </row>
     <row r="39" ht="20" customHeight="1">
       <c r="A39" s="1" t="n">
@@ -15398,6 +15515,9 @@
       <c r="DT39" s="3" t="n">
         <v>128</v>
       </c>
+      <c r="DU39" s="1" t="n">
+        <v>167.5</v>
+      </c>
     </row>
     <row r="40" ht="20" customHeight="1">
       <c r="A40" s="1" t="n">
@@ -15772,6 +15892,9 @@
       <c r="DT40" s="1" t="n">
         <v>142.2</v>
       </c>
+      <c r="DU40" s="3" t="n">
+        <v>134.9</v>
+      </c>
     </row>
     <row r="41" ht="20" customHeight="1">
       <c r="A41" s="1" t="n">
@@ -16145,6 +16268,9 @@
       </c>
       <c r="DT41" s="1" t="n">
         <v>152.5</v>
+      </c>
+      <c r="DU41" s="1" t="n">
+        <v>212.8</v>
       </c>
     </row>
     <row r="42" ht="20" customHeight="1">
@@ -16482,6 +16608,7 @@
       <c r="DR42" s="1" t="n"/>
       <c r="DS42" s="1" t="n"/>
       <c r="DT42" s="1" t="n"/>
+      <c r="DU42" s="1" t="n"/>
     </row>
     <row r="43" ht="20" customHeight="1">
       <c r="A43" s="1" t="n">
@@ -16818,6 +16945,7 @@
       <c r="DR43" s="1" t="n"/>
       <c r="DS43" s="1" t="n"/>
       <c r="DT43" s="1" t="n"/>
+      <c r="DU43" s="1" t="n"/>
     </row>
     <row r="44" ht="20" customHeight="1">
       <c r="A44" s="1" t="n">
@@ -17192,6 +17320,9 @@
       <c r="DT44" s="1" t="n">
         <v>161.1</v>
       </c>
+      <c r="DU44" s="1" t="n">
+        <v>147.8</v>
+      </c>
     </row>
     <row r="45" ht="20" customHeight="1">
       <c r="A45" s="1" t="n">
@@ -17566,6 +17697,9 @@
       <c r="DT45" s="1" t="n">
         <v>181.2</v>
       </c>
+      <c r="DU45" s="1" t="n">
+        <v>148.3</v>
+      </c>
     </row>
     <row r="46" ht="20" customHeight="1">
       <c r="A46" s="1" t="n">
@@ -17940,6 +18074,9 @@
       <c r="DT46" s="1" t="n">
         <v>144.6</v>
       </c>
+      <c r="DU46" s="1" t="n">
+        <v>151.5</v>
+      </c>
     </row>
     <row r="47" ht="20" customHeight="1">
       <c r="A47" s="1" t="n">
@@ -18314,6 +18451,9 @@
       <c r="DT47" s="3" t="n">
         <v>136</v>
       </c>
+      <c r="DU47" s="3" t="n">
+        <v>135.8</v>
+      </c>
     </row>
     <row r="48" ht="20" customHeight="1">
       <c r="A48" s="1" t="n">
@@ -18688,6 +18828,9 @@
       <c r="DT48" s="1" t="n">
         <v>159.2</v>
       </c>
+      <c r="DU48" s="3" t="n">
+        <v>133.1</v>
+      </c>
     </row>
     <row r="49" ht="20" customHeight="1">
       <c r="A49" s="1" t="n">
@@ -19062,6 +19205,9 @@
       <c r="DT49" s="1" t="n">
         <v>143.6</v>
       </c>
+      <c r="DU49" s="1" t="n">
+        <v>169.5</v>
+      </c>
     </row>
     <row r="50" ht="20" customHeight="1">
       <c r="A50" s="1" t="n">
@@ -19436,6 +19582,9 @@
       <c r="DT50" s="1" t="n">
         <v>162.3</v>
       </c>
+      <c r="DU50" s="1" t="n">
+        <v>152.4</v>
+      </c>
     </row>
     <row r="51" ht="20" customHeight="1">
       <c r="A51" s="1" t="n">
@@ -19810,6 +19959,9 @@
       <c r="DT51" s="1" t="n">
         <v>145.6</v>
       </c>
+      <c r="DU51" s="1" t="n">
+        <v>155.5</v>
+      </c>
     </row>
     <row r="52" ht="20" customHeight="1">
       <c r="A52" s="1" t="n">
@@ -20184,6 +20336,9 @@
       <c r="DT52" s="1" t="n">
         <v>223.1</v>
       </c>
+      <c r="DU52" s="3" t="n">
+        <v>139.2</v>
+      </c>
     </row>
     <row r="53" ht="20" customHeight="1">
       <c r="A53" s="1" t="n">
@@ -20557,6 +20712,9 @@
       </c>
       <c r="DT53" s="3" t="n">
         <v>132.2</v>
+      </c>
+      <c r="DU53" s="1" t="n">
+        <v>149.3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2025-01-12
</commit_message>
<xml_diff>
--- a/マイジャグラーV_塗りつぶし済み.xlsx
+++ b/マイジャグラーV_塗りつぶし済み.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:DU53"/>
+  <dimension ref="A1:DV53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -564,6 +564,7 @@
     <col width="12" customWidth="1" min="123" max="123"/>
     <col width="12" customWidth="1" min="124" max="124"/>
     <col width="12" customWidth="1" min="125" max="125"/>
+    <col width="12" customWidth="1" min="126" max="126"/>
   </cols>
   <sheetData>
     <row r="1" ht="20" customHeight="1">
@@ -1192,6 +1193,11 @@
           <t>2025/01/11</t>
         </is>
       </c>
+      <c r="DV1" s="1" t="inlineStr">
+        <is>
+          <t>2025/01/12</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="20" customHeight="1">
       <c r="A2" s="1" t="n">
@@ -1569,6 +1575,9 @@
       <c r="DU2" s="1" t="n">
         <v>178</v>
       </c>
+      <c r="DV2" s="1" t="n">
+        <v>151.1</v>
+      </c>
     </row>
     <row r="3" ht="20" customHeight="1">
       <c r="A3" s="1" t="n">
@@ -1946,6 +1955,9 @@
       <c r="DU3" s="1" t="n">
         <v>204.4</v>
       </c>
+      <c r="DV3" s="1" t="n">
+        <v>196.9</v>
+      </c>
     </row>
     <row r="4" ht="20" customHeight="1">
       <c r="A4" s="1" t="n">
@@ -2323,6 +2335,9 @@
       <c r="DU4" s="1" t="n">
         <v>152.8</v>
       </c>
+      <c r="DV4" s="1" t="n">
+        <v>156.6</v>
+      </c>
     </row>
     <row r="5" ht="20" customHeight="1">
       <c r="A5" s="1" t="n">
@@ -2700,6 +2715,9 @@
       <c r="DU5" s="1" t="n">
         <v>179.7</v>
       </c>
+      <c r="DV5" s="3" t="n">
+        <v>129.5</v>
+      </c>
     </row>
     <row r="6" ht="20" customHeight="1">
       <c r="A6" s="1" t="n">
@@ -3077,6 +3095,9 @@
       <c r="DU6" s="3" t="n">
         <v>131.1</v>
       </c>
+      <c r="DV6" s="1" t="n">
+        <v>147.2</v>
+      </c>
     </row>
     <row r="7" ht="20" customHeight="1">
       <c r="A7" s="1" t="n">
@@ -3454,6 +3475,9 @@
       <c r="DU7" s="1" t="n">
         <v>154.7</v>
       </c>
+      <c r="DV7" s="1" t="n">
+        <v>160.4</v>
+      </c>
     </row>
     <row r="8" ht="20" customHeight="1">
       <c r="A8" s="1" t="n">
@@ -3831,6 +3855,9 @@
       <c r="DU8" s="3" t="n">
         <v>138</v>
       </c>
+      <c r="DV8" s="1" t="n">
+        <v>151.8</v>
+      </c>
     </row>
     <row r="9" ht="20" customHeight="1">
       <c r="A9" s="1" t="n">
@@ -4208,6 +4235,9 @@
       <c r="DU9" s="1" t="n">
         <v>144.8</v>
       </c>
+      <c r="DV9" s="3" t="n">
+        <v>136.2</v>
+      </c>
     </row>
     <row r="10" ht="20" customHeight="1">
       <c r="A10" s="1" t="n">
@@ -4585,6 +4615,9 @@
       <c r="DU10" s="1" t="n">
         <v>157.2</v>
       </c>
+      <c r="DV10" s="1" t="n">
+        <v>184.9</v>
+      </c>
     </row>
     <row r="11" ht="20" customHeight="1">
       <c r="A11" s="1" t="n">
@@ -4962,6 +4995,9 @@
       <c r="DU11" s="1" t="n">
         <v>144.6</v>
       </c>
+      <c r="DV11" s="1" t="n">
+        <v>229.2</v>
+      </c>
     </row>
     <row r="12" ht="20" customHeight="1">
       <c r="A12" s="1" t="n">
@@ -5339,6 +5375,9 @@
       <c r="DU12" s="1" t="n">
         <v>175.3</v>
       </c>
+      <c r="DV12" s="1" t="n">
+        <v>143.2</v>
+      </c>
     </row>
     <row r="13" ht="20" customHeight="1">
       <c r="A13" s="1" t="n">
@@ -5716,6 +5755,9 @@
       <c r="DU13" s="3" t="n">
         <v>137.7</v>
       </c>
+      <c r="DV13" s="3" t="n">
+        <v>139</v>
+      </c>
     </row>
     <row r="14" ht="20" customHeight="1">
       <c r="A14" s="1" t="n">
@@ -6093,6 +6135,9 @@
       <c r="DU14" s="2" t="n">
         <v>115.2</v>
       </c>
+      <c r="DV14" s="1" t="n">
+        <v>155.4</v>
+      </c>
     </row>
     <row r="15" ht="20" customHeight="1">
       <c r="A15" s="1" t="n">
@@ -6470,6 +6515,9 @@
       <c r="DU15" s="1" t="n">
         <v>199</v>
       </c>
+      <c r="DV15" s="1" t="n">
+        <v>152.7</v>
+      </c>
     </row>
     <row r="16" ht="20" customHeight="1">
       <c r="A16" s="1" t="n">
@@ -6847,6 +6895,9 @@
       <c r="DU16" s="1" t="n">
         <v>149.5</v>
       </c>
+      <c r="DV16" s="3" t="n">
+        <v>133.6</v>
+      </c>
     </row>
     <row r="17" ht="20" customHeight="1">
       <c r="A17" s="1" t="n">
@@ -7224,6 +7275,9 @@
       <c r="DU17" s="1" t="n">
         <v>190.4</v>
       </c>
+      <c r="DV17" s="1" t="n">
+        <v>155</v>
+      </c>
     </row>
     <row r="18" ht="20" customHeight="1">
       <c r="A18" s="1" t="n">
@@ -7601,6 +7655,9 @@
       <c r="DU18" s="1" t="n">
         <v>162.6</v>
       </c>
+      <c r="DV18" s="3" t="n">
+        <v>132.9</v>
+      </c>
     </row>
     <row r="19" ht="20" customHeight="1">
       <c r="A19" s="1" t="n">
@@ -7978,6 +8035,9 @@
       <c r="DU19" s="1" t="n">
         <v>160.8</v>
       </c>
+      <c r="DV19" s="3" t="n">
+        <v>129.5</v>
+      </c>
     </row>
     <row r="20" ht="20" customHeight="1">
       <c r="A20" s="1" t="n">
@@ -8355,6 +8415,9 @@
       <c r="DU20" s="1" t="n">
         <v>207.5</v>
       </c>
+      <c r="DV20" s="1" t="n">
+        <v>170.5</v>
+      </c>
     </row>
     <row r="21" ht="20" customHeight="1">
       <c r="A21" s="1" t="n">
@@ -8732,6 +8795,9 @@
       <c r="DU21" s="3" t="n">
         <v>138.5</v>
       </c>
+      <c r="DV21" s="3" t="n">
+        <v>135.8</v>
+      </c>
     </row>
     <row r="22" ht="20" customHeight="1">
       <c r="A22" s="1" t="n">
@@ -9109,6 +9175,9 @@
       <c r="DU22" s="2" t="n">
         <v>117.9</v>
       </c>
+      <c r="DV22" s="1" t="n">
+        <v>161.1</v>
+      </c>
     </row>
     <row r="23" ht="20" customHeight="1">
       <c r="A23" s="1" t="n">
@@ -9486,6 +9555,9 @@
       <c r="DU23" s="1" t="n">
         <v>159.3</v>
       </c>
+      <c r="DV23" s="1" t="n">
+        <v>208.4</v>
+      </c>
     </row>
     <row r="24" ht="20" customHeight="1">
       <c r="A24" s="1" t="n">
@@ -9863,6 +9935,9 @@
       <c r="DU24" s="3" t="n">
         <v>133.8</v>
       </c>
+      <c r="DV24" s="1" t="n">
+        <v>194.7</v>
+      </c>
     </row>
     <row r="25" ht="20" customHeight="1">
       <c r="A25" s="1" t="n">
@@ -10240,6 +10315,9 @@
       <c r="DU25" s="3" t="n">
         <v>131.1</v>
       </c>
+      <c r="DV25" s="3" t="n">
+        <v>131.1</v>
+      </c>
     </row>
     <row r="26" ht="20" customHeight="1">
       <c r="A26" s="1" t="n">
@@ -10617,6 +10695,9 @@
       <c r="DU26" s="3" t="n">
         <v>139.8</v>
       </c>
+      <c r="DV26" s="1" t="n">
+        <v>191.9</v>
+      </c>
     </row>
     <row r="27" ht="20" customHeight="1">
       <c r="A27" s="1" t="n">
@@ -10994,6 +11075,9 @@
       <c r="DU27" s="1" t="n">
         <v>190.3</v>
       </c>
+      <c r="DV27" s="1" t="n">
+        <v>190.2</v>
+      </c>
     </row>
     <row r="28" ht="20" customHeight="1">
       <c r="A28" s="1" t="n">
@@ -11371,6 +11455,9 @@
       <c r="DU28" s="1" t="n">
         <v>213.6</v>
       </c>
+      <c r="DV28" s="1" t="n">
+        <v>161.1</v>
+      </c>
     </row>
     <row r="29" ht="20" customHeight="1">
       <c r="A29" s="1" t="n">
@@ -11748,6 +11835,9 @@
       <c r="DU29" s="1" t="n">
         <v>160.6</v>
       </c>
+      <c r="DV29" s="1" t="n">
+        <v>161.8</v>
+      </c>
     </row>
     <row r="30" ht="20" customHeight="1">
       <c r="A30" s="1" t="n">
@@ -12125,6 +12215,9 @@
       <c r="DU30" s="1" t="n">
         <v>176.1</v>
       </c>
+      <c r="DV30" s="1" t="n">
+        <v>152.5</v>
+      </c>
     </row>
     <row r="31" ht="20" customHeight="1">
       <c r="A31" s="1" t="n">
@@ -12502,6 +12595,9 @@
       <c r="DU31" s="1" t="n">
         <v>147.9</v>
       </c>
+      <c r="DV31" s="3" t="n">
+        <v>136.1</v>
+      </c>
     </row>
     <row r="32" ht="20" customHeight="1">
       <c r="A32" s="1" t="n">
@@ -12879,6 +12975,9 @@
       <c r="DU32" s="1" t="n">
         <v>174.9</v>
       </c>
+      <c r="DV32" s="1" t="n">
+        <v>158.8</v>
+      </c>
     </row>
     <row r="33" ht="20" customHeight="1">
       <c r="A33" s="1" t="n">
@@ -13256,6 +13355,9 @@
       <c r="DU33" s="1" t="n">
         <v>221.8</v>
       </c>
+      <c r="DV33" s="3" t="n">
+        <v>126.1</v>
+      </c>
     </row>
     <row r="34" ht="20" customHeight="1">
       <c r="A34" s="1" t="n">
@@ -13633,6 +13735,9 @@
       <c r="DU34" s="1" t="n">
         <v>175.9</v>
       </c>
+      <c r="DV34" s="2" t="n">
+        <v>117.6</v>
+      </c>
     </row>
     <row r="35" ht="20" customHeight="1">
       <c r="A35" s="1" t="n">
@@ -14010,6 +14115,9 @@
       <c r="DU35" s="2" t="n">
         <v>124.9</v>
       </c>
+      <c r="DV35" s="1" t="n">
+        <v>209.1</v>
+      </c>
     </row>
     <row r="36" ht="20" customHeight="1">
       <c r="A36" s="1" t="n">
@@ -14387,6 +14495,9 @@
       <c r="DU36" s="1" t="n">
         <v>150.1</v>
       </c>
+      <c r="DV36" s="1" t="n">
+        <v>180.6</v>
+      </c>
     </row>
     <row r="37" ht="20" customHeight="1">
       <c r="A37" s="1" t="n">
@@ -14764,6 +14875,9 @@
       <c r="DU37" s="1" t="n">
         <v>140.9</v>
       </c>
+      <c r="DV37" s="3" t="n">
+        <v>136.7</v>
+      </c>
     </row>
     <row r="38" ht="20" customHeight="1">
       <c r="A38" s="1" t="n">
@@ -15141,6 +15255,9 @@
       <c r="DU38" s="2" t="n">
         <v>118.8</v>
       </c>
+      <c r="DV38" s="3" t="n">
+        <v>130.5</v>
+      </c>
     </row>
     <row r="39" ht="20" customHeight="1">
       <c r="A39" s="1" t="n">
@@ -15518,6 +15635,9 @@
       <c r="DU39" s="1" t="n">
         <v>167.5</v>
       </c>
+      <c r="DV39" s="1" t="n">
+        <v>203.8</v>
+      </c>
     </row>
     <row r="40" ht="20" customHeight="1">
       <c r="A40" s="1" t="n">
@@ -15895,6 +16015,9 @@
       <c r="DU40" s="3" t="n">
         <v>134.9</v>
       </c>
+      <c r="DV40" s="3" t="n">
+        <v>138.2</v>
+      </c>
     </row>
     <row r="41" ht="20" customHeight="1">
       <c r="A41" s="1" t="n">
@@ -16271,6 +16394,9 @@
       </c>
       <c r="DU41" s="1" t="n">
         <v>212.8</v>
+      </c>
+      <c r="DV41" s="1" t="n">
+        <v>165.4</v>
       </c>
     </row>
     <row r="42" ht="20" customHeight="1">
@@ -16609,6 +16735,7 @@
       <c r="DS42" s="1" t="n"/>
       <c r="DT42" s="1" t="n"/>
       <c r="DU42" s="1" t="n"/>
+      <c r="DV42" s="1" t="n"/>
     </row>
     <row r="43" ht="20" customHeight="1">
       <c r="A43" s="1" t="n">
@@ -16946,6 +17073,7 @@
       <c r="DS43" s="1" t="n"/>
       <c r="DT43" s="1" t="n"/>
       <c r="DU43" s="1" t="n"/>
+      <c r="DV43" s="1" t="n"/>
     </row>
     <row r="44" ht="20" customHeight="1">
       <c r="A44" s="1" t="n">
@@ -17323,6 +17451,9 @@
       <c r="DU44" s="1" t="n">
         <v>147.8</v>
       </c>
+      <c r="DV44" s="1" t="n">
+        <v>169.6</v>
+      </c>
     </row>
     <row r="45" ht="20" customHeight="1">
       <c r="A45" s="1" t="n">
@@ -17700,6 +17831,9 @@
       <c r="DU45" s="1" t="n">
         <v>148.3</v>
       </c>
+      <c r="DV45" s="1" t="n">
+        <v>172.4</v>
+      </c>
     </row>
     <row r="46" ht="20" customHeight="1">
       <c r="A46" s="1" t="n">
@@ -18077,6 +18211,9 @@
       <c r="DU46" s="1" t="n">
         <v>151.5</v>
       </c>
+      <c r="DV46" s="1" t="n">
+        <v>147.6</v>
+      </c>
     </row>
     <row r="47" ht="20" customHeight="1">
       <c r="A47" s="1" t="n">
@@ -18454,6 +18591,9 @@
       <c r="DU47" s="3" t="n">
         <v>135.8</v>
       </c>
+      <c r="DV47" s="1" t="n">
+        <v>148.3</v>
+      </c>
     </row>
     <row r="48" ht="20" customHeight="1">
       <c r="A48" s="1" t="n">
@@ -18831,6 +18971,9 @@
       <c r="DU48" s="3" t="n">
         <v>133.1</v>
       </c>
+      <c r="DV48" s="1" t="n">
+        <v>217.9</v>
+      </c>
     </row>
     <row r="49" ht="20" customHeight="1">
       <c r="A49" s="1" t="n">
@@ -19208,6 +19351,9 @@
       <c r="DU49" s="1" t="n">
         <v>169.5</v>
       </c>
+      <c r="DV49" s="3" t="n">
+        <v>138.6</v>
+      </c>
     </row>
     <row r="50" ht="20" customHeight="1">
       <c r="A50" s="1" t="n">
@@ -19585,6 +19731,9 @@
       <c r="DU50" s="1" t="n">
         <v>152.4</v>
       </c>
+      <c r="DV50" s="3" t="n">
+        <v>126.9</v>
+      </c>
     </row>
     <row r="51" ht="20" customHeight="1">
       <c r="A51" s="1" t="n">
@@ -19962,6 +20111,9 @@
       <c r="DU51" s="1" t="n">
         <v>155.5</v>
       </c>
+      <c r="DV51" s="1" t="n">
+        <v>154</v>
+      </c>
     </row>
     <row r="52" ht="20" customHeight="1">
       <c r="A52" s="1" t="n">
@@ -20339,6 +20491,9 @@
       <c r="DU52" s="3" t="n">
         <v>139.2</v>
       </c>
+      <c r="DV52" s="1" t="n">
+        <v>146</v>
+      </c>
     </row>
     <row r="53" ht="20" customHeight="1">
       <c r="A53" s="1" t="n">
@@ -20715,6 +20870,9 @@
       </c>
       <c r="DU53" s="1" t="n">
         <v>149.3</v>
+      </c>
+      <c r="DV53" s="2" t="n">
+        <v>122.9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2025-03-28
</commit_message>
<xml_diff>
--- a/マイジャグラーV_塗りつぶし済み.xlsx
+++ b/マイジャグラーV_塗りつぶし済み.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:FP51"/>
+  <dimension ref="A1:FQ51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -611,6 +611,7 @@
     <col width="12" customWidth="1" min="170" max="170"/>
     <col width="12" customWidth="1" min="171" max="171"/>
     <col width="12" customWidth="1" min="172" max="172"/>
+    <col width="12" customWidth="1" min="173" max="173"/>
   </cols>
   <sheetData>
     <row r="1" ht="20" customHeight="1">
@@ -1474,6 +1475,11 @@
           <t>2025/02/27</t>
         </is>
       </c>
+      <c r="FQ1" s="1" t="inlineStr">
+        <is>
+          <t>2025/03/28</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="20" customHeight="1">
       <c r="A2" s="1" t="n">
@@ -1992,6 +1998,9 @@
       <c r="FP2" s="1" t="n">
         <v>178.8</v>
       </c>
+      <c r="FQ2" s="1" t="n">
+        <v>149.3</v>
+      </c>
     </row>
     <row r="3" ht="20" customHeight="1">
       <c r="A3" s="1" t="n">
@@ -2510,6 +2519,9 @@
       <c r="FP3" s="1" t="n">
         <v>191.4</v>
       </c>
+      <c r="FQ3" s="1" t="n">
+        <v>184</v>
+      </c>
     </row>
     <row r="4" ht="20" customHeight="1">
       <c r="A4" s="1" t="n">
@@ -3028,6 +3040,9 @@
       <c r="FP4" s="1" t="n">
         <v>177.6</v>
       </c>
+      <c r="FQ4" s="3" t="n">
+        <v>134.1</v>
+      </c>
     </row>
     <row r="5" ht="20" customHeight="1">
       <c r="A5" s="1" t="n">
@@ -3546,6 +3561,9 @@
       <c r="FP5" s="1" t="n">
         <v>201.6</v>
       </c>
+      <c r="FQ5" s="3" t="n">
+        <v>126.3</v>
+      </c>
     </row>
     <row r="6" ht="20" customHeight="1">
       <c r="A6" s="1" t="n">
@@ -4064,6 +4082,9 @@
       <c r="FP6" s="1" t="n">
         <v>145.9</v>
       </c>
+      <c r="FQ6" s="1" t="n">
+        <v>155.6</v>
+      </c>
     </row>
     <row r="7" ht="20" customHeight="1">
       <c r="A7" s="1" t="n">
@@ -4582,6 +4603,9 @@
       <c r="FP7" s="1" t="n">
         <v>141.1</v>
       </c>
+      <c r="FQ7" s="1" t="n">
+        <v>161.1</v>
+      </c>
     </row>
     <row r="8" ht="20" customHeight="1">
       <c r="A8" s="1" t="n">
@@ -5100,6 +5124,9 @@
       <c r="FP8" s="3" t="n">
         <v>139.2</v>
       </c>
+      <c r="FQ8" s="2" t="n">
+        <v>116.2</v>
+      </c>
     </row>
     <row r="9" ht="20" customHeight="1">
       <c r="A9" s="1" t="n">
@@ -5618,6 +5645,9 @@
       <c r="FP9" s="2" t="n">
         <v>124.9</v>
       </c>
+      <c r="FQ9" s="1" t="n">
+        <v>148.3</v>
+      </c>
     </row>
     <row r="10" ht="20" customHeight="1">
       <c r="A10" s="1" t="n">
@@ -6136,6 +6166,9 @@
       <c r="FP10" s="1" t="n">
         <v>168.4</v>
       </c>
+      <c r="FQ10" s="1" t="n">
+        <v>167.1</v>
+      </c>
     </row>
     <row r="11" ht="20" customHeight="1">
       <c r="A11" s="1" t="n">
@@ -6654,6 +6687,9 @@
       <c r="FP11" s="1" t="n">
         <v>167.2</v>
       </c>
+      <c r="FQ11" s="1" t="n">
+        <v>170.5</v>
+      </c>
     </row>
     <row r="12" ht="20" customHeight="1">
       <c r="A12" s="1" t="n">
@@ -7172,6 +7208,9 @@
       <c r="FP12" s="1" t="n">
         <v>153.5</v>
       </c>
+      <c r="FQ12" s="3" t="n">
+        <v>130.7</v>
+      </c>
     </row>
     <row r="13" ht="20" customHeight="1">
       <c r="A13" s="1" t="n">
@@ -7690,6 +7729,9 @@
       <c r="FP13" s="1" t="n">
         <v>219.2</v>
       </c>
+      <c r="FQ13" s="2" t="n">
+        <v>124.3</v>
+      </c>
     </row>
     <row r="14" ht="20" customHeight="1">
       <c r="A14" s="1" t="n">
@@ -8208,6 +8250,9 @@
       <c r="FP14" s="1" t="n">
         <v>191.3</v>
       </c>
+      <c r="FQ14" s="1" t="n">
+        <v>146</v>
+      </c>
     </row>
     <row r="15" ht="20" customHeight="1">
       <c r="A15" s="1" t="n">
@@ -8726,6 +8771,9 @@
       <c r="FP15" s="1" t="n">
         <v>174.5</v>
       </c>
+      <c r="FQ15" s="1" t="n">
+        <v>153.5</v>
+      </c>
     </row>
     <row r="16" ht="20" customHeight="1">
       <c r="A16" s="1" t="n">
@@ -9244,6 +9292,9 @@
       <c r="FP16" s="1" t="n">
         <v>168.7</v>
       </c>
+      <c r="FQ16" s="1" t="n">
+        <v>155.3</v>
+      </c>
     </row>
     <row r="17" ht="20" customHeight="1">
       <c r="A17" s="1" t="n">
@@ -9762,6 +9813,9 @@
       <c r="FP17" s="2" t="n">
         <v>120.6</v>
       </c>
+      <c r="FQ17" s="1" t="n">
+        <v>224.5</v>
+      </c>
     </row>
     <row r="18" ht="20" customHeight="1">
       <c r="A18" s="1" t="n">
@@ -10280,6 +10334,9 @@
       <c r="FP18" s="1" t="n">
         <v>170.1</v>
       </c>
+      <c r="FQ18" s="1" t="n">
+        <v>174.9</v>
+      </c>
     </row>
     <row r="19" ht="20" customHeight="1">
       <c r="A19" s="1" t="n">
@@ -10798,6 +10855,9 @@
       <c r="FP19" s="2" t="n">
         <v>116</v>
       </c>
+      <c r="FQ19" s="1" t="n">
+        <v>212.1</v>
+      </c>
     </row>
     <row r="20" ht="20" customHeight="1">
       <c r="A20" s="1" t="n">
@@ -11316,6 +11376,9 @@
       <c r="FP20" s="1" t="n">
         <v>155.8</v>
       </c>
+      <c r="FQ20" s="1" t="n">
+        <v>143.3</v>
+      </c>
     </row>
     <row r="21" ht="20" customHeight="1">
       <c r="A21" s="1" t="n">
@@ -11834,6 +11897,9 @@
       <c r="FP21" s="1" t="n">
         <v>165.7</v>
       </c>
+      <c r="FQ21" s="1" t="n">
+        <v>179.5</v>
+      </c>
     </row>
     <row r="22" ht="20" customHeight="1">
       <c r="A22" s="1" t="n">
@@ -12352,6 +12418,9 @@
       <c r="FP22" s="1" t="n">
         <v>156.8</v>
       </c>
+      <c r="FQ22" s="1" t="n">
+        <v>278.4</v>
+      </c>
     </row>
     <row r="23" ht="20" customHeight="1">
       <c r="A23" s="1" t="n">
@@ -12870,6 +12939,9 @@
       <c r="FP23" s="1" t="n">
         <v>166.5</v>
       </c>
+      <c r="FQ23" s="2" t="n">
+        <v>109.5</v>
+      </c>
     </row>
     <row r="24" ht="20" customHeight="1">
       <c r="A24" s="1" t="n">
@@ -13388,6 +13460,9 @@
       <c r="FP24" s="1" t="n">
         <v>174.6</v>
       </c>
+      <c r="FQ24" s="2" t="n">
+        <v>120.2</v>
+      </c>
     </row>
     <row r="25" ht="20" customHeight="1">
       <c r="A25" s="1" t="n">
@@ -13906,6 +13981,9 @@
       <c r="FP25" s="1" t="n">
         <v>153.4</v>
       </c>
+      <c r="FQ25" s="3" t="n">
+        <v>129.5</v>
+      </c>
     </row>
     <row r="26" ht="20" customHeight="1">
       <c r="A26" s="1" t="n">
@@ -14424,6 +14502,9 @@
       <c r="FP26" s="1" t="n">
         <v>151.8</v>
       </c>
+      <c r="FQ26" s="1" t="n">
+        <v>167.4</v>
+      </c>
     </row>
     <row r="27" ht="20" customHeight="1">
       <c r="A27" s="1" t="n">
@@ -14942,6 +15023,9 @@
       <c r="FP27" s="1" t="n">
         <v>147.7</v>
       </c>
+      <c r="FQ27" s="1" t="n">
+        <v>175.8</v>
+      </c>
     </row>
     <row r="28" ht="20" customHeight="1">
       <c r="A28" s="1" t="n">
@@ -15460,6 +15544,9 @@
       <c r="FP28" s="1" t="n">
         <v>189.3</v>
       </c>
+      <c r="FQ28" s="1" t="n">
+        <v>163.2</v>
+      </c>
     </row>
     <row r="29" ht="20" customHeight="1">
       <c r="A29" s="1" t="n">
@@ -15978,6 +16065,9 @@
       <c r="FP29" s="1" t="n">
         <v>156.7</v>
       </c>
+      <c r="FQ29" s="1" t="n">
+        <v>202.9</v>
+      </c>
     </row>
     <row r="30" ht="20" customHeight="1">
       <c r="A30" s="1" t="n">
@@ -16496,6 +16586,9 @@
       <c r="FP30" s="1" t="n">
         <v>153.1</v>
       </c>
+      <c r="FQ30" s="1" t="n">
+        <v>184.9</v>
+      </c>
     </row>
     <row r="31" ht="20" customHeight="1">
       <c r="A31" s="1" t="n">
@@ -17014,6 +17107,9 @@
       <c r="FP31" s="1" t="n">
         <v>196.4</v>
       </c>
+      <c r="FQ31" s="1" t="n">
+        <v>159</v>
+      </c>
     </row>
     <row r="32" ht="20" customHeight="1">
       <c r="A32" s="1" t="n">
@@ -17532,6 +17628,9 @@
       <c r="FP32" s="1" t="n">
         <v>163.4</v>
       </c>
+      <c r="FQ32" s="1" t="n">
+        <v>150</v>
+      </c>
     </row>
     <row r="33" ht="20" customHeight="1">
       <c r="A33" s="1" t="n">
@@ -18050,6 +18149,9 @@
       <c r="FP33" s="3" t="n">
         <v>133.9</v>
       </c>
+      <c r="FQ33" s="3" t="n">
+        <v>126.1</v>
+      </c>
     </row>
     <row r="34" ht="20" customHeight="1">
       <c r="A34" s="1" t="n">
@@ -18568,6 +18670,9 @@
       <c r="FP34" s="2" t="n">
         <v>112.6</v>
       </c>
+      <c r="FQ34" s="1" t="n">
+        <v>245.1</v>
+      </c>
     </row>
     <row r="35" ht="20" customHeight="1">
       <c r="A35" s="1" t="n">
@@ -19086,6 +19191,9 @@
       <c r="FP35" s="1" t="n">
         <v>155.4</v>
       </c>
+      <c r="FQ35" s="1" t="n">
+        <v>206.8</v>
+      </c>
     </row>
     <row r="36" ht="20" customHeight="1">
       <c r="A36" s="1" t="n">
@@ -19604,6 +19712,9 @@
       <c r="FP36" s="3" t="n">
         <v>130.9</v>
       </c>
+      <c r="FQ36" s="3" t="n">
+        <v>132.3</v>
+      </c>
     </row>
     <row r="37" ht="20" customHeight="1">
       <c r="A37" s="1" t="n">
@@ -20122,6 +20233,9 @@
       <c r="FP37" s="1" t="n">
         <v>157</v>
       </c>
+      <c r="FQ37" s="1" t="n">
+        <v>144.8</v>
+      </c>
     </row>
     <row r="38" ht="20" customHeight="1">
       <c r="A38" s="1" t="n">
@@ -20640,6 +20754,9 @@
       <c r="FP38" s="1" t="n">
         <v>163.8</v>
       </c>
+      <c r="FQ38" s="1" t="n">
+        <v>150</v>
+      </c>
     </row>
     <row r="39" ht="20" customHeight="1">
       <c r="A39" s="1" t="n">
@@ -21158,6 +21275,9 @@
       <c r="FP39" s="3" t="n">
         <v>131.7</v>
       </c>
+      <c r="FQ39" s="1" t="n">
+        <v>165.4</v>
+      </c>
     </row>
     <row r="40" ht="20" customHeight="1">
       <c r="A40" s="1" t="n">
@@ -21676,6 +21796,9 @@
       <c r="FP40" s="1" t="n">
         <v>146.6</v>
       </c>
+      <c r="FQ40" s="1" t="n">
+        <v>174.1</v>
+      </c>
     </row>
     <row r="41" ht="20" customHeight="1">
       <c r="A41" s="1" t="n">
@@ -22194,6 +22317,9 @@
       <c r="FP41" s="1" t="n">
         <v>184</v>
       </c>
+      <c r="FQ41" s="1" t="n">
+        <v>149.9</v>
+      </c>
     </row>
     <row r="42" ht="20" customHeight="1">
       <c r="A42" s="1" t="n">
@@ -22712,6 +22838,9 @@
       <c r="FP42" s="3" t="n">
         <v>127.8</v>
       </c>
+      <c r="FQ42" s="1" t="n">
+        <v>240.1</v>
+      </c>
     </row>
     <row r="43" ht="20" customHeight="1">
       <c r="A43" s="1" t="n">
@@ -23230,6 +23359,9 @@
       <c r="FP43" s="1" t="n">
         <v>226.2</v>
       </c>
+      <c r="FQ43" s="3" t="n">
+        <v>133.4</v>
+      </c>
     </row>
     <row r="44" ht="20" customHeight="1">
       <c r="A44" s="1" t="n">
@@ -23748,6 +23880,9 @@
       <c r="FP44" s="1" t="n">
         <v>148</v>
       </c>
+      <c r="FQ44" s="1" t="n">
+        <v>153.3</v>
+      </c>
     </row>
     <row r="45" ht="20" customHeight="1">
       <c r="A45" s="1" t="n">
@@ -24266,6 +24401,9 @@
       <c r="FP45" s="1" t="n">
         <v>172.9</v>
       </c>
+      <c r="FQ45" s="1" t="n">
+        <v>153</v>
+      </c>
     </row>
     <row r="46" ht="20" customHeight="1">
       <c r="A46" s="1" t="n">
@@ -24784,6 +24922,9 @@
       <c r="FP46" s="1" t="n">
         <v>163.7</v>
       </c>
+      <c r="FQ46" s="3" t="n">
+        <v>128.1</v>
+      </c>
     </row>
     <row r="47" ht="20" customHeight="1">
       <c r="A47" s="1" t="n">
@@ -25302,6 +25443,9 @@
       <c r="FP47" s="1" t="n">
         <v>156.1</v>
       </c>
+      <c r="FQ47" s="3" t="n">
+        <v>138.3</v>
+      </c>
     </row>
     <row r="48" ht="20" customHeight="1">
       <c r="A48" s="1" t="n">
@@ -25820,6 +25964,9 @@
       <c r="FP48" s="1" t="n">
         <v>152.6</v>
       </c>
+      <c r="FQ48" s="1" t="n">
+        <v>168.1</v>
+      </c>
     </row>
     <row r="49" ht="20" customHeight="1">
       <c r="A49" s="1" t="n">
@@ -26338,6 +26485,9 @@
       <c r="FP49" s="2" t="n">
         <v>123.3</v>
       </c>
+      <c r="FQ49" s="1" t="n">
+        <v>145.4</v>
+      </c>
     </row>
     <row r="50" ht="20" customHeight="1">
       <c r="A50" s="1" t="n">
@@ -26856,6 +27006,9 @@
       <c r="FP50" s="1" t="n">
         <v>141.7</v>
       </c>
+      <c r="FQ50" s="3" t="n">
+        <v>134.8</v>
+      </c>
     </row>
     <row r="51" ht="20" customHeight="1">
       <c r="A51" s="1" t="n">
@@ -27373,6 +27526,9 @@
       </c>
       <c r="FP51" s="1" t="n">
         <v>142.4</v>
+      </c>
+      <c r="FQ51" s="3" t="n">
+        <v>134</v>
       </c>
     </row>
   </sheetData>

</xml_diff>